<commit_message>
Shop Popup: Development - Full re-implementation of the popup and pills logic. Added offers tab support. Offers: Content - Added IAP sku field. Chests Screen: Refactor - Created own folder for scripts. Global Events Screen: Refactor - Created own folder for scripts.
Former-commit-id: c3e54635765b47b88a031ee72cabb53b65d8c312
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6A82CA15-AF8F-B94E-A079-912B071E57A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -152,12 +153,39 @@
   </si>
   <si>
     <t>endDate</t>
+  </si>
+  <si>
+    <t>[iapSku]</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_2</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_3</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_4</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_1</t>
+  </si>
+  <si>
+    <t>[tidName]</t>
+  </si>
+  <si>
+    <t>TID_OFFER_PACK_MEGA</t>
+  </si>
+  <si>
+    <t>TID_OFFER_PACK_SUPER</t>
+  </si>
+  <si>
+    <t>TID_OFFER_PACK_BASIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -279,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -359,11 +387,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -411,11 +465,169 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -887,83 +1099,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -978,20 +1113,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B4:L31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="B4:L31"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="10"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="8"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="7"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="6"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="5"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="4"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="3"/>
-    <tableColumn id="4" name="[order]" dataDxfId="2"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="1"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B4:N31" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+  <autoFilter ref="B4:N31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[paramValue]" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[itemType]" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[itemAmount]" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[itemSku]" dataDxfId="14"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[itemFeatured]" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[minAppVersion]" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[order]" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[refPrice]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[discount]" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{EC30BFE9-93AC-B341-A6DF-2464A465E69D}" name="[iapSku]" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{CAF1E60A-0F22-9F48-B595-4C0BDBEE3450}" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1293,11 +1430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,6 +1449,8 @@
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1382,6 +1521,12 @@
       <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
@@ -1407,6 +1552,12 @@
       <c r="L5" s="12">
         <v>0.5</v>
       </c>
+      <c r="M5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1432,6 +1583,8 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
@@ -1453,6 +1606,8 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
@@ -1474,6 +1629,8 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="13"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
@@ -1493,6 +1650,8 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
@@ -1512,6 +1671,8 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
@@ -1531,6 +1692,8 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
@@ -1550,6 +1713,8 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
@@ -1569,6 +1734,8 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="13"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
@@ -1588,6 +1755,8 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="13"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
@@ -1613,6 +1782,12 @@
       <c r="L15" s="12">
         <v>0.75</v>
       </c>
+      <c r="M15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
@@ -1636,8 +1811,10 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -1657,8 +1834,10 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -1678,8 +1857,10 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="13"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1697,8 +1878,10 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1716,8 +1899,10 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -1735,8 +1920,10 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -1754,8 +1941,10 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1773,8 +1962,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -1792,8 +1983,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
@@ -1817,8 +2010,14 @@
       <c r="L25" s="12">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M25" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1838,8 +2037,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
@@ -1859,8 +2060,10 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="13"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>17</v>
       </c>
@@ -1878,8 +2081,10 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="13"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
@@ -1903,8 +2108,14 @@
       <c r="L29" s="12">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>6</v>
       </c>
@@ -1926,8 +2137,10 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -1945,51 +2158,53 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="13"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I5:L31">
-    <cfRule type="expression" dxfId="21" priority="9">
+  <conditionalFormatting sqref="I5:N31">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H22 F23:H23 E24:H31">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14 D25:D31">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D24">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$B15&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:D23 B5:L22 F23:L23 B24:L31">
-    <cfRule type="expression" dxfId="17" priority="3">
+  <conditionalFormatting sqref="B23:D23 B5:L22 F23:L23 B24:L31 M5:N31">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B23&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$B23="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B31">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C5:C31">
+    <dataValidation type="list" allowBlank="1" sqref="C5:C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"featured,startDate,endDate,countriesAllowed,countriesExcluded,gamesPlayed,frequency,maxViews,zone,payerType,minSpent,dragonOwned,dragonUnlocked,scBalanceRange,hcBalanceRange,openedEggs,petsOwnedCount,petsOwned,progressionRange,skinsUnlocked,skinsOwned"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E5:E22 E24:E31">
+    <dataValidation type="list" allowBlank="1" sqref="E5:E22 E24:E31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Offer Pack: Content - Added new segmentation parameters (dragonNotOwned, petsNotOwned, skinsNotOwned).
Former-commit-id: a1a79601b2b17a0ca05650df817058f26cb94b48
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6A82CA15-AF8F-B94E-A079-912B071E57A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C96F9033-5749-F447-9523-85F9E05BEDB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidationData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -106,12 +107,6 @@
   </si>
   <si>
     <t>dragonSelection</t>
-  </si>
-  <si>
-    <t>offer_pack_test_1</t>
-  </si>
-  <si>
-    <t>offer_pack_test_2</t>
   </si>
   <si>
     <t>egg</t>
@@ -127,9 +122,6 @@
 Use a tool like https://www.epochconverter.com/ for timestamps</t>
   </si>
   <si>
-    <t>offer_pack_test_3</t>
-  </si>
-  <si>
     <t>[refPrice]</t>
   </si>
   <si>
@@ -137,9 +129,6 @@
   </si>
   <si>
     <t>gamesPlayed</t>
-  </si>
-  <si>
-    <t>offer_pack_test_4</t>
   </si>
   <si>
     <t>openedEggs</t>
@@ -180,13 +169,94 @@
   </si>
   <si>
     <t>TID_OFFER_PACK_BASIC</t>
+  </si>
+  <si>
+    <t>Segmentation Parameters</t>
+  </si>
+  <si>
+    <t>Item Types</t>
+  </si>
+  <si>
+    <t>countriesAllowed</t>
+  </si>
+  <si>
+    <t>countriesExcluded</t>
+  </si>
+  <si>
+    <t>payerType</t>
+  </si>
+  <si>
+    <t>minSpent</t>
+  </si>
+  <si>
+    <t>dragonOwned</t>
+  </si>
+  <si>
+    <t>dragonUnlocked</t>
+  </si>
+  <si>
+    <t>scBalanceRange</t>
+  </si>
+  <si>
+    <t>hcBalanceRange</t>
+  </si>
+  <si>
+    <t>petsOwnedCount</t>
+  </si>
+  <si>
+    <t>petsOwned</t>
+  </si>
+  <si>
+    <t>progressionRange</t>
+  </si>
+  <si>
+    <t>skinsUnlocked</t>
+  </si>
+  <si>
+    <t>skinsOwned</t>
+  </si>
+  <si>
+    <t>skinsNotOwned</t>
+  </si>
+  <si>
+    <t>petsNotOwned</t>
+  </si>
+  <si>
+    <t>dragonNotOwned</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>skin</t>
+  </si>
+  <si>
+    <t>offer_pack_test_2items</t>
+  </si>
+  <si>
+    <t>offer_pack_test_egg</t>
+  </si>
+  <si>
+    <t>offer_pack_test_pet</t>
+  </si>
+  <si>
+    <t>offer_pack_test_1item</t>
+  </si>
+  <si>
+    <t>offer_pack_test_skin</t>
+  </si>
+  <si>
+    <t>dragon_chinese_3</t>
+  </si>
+  <si>
+    <t>dragon_chinese</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,6 +309,14 @@
     <font>
       <i/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -417,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -474,11 +552,288 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -514,83 +869,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1113,22 +1391,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B4:N31" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
-  <autoFilter ref="B4:N31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
+  <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[paramValue]" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[itemType]" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[itemAmount]" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[itemSku]" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[itemFeatured]" dataDxfId="13"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[minAppVersion]" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[order]" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[refPrice]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[discount]" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{EC30BFE9-93AC-B341-A6DF-2464A465E69D}" name="[iapSku]" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{CAF1E60A-0F22-9F48-B595-4C0BDBEE3450}" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[paramValue]" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[itemType]" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[itemAmount]" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[itemSku]" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[itemFeatured]" dataDxfId="31"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[minAppVersion]" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[order]" dataDxfId="29"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[refPrice]" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[discount]" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{EC30BFE9-93AC-B341-A6DF-2464A465E69D}" name="[iapSku]" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{CAF1E60A-0F22-9F48-B595-4C0BDBEE3450}" name="[tidName]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1431,10 +1709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P31"/>
+  <dimension ref="B1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="131" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,7 +1723,7 @@
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
@@ -1475,16 +1753,16 @@
     </row>
     <row r="3" spans="2:16" s="16" customFormat="1" ht="182" x14ac:dyDescent="0.2">
       <c r="D3" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="112" x14ac:dyDescent="0.2">
@@ -1516,16 +1794,16 @@
         <v>2</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
@@ -1533,7 +1811,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="10"/>
@@ -1553,10 +1831,10 @@
         <v>0.5</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
@@ -1595,10 +1873,10 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="11" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="F7" s="11">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="15"/>
@@ -1658,7 +1936,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="7">
         <v>1519057687</v>
@@ -1679,10 +1957,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7">
-        <v>1519835287</v>
+        <v>1522257000</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1760,76 +2038,76 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="6">
-        <v>1</v>
-      </c>
-      <c r="K15" s="6">
-        <v>200</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0.75</v>
-      </c>
-      <c r="M15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="N15" s="18" t="s">
-        <v>48</v>
-      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="10">
-        <v>2</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
+      <c r="I16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6">
+        <v>200</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="11">
-        <v>100</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="15"/>
+      <c r="E17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1842,42 +2120,44 @@
         <v>6</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F18" s="11">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="15"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="13"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="11">
+        <v>10000</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="15"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
     </row>
@@ -1886,10 +2166,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1519230487</v>
+        <v>15</v>
+      </c>
+      <c r="D20" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1907,10 +2187,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7">
-        <v>1519576087</v>
+        <v>1519230487</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1928,10 +2208,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D22" s="7">
-        <v>10</v>
+        <v>1522257000</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -1949,10 +2229,10 @@
         <v>17</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -1961,7 +2241,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="13"/>
+      <c r="L23" s="6"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
@@ -1970,10 +2250,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -1988,155 +2268,147 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="6">
-        <v>2</v>
-      </c>
-      <c r="K25" s="6">
-        <v>50</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="M25" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N25" s="18" t="s">
-        <v>50</v>
-      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="11">
-        <v>50</v>
-      </c>
-      <c r="G26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
+      <c r="I26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6">
+        <v>200</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="11">
-        <v>5000</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="15"/>
+      <c r="E27" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="13"/>
+      <c r="L27" s="6"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="7">
-        <v>5</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="11">
+        <v>100</v>
+      </c>
       <c r="G28" s="11"/>
       <c r="H28" s="15"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="13"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="11">
+        <v>10000</v>
+      </c>
       <c r="G29" s="11"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="6">
-        <v>3</v>
-      </c>
-      <c r="K29" s="6">
-        <v>20</v>
-      </c>
-      <c r="L29" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="M29" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N29" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="11">
-        <v>5</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>35</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="15"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="13"/>
+      <c r="L30" s="6"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
     </row>
@@ -2145,10 +2417,10 @@
         <v>17</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" s="7">
-        <v>3</v>
+        <v>1519230487</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -2157,55 +2429,440 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1522257000</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="7">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="6">
+        <v>2</v>
+      </c>
+      <c r="K38" s="6">
+        <v>50</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="11">
+        <v>50</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="11">
+        <v>5000</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="7">
+        <v>5</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="6">
+        <v>3</v>
+      </c>
+      <c r="K42" s="6">
+        <v>20</v>
+      </c>
+      <c r="L42" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N42" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="11">
+        <v>5</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="15"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="7">
+        <v>3</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I5:N31">
-    <cfRule type="expression" dxfId="7" priority="9">
+  <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
+    <cfRule type="expression" dxfId="24" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:H22 F23:H23 E24:H31">
-    <cfRule type="expression" dxfId="6" priority="8">
+  <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D14 D25:D31">
-    <cfRule type="expression" dxfId="5" priority="7">
+  <conditionalFormatting sqref="D5:D13 D15 D38:D44">
+    <cfRule type="expression" dxfId="22" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D24">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>$B15&lt;&gt;"&lt;Param&gt;"</formula>
+  <conditionalFormatting sqref="D16:D25">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:D23 B5:L22 F23:L23 B24:L31 M5:N31">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$B23&lt;&gt;"&lt;Item&gt;"</formula>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$B23="&lt;Definition&gt;"</formula>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <conditionalFormatting sqref="I14:N14">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:H14">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:N14">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>$B14="&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:N34 I37:N37">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D34 D37">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>$B26="&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>$B34="&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35:N35">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:H35">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:N35">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$B35="&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36:N36">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36:H36">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:N36">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B36="&lt;Definition&gt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C5:C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"featured,startDate,endDate,countriesAllowed,countriesExcluded,gamesPlayed,frequency,maxViews,zone,payerType,minSpent,dragonOwned,dragonUnlocked,scBalanceRange,hcBalanceRange,openedEggs,petsOwnedCount,petsOwned,progressionRange,skinsUnlocked,skinsOwned"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E5:E22 E24:E31" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2213,5 +2870,210 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B978484-C36D-FE48-9BB2-8C5B7593D4D5}">
+          <x14:formula1>
+            <xm:f>ValidationData!$B$4:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5:E44</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{B0D0AF8C-4D09-EC43-BF46-CC111321D414}">
+          <x14:formula1>
+            <xm:f>ValidationData!$D$4:$D$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C44</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DFF118-E2C0-E64C-BF6C-DD3AD8042DF7}">
+  <dimension ref="B2:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Offers: Development - New content format, splitting packsDefinitions with itemDefinitions in two single-dimension tables.
Former-commit-id: b6bd2abb3dad8ad0cd5f3b3f2e54b8271f536795
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C96F9033-5749-F447-9523-85F9E05BEDB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7297086F-3DD4-7542-A532-E86AE4187E92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ValidationData" sheetId="2" r:id="rId2"/>
+    <sheet name="Packs" sheetId="3" r:id="rId1"/>
+    <sheet name="Items" sheetId="4" r:id="rId2"/>
+    <sheet name="OLD" sheetId="1" r:id="rId3"/>
+    <sheet name="ValidationData" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="166">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -250,13 +252,289 @@
   </si>
   <si>
     <t>dragon_chinese</t>
+  </si>
+  <si>
+    <t>offerPacksDefinitions_OLD</t>
+  </si>
+  <si>
+    <t>[enabled]</t>
+  </si>
+  <si>
+    <t>offer_pack_1</t>
+  </si>
+  <si>
+    <t>[featured]</t>
+  </si>
+  <si>
+    <t>[startDate]</t>
+  </si>
+  <si>
+    <t>[endDate]</t>
+  </si>
+  <si>
+    <t>[countriesAllowed]</t>
+  </si>
+  <si>
+    <t>[countriesExcluded]</t>
+  </si>
+  <si>
+    <t>[gamesPlayed]</t>
+  </si>
+  <si>
+    <t>[frequency]</t>
+  </si>
+  <si>
+    <t>[maxViews]</t>
+  </si>
+  <si>
+    <t>[zone]</t>
+  </si>
+  <si>
+    <t>[payerType]</t>
+  </si>
+  <si>
+    <t>[minSpent]</t>
+  </si>
+  <si>
+    <t>[dragonUnlocked]</t>
+  </si>
+  <si>
+    <t>[dragonOwned]</t>
+  </si>
+  <si>
+    <t>[dragonNotOwned]</t>
+  </si>
+  <si>
+    <t>[scBalanceRange]</t>
+  </si>
+  <si>
+    <t>[hcBalanceRange]</t>
+  </si>
+  <si>
+    <t>[openedEggs]</t>
+  </si>
+  <si>
+    <t>[petsOwnedCount]</t>
+  </si>
+  <si>
+    <t>[petsOwned]</t>
+  </si>
+  <si>
+    <t>[petsNotOwned]</t>
+  </si>
+  <si>
+    <t>[progressionRange]</t>
+  </si>
+  <si>
+    <t>[skinsUnlocked]</t>
+  </si>
+  <si>
+    <t>[skinsOwned]</t>
+  </si>
+  <si>
+    <t>4.99</t>
+  </si>
+  <si>
+    <t>Check Confluence doc for each parameter's format.</t>
+  </si>
+  <si>
+    <t>Use a tool like https://www.epochconverter.com/ for timestamps</t>
+  </si>
+  <si>
+    <t>offer_pack_2</t>
+  </si>
+  <si>
+    <t>offer_pack_3</t>
+  </si>
+  <si>
+    <t>offer_pack_4</t>
+  </si>
+  <si>
+    <t>offer_pack_5</t>
+  </si>
+  <si>
+    <t>offer_pack_6</t>
+  </si>
+  <si>
+    <t>offer_pack_7</t>
+  </si>
+  <si>
+    <t>offer_pack_8</t>
+  </si>
+  <si>
+    <t>offer_pack_9</t>
+  </si>
+  <si>
+    <t>offer_pack_10</t>
+  </si>
+  <si>
+    <t>offer_pack_11</t>
+  </si>
+  <si>
+    <t>offer_pack_12</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_5</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_6</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_7</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_8</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_9</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_10</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_11</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.offer_pack_12</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>{offerItemsDefinitions}</t>
+  </si>
+  <si>
+    <t>[item1]</t>
+  </si>
+  <si>
+    <t>[item2]</t>
+  </si>
+  <si>
+    <t>[item3]</t>
+  </si>
+  <si>
+    <t>[skinsNotOwned]</t>
+  </si>
+  <si>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>[amount]</t>
+  </si>
+  <si>
+    <t>offer_item_1</t>
+  </si>
+  <si>
+    <t>offer_item_2</t>
+  </si>
+  <si>
+    <t>offer_item_3</t>
+  </si>
+  <si>
+    <t>offer_item_4</t>
+  </si>
+  <si>
+    <t>offer_item_5</t>
+  </si>
+  <si>
+    <t>offer_item_6</t>
+  </si>
+  <si>
+    <t>offer_item_7</t>
+  </si>
+  <si>
+    <t>offer_item_8</t>
+  </si>
+  <si>
+    <t>offer_item_9</t>
+  </si>
+  <si>
+    <t>offer_item_10</t>
+  </si>
+  <si>
+    <t>offer_item_11</t>
+  </si>
+  <si>
+    <t>offer_item_12</t>
+  </si>
+  <si>
+    <t>offer_item_13</t>
+  </si>
+  <si>
+    <t>offer_item_14</t>
+  </si>
+  <si>
+    <t>offer_item_15</t>
+  </si>
+  <si>
+    <t>offer_item_16</t>
+  </si>
+  <si>
+    <t>offer_item_17</t>
+  </si>
+  <si>
+    <t>offer_item_18</t>
+  </si>
+  <si>
+    <t>offer_item_19</t>
+  </si>
+  <si>
+    <t>offer_item_20</t>
+  </si>
+  <si>
+    <t>offer_item_21</t>
+  </si>
+  <si>
+    <t>offer_item_22</t>
+  </si>
+  <si>
+    <t>offer_item_23</t>
+  </si>
+  <si>
+    <t>offer_item_24</t>
+  </si>
+  <si>
+    <t>offer_item_25</t>
+  </si>
+  <si>
+    <t>offer_item_26</t>
+  </si>
+  <si>
+    <t>offer_item_27</t>
+  </si>
+  <si>
+    <t>offer_item_28</t>
+  </si>
+  <si>
+    <t>offer_item_29</t>
+  </si>
+  <si>
+    <t>offer_item_30</t>
+  </si>
+  <si>
+    <t>offer_item_31</t>
+  </si>
+  <si>
+    <t>offer_item_32</t>
+  </si>
+  <si>
+    <t>offer_item_33</t>
+  </si>
+  <si>
+    <t>offer_item_34</t>
+  </si>
+  <si>
+    <t>offer_item_35</t>
+  </si>
+  <si>
+    <t>offer_item_36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -322,8 +600,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +670,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA8ED0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3DAEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -491,11 +801,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -554,11 +934,102 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="89">
     <dxf>
       <font>
         <b/>
@@ -1377,8 +1848,1746 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE3DAEF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE3DAEF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE3DAEF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE3DAEF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF95B3D7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE3DAEF"/>
+      <color rgb="FFAA8ED0"/>
+      <color rgb="FFC88ED0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1391,10 +3600,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ED1A36F1-C81C-E240-B69D-05233E25FFBE}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AK14" totalsRowShown="0" headerRowDxfId="88" headerRowBorderDxfId="87" tableBorderDxfId="86">
+  <autoFilter ref="B2:AK14" xr:uid="{4F9A3A4D-2285-5F44-B96F-898511E3F95B}"/>
+  <tableColumns count="36">
+    <tableColumn id="1" xr3:uid="{5AA55AC3-7CB6-FC44-B07D-F51D2A78CC7F}" name="{offerPacksDefinitions}" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{769B23B4-E9A6-284B-90FD-39F89B1ACB9C}" name="[sku]" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{C2ECF4B3-5C1E-FA40-B693-9309C7BCA56C}" name="[enabled]" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{775C3509-403A-644A-86AD-77F63EA7574E}" name="[item1]" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{93FE19D6-1AD6-614B-A400-0C80FB077313}" name="[item2]" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{9A9C4E04-C2C4-9A4E-8267-2ED259FD6396}" name="[item3]" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{3DF96E69-A350-B74B-87E8-962A5358D4FE}" name="[order]" dataDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{960853A1-6A63-CE44-AAA8-91A8A20AF5D0}" name="[refPrice]" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{686163E9-209F-D64B-8FC7-4F6917B59535}" name="[discount]" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{70F61F4A-125E-6643-9427-3AF37756BF1D}" name="[iapSku]" dataDxfId="76"/>
+    <tableColumn id="11" xr3:uid="{392047DC-2DF0-A248-BD8D-C510711B2715}" name="[tidName]" dataDxfId="75"/>
+    <tableColumn id="12" xr3:uid="{1A9730B6-30B6-1C4D-942F-461C1D96445D}" name="[featured]" dataDxfId="74"/>
+    <tableColumn id="13" xr3:uid="{4E307595-D830-8545-8566-5F0470CF29AB}" name="[maxViews]" dataDxfId="73"/>
+    <tableColumn id="14" xr3:uid="{FB4C12FD-07EB-1F4B-93B8-AD797245A23C}" name="[zone]" dataDxfId="72"/>
+    <tableColumn id="15" xr3:uid="{8D2DE5F3-FBDD-604E-A6FB-081C887B0E61}" name="[frequency]" dataDxfId="71"/>
+    <tableColumn id="16" xr3:uid="{3E5B5816-0024-0E47-AAF3-D9442AABDBC4}" name="[startDate]" dataDxfId="70"/>
+    <tableColumn id="17" xr3:uid="{6F9129DD-4054-AB4D-9D66-876B6196FB57}" name="[endDate]" dataDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{3D155EBB-7C6E-4C4C-B541-2CE516975490}" name="[minAppVersion]" dataDxfId="68"/>
+    <tableColumn id="19" xr3:uid="{D3F1299F-F88F-D141-8EB7-0BFF97FC7451}" name="[countriesAllowed]" dataDxfId="67"/>
+    <tableColumn id="20" xr3:uid="{4BD03573-B9AE-E142-B845-87458F1C146E}" name="[countriesExcluded]" dataDxfId="66"/>
+    <tableColumn id="21" xr3:uid="{B7105B3F-72DE-C14C-9A41-5EC27FCB4916}" name="[gamesPlayed]" dataDxfId="65"/>
+    <tableColumn id="22" xr3:uid="{87DF1AE4-1EE5-E54B-AD5A-C43DE78722FA}" name="[payerType]" dataDxfId="64"/>
+    <tableColumn id="23" xr3:uid="{7DF15487-16A4-C64D-9B10-94ACDAA98F79}" name="[minSpent]" dataDxfId="63"/>
+    <tableColumn id="24" xr3:uid="{F92FED66-4C4F-A946-8E91-8023959BBA02}" name="[dragonUnlocked]" dataDxfId="62"/>
+    <tableColumn id="25" xr3:uid="{14A8C544-806C-354E-9E67-F45B793458A6}" name="[dragonOwned]" dataDxfId="61"/>
+    <tableColumn id="26" xr3:uid="{438DC746-388B-B04F-945D-53D911FFA0F7}" name="[dragonNotOwned]" dataDxfId="60"/>
+    <tableColumn id="27" xr3:uid="{0695E1EC-C75A-3646-8FA9-71A912B6B9AC}" name="[scBalanceRange]" dataDxfId="59"/>
+    <tableColumn id="28" xr3:uid="{2E794ABE-BB5B-1B46-BC02-2A0CA0443719}" name="[hcBalanceRange]" dataDxfId="58"/>
+    <tableColumn id="29" xr3:uid="{AA2978B6-89A3-8A4A-8060-29A4779643D5}" name="[openedEggs]" dataDxfId="57"/>
+    <tableColumn id="30" xr3:uid="{F1B00789-E048-674E-AE95-47F1DF292AC1}" name="[petsOwnedCount]" dataDxfId="56"/>
+    <tableColumn id="31" xr3:uid="{897170A1-2C50-9C4E-8236-A916C2ED996F}" name="[petsOwned]" dataDxfId="55"/>
+    <tableColumn id="32" xr3:uid="{779EAF2B-15DF-414D-9D3D-DEF167C11DBA}" name="[petsNotOwned]" dataDxfId="54"/>
+    <tableColumn id="33" xr3:uid="{4A6A119E-C556-EB4E-880F-1E1B883AC642}" name="[progressionRange]" dataDxfId="53"/>
+    <tableColumn id="34" xr3:uid="{AD71F6AD-47E0-5543-B2E3-10FCB940B2C0}" name="[skinsUnlocked]" dataDxfId="52"/>
+    <tableColumn id="35" xr3:uid="{A84F0E68-2635-2342-8D34-F24736CE36B2}" name="[skinsOwned]" dataDxfId="51"/>
+    <tableColumn id="36" xr3:uid="{3817307B-BA2C-4E4D-B2A1-ABCA643213CA}" name="[skinsNotOwned]" dataDxfId="50"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{04610754-5ED0-5E41-B954-7462132FFEC2}" name="offerItemsDefinitions" displayName="offerItemsDefinitions" ref="B2:G38" totalsRowShown="0" headerRowBorderDxfId="49" tableBorderDxfId="48">
+  <autoFilter ref="B2:G38" xr:uid="{D4C0794A-5423-DF44-BB3E-4FEE91E963EF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{CDFF9D76-676F-CD42-843F-D81014EF49E4}" name="{offerItemsDefinitions}" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{4332E9A8-FF36-0946-B7F9-01362FCB91F0}" name="[sku]" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{6F915615-A632-534B-9CEC-EF0355B21B34}" name="[featured]" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{9CA5F155-FA3C-C148-8CA8-8B53398F8C04}" name="[type]" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{DEB48AFA-7AB3-E14F-9F10-B40C4A5D5330}" name="[amount]" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{07284125-DDB0-ED4B-84EA-A93ECC9950CD}" name="[itemSku]" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
   <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="offerPacksDefinitions_OLD" dataDxfId="37"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="36"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[paramValue]" dataDxfId="35"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[itemType]" dataDxfId="34"/>
@@ -1708,11 +3977,1409 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C213BC37-2D64-1C49-9206-ADFE266D60BF}">
+  <dimension ref="B1:AK14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="37" customWidth="1"/>
+    <col min="12" max="12" width="30.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="21.83203125" customWidth="1"/>
+    <col min="21" max="21" width="22.83203125" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" customWidth="1"/>
+    <col min="26" max="26" width="18.83203125" customWidth="1"/>
+    <col min="27" max="27" width="22.5" customWidth="1"/>
+    <col min="28" max="28" width="20.5" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" customWidth="1"/>
+    <col min="31" max="31" width="22" customWidth="1"/>
+    <col min="32" max="32" width="15.83203125" customWidth="1"/>
+    <col min="33" max="33" width="19.6640625" customWidth="1"/>
+    <col min="34" max="34" width="22.33203125" customWidth="1"/>
+    <col min="35" max="35" width="19" customWidth="1"/>
+    <col min="36" max="36" width="16.5" customWidth="1"/>
+    <col min="37" max="37" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:37" s="26" customFormat="1" ht="154" x14ac:dyDescent="0.2">
+      <c r="H1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="52"/>
+      <c r="S1" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+    </row>
+    <row r="2" spans="2:37" ht="112" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z2" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB2" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE2" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG2" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH2" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI2" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ2" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK2" s="40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="29">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="47"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="49"/>
+    </row>
+    <row r="4" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="29">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="49"/>
+    </row>
+    <row r="5" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="29">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="48"/>
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="49"/>
+    </row>
+    <row r="6" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="29">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="47"/>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="47"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="48"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
+      <c r="AG6" s="47"/>
+      <c r="AH6" s="47"/>
+      <c r="AI6" s="48"/>
+      <c r="AJ6" s="48"/>
+      <c r="AK6" s="49"/>
+    </row>
+    <row r="7" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="29">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="48"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="48"/>
+      <c r="AK7" s="49"/>
+    </row>
+    <row r="8" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="29">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="48"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="49"/>
+    </row>
+    <row r="9" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="29">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="47"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="48"/>
+      <c r="AD9" s="48"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="48"/>
+      <c r="AK9" s="49"/>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="29">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
+      <c r="AG10" s="47"/>
+      <c r="AH10" s="47"/>
+      <c r="AI10" s="48"/>
+      <c r="AJ10" s="48"/>
+      <c r="AK10" s="49"/>
+    </row>
+    <row r="11" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="29">
+        <v>0</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="47"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="48"/>
+      <c r="AD11" s="48"/>
+      <c r="AE11" s="47"/>
+      <c r="AF11" s="47"/>
+      <c r="AG11" s="47"/>
+      <c r="AH11" s="47"/>
+      <c r="AI11" s="48"/>
+      <c r="AJ11" s="48"/>
+      <c r="AK11" s="49"/>
+    </row>
+    <row r="12" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="29">
+        <v>0</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="47"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="47"/>
+      <c r="AH12" s="47"/>
+      <c r="AI12" s="48"/>
+      <c r="AJ12" s="48"/>
+      <c r="AK12" s="49"/>
+    </row>
+    <row r="13" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="29">
+        <v>0</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="48"/>
+      <c r="AD13" s="48"/>
+      <c r="AE13" s="47"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="47"/>
+      <c r="AH13" s="47"/>
+      <c r="AI13" s="48"/>
+      <c r="AJ13" s="48"/>
+      <c r="AK13" s="49"/>
+    </row>
+    <row r="14" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="36">
+        <v>0</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14" s="50"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="48"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="47"/>
+      <c r="AH14" s="47"/>
+      <c r="AI14" s="48"/>
+      <c r="AJ14" s="48"/>
+      <c r="AK14" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Q1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED217350-C2FE-AD4B-876A-D4EF0AF3C693}">
+  <dimension ref="B1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="2:7" ht="112" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="32">
+        <v>1</v>
+      </c>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="31"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="31"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="31"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="31"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="31"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="31"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="31"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="31"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{82F0CDD5-614E-894D-B344-C4AC23E531DA}">
+          <x14:formula1>
+            <xm:f>ValidationData!$B$4:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E38</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="131" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1765,9 +5432,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="112" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="127" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -2891,12 +6558,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DFF118-E2C0-E64C-BF6C-DD3AD8042DF7}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D8" sqref="D8:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Content - Add progression offers in content
Former-commit-id: 2a5aab6d2e307095df8b2bd065c2e4b1c4a9aed7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F9C48722-F3B0-A84B-B401-9FBFABCE125C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="198">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -524,12 +523,111 @@
   </si>
   <si>
     <t>[durationMinutes]</t>
+  </si>
+  <si>
+    <t>intermediatePackPet</t>
+  </si>
+  <si>
+    <t>currencyCatchupPack1</t>
+  </si>
+  <si>
+    <t>valueGatchaPack</t>
+  </si>
+  <si>
+    <t>valueCurrencyPack</t>
+  </si>
+  <si>
+    <t>smallGatchaPack</t>
+  </si>
+  <si>
+    <t>smallCurrencyPack</t>
+  </si>
+  <si>
+    <t>megaGatchaPack</t>
+  </si>
+  <si>
+    <t>currencyCatchupPack2</t>
+  </si>
+  <si>
+    <t>megaHCPackClassic</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.intermediatepackpet</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.currencycatchuppack1</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.valuegatchapack</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.valuecurrencypack</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.smallgatchapack</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.smallcurrencypack</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.megagatchapack</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.currencycatchuppack2</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.megahcpackclassic</t>
+  </si>
+  <si>
+    <t>pet_34</t>
+  </si>
+  <si>
+    <t>egg_offer</t>
+  </si>
+  <si>
+    <t>nonPayer</t>
+  </si>
+  <si>
+    <t>payer</t>
+  </si>
+  <si>
+    <t>30:999</t>
+  </si>
+  <si>
+    <t>38:999</t>
+  </si>
+  <si>
+    <t>44:999</t>
+  </si>
+  <si>
+    <t>53:999</t>
+  </si>
+  <si>
+    <t>69:999</t>
+  </si>
+  <si>
+    <t>TID_OFFER_PACK_INTERMEDIATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -612,7 +710,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -745,8 +843,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -896,11 +1006,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1047,13 +1168,46 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1061,45 +1215,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="91">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2663,6 +2778,44 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -3060,7 +3213,6 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3074,42 +3226,6 @@
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFF9E6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
         <top/>
         <bottom style="thin">
           <color auto="1"/>
@@ -3165,50 +3281,13 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF9E6"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3272,14 +3351,13 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFEDB3"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3308,14 +3386,13 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFEDB3"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3379,7 +3456,76 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFEDB3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFEDB3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3417,7 +3563,6 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3492,7 +3637,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -3660,77 +3804,77 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AU23" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88">
-  <autoFilter ref="B2:AU23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AU32" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88">
+  <autoFilter ref="B2:AU32"/>
   <tableColumns count="46">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="45" xr3:uid="{44CF430E-7666-B44F-8C90-8B9AFA5061FC}" name="[uniqueId]" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="84"/>
-    <tableColumn id="39" xr3:uid="{BDE36CE7-C3EE-CF46-9E65-256BF79847A1}" name="[purchaseLimit]" dataDxfId="83"/>
-    <tableColumn id="38" xr3:uid="{549D4FA4-F5FE-7E41-8EE1-D5AC64E6CC50}" name="[item1Featured]" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="81"/>
-    <tableColumn id="37" xr3:uid="{5FB302D5-DFC3-434A-B077-2D1D2138B668}" name="[item1Amount]" dataDxfId="80"/>
-    <tableColumn id="40" xr3:uid="{6455B275-094E-2345-9FD4-2C5DC35C6A9F}" name="[item1Sku]" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="78"/>
-    <tableColumn id="41" xr3:uid="{ED68C080-ED0B-9E43-B505-291AD4921579}" name="[item2Amount]" dataDxfId="77"/>
-    <tableColumn id="42" xr3:uid="{BFF33F2B-41F5-5A4C-93AB-DEB983FA7B88}" name="[item2Sku]" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="75"/>
-    <tableColumn id="43" xr3:uid="{3E8BF91C-560F-7741-8332-6A6D5E4E61A3}" name="[item3Amount]" dataDxfId="74"/>
-    <tableColumn id="44" xr3:uid="{4BD3AFA7-A608-A344-82A9-163AFF411CC3}" name="[item3Sku]" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="66"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="65"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="64"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="63"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="62"/>
-    <tableColumn id="46" xr3:uid="{F0E8F3EC-0A78-E14A-AE70-991D0323870C}" name="[durationMinutes]" dataDxfId="0"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="61"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="60"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="59"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="58"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="57"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="56"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="55"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="54"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="53"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="52"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="51"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="50"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="49"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="48"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="47"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="46"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="45"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="44"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="43"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="85"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="84"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="83"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="82"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="81"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="80"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="79"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="78"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="77"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="76"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="75"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="74"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="73"/>
+    <tableColumn id="7" name="[order]" dataDxfId="72"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="71"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="70"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="69"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="68"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="67"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="66"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="65"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="64"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="63"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="62"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="61"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="60"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="59"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="58"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="57"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="56"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="55"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
-  <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
+  <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="offerPacksDefinitions_OLD" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="37"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="[paramValue]" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[itemType]" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="[itemAmount]" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="[itemSku]" dataDxfId="33"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="[itemFeatured]" dataDxfId="32"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="[minAppVersion]" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[order]" dataDxfId="30"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="[refPrice]" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="[discount]" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[iapSku]" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="26"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="37"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="36"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="35"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="34"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="33"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="32"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="31"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="30"/>
+    <tableColumn id="4" name="[order]" dataDxfId="29"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="28"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="27"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="26"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4032,26 +4176,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AU23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="16" width="5.83203125" customWidth="1"/>
-    <col min="17" max="19" width="14.83203125" customWidth="1"/>
-    <col min="20" max="20" width="40.83203125" customWidth="1"/>
-    <col min="21" max="21" width="25.83203125" customWidth="1"/>
-    <col min="22" max="47" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="32" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="34" max="47" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:47" s="25" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:47" s="25" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
       <c r="Q1" s="16" t="s">
         <v>29</v>
       </c>
@@ -4061,34 +4213,34 @@
       <c r="S1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="52" t="s">
+      <c r="Z1" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="52"/>
+      <c r="AA1" s="53"/>
       <c r="AB1" s="49"/>
-      <c r="AC1" s="53" t="s">
+      <c r="AC1" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-    </row>
-    <row r="2" spans="2:47" ht="112" x14ac:dyDescent="0.2">
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+    </row>
+    <row r="2" spans="2:47" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4228,7 +4380,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
@@ -4296,7 +4448,7 @@
         <v>151</v>
       </c>
       <c r="X3" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y3" s="36" t="s">
         <v>151</v>
@@ -4368,12 +4520,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="51" t="s">
         <v>151</v>
@@ -4418,13 +4570,13 @@
         <v>0</v>
       </c>
       <c r="R4" s="29" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="S4" s="30">
         <v>0.5</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U4" s="22" t="s">
         <v>44</v>
@@ -4436,7 +4588,7 @@
         <v>151</v>
       </c>
       <c r="X4" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y4" s="36" t="s">
         <v>151</v>
@@ -4508,12 +4660,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>151</v>
@@ -4558,13 +4710,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S5" s="30">
         <v>0.5</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U5" s="22" t="s">
         <v>44</v>
@@ -4576,7 +4728,7 @@
         <v>151</v>
       </c>
       <c r="X5" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y5" s="36" t="s">
         <v>151</v>
@@ -4587,7 +4739,7 @@
       <c r="AA5" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB5" s="39" t="s">
+      <c r="AB5" s="52" t="s">
         <v>151</v>
       </c>
       <c r="AC5" s="37" t="s">
@@ -4648,12 +4800,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6" s="51" t="s">
         <v>151</v>
@@ -4698,13 +4850,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="29" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="S6" s="30">
         <v>0.5</v>
       </c>
       <c r="T6" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U6" s="22" t="s">
         <v>44</v>
@@ -4716,7 +4868,7 @@
         <v>151</v>
       </c>
       <c r="X6" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y6" s="36" t="s">
         <v>151</v>
@@ -4727,7 +4879,7 @@
       <c r="AA6" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB6" s="54" t="s">
+      <c r="AB6" s="39" t="s">
         <v>151</v>
       </c>
       <c r="AC6" s="37" t="s">
@@ -4788,12 +4940,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>151</v>
@@ -4838,13 +4990,13 @@
         <v>0</v>
       </c>
       <c r="R7" s="29" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="S7" s="30">
         <v>0.5</v>
       </c>
       <c r="T7" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U7" s="22" t="s">
         <v>44</v>
@@ -4856,7 +5008,7 @@
         <v>151</v>
       </c>
       <c r="X7" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y7" s="36" t="s">
         <v>151</v>
@@ -4928,12 +5080,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D8" s="51" t="s">
         <v>151</v>
@@ -4978,13 +5130,13 @@
         <v>0</v>
       </c>
       <c r="R8" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S8" s="30">
         <v>0.5</v>
       </c>
       <c r="T8" s="26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U8" s="22" t="s">
         <v>44</v>
@@ -4996,7 +5148,7 @@
         <v>151</v>
       </c>
       <c r="X8" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y8" s="36" t="s">
         <v>151</v>
@@ -5068,12 +5220,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>151</v>
@@ -5118,13 +5270,13 @@
         <v>0</v>
       </c>
       <c r="R9" s="29" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="S9" s="30">
         <v>0.5</v>
       </c>
       <c r="T9" s="26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U9" s="22" t="s">
         <v>44</v>
@@ -5136,7 +5288,7 @@
         <v>151</v>
       </c>
       <c r="X9" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y9" s="36" t="s">
         <v>151</v>
@@ -5208,12 +5360,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D10" s="51" t="s">
         <v>151</v>
@@ -5258,13 +5410,13 @@
         <v>0</v>
       </c>
       <c r="R10" s="29" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="S10" s="30">
         <v>0.5</v>
       </c>
       <c r="T10" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U10" s="22" t="s">
         <v>44</v>
@@ -5276,7 +5428,7 @@
         <v>151</v>
       </c>
       <c r="X10" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y10" s="36" t="s">
         <v>151</v>
@@ -5348,12 +5500,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>151</v>
@@ -5398,13 +5550,13 @@
         <v>0</v>
       </c>
       <c r="R11" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S11" s="30">
         <v>0.5</v>
       </c>
       <c r="T11" s="26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U11" s="22" t="s">
         <v>44</v>
@@ -5416,7 +5568,7 @@
         <v>151</v>
       </c>
       <c r="X11" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y11" s="36" t="s">
         <v>151</v>
@@ -5488,12 +5640,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>151</v>
@@ -5538,13 +5690,13 @@
         <v>0</v>
       </c>
       <c r="R12" s="29" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="S12" s="30">
         <v>0.5</v>
       </c>
       <c r="T12" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U12" s="22" t="s">
         <v>44</v>
@@ -5556,7 +5708,7 @@
         <v>151</v>
       </c>
       <c r="X12" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y12" s="36" t="s">
         <v>151</v>
@@ -5628,12 +5780,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>140</v>
+      <c r="C13" s="31" t="s">
+        <v>141</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>151</v>
@@ -5674,17 +5826,17 @@
       <c r="P13" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="Q13" s="32">
         <v>0</v>
       </c>
-      <c r="R13" s="29" t="s">
-        <v>99</v>
+      <c r="R13" s="35" t="s">
+        <v>126</v>
       </c>
       <c r="S13" s="30">
         <v>0.5</v>
       </c>
       <c r="T13" s="26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="U13" s="22" t="s">
         <v>44</v>
@@ -5696,7 +5848,7 @@
         <v>151</v>
       </c>
       <c r="X13" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y13" s="36" t="s">
         <v>151</v>
@@ -5768,12 +5920,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D14" s="51" t="s">
         <v>151</v>
@@ -5818,13 +5970,13 @@
         <v>0</v>
       </c>
       <c r="R14" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S14" s="30">
         <v>0.5</v>
       </c>
       <c r="T14" s="26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U14" s="22" t="s">
         <v>44</v>
@@ -5836,7 +5988,7 @@
         <v>151</v>
       </c>
       <c r="X14" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y14" s="36" t="s">
         <v>151</v>
@@ -5908,12 +6060,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>151</v>
@@ -5958,13 +6110,13 @@
         <v>0</v>
       </c>
       <c r="R15" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="S15" s="30">
         <v>0.5</v>
       </c>
       <c r="T15" s="26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U15" s="22" t="s">
         <v>44</v>
@@ -5976,7 +6128,7 @@
         <v>151</v>
       </c>
       <c r="X15" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y15" s="36" t="s">
         <v>151</v>
@@ -6048,12 +6200,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D16" s="51" t="s">
         <v>151</v>
@@ -6098,13 +6250,13 @@
         <v>0</v>
       </c>
       <c r="R16" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="S16" s="30">
         <v>0.5</v>
       </c>
       <c r="T16" s="26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="U16" s="22" t="s">
         <v>44</v>
@@ -6116,7 +6268,7 @@
         <v>151</v>
       </c>
       <c r="X16" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y16" s="36" t="s">
         <v>151</v>
@@ -6188,12 +6340,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>151</v>
@@ -6238,13 +6390,13 @@
         <v>0</v>
       </c>
       <c r="R17" s="35" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="S17" s="30">
         <v>0.5</v>
       </c>
       <c r="T17" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="U17" s="22" t="s">
         <v>44</v>
@@ -6256,7 +6408,7 @@
         <v>151</v>
       </c>
       <c r="X17" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y17" s="36" t="s">
         <v>151</v>
@@ -6328,12 +6480,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>151</v>
@@ -6378,13 +6530,13 @@
         <v>0</v>
       </c>
       <c r="R18" s="35" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="S18" s="30">
         <v>0.5</v>
       </c>
       <c r="T18" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="U18" s="22" t="s">
         <v>44</v>
@@ -6396,7 +6548,7 @@
         <v>151</v>
       </c>
       <c r="X18" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y18" s="36" t="s">
         <v>151</v>
@@ -6468,12 +6620,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>151</v>
@@ -6518,13 +6670,13 @@
         <v>0</v>
       </c>
       <c r="R19" s="35" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="S19" s="30">
         <v>0.5</v>
       </c>
       <c r="T19" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="U19" s="22" t="s">
         <v>44</v>
@@ -6536,7 +6688,7 @@
         <v>151</v>
       </c>
       <c r="X19" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y19" s="36" t="s">
         <v>151</v>
@@ -6608,12 +6760,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>151</v>
@@ -6658,13 +6810,13 @@
         <v>0</v>
       </c>
       <c r="R20" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S20" s="30">
         <v>0.5</v>
       </c>
       <c r="T20" s="26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="U20" s="22" t="s">
         <v>44</v>
@@ -6676,7 +6828,7 @@
         <v>151</v>
       </c>
       <c r="X20" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y20" s="36" t="s">
         <v>151</v>
@@ -6748,12 +6900,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>151</v>
@@ -6798,13 +6950,13 @@
         <v>0</v>
       </c>
       <c r="R21" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="S21" s="30">
         <v>0.5</v>
       </c>
       <c r="T21" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="U21" s="22" t="s">
         <v>44</v>
@@ -6816,7 +6968,7 @@
         <v>151</v>
       </c>
       <c r="X21" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y21" s="36" t="s">
         <v>151</v>
@@ -6888,12 +7040,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:47" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="31" t="s">
-        <v>149</v>
+      <c r="C22" s="38" t="s">
+        <v>150</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>151</v>
@@ -6937,14 +7089,14 @@
       <c r="Q22" s="32">
         <v>0</v>
       </c>
-      <c r="R22" s="35" t="s">
-        <v>128</v>
+      <c r="R22" s="29" t="s">
+        <v>129</v>
       </c>
       <c r="S22" s="30">
         <v>0.5</v>
       </c>
       <c r="T22" s="26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="U22" s="22" t="s">
         <v>44</v>
@@ -6956,7 +7108,7 @@
         <v>151</v>
       </c>
       <c r="X22" s="36" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="Y22" s="36" t="s">
         <v>151</v>
@@ -7028,143 +7180,1397 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+    <row r="23" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B23" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="40" t="b">
+      <c r="C23" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="58">
+        <v>1</v>
+      </c>
+      <c r="G23" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="58">
+        <v>1</v>
+      </c>
+      <c r="J23" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="K23" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="58">
+        <v>60</v>
+      </c>
+      <c r="M23" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="N23" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="O23" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="P23" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q23" s="59">
         <v>0</v>
       </c>
-      <c r="F23" s="48">
+      <c r="R23" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="S23" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="T23" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="U23" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="V23" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="W23" s="64">
+        <v>0</v>
+      </c>
+      <c r="X23" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y23" s="64">
+        <v>10</v>
+      </c>
+      <c r="Z23" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA23" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB23" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC23" s="65">
+        <v>1.6</v>
+      </c>
+      <c r="AD23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF23" s="65">
+        <v>4</v>
+      </c>
+      <c r="AG23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN23" s="65"/>
+      <c r="AO23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP23" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="AQ23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR23" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="AS23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT23" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU23" s="65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="G23" s="43" t="b">
+      <c r="F24" s="48">
+        <v>1</v>
+      </c>
+      <c r="G24" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="43">
+        <v>4</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="K24" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="47">
+        <v>3000</v>
+      </c>
+      <c r="M24" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N24" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O24" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P24" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="32">
         <v>0</v>
       </c>
-      <c r="H23" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="I23" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="J23" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="K23" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="L23" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="M23" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="N23" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="O23" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="P23" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q23" s="32">
+      <c r="R24" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="S24" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="T24" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="U24" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="V24" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W24" s="36">
         <v>0</v>
       </c>
-      <c r="R23" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="S23" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="T23" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="U23" s="22" t="s">
+      <c r="X24" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y24" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z24" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA24" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB24" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC24" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF24" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN24" s="37">
+        <v>10</v>
+      </c>
+      <c r="AO24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR24" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AS24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU24" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="48">
+        <v>1</v>
+      </c>
+      <c r="G25" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="43">
+        <v>50000</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K25" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="47">
+        <v>60</v>
+      </c>
+      <c r="M25" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N25" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O25" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P25" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="32">
+        <v>0</v>
+      </c>
+      <c r="R25" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="S25" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="T25" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="U25" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="V25" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W25" s="36">
+        <v>0</v>
+      </c>
+      <c r="X25" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y25" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z25" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA25" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB25" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC25" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF25" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG25" s="37"/>
+      <c r="AH25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR25" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AS25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU25" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="48">
+        <v>1</v>
+      </c>
+      <c r="G26" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="43">
+        <v>6</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="K26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="47">
+        <v>3000</v>
+      </c>
+      <c r="M26" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N26" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O26" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P26" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q26" s="32">
+        <v>0</v>
+      </c>
+      <c r="R26" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="S26" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="T26" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="U26" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V26" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W26" s="36">
+        <v>0</v>
+      </c>
+      <c r="X26" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y26" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z26" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA26" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB26" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC26" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF26" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG26" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN26" s="37">
+        <v>20</v>
+      </c>
+      <c r="AO26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR26" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU26" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="48">
+        <v>1</v>
+      </c>
+      <c r="G27" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="43">
+        <v>200</v>
+      </c>
+      <c r="J27" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K27" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="47">
+        <v>100000</v>
+      </c>
+      <c r="M27" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N27" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O27" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P27" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q27" s="32">
+        <v>0</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="S27" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="T27" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="U27" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="W23" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="X23" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y23" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z23" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA23" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB23" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC23" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU23" s="37" t="s">
+      <c r="V27" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W27" s="36">
+        <v>0</v>
+      </c>
+      <c r="X27" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y27" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z27" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA27" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB27" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC27" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF27" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG27" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR27" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU27" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="48">
+        <v>1</v>
+      </c>
+      <c r="G28" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="43">
+        <v>4</v>
+      </c>
+      <c r="J28" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="K28" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="47">
+        <v>3000</v>
+      </c>
+      <c r="M28" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N28" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O28" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P28" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q28" s="32">
+        <v>0</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="S28" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="T28" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="U28" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V28" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W28" s="36">
+        <v>0</v>
+      </c>
+      <c r="X28" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y28" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA28" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB28" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC28" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF28" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH28" s="37">
+        <v>5</v>
+      </c>
+      <c r="AI28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN28" s="37">
+        <v>20</v>
+      </c>
+      <c r="AO28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR28" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU28" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="48">
+        <v>1</v>
+      </c>
+      <c r="G29" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="43">
+        <v>100</v>
+      </c>
+      <c r="J29" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K29" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="47">
+        <v>100000</v>
+      </c>
+      <c r="M29" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N29" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O29" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P29" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q29" s="32">
+        <v>0</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="S29" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="T29" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="U29" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V29" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W29" s="36">
+        <v>0</v>
+      </c>
+      <c r="X29" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y29" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z29" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA29" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB29" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC29" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF29" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG29" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH29" s="37">
+        <v>5</v>
+      </c>
+      <c r="AI29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR29" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU29" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="48">
+        <v>1</v>
+      </c>
+      <c r="G30" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="43">
+        <v>10</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="47">
+        <v>3000</v>
+      </c>
+      <c r="M30" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N30" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O30" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P30" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q30" s="32">
+        <v>0</v>
+      </c>
+      <c r="R30" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="S30" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="T30" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="U30" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V30" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W30" s="36">
+        <v>0</v>
+      </c>
+      <c r="X30" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y30" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z30" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA30" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB30" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC30" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF30" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG30" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH30" s="37">
+        <v>40</v>
+      </c>
+      <c r="AI30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN30" s="37">
+        <v>20</v>
+      </c>
+      <c r="AO30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR30" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU30" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="48">
+        <v>1</v>
+      </c>
+      <c r="G31" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="43">
+        <v>150000</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K31" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="47">
+        <v>60</v>
+      </c>
+      <c r="M31" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N31" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O31" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P31" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q31" s="32">
+        <v>0</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="T31" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="U31" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="V31" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W31" s="36">
+        <v>0</v>
+      </c>
+      <c r="X31" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y31" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z31" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA31" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB31" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC31" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF31" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP31" s="37"/>
+      <c r="AQ31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR31" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU31" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="48">
+        <v>1</v>
+      </c>
+      <c r="G32" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="43">
+        <v>900</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K32" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="47">
+        <v>300000</v>
+      </c>
+      <c r="M32" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="N32" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O32" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P32" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q32" s="32">
+        <v>0</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="S32" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="T32" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="U32" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="V32" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W32" s="36">
+        <v>0</v>
+      </c>
+      <c r="X32" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y32" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z32" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA32" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB32" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC32" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="AD32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF32" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG32" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH32" s="37">
+        <v>50</v>
+      </c>
+      <c r="AI32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR32" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU32" s="37" t="s">
         <v>151</v>
       </c>
     </row>
@@ -7174,39 +8580,39 @@
     <mergeCell ref="AC1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7225,7 +8631,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="2:16" s="16" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" s="16" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
@@ -7239,7 +8645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="127" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
@@ -7280,7 +8686,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -7311,7 +8717,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -7338,7 +8744,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -7361,7 +8767,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -7384,7 +8790,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -7405,7 +8811,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -7426,7 +8832,7 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -7447,7 +8853,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -7468,7 +8874,7 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
@@ -7489,7 +8895,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -7510,7 +8916,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -7531,7 +8937,7 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -7562,7 +8968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -7589,7 +8995,7 @@
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -7612,7 +9018,7 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -7635,7 +9041,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -7656,7 +9062,7 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -7677,7 +9083,7 @@
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -7698,7 +9104,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -7719,7 +9125,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -7740,7 +9146,7 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
@@ -7761,7 +9167,7 @@
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -7792,7 +9198,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
@@ -7819,7 +9225,7 @@
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
@@ -7842,7 +9248,7 @@
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
@@ -7865,7 +9271,7 @@
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -7886,7 +9292,7 @@
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -7907,7 +9313,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -7928,7 +9334,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -7949,7 +9355,7 @@
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
@@ -7970,7 +9376,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -7991,7 +9397,7 @@
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
@@ -8012,7 +9418,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
@@ -8033,7 +9439,7 @@
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
@@ -8064,7 +9470,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
@@ -8087,7 +9493,7 @@
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
@@ -8110,7 +9516,7 @@
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
@@ -8131,7 +9537,7 @@
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
@@ -8162,7 +9568,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
@@ -8187,7 +9593,7 @@
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
@@ -8210,132 +9616,132 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="24" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="22" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="18" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8347,13 +9753,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationData!$B$4:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>ValidationData!$D$4:$D$31</xm:f>
           </x14:formula1>
@@ -8366,19 +9772,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>48</v>
       </c>
@@ -8387,10 +9793,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -8398,7 +9804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -8406,7 +9812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -8414,13 +9820,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -8428,7 +9834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -8436,7 +9842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>151</v>
       </c>
@@ -8444,107 +9850,107 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Content - Add date and unique ID to offers
Former-commit-id: c8bfcbacc4fad041b44eb65fd3b0ae167286210a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="199">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -622,15 +622,25 @@
   </si>
   <si>
     <t>TID_OFFER_PACK_INTERMEDIATE</t>
+  </si>
+  <si>
+    <t>intermediatePack2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1021,200 +1031,731 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="91">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1492,534 +2033,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3859,22 +3872,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="37"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="36"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="35"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="34"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="33"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="32"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="31"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="30"/>
-    <tableColumn id="4" name="[order]" dataDxfId="29"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="28"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="27"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="26"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="25"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
+    <tableColumn id="4" name="[order]" dataDxfId="4"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4179,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4198,7 +4211,9 @@
     <col min="21" max="21" width="19.875" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="7.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="32" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="7.5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.25" bestFit="1" customWidth="1"/>
     <col min="34" max="47" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -4213,32 +4228,32 @@
       <c r="S1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="53" t="s">
+      <c r="Z1" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="53"/>
+      <c r="AA1" s="64"/>
       <c r="AB1" s="49"/>
-      <c r="AC1" s="54" t="s">
+      <c r="AC1" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
     </row>
     <row r="2" spans="2:47" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -7181,140 +7196,140 @@
       </c>
     </row>
     <row r="23" spans="2:47" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="58" t="b">
+      <c r="D23" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="56">
         <v>1</v>
       </c>
-      <c r="G23" s="58" t="b">
+      <c r="G23" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="58">
+      <c r="I23" s="56">
         <v>1</v>
       </c>
-      <c r="J23" s="58" t="s">
+      <c r="J23" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="58">
+      <c r="L23" s="56">
         <v>60</v>
       </c>
-      <c r="M23" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="N23" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="O23" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="P23" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q23" s="59">
+      <c r="M23" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="N23" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="O23" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="P23" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q23" s="57">
         <v>0</v>
       </c>
-      <c r="R23" s="60" t="s">
+      <c r="R23" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="S23" s="61" t="s">
+      <c r="S23" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="T23" s="62" t="s">
+      <c r="T23" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="U23" s="63" t="s">
+      <c r="U23" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="V23" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="W23" s="64">
+      <c r="V23" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="W23" s="62">
         <v>0</v>
       </c>
-      <c r="X23" s="64" t="s">
+      <c r="X23" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="Y23" s="64">
+      <c r="Y23" s="62">
         <v>10</v>
       </c>
-      <c r="Z23" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA23" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB23" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC23" s="65">
+      <c r="Z23" s="62">
+        <v>1528070400</v>
+      </c>
+      <c r="AA23" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB23" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC23" s="63">
         <v>1.6</v>
       </c>
-      <c r="AD23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF23" s="65">
+      <c r="AD23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF23" s="63">
         <v>4</v>
       </c>
-      <c r="AG23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN23" s="65"/>
-      <c r="AO23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP23" s="65" t="s">
+      <c r="AG23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN23" s="63"/>
+      <c r="AO23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP23" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="AQ23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR23" s="65" t="s">
+      <c r="AQ23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR23" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="AS23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT23" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU23" s="65" t="s">
+      <c r="AS23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU23" s="63" t="s">
         <v>151</v>
       </c>
     </row>
@@ -7391,8 +7406,8 @@
       <c r="Y24" s="36">
         <v>10</v>
       </c>
-      <c r="Z24" s="39" t="s">
-        <v>151</v>
+      <c r="Z24" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA24" s="39" t="s">
         <v>151</v>
@@ -7531,8 +7546,8 @@
       <c r="Y25" s="36">
         <v>10</v>
       </c>
-      <c r="Z25" s="39" t="s">
-        <v>151</v>
+      <c r="Z25" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA25" s="39" t="s">
         <v>151</v>
@@ -7603,8 +7618,8 @@
       <c r="C26" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="51" t="s">
-        <v>167</v>
+      <c r="D26" s="66" t="s">
+        <v>198</v>
       </c>
       <c r="E26" s="40" t="b">
         <v>1</v>
@@ -7669,8 +7684,8 @@
       <c r="Y26" s="36">
         <v>10</v>
       </c>
-      <c r="Z26" s="39" t="s">
-        <v>151</v>
+      <c r="Z26" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA26" s="39" t="s">
         <v>151</v>
@@ -7743,8 +7758,8 @@
       <c r="C27" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="51" t="s">
-        <v>168</v>
+      <c r="D27" s="66" t="s">
+        <v>198</v>
       </c>
       <c r="E27" s="40" t="b">
         <v>1</v>
@@ -7809,8 +7824,8 @@
       <c r="Y27" s="36">
         <v>10</v>
       </c>
-      <c r="Z27" s="39" t="s">
-        <v>151</v>
+      <c r="Z27" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA27" s="39" t="s">
         <v>151</v>
@@ -7883,8 +7898,8 @@
       <c r="C28" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="D28" s="51" t="s">
-        <v>169</v>
+      <c r="D28" s="66" t="s">
+        <v>198</v>
       </c>
       <c r="E28" s="40" t="b">
         <v>1</v>
@@ -7949,8 +7964,8 @@
       <c r="Y28" s="36">
         <v>10</v>
       </c>
-      <c r="Z28" s="39" t="s">
-        <v>151</v>
+      <c r="Z28" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA28" s="39" t="s">
         <v>151</v>
@@ -8023,8 +8038,8 @@
       <c r="C29" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="51" t="s">
-        <v>170</v>
+      <c r="D29" s="66" t="s">
+        <v>198</v>
       </c>
       <c r="E29" s="40" t="b">
         <v>1</v>
@@ -8089,8 +8104,8 @@
       <c r="Y29" s="36">
         <v>10</v>
       </c>
-      <c r="Z29" s="39" t="s">
-        <v>151</v>
+      <c r="Z29" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA29" s="39" t="s">
         <v>151</v>
@@ -8163,8 +8178,8 @@
       <c r="C30" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="51" t="s">
-        <v>171</v>
+      <c r="D30" s="66" t="s">
+        <v>198</v>
       </c>
       <c r="E30" s="40" t="b">
         <v>1</v>
@@ -8229,8 +8244,8 @@
       <c r="Y30" s="36">
         <v>10</v>
       </c>
-      <c r="Z30" s="39" t="s">
-        <v>151</v>
+      <c r="Z30" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA30" s="39" t="s">
         <v>151</v>
@@ -8369,8 +8384,8 @@
       <c r="Y31" s="36">
         <v>10</v>
       </c>
-      <c r="Z31" s="39" t="s">
-        <v>151</v>
+      <c r="Z31" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA31" s="39" t="s">
         <v>151</v>
@@ -8507,8 +8522,8 @@
       <c r="Y32" s="36">
         <v>10</v>
       </c>
-      <c r="Z32" s="39" t="s">
-        <v>151</v>
+      <c r="Z32" s="39">
+        <v>1528070400</v>
       </c>
       <c r="AA32" s="39" t="s">
         <v>151</v>
@@ -9616,127 +9631,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="41" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="23" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="22" priority="25">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="36" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Content - Add duration to special offers
Former-commit-id: a0f915bc8ce8ee4ade21a31523168f2ebba518c1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="199">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -1214,14 +1214,14 @@
     <xf numFmtId="0" fontId="6" fillId="24" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4192,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4228,32 +4228,32 @@
       <c r="S1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="64" t="s">
+      <c r="Z1" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="64"/>
+      <c r="AA1" s="65"/>
       <c r="AB1" s="49"/>
-      <c r="AC1" s="65" t="s">
+      <c r="AC1" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="65"/>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="65"/>
-      <c r="AS1" s="65"/>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="65"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="66"/>
     </row>
     <row r="2" spans="2:47" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -7274,8 +7274,8 @@
       <c r="AA23" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="AB23" s="62" t="s">
-        <v>151</v>
+      <c r="AB23" s="62">
+        <v>1440</v>
       </c>
       <c r="AC23" s="63">
         <v>1.6</v>
@@ -7412,8 +7412,8 @@
       <c r="AA24" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB24" s="39" t="s">
-        <v>151</v>
+      <c r="AB24" s="39">
+        <v>1440</v>
       </c>
       <c r="AC24" s="37">
         <v>1.6</v>
@@ -7552,8 +7552,8 @@
       <c r="AA25" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB25" s="39" t="s">
-        <v>151</v>
+      <c r="AB25" s="39">
+        <v>2880</v>
       </c>
       <c r="AC25" s="37">
         <v>1.6</v>
@@ -7618,7 +7618,7 @@
       <c r="C26" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="66" t="s">
+      <c r="D26" s="64" t="s">
         <v>198</v>
       </c>
       <c r="E26" s="40" t="b">
@@ -7690,8 +7690,8 @@
       <c r="AA26" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB26" s="39" t="s">
-        <v>151</v>
+      <c r="AB26" s="39">
+        <v>1440</v>
       </c>
       <c r="AC26" s="37">
         <v>1.6</v>
@@ -7758,7 +7758,7 @@
       <c r="C27" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="64" t="s">
         <v>198</v>
       </c>
       <c r="E27" s="40" t="b">
@@ -7830,8 +7830,8 @@
       <c r="AA27" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB27" s="39" t="s">
-        <v>151</v>
+      <c r="AB27" s="39">
+        <v>1440</v>
       </c>
       <c r="AC27" s="37">
         <v>1.6</v>
@@ -7898,7 +7898,7 @@
       <c r="C28" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="64" t="s">
         <v>198</v>
       </c>
       <c r="E28" s="40" t="b">
@@ -7970,8 +7970,8 @@
       <c r="AA28" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB28" s="39" t="s">
-        <v>151</v>
+      <c r="AB28" s="39">
+        <v>1440</v>
       </c>
       <c r="AC28" s="37">
         <v>1.6</v>
@@ -8038,7 +8038,7 @@
       <c r="C29" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="64" t="s">
         <v>198</v>
       </c>
       <c r="E29" s="40" t="b">
@@ -8110,8 +8110,8 @@
       <c r="AA29" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB29" s="39" t="s">
-        <v>151</v>
+      <c r="AB29" s="39">
+        <v>1440</v>
       </c>
       <c r="AC29" s="37">
         <v>1.6</v>
@@ -8178,7 +8178,7 @@
       <c r="C30" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="64" t="s">
         <v>198</v>
       </c>
       <c r="E30" s="40" t="b">
@@ -8250,8 +8250,8 @@
       <c r="AA30" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB30" s="39" t="s">
-        <v>151</v>
+      <c r="AB30" s="39">
+        <v>1440</v>
       </c>
       <c r="AC30" s="37">
         <v>1.6</v>
@@ -8390,8 +8390,8 @@
       <c r="AA31" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB31" s="39" t="s">
-        <v>151</v>
+      <c r="AB31" s="39">
+        <v>2880</v>
       </c>
       <c r="AC31" s="37">
         <v>1.6</v>
@@ -8528,8 +8528,8 @@
       <c r="AA32" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB32" s="39" t="s">
-        <v>151</v>
+      <c r="AB32" s="39">
+        <v>4320</v>
       </c>
       <c r="AC32" s="37">
         <v>1.6</v>

</xml_diff>

<commit_message>
Content - Fix offer packs
Former-commit-id: 00a6a6450f679cf9346db647cda54aa70de35120
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="200">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -625,6 +625,9 @@
   </si>
   <si>
     <t>intermediatePack2</t>
+  </si>
+  <si>
+    <t>1.6</t>
   </si>
 </sst>
 </file>
@@ -4192,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4208,14 +4211,21 @@
     <col min="18" max="18" width="14.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.25" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.875" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="7.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="31" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.25" customWidth="1"/>
     <col min="33" max="33" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="34" max="47" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.375" customWidth="1"/>
+    <col min="35" max="39" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.875" customWidth="1"/>
+    <col min="41" max="41" width="16.125" customWidth="1"/>
+    <col min="42" max="42" width="14.625" customWidth="1"/>
+    <col min="43" max="43" width="20.25" customWidth="1"/>
+    <col min="44" max="47" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:47" s="25" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
@@ -7256,8 +7266,8 @@
       <c r="U23" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="V23" s="62" t="s">
-        <v>151</v>
+      <c r="V23" s="62" t="b">
+        <v>1</v>
       </c>
       <c r="W23" s="62">
         <v>0</v>
@@ -7277,8 +7287,8 @@
       <c r="AB23" s="62">
         <v>1440</v>
       </c>
-      <c r="AC23" s="63">
-        <v>1.6</v>
+      <c r="AC23" s="63" t="s">
+        <v>199</v>
       </c>
       <c r="AD23" s="63" t="s">
         <v>151</v>
@@ -7315,10 +7325,10 @@
         <v>151</v>
       </c>
       <c r="AP23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ23" s="63" t="s">
         <v>188</v>
-      </c>
-      <c r="AQ23" s="63" t="s">
-        <v>151</v>
       </c>
       <c r="AR23" s="63" t="s">
         <v>192</v>
@@ -7394,8 +7404,8 @@
       <c r="U24" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="V24" s="36" t="s">
-        <v>151</v>
+      <c r="V24" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W24" s="36">
         <v>0</v>
@@ -7407,7 +7417,7 @@
         <v>10</v>
       </c>
       <c r="Z24" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA24" s="39" t="s">
         <v>151</v>
@@ -7415,8 +7425,8 @@
       <c r="AB24" s="39">
         <v>1440</v>
       </c>
-      <c r="AC24" s="37">
-        <v>1.6</v>
+      <c r="AC24" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD24" s="37" t="s">
         <v>151</v>
@@ -7532,10 +7542,10 @@
         <v>180</v>
       </c>
       <c r="U25" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="V25" s="36" t="s">
-        <v>151</v>
+        <v>45</v>
+      </c>
+      <c r="V25" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W25" s="36">
         <v>0</v>
@@ -7547,7 +7557,7 @@
         <v>10</v>
       </c>
       <c r="Z25" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA25" s="39" t="s">
         <v>151</v>
@@ -7555,8 +7565,8 @@
       <c r="AB25" s="39">
         <v>2880</v>
       </c>
-      <c r="AC25" s="37">
-        <v>1.6</v>
+      <c r="AC25" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD25" s="37" t="s">
         <v>151</v>
@@ -7672,8 +7682,8 @@
       <c r="U26" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="V26" s="36" t="s">
-        <v>151</v>
+      <c r="V26" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W26" s="36">
         <v>0</v>
@@ -7693,8 +7703,8 @@
       <c r="AB26" s="39">
         <v>1440</v>
       </c>
-      <c r="AC26" s="37">
-        <v>1.6</v>
+      <c r="AC26" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD26" s="37" t="s">
         <v>151</v>
@@ -7812,8 +7822,8 @@
       <c r="U27" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="V27" s="36" t="s">
-        <v>151</v>
+      <c r="V27" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W27" s="36">
         <v>0</v>
@@ -7833,8 +7843,8 @@
       <c r="AB27" s="39">
         <v>1440</v>
       </c>
-      <c r="AC27" s="37">
-        <v>1.6</v>
+      <c r="AC27" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD27" s="37" t="s">
         <v>151</v>
@@ -7952,8 +7962,8 @@
       <c r="U28" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="V28" s="36" t="s">
-        <v>151</v>
+      <c r="V28" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W28" s="36">
         <v>0</v>
@@ -7973,8 +7983,8 @@
       <c r="AB28" s="39">
         <v>1440</v>
       </c>
-      <c r="AC28" s="37">
-        <v>1.6</v>
+      <c r="AC28" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD28" s="37" t="s">
         <v>151</v>
@@ -8092,8 +8102,8 @@
       <c r="U29" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="V29" s="36" t="s">
-        <v>151</v>
+      <c r="V29" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W29" s="36">
         <v>0</v>
@@ -8113,8 +8123,8 @@
       <c r="AB29" s="39">
         <v>1440</v>
       </c>
-      <c r="AC29" s="37">
-        <v>1.6</v>
+      <c r="AC29" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD29" s="37" t="s">
         <v>151</v>
@@ -8232,8 +8242,8 @@
       <c r="U30" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="V30" s="36" t="s">
-        <v>151</v>
+      <c r="V30" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W30" s="36">
         <v>0</v>
@@ -8253,8 +8263,8 @@
       <c r="AB30" s="39">
         <v>1440</v>
       </c>
-      <c r="AC30" s="37">
-        <v>1.6</v>
+      <c r="AC30" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD30" s="37" t="s">
         <v>151</v>
@@ -8370,10 +8380,10 @@
         <v>186</v>
       </c>
       <c r="U31" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="V31" s="36" t="s">
-        <v>151</v>
+        <v>45</v>
+      </c>
+      <c r="V31" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W31" s="36">
         <v>0</v>
@@ -8393,8 +8403,8 @@
       <c r="AB31" s="39">
         <v>2880</v>
       </c>
-      <c r="AC31" s="37">
-        <v>1.6</v>
+      <c r="AC31" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD31" s="37" t="s">
         <v>151</v>
@@ -8510,8 +8520,8 @@
       <c r="U32" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="V32" s="36" t="s">
-        <v>151</v>
+      <c r="V32" s="36" t="b">
+        <v>1</v>
       </c>
       <c r="W32" s="36">
         <v>0</v>
@@ -8531,8 +8541,8 @@
       <c r="AB32" s="39">
         <v>4320</v>
       </c>
-      <c r="AC32" s="37">
-        <v>1.6</v>
+      <c r="AC32" s="37" t="s">
+        <v>199</v>
       </c>
       <c r="AD32" s="37" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Content Offers - remove featured for pack with only 2 items
Former-commit-id: 1aae231fe094c0693fdf993acadcbba47d9fb5ee
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -16,7 +16,7 @@
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4195,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" activeCellId="1" sqref="G24:G32 I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4204,7 +4204,9 @@
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="7.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
@@ -7222,7 +7224,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="56" t="s">
         <v>18</v>
@@ -7360,7 +7362,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="43" t="s">
         <v>27</v>
@@ -7500,7 +7502,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="43" t="s">
         <v>21</v>
@@ -7638,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="43" t="s">
         <v>27</v>
@@ -7778,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="43" t="s">
         <v>19</v>
@@ -7918,7 +7920,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>27</v>
@@ -8058,7 +8060,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="43" t="s">
         <v>19</v>
@@ -8198,7 +8200,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="43" t="s">
         <v>27</v>
@@ -8338,7 +8340,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="43" t="s">
         <v>21</v>
@@ -8476,7 +8478,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="43" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Content - Roll back previous commit
Former-commit-id: 17d98e8a908bef9a55c2a56b800dafeaf190256d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -4196,7 +4196,7 @@
   <dimension ref="B1:AU32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" activeCellId="1" sqref="G24:G32 I25"/>
+      <selection activeCell="G24" sqref="G24:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7224,7 +7224,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="56" t="s">
         <v>18</v>
@@ -7362,7 +7362,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="43" t="s">
         <v>27</v>
@@ -7502,7 +7502,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="43" t="s">
         <v>21</v>
@@ -7640,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="43" t="s">
         <v>27</v>
@@ -7780,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="43" t="s">
         <v>19</v>
@@ -7920,7 +7920,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>27</v>
@@ -8060,7 +8060,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="43" t="s">
         <v>19</v>
@@ -8200,7 +8200,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="43" t="s">
         <v>27</v>
@@ -8340,7 +8340,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="43" t="s">
         <v>21</v>
@@ -8478,7 +8478,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="43" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Content - Fix timestamp offers
Former-commit-id: 38a563878a3358f91e2cb429f42ed98da63ade99
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -4195,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G32"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7281,7 +7281,7 @@
         <v>10</v>
       </c>
       <c r="Z23" s="62">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA23" s="62" t="s">
         <v>151</v>
@@ -7697,7 +7697,7 @@
         <v>10</v>
       </c>
       <c r="Z26" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA26" s="39" t="s">
         <v>151</v>
@@ -7837,7 +7837,7 @@
         <v>10</v>
       </c>
       <c r="Z27" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA27" s="39" t="s">
         <v>151</v>
@@ -7977,7 +7977,7 @@
         <v>10</v>
       </c>
       <c r="Z28" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA28" s="39" t="s">
         <v>151</v>
@@ -8117,7 +8117,7 @@
         <v>10</v>
       </c>
       <c r="Z29" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA29" s="39" t="s">
         <v>151</v>
@@ -8257,7 +8257,7 @@
         <v>10</v>
       </c>
       <c r="Z30" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA30" s="39" t="s">
         <v>151</v>
@@ -8397,7 +8397,7 @@
         <v>10</v>
       </c>
       <c r="Z31" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA31" s="39" t="s">
         <v>151</v>
@@ -8535,7 +8535,7 @@
         <v>10</v>
       </c>
       <c r="Z32" s="39">
-        <v>1528070400</v>
+        <v>1526342400</v>
       </c>
       <c r="AA32" s="39" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Content - Add order variable to the packDefinition
Former-commit-id: 35a7184181557de9e7616c6621e2f81b5d06449b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -4195,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="Z35" sqref="Z35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7254,7 +7254,7 @@
         <v>151</v>
       </c>
       <c r="Q23" s="57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R23" s="58" t="s">
         <v>99</v>
@@ -7392,7 +7392,7 @@
         <v>151</v>
       </c>
       <c r="Q24" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="29" t="s">
         <v>99</v>
@@ -7532,7 +7532,7 @@
         <v>151</v>
       </c>
       <c r="Q25" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" s="29" t="s">
         <v>99</v>
@@ -7670,7 +7670,7 @@
         <v>151</v>
       </c>
       <c r="Q26" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="29" t="s">
         <v>99</v>
@@ -7810,7 +7810,7 @@
         <v>151</v>
       </c>
       <c r="Q27" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R27" s="29" t="s">
         <v>125</v>
@@ -7950,7 +7950,7 @@
         <v>151</v>
       </c>
       <c r="Q28" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="29" t="s">
         <v>125</v>
@@ -8090,7 +8090,7 @@
         <v>151</v>
       </c>
       <c r="Q29" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R29" s="29" t="s">
         <v>99</v>
@@ -8230,7 +8230,7 @@
         <v>151</v>
       </c>
       <c r="Q30" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="29" t="s">
         <v>99</v>
@@ -8370,7 +8370,7 @@
         <v>151</v>
       </c>
       <c r="Q31" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="29" t="s">
         <v>126</v>
@@ -8508,7 +8508,7 @@
         <v>151</v>
       </c>
       <c r="Q32" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R32" s="29" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Offers: Development - Implemented minSpent and added minNumberOfPurchases and timeSinceLastPurchase parameters.
Former-commit-id: 99d4658edbe567dbb0727207ae8e33ae3a71cc13
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA69E686-AFD9-0F45-81E0-6A3E4971EA12}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="202">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -628,12 +629,18 @@
   </si>
   <si>
     <t>1.6</t>
+  </si>
+  <si>
+    <t>[minNumberOfPurchases]</t>
+  </si>
+  <si>
+    <t>[minutesSinceLastPurchase]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1230,112 +1237,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="93">
     <dxf>
       <font>
         <b val="0"/>
@@ -1350,15 +1252,17 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
           <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1374,389 +1278,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2048,6 +1569,576 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3820,77 +3911,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AU32" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88">
-  <autoFilter ref="B2:AU32"/>
-  <tableColumns count="46">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="85"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="84"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="83"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="82"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="81"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="80"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="79"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="78"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="77"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="76"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="75"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="74"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="73"/>
-    <tableColumn id="7" name="[order]" dataDxfId="72"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="71"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="70"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="69"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="68"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="67"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="66"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="65"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="64"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="63"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="62"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="61"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="60"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="59"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="58"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="57"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="56"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="55"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AW32" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90">
+  <autoFilter ref="B2:AW32" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[uniqueId]" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="86"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[purchaseLimit]" dataDxfId="85"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[item1Featured]" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="83"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[item1Amount]" dataDxfId="82"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[item1Sku]" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="80"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[item2Amount]" dataDxfId="79"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[item2Sku]" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="77"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[item3Amount]" dataDxfId="76"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[item3Sku]" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="70"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="69"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="67"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="66"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="65"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="64"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[durationMinutes]" dataDxfId="63"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="62"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="61"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="60"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="59"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="58"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="57"/>
+    <tableColumn id="47" xr3:uid="{AED225FC-C091-2342-9B9A-0BC4A5AA4B98}" name="[minNumberOfPurchases]" dataDxfId="26"/>
+    <tableColumn id="48" xr3:uid="{EDC99988-F22B-2C41-BBCD-4DF3558834B7}" name="[minutesSinceLastPurchase]" dataDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="56"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="55"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="54"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="53"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="52"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="51"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="50"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="49"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="48"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="47"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="46"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="45"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="B4:N44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
+  <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
-    <tableColumn id="4" name="[order]" dataDxfId="4"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="offerPacksDefinitions_OLD" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="38"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="[paramValue]" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[itemType]" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[itemAmount]" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[itemSku]" dataDxfId="34"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="[itemFeatured]" dataDxfId="33"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="[minAppVersion]" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[order]" dataDxfId="31"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="[refPrice]" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[discount]" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[iapSku]" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4192,45 +4285,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AU32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:AW32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
     <col min="8" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="31" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.25" customWidth="1"/>
-    <col min="33" max="33" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.375" customWidth="1"/>
+    <col min="32" max="32" width="20.1640625" customWidth="1"/>
+    <col min="33" max="33" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.33203125" customWidth="1"/>
     <col min="35" max="39" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.875" customWidth="1"/>
-    <col min="41" max="41" width="16.125" customWidth="1"/>
-    <col min="42" max="42" width="14.625" customWidth="1"/>
-    <col min="43" max="43" width="20.25" customWidth="1"/>
+    <col min="40" max="40" width="16.83203125" customWidth="1"/>
+    <col min="41" max="41" width="16.1640625" customWidth="1"/>
+    <col min="42" max="42" width="14.6640625" customWidth="1"/>
+    <col min="43" max="43" width="20.1640625" customWidth="1"/>
     <col min="44" max="47" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:47" s="25" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:49" s="25" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="Q1" s="16" t="s">
         <v>29</v>
       </c>
@@ -4266,8 +4359,10 @@
       <c r="AS1" s="66"/>
       <c r="AT1" s="66"/>
       <c r="AU1" s="66"/>
-    </row>
-    <row r="2" spans="2:47" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="AV1" s="66"/>
+      <c r="AW1" s="66"/>
+    </row>
+    <row r="2" spans="2:49" ht="135" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4368,46 +4463,52 @@
         <v>86</v>
       </c>
       <c r="AI2" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ2" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK2" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="AJ2" s="33" t="s">
+      <c r="AL2" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="AK2" s="33" t="s">
+      <c r="AM2" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="AL2" s="33" t="s">
+      <c r="AN2" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="AM2" s="33" t="s">
+      <c r="AO2" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="AN2" s="33" t="s">
+      <c r="AP2" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="AO2" s="33" t="s">
+      <c r="AQ2" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="AP2" s="33" t="s">
+      <c r="AR2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="AQ2" s="33" t="s">
+      <c r="AS2" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="AR2" s="33" t="s">
+      <c r="AT2" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="AS2" s="33" t="s">
+      <c r="AU2" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="AT2" s="33" t="s">
+      <c r="AV2" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="AU2" s="34" t="s">
+      <c r="AW2" s="34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
@@ -4546,8 +4647,14 @@
       <c r="AU3" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW3" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
@@ -4686,8 +4793,14 @@
       <c r="AU4" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV4" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW4" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
@@ -4826,8 +4939,14 @@
       <c r="AU5" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV5" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW5" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -4966,8 +5085,14 @@
       <c r="AU6" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW6" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
@@ -5106,8 +5231,14 @@
       <c r="AU7" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV7" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW7" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
@@ -5246,8 +5377,14 @@
       <c r="AU8" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV8" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW8" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
@@ -5386,8 +5523,14 @@
       <c r="AU9" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV9" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW9" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
@@ -5526,8 +5669,14 @@
       <c r="AU10" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV10" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW10" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
@@ -5666,8 +5815,14 @@
       <c r="AU11" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV11" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW11" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
@@ -5806,8 +5961,14 @@
       <c r="AU12" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV12" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW12" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
@@ -5946,8 +6107,14 @@
       <c r="AU13" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV13" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW13" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B14" s="14" t="s">
         <v>3</v>
       </c>
@@ -6086,8 +6253,14 @@
       <c r="AU14" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV14" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW14" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
@@ -6226,8 +6399,14 @@
       <c r="AU15" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV15" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW15" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
@@ -6366,8 +6545,14 @@
       <c r="AU16" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV16" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW16" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>3</v>
       </c>
@@ -6506,8 +6691,14 @@
       <c r="AU17" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV17" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW17" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>3</v>
       </c>
@@ -6646,8 +6837,14 @@
       <c r="AU18" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV18" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW18" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
@@ -6786,8 +6983,14 @@
       <c r="AU19" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV19" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW19" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
@@ -6926,8 +7129,14 @@
       <c r="AU20" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV20" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW20" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
         <v>3</v>
       </c>
@@ -7066,8 +7275,14 @@
       <c r="AU21" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="22" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV21" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW21" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
@@ -7206,8 +7421,14 @@
       <c r="AU22" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="23" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV22" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW22" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
@@ -7322,30 +7543,36 @@
       <c r="AM23" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="AN23" s="63"/>
+      <c r="AN23" s="63" t="s">
+        <v>151</v>
+      </c>
       <c r="AO23" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="AP23" s="63" t="s">
-        <v>151</v>
-      </c>
+      <c r="AP23" s="63"/>
       <c r="AQ23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS23" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="AR23" s="63" t="s">
+      <c r="AT23" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="AS23" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT23" s="63" t="s">
-        <v>151</v>
-      </c>
       <c r="AU23" s="63" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="24" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV23" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW23" s="63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
         <v>3</v>
       </c>
@@ -7460,32 +7687,38 @@
       <c r="AM24" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AN24" s="37">
+      <c r="AN24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP24" s="37">
         <v>10</v>
       </c>
-      <c r="AO24" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP24" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AQ24" s="37" t="s">
         <v>151</v>
       </c>
       <c r="AR24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT24" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="AS24" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT24" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU24" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="25" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW24" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B25" s="14" t="s">
         <v>3</v>
       </c>
@@ -7611,19 +7844,25 @@
         <v>151</v>
       </c>
       <c r="AR25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT25" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="AS25" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT25" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU25" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="26" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW25" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B26" s="14" t="s">
         <v>3</v>
       </c>
@@ -7738,32 +7977,38 @@
       <c r="AM26" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AN26" s="37">
+      <c r="AN26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP26" s="37">
         <v>20</v>
       </c>
-      <c r="AO26" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP26" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AQ26" s="37" t="s">
         <v>151</v>
       </c>
       <c r="AR26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT26" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AS26" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT26" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU26" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="27" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW26" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B27" s="14" t="s">
         <v>3</v>
       </c>
@@ -7891,19 +8136,25 @@
         <v>151</v>
       </c>
       <c r="AR27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT27" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AS27" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT27" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU27" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="28" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW27" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B28" s="14" t="s">
         <v>3</v>
       </c>
@@ -8018,32 +8269,38 @@
       <c r="AM28" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AN28" s="37">
+      <c r="AN28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP28" s="37">
         <v>20</v>
       </c>
-      <c r="AO28" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP28" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AQ28" s="37" t="s">
         <v>151</v>
       </c>
       <c r="AR28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT28" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AS28" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT28" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU28" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="29" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW28" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B29" s="14" t="s">
         <v>3</v>
       </c>
@@ -8171,19 +8428,25 @@
         <v>151</v>
       </c>
       <c r="AR29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT29" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AS29" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT29" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU29" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="30" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW29" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>3</v>
       </c>
@@ -8298,32 +8561,38 @@
       <c r="AM30" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AN30" s="37">
+      <c r="AN30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP30" s="37">
         <v>20</v>
       </c>
-      <c r="AO30" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP30" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AQ30" s="37" t="s">
         <v>151</v>
       </c>
       <c r="AR30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT30" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AS30" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT30" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU30" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="31" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV30" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW30" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>3</v>
       </c>
@@ -8444,24 +8713,30 @@
       <c r="AO31" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AP31" s="37"/>
+      <c r="AP31" s="37" t="s">
+        <v>151</v>
+      </c>
       <c r="AQ31" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AR31" s="37" t="s">
+      <c r="AR31" s="37"/>
+      <c r="AS31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT31" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="AS31" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT31" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU31" s="37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="32" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AV31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW31" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
         <v>3</v>
       </c>
@@ -8589,22 +8864,28 @@
         <v>151</v>
       </c>
       <c r="AR32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT32" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="AS32" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT32" s="37" t="s">
-        <v>151</v>
-      </c>
       <c r="AU32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV32" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW32" s="37" t="s">
         <v>151</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AC1:AU1"/>
+    <mergeCell ref="AC1:AW1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8615,31 +8896,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8658,7 +8939,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="2:16" s="16" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" s="16" customFormat="1" ht="182" x14ac:dyDescent="0.2">
       <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
@@ -8672,7 +8953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="129.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="127" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
@@ -8713,7 +8994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -8744,7 +9025,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -8771,7 +9052,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -8794,7 +9075,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -8817,7 +9098,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -8838,7 +9119,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -8859,7 +9140,7 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -8880,7 +9161,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -8901,7 +9182,7 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
@@ -8922,7 +9203,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -8943,7 +9224,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -8964,7 +9245,7 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -8995,7 +9276,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -9022,7 +9303,7 @@
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -9045,7 +9326,7 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -9068,7 +9349,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -9089,7 +9370,7 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -9110,7 +9391,7 @@
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -9131,7 +9412,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -9152,7 +9433,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -9173,7 +9454,7 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
@@ -9194,7 +9475,7 @@
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -9225,7 +9506,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
@@ -9252,7 +9533,7 @@
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
@@ -9275,7 +9556,7 @@
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
@@ -9298,7 +9579,7 @@
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -9319,7 +9600,7 @@
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -9340,7 +9621,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -9361,7 +9642,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -9382,7 +9663,7 @@
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
@@ -9403,7 +9684,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -9424,7 +9705,7 @@
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
@@ -9445,7 +9726,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
@@ -9466,7 +9747,7 @@
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
@@ -9497,7 +9778,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
@@ -9520,7 +9801,7 @@
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
@@ -9543,7 +9824,7 @@
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
@@ -9564,7 +9845,7 @@
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
@@ -9595,7 +9876,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
@@ -9620,7 +9901,7 @@
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
@@ -9643,132 +9924,132 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="39" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="22" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="36" priority="20">
+    <cfRule type="expression" dxfId="20" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="35" priority="19">
+    <cfRule type="expression" dxfId="19" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="26" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9780,13 +10061,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>ValidationData!$B$4:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>ValidationData!$D$4:$D$31</xm:f>
           </x14:formula1>
@@ -9799,19 +10080,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
         <v>48</v>
       </c>
@@ -9820,10 +10101,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -9831,7 +10112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -9839,7 +10120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -9847,13 +10128,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -9861,7 +10142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -9869,7 +10150,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>151</v>
       </c>
@@ -9877,107 +10158,107 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Content - Starter pack is back
Former-commit-id: 16b77d56694315126b22e7ae4e657836b4d177c4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA69E686-AFD9-0F45-81E0-6A3E4971EA12}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="204">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -635,12 +634,18 @@
   </si>
   <si>
     <t>[minutesSinceLastPurchase]</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_STARTERPACK</t>
+  </si>
+  <si>
+    <t>6:999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1041,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,11 +1238,122 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1252,17 +1368,15 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
           <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1278,6 +1392,389 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1569,576 +2066,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2628,6 +2555,88 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3911,79 +3920,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AW32" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90">
-  <autoFilter ref="B2:AW32" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AW32" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90">
+  <autoFilter ref="B2:AW32"/>
   <tableColumns count="48">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[uniqueId]" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="86"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[purchaseLimit]" dataDxfId="85"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[item1Featured]" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="83"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[item1Amount]" dataDxfId="82"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[item1Sku]" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="80"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[item2Amount]" dataDxfId="79"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[item2Sku]" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="77"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[item3Amount]" dataDxfId="76"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[item3Sku]" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="70"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="69"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="68"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="67"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="66"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="65"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="64"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[durationMinutes]" dataDxfId="63"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="62"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="61"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="60"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="59"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="58"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="57"/>
-    <tableColumn id="47" xr3:uid="{AED225FC-C091-2342-9B9A-0BC4A5AA4B98}" name="[minNumberOfPurchases]" dataDxfId="26"/>
-    <tableColumn id="48" xr3:uid="{EDC99988-F22B-2C41-BBCD-4DF3558834B7}" name="[minutesSinceLastPurchase]" dataDxfId="0"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="56"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="55"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="54"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="53"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="52"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="51"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="50"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="49"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="48"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="47"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="46"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="45"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="44"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="87"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="86"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="85"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="84"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="83"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="82"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="81"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="80"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="79"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="78"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="77"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="76"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="75"/>
+    <tableColumn id="7" name="[order]" dataDxfId="74"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="73"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="72"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="71"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="70"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="69"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="68"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="67"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="66"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="65"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="64"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="63"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="62"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="61"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="60"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="59"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="58"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="57"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="56"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="55"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
-  <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="offerPacksDefinitions_OLD" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="38"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="[paramValue]" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[itemType]" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[itemAmount]" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[itemSku]" dataDxfId="34"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="[itemFeatured]" dataDxfId="33"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="[minAppVersion]" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[order]" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="[refPrice]" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[discount]" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[iapSku]" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="27"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
+    <tableColumn id="4" name="[order]" dataDxfId="4"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4285,45 +4294,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
     <col min="8" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.875" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
     <col min="27" max="31" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.1640625" customWidth="1"/>
-    <col min="33" max="33" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.33203125" customWidth="1"/>
+    <col min="32" max="32" width="20.125" customWidth="1"/>
+    <col min="33" max="33" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.375" customWidth="1"/>
     <col min="35" max="39" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.83203125" customWidth="1"/>
-    <col min="41" max="41" width="16.1640625" customWidth="1"/>
-    <col min="42" max="42" width="14.6640625" customWidth="1"/>
-    <col min="43" max="43" width="20.1640625" customWidth="1"/>
+    <col min="40" max="40" width="16.875" customWidth="1"/>
+    <col min="41" max="41" width="16.125" customWidth="1"/>
+    <col min="42" max="42" width="14.625" customWidth="1"/>
+    <col min="43" max="43" width="20.125" customWidth="1"/>
     <col min="44" max="47" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:49" s="25" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:49" s="25" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
       <c r="Q1" s="16" t="s">
         <v>29</v>
       </c>
@@ -4362,7 +4371,7 @@
       <c r="AV1" s="66"/>
       <c r="AW1" s="66"/>
     </row>
-    <row r="2" spans="2:49" ht="135" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:49" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4508,7 +4517,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
@@ -4519,37 +4528,37 @@
         <v>151</v>
       </c>
       <c r="E3" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="48">
         <v>1</v>
       </c>
       <c r="G3" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="I3" s="43" t="s">
-        <v>151</v>
+        <v>27</v>
+      </c>
+      <c r="I3" s="43">
+        <v>3</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="K3" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="L3" s="47" t="s">
-        <v>151</v>
+        <v>19</v>
+      </c>
+      <c r="L3" s="47">
+        <v>80</v>
       </c>
       <c r="M3" s="47" t="s">
         <v>151</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>151</v>
+        <v>21</v>
+      </c>
+      <c r="O3" s="42">
+        <v>30000</v>
       </c>
       <c r="P3" s="42" t="s">
         <v>151</v>
@@ -4560,38 +4569,36 @@
       <c r="R3" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="S3" s="30">
-        <v>0.5</v>
+      <c r="S3" s="67" t="s">
+        <v>178</v>
       </c>
       <c r="T3" s="26" t="s">
         <v>104</v>
       </c>
       <c r="U3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="W3" s="36" t="s">
-        <v>151</v>
+        <v>202</v>
+      </c>
+      <c r="V3" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" s="36">
+        <v>0</v>
       </c>
       <c r="X3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z3" s="39" t="s">
-        <v>151</v>
-      </c>
+      <c r="Y3" s="36">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="39"/>
       <c r="AA3" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB3" s="39" t="s">
-        <v>151</v>
+      <c r="AB3" s="39">
+        <v>1440</v>
       </c>
       <c r="AC3" s="37" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="AD3" s="37" t="s">
         <v>151</v>
@@ -4599,8 +4606,8 @@
       <c r="AE3" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AF3" s="37" t="s">
-        <v>151</v>
+      <c r="AF3" s="37">
+        <v>4</v>
       </c>
       <c r="AG3" s="37" t="s">
         <v>151</v>
@@ -4641,8 +4648,8 @@
       <c r="AS3" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AT3" s="37" t="s">
-        <v>151</v>
+      <c r="AT3" s="68" t="s">
+        <v>203</v>
       </c>
       <c r="AU3" s="37" t="s">
         <v>151</v>
@@ -4654,7 +4661,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
@@ -4800,7 +4807,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
@@ -4946,7 +4953,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -5092,7 +5099,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
@@ -5238,7 +5245,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
@@ -5384,7 +5391,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
@@ -5530,7 +5537,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
@@ -5676,7 +5683,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
@@ -5822,7 +5829,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
@@ -5968,7 +5975,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
@@ -6114,7 +6121,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>3</v>
       </c>
@@ -6260,7 +6267,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
@@ -6406,7 +6413,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
@@ -6552,7 +6559,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>3</v>
       </c>
@@ -6698,7 +6705,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>3</v>
       </c>
@@ -6844,7 +6851,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
@@ -6990,7 +6997,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
@@ -7136,7 +7143,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>3</v>
       </c>
@@ -7282,7 +7289,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
@@ -7428,7 +7435,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
@@ -7572,7 +7579,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>3</v>
       </c>
@@ -7718,7 +7725,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>3</v>
       </c>
@@ -7862,7 +7869,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>3</v>
       </c>
@@ -8008,7 +8015,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>3</v>
       </c>
@@ -8154,7 +8161,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>3</v>
       </c>
@@ -8300,7 +8307,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>3</v>
       </c>
@@ -8446,7 +8453,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>3</v>
       </c>
@@ -8592,7 +8599,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>3</v>
       </c>
@@ -8736,7 +8743,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="2:49" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>3</v>
       </c>
@@ -8896,31 +8903,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8939,7 +8946,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="2:16" s="16" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" s="16" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
@@ -8953,7 +8960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="127" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
@@ -8994,7 +9001,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -9025,7 +9032,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -9052,7 +9059,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -9075,7 +9082,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -9098,7 +9105,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -9119,7 +9126,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -9140,7 +9147,7 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -9161,7 +9168,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -9182,7 +9189,7 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
@@ -9203,7 +9210,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -9224,7 +9231,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -9245,7 +9252,7 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -9276,7 +9283,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -9303,7 +9310,7 @@
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -9326,7 +9333,7 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -9349,7 +9356,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -9370,7 +9377,7 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -9391,7 +9398,7 @@
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -9412,7 +9419,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -9433,7 +9440,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -9454,7 +9461,7 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
@@ -9475,7 +9482,7 @@
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -9506,7 +9513,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
@@ -9533,7 +9540,7 @@
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
@@ -9556,7 +9563,7 @@
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
@@ -9579,7 +9586,7 @@
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -9600,7 +9607,7 @@
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -9621,7 +9628,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -9642,7 +9649,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -9663,7 +9670,7 @@
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
@@ -9684,7 +9691,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -9705,7 +9712,7 @@
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
@@ -9726,7 +9733,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
@@ -9747,7 +9754,7 @@
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
@@ -9778,7 +9785,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
@@ -9801,7 +9808,7 @@
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
@@ -9824,7 +9831,7 @@
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
@@ -9845,7 +9852,7 @@
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
@@ -9876,7 +9883,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
@@ -9901,7 +9908,7 @@
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
@@ -9924,132 +9931,132 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="41" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="36" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="18" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10061,13 +10068,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationData!$B$4:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>ValidationData!$D$4:$D$31</xm:f>
           </x14:formula1>
@@ -10080,19 +10087,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>48</v>
       </c>
@@ -10101,10 +10108,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -10112,7 +10119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -10120,7 +10127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -10128,13 +10135,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -10142,7 +10149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -10150,7 +10157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>151</v>
       </c>
@@ -10158,107 +10165,107 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Content - Add promoted IAPs
Former-commit-id: 9477efff2846f77edb927e477401f229d4c8e1f6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="207">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -640,6 +640,15 @@
   </si>
   <si>
     <t>6:999</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.promoted3</t>
+  </si>
+  <si>
+    <t>promoted3</t>
+  </si>
+  <si>
+    <t>1.10</t>
   </si>
 </sst>
 </file>
@@ -1232,551 +1241,23 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2054,6 +1535,534 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3920,8 +3929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AW32" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90">
-  <autoFilter ref="B2:AW32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AW33" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90">
+  <autoFilter ref="B2:AW33"/>
   <tableColumns count="48">
     <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="89"/>
     <tableColumn id="2" name="[sku]" dataDxfId="88"/>
@@ -3977,22 +3986,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
   <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
-    <tableColumn id="4" name="[order]" dataDxfId="4"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="37"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="36"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="35"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="34"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="33"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="32"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="31"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="30"/>
+    <tableColumn id="4" name="[order]" dataDxfId="29"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="28"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="27"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="26"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4295,10 +4304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AW32"/>
+  <dimension ref="B1:AW33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4342,34 +4351,34 @@
       <c r="S1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="65" t="s">
+      <c r="Z1" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="65"/>
+      <c r="AA1" s="67"/>
       <c r="AB1" s="49"/>
-      <c r="AC1" s="66" t="s">
+      <c r="AC1" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="66"/>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="66"/>
-      <c r="AV1" s="66"/>
-      <c r="AW1" s="66"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="68"/>
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="68"/>
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
     </row>
     <row r="2" spans="2:49" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -4569,7 +4578,7 @@
       <c r="R3" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="S3" s="67" t="s">
+      <c r="S3" s="65" t="s">
         <v>178</v>
       </c>
       <c r="T3" s="26" t="s">
@@ -4648,7 +4657,7 @@
       <c r="AS3" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AT3" s="68" t="s">
+      <c r="AT3" s="66" t="s">
         <v>203</v>
       </c>
       <c r="AU3" s="37" t="s">
@@ -8886,6 +8895,144 @@
         <v>151</v>
       </c>
       <c r="AW32" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="48">
+        <v>1</v>
+      </c>
+      <c r="G33" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="43">
+        <v>100</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="K33" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="47">
+        <v>20000</v>
+      </c>
+      <c r="M33" s="47"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="32">
+        <v>1</v>
+      </c>
+      <c r="R33" s="29">
+        <v>4.99</v>
+      </c>
+      <c r="S33" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="T33" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="U33" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V33" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="W33" s="36">
+        <v>0</v>
+      </c>
+      <c r="X33" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y33" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z33" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA33" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB33" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC33" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF33" s="37">
+        <v>4</v>
+      </c>
+      <c r="AG33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV33" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW33" s="37" t="s">
         <v>151</v>
       </c>
     </row>
@@ -9931,127 +10078,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="24" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="39" priority="25">
+    <cfRule type="expression" dxfId="22" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="36" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="35" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="26" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Content - Fix bug with offers
Former-commit-id: 0ecd581cca229fcd8e78e55ee272468126af0339
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1291,12 +1291,6 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1347,6 +1341,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4401,8 +4401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4446,34 +4446,34 @@
       <c r="S1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="67" t="s">
+      <c r="Z1" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="67"/>
+      <c r="AA1" s="84"/>
       <c r="AB1" s="49"/>
-      <c r="AC1" s="68" t="s">
+      <c r="AC1" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="68"/>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="85"/>
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="85"/>
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="85"/>
+      <c r="AM1" s="85"/>
+      <c r="AN1" s="85"/>
+      <c r="AO1" s="85"/>
+      <c r="AP1" s="85"/>
+      <c r="AQ1" s="85"/>
+      <c r="AR1" s="85"/>
+      <c r="AS1" s="85"/>
+      <c r="AT1" s="85"/>
+      <c r="AU1" s="85"/>
+      <c r="AV1" s="85"/>
+      <c r="AW1" s="85"/>
     </row>
     <row r="2" spans="2:49" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -9132,17 +9132,17 @@
       </c>
     </row>
     <row r="34" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="D34" s="69" t="s">
         <v>207</v>
       </c>
-      <c r="E34" s="72" t="b">
-        <v>1</v>
+      <c r="E34" s="70" t="b">
+        <v>0</v>
       </c>
       <c r="F34" s="48">
         <v>1</v>
@@ -9150,16 +9150,16 @@
       <c r="G34" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="75"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="77">
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="75">
         <v>1</v>
       </c>
       <c r="R34" s="29">
@@ -9171,31 +9171,31 @@
       <c r="T34" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="U34" s="78" t="s">
+      <c r="U34" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="V34" s="79" t="b">
+      <c r="V34" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="W34" s="79">
+      <c r="W34" s="77">
         <v>0</v>
       </c>
-      <c r="X34" s="79" t="s">
+      <c r="X34" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="Y34" s="80">
+      <c r="Y34" s="78">
         <v>10</v>
       </c>
-      <c r="Z34" s="81" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA34" s="82" t="s">
+      <c r="Z34" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA34" s="80" t="s">
         <v>151</v>
       </c>
       <c r="AB34" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AC34" s="83" t="s">
+      <c r="AC34" s="81" t="s">
         <v>209</v>
       </c>
       <c r="AD34" s="37" t="s">
@@ -9207,10 +9207,10 @@
       <c r="AF34" s="37">
         <v>4</v>
       </c>
-      <c r="AG34" s="84" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH34" s="84" t="s">
+      <c r="AG34" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH34" s="82" t="s">
         <v>151</v>
       </c>
       <c r="AI34" s="37" t="s">
@@ -9231,10 +9231,10 @@
       <c r="AN34" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AO34" s="84" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP34" s="84" t="s">
+      <c r="AO34" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP34" s="82" t="s">
         <v>151</v>
       </c>
       <c r="AQ34" s="37" t="s">
@@ -9249,13 +9249,13 @@
       <c r="AT34" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AU34" s="84" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV34" s="84" t="s">
-        <v>151</v>
-      </c>
-      <c r="AW34" s="85" t="s">
+      <c r="AU34" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV34" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW34" s="83" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Content - Starter pack - 30 000 coins :D
Former-commit-id: 568fb19f4dda3375ce0968377ce210c7495bdcc8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -4401,8 +4401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4659,10 +4659,10 @@
         <v>151</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="42">
-        <v>30000</v>
+        <v>151</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>151</v>
       </c>
       <c r="P3" s="42" t="s">
         <v>151</v>
@@ -4673,8 +4673,8 @@
       <c r="R3" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="S3" s="65" t="s">
-        <v>178</v>
+      <c r="S3" s="65">
+        <v>0.85</v>
       </c>
       <c r="T3" s="26" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Content - Delta - Change starter pack from $2 to $5
Former-commit-id: b85101b8c8fb6b7bcc99040c40a58642dda6d9ea
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="210">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -4402,7 +4402,7 @@
   <dimension ref="B1:AW34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4632,7 +4632,7 @@
         <v>151</v>
       </c>
       <c r="E3" s="40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="48">
         <v>1</v>
@@ -5068,28 +5068,28 @@
         <v>151</v>
       </c>
       <c r="E6" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="48">
         <v>1</v>
       </c>
       <c r="G6" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>151</v>
+        <v>27</v>
+      </c>
+      <c r="I6" s="43">
+        <v>3</v>
       </c>
       <c r="J6" s="43" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="L6" s="47" t="s">
-        <v>151</v>
+        <v>19</v>
+      </c>
+      <c r="L6" s="47">
+        <v>80</v>
       </c>
       <c r="M6" s="47" t="s">
         <v>151</v>
@@ -5116,31 +5116,29 @@
         <v>108</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="V6" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="W6" s="36" t="s">
-        <v>151</v>
+        <v>202</v>
+      </c>
+      <c r="V6" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="W6" s="36">
+        <v>0</v>
       </c>
       <c r="X6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z6" s="39" t="s">
-        <v>151</v>
-      </c>
+      <c r="Y6" s="36">
+        <v>20</v>
+      </c>
+      <c r="Z6" s="39"/>
       <c r="AA6" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="AB6" s="39" t="s">
-        <v>151</v>
+      <c r="AB6" s="39">
+        <v>1440</v>
       </c>
       <c r="AC6" s="37" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="AD6" s="37" t="s">
         <v>151</v>
@@ -5148,8 +5146,8 @@
       <c r="AE6" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AF6" s="37" t="s">
-        <v>151</v>
+      <c r="AF6" s="37">
+        <v>4</v>
       </c>
       <c r="AG6" s="37" t="s">
         <v>151</v>
@@ -5190,8 +5188,8 @@
       <c r="AS6" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="AT6" s="37" t="s">
-        <v>151</v>
+      <c r="AT6" s="66" t="s">
+        <v>203</v>
       </c>
       <c r="AU6" s="37" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Content - Change discount % for new starter pack
Former-commit-id: d2b84056ff026850ed8c2fa81e39d607f0c86904
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -4401,8 +4401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5110,7 +5110,7 @@
         <v>99</v>
       </c>
       <c r="S6" s="30">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="T6" s="26" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Rotational Offers: Fix - Wrong Egg sku.
Former-commit-id: 810647cb333a3acfb579ce2488a4c005614eee40
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC2B415-0D77-3C49-AE62-CD477A7DF558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="32700" windowHeight="20535"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -810,7 +811,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4755,81 +4756,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY70" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92">
-  <autoFilter ref="B2:AY70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY70" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92">
+  <autoFilter ref="B2:AY70" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="50">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="91"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="89"/>
-    <tableColumn id="49" name="[type]" dataDxfId="88"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="87"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="86"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="85"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="84"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="83"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="82"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="81"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="80"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="79"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="78"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="77"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="76"/>
-    <tableColumn id="7" name="[order]" dataDxfId="75"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="74"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="73"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="72"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="71"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="70"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="69"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="68"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="67"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="66"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="65"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="64"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="63"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="62"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="61"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="60"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="59"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="58"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="57"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="56"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="55"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="90"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[uniqueId]" dataDxfId="89"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[type]" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="87"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[purchaseLimit]" dataDxfId="86"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[item1Featured]" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="84"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[item1Amount]" dataDxfId="83"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[item1Sku]" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="81"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[item2Amount]" dataDxfId="80"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[item2Sku]" dataDxfId="79"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="78"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[item3Amount]" dataDxfId="77"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[item3Sku]" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="73"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="72"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="71"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="70"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="69"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="68"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="67"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="66"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="65"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[durationMinutes]" dataDxfId="64"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="63"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="62"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="61"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="60"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="59"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="58"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[maxSpent]" dataDxfId="57"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[minNumberOfPurchases]" dataDxfId="56"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[minutesSinceLastPurchase]" dataDxfId="55"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="54"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="53"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="52"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="51"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="50"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="49"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="48"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="47"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="46"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="45"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="44"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="43"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="B4:N44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="B4:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
-    <tableColumn id="4" name="[order]" dataDxfId="4"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="[paramValue]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[itemType]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[itemAmount]" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[itemSku]" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="[itemFeatured]" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="[minAppVersion]" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[order]" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="[refPrice]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[discount]" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[iapSku]" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5131,51 +5132,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AY70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="32" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" customWidth="1"/>
-    <col min="34" max="34" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="19.375" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="19.33203125" customWidth="1"/>
     <col min="37" max="41" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.875" customWidth="1"/>
-    <col min="43" max="43" width="16.125" customWidth="1"/>
-    <col min="44" max="44" width="14.625" customWidth="1"/>
-    <col min="45" max="45" width="20.125" customWidth="1"/>
+    <col min="42" max="42" width="16.83203125" customWidth="1"/>
+    <col min="43" max="43" width="16.1640625" customWidth="1"/>
+    <col min="44" max="44" width="14.6640625" customWidth="1"/>
+    <col min="45" max="45" width="20.1640625" customWidth="1"/>
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="24" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="24" customFormat="1" ht="135" x14ac:dyDescent="0.2">
       <c r="R1" s="16" t="s">
         <v>29</v>
       </c>
@@ -5215,7 +5216,7 @@
       <c r="AX1" s="132"/>
       <c r="AY1" s="132"/>
     </row>
-    <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:51" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -5367,7 +5368,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B3" s="44" t="s">
         <v>3</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B4" s="44" t="s">
         <v>3</v>
       </c>
@@ -5669,7 +5670,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
@@ -5821,7 +5822,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -5971,7 +5972,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B7" s="44" t="s">
         <v>3</v>
       </c>
@@ -6123,7 +6124,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B8" s="44" t="s">
         <v>3</v>
       </c>
@@ -6275,7 +6276,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
@@ -6579,7 +6580,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B11" s="44" t="s">
         <v>3</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B12" s="44" t="s">
         <v>3</v>
       </c>
@@ -6883,7 +6884,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B13" s="44" t="s">
         <v>3</v>
       </c>
@@ -7035,7 +7036,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B14" s="44" t="s">
         <v>3</v>
       </c>
@@ -7187,7 +7188,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B15" s="44" t="s">
         <v>3</v>
       </c>
@@ -7339,7 +7340,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -7491,7 +7492,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B17" s="44" t="s">
         <v>3</v>
       </c>
@@ -7643,7 +7644,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -7795,7 +7796,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B19" s="44" t="s">
         <v>3</v>
       </c>
@@ -7947,7 +7948,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B20" s="44" t="s">
         <v>3</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
         <v>3</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B22" s="44" t="s">
         <v>3</v>
       </c>
@@ -8403,7 +8404,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B23" s="58" t="s">
         <v>3</v>
       </c>
@@ -8553,7 +8554,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -8705,7 +8706,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B25" s="44" t="s">
         <v>3</v>
       </c>
@@ -8855,7 +8856,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -9007,7 +9008,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B27" s="44" t="s">
         <v>3</v>
       </c>
@@ -9159,7 +9160,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B29" s="44" t="s">
         <v>3</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B30" s="44" t="s">
         <v>3</v>
       </c>
@@ -9615,7 +9616,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B31" s="44" t="s">
         <v>3</v>
       </c>
@@ -9765,7 +9766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B32" s="44" t="s">
         <v>3</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B33" s="44" t="s">
         <v>3</v>
       </c>
@@ -10061,7 +10062,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B34" s="100" t="s">
         <v>3</v>
       </c>
@@ -10195,7 +10196,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B35" s="116" t="s">
         <v>3</v>
       </c>
@@ -10233,7 +10234,7 @@
         <v>4</v>
       </c>
       <c r="N35" s="120" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="O35" s="121"/>
       <c r="P35" s="121"/>
@@ -10342,7 +10343,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B36" s="42" t="s">
         <v>3</v>
       </c>
@@ -10483,7 +10484,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B37" s="42" t="s">
         <v>3</v>
       </c>
@@ -10624,7 +10625,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B38" s="42" t="s">
         <v>3</v>
       </c>
@@ -10765,7 +10766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B39" s="42" t="s">
         <v>3</v>
       </c>
@@ -10910,7 +10911,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B40" s="42" t="s">
         <v>3</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B41" s="42" t="s">
         <v>3</v>
       </c>
@@ -11206,7 +11207,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B42" s="42" t="s">
         <v>3</v>
       </c>
@@ -11351,7 +11352,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B43" s="42" t="s">
         <v>3</v>
       </c>
@@ -11496,7 +11497,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B44" s="42" t="s">
         <v>3</v>
       </c>
@@ -11641,7 +11642,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B45" s="42" t="s">
         <v>3</v>
       </c>
@@ -11786,7 +11787,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B46" s="85" t="s">
         <v>3</v>
       </c>
@@ -11931,7 +11932,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B47" s="116" t="s">
         <v>3</v>
       </c>
@@ -12078,7 +12079,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B48" s="42" t="s">
         <v>3</v>
       </c>
@@ -12219,7 +12220,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B49" s="42" t="s">
         <v>3</v>
       </c>
@@ -12360,7 +12361,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B50" s="42" t="s">
         <v>3</v>
       </c>
@@ -12501,7 +12502,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B51" s="42" t="s">
         <v>3</v>
       </c>
@@ -12642,7 +12643,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B52" s="42" t="s">
         <v>3</v>
       </c>
@@ -12783,7 +12784,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B53" s="42" t="s">
         <v>3</v>
       </c>
@@ -12930,7 +12931,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B54" s="42" t="s">
         <v>3</v>
       </c>
@@ -13077,7 +13078,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B55" s="42" t="s">
         <v>3</v>
       </c>
@@ -13218,7 +13219,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B56" s="42" t="s">
         <v>3</v>
       </c>
@@ -13363,7 +13364,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B57" s="42" t="s">
         <v>3</v>
       </c>
@@ -13504,7 +13505,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B58" s="85" t="s">
         <v>3</v>
       </c>
@@ -13649,7 +13650,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B59" s="70" t="s">
         <v>3</v>
       </c>
@@ -13796,7 +13797,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B60" s="42" t="s">
         <v>3</v>
       </c>
@@ -13943,7 +13944,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B61" s="42" t="s">
         <v>3</v>
       </c>
@@ -14096,7 +14097,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B62" s="42" t="s">
         <v>3</v>
       </c>
@@ -14237,7 +14238,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B63" s="42" t="s">
         <v>3</v>
       </c>
@@ -14378,7 +14379,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B64" s="42" t="s">
         <v>3</v>
       </c>
@@ -14519,7 +14520,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B65" s="42" t="s">
         <v>3</v>
       </c>
@@ -14670,7 +14671,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B66" s="42" t="s">
         <v>3</v>
       </c>
@@ -14821,7 +14822,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B67" s="42" t="s">
         <v>3</v>
       </c>
@@ -14972,7 +14973,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B68" s="42" t="s">
         <v>3</v>
       </c>
@@ -15117,7 +15118,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B69" s="42" t="s">
         <v>3</v>
       </c>
@@ -15258,7 +15259,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B70" s="42" t="s">
         <v>3</v>
       </c>
@@ -15417,31 +15418,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -15460,7 +15461,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="2:16" s="16" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" s="16" customFormat="1" ht="195" x14ac:dyDescent="0.2">
       <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
@@ -15474,7 +15475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="129.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="127" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
@@ -15515,7 +15516,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -15546,7 +15547,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -15573,7 +15574,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -15596,7 +15597,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -15619,7 +15620,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -15640,7 +15641,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -15661,7 +15662,7 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -15682,7 +15683,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -15703,7 +15704,7 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
@@ -15724,7 +15725,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -15745,7 +15746,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -15766,7 +15767,7 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -15797,7 +15798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -15824,7 +15825,7 @@
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -15847,7 +15848,7 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -15870,7 +15871,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -15891,7 +15892,7 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -15912,7 +15913,7 @@
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -15933,7 +15934,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -15954,7 +15955,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -15975,7 +15976,7 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
@@ -15996,7 +15997,7 @@
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -16027,7 +16028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
@@ -16054,7 +16055,7 @@
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
@@ -16077,7 +16078,7 @@
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
@@ -16100,7 +16101,7 @@
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -16121,7 +16122,7 @@
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -16142,7 +16143,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -16163,7 +16164,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -16184,7 +16185,7 @@
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
@@ -16205,7 +16206,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -16226,7 +16227,7 @@
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
@@ -16247,7 +16248,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
@@ -16268,7 +16269,7 @@
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
@@ -16299,7 +16300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
@@ -16322,7 +16323,7 @@
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
@@ -16345,7 +16346,7 @@
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
@@ -16366,7 +16367,7 @@
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
@@ -16397,7 +16398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
@@ -16422,7 +16423,7 @@
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
@@ -16570,7 +16571,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B44" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"&lt;Definition&gt;,&lt;Item&gt;,&lt;Param&gt;"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16582,13 +16583,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>ValidationData!$B$4:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>ValidationData!$D$4:$D$31</xm:f>
           </x14:formula1>
@@ -16601,19 +16602,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
         <v>48</v>
       </c>
@@ -16622,10 +16623,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -16633,7 +16634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -16641,7 +16642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -16649,13 +16650,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -16663,7 +16664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -16671,7 +16672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>151</v>
       </c>
@@ -16679,107 +16680,107 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Content - Change pack content for DOS
Former-commit-id: 3c13558d74751d3a323603fed496ed4e00c1019a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2795" uniqueCount="295">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -5242,8 +5242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35:U70"/>
+    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10900,12 +10900,8 @@
       <c r="K39" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="L39" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="M39" s="48">
-        <v>2222</v>
-      </c>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
       <c r="N39" s="48"/>
       <c r="O39" s="49"/>
       <c r="P39" s="49"/>
@@ -11044,12 +11040,8 @@
       <c r="K40" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="L40" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40" s="48">
-        <v>3333</v>
-      </c>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
       <c r="N40" s="48"/>
       <c r="O40" s="49"/>
       <c r="P40" s="49"/>

</xml_diff>

<commit_message>
Content - Final balance for the new progression offers
Former-commit-id: 718cce36f5f2e7569dd1691e9a71b008c428f2b2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="322">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -978,9 +978,6 @@
     <t>1.26</t>
   </si>
   <si>
-    <t>19:999</t>
-  </si>
-  <si>
     <t>TID_STORE_PACK_SMALLGATCHAPACK</t>
   </si>
   <si>
@@ -991,6 +988,12 @@
   </si>
   <si>
     <t>TID_STORE_PACK_MEGAHCPACKCLASSIC</t>
+  </si>
+  <si>
+    <t>18:999</t>
+  </si>
+  <si>
+    <t>28:999</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1694,9 +1697,6 @@
     <xf numFmtId="0" fontId="10" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1768,12 +1768,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1874,264 +1868,17 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="97">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3049,6 +2796,123 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -4160,6 +4024,122 @@
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -4955,6 +4935,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4983,84 +4983,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY76" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY76" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="B2:AY76"/>
   <sortState ref="B3:AY76">
     <sortCondition descending="1" ref="F2:F76"/>
   </sortState>
   <tableColumns count="50">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="93"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="91"/>
-    <tableColumn id="49" name="[type]" dataDxfId="90"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="89"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="88"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="87"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="86"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="85"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="84"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="83"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="82"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="81"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="80"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="79"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="78"/>
-    <tableColumn id="7" name="[order]" dataDxfId="77"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="7"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="5"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="76"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="75"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="74"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="73"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="72"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="71"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="70"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="69"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="68"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="67"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="66"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="65"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="64"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="63"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="62"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="61"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="60"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="59"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="58"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="57"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="56"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="55"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="54"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="53"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="52"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="2"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="0"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="1"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="51"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="50"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="91"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="89"/>
+    <tableColumn id="49" name="[type]" dataDxfId="88"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="87"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="86"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="85"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="84"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="83"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="82"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="81"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="80"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="79"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="78"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="77"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="76"/>
+    <tableColumn id="7" name="[order]" dataDxfId="75"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="74"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="73"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="72"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="71"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="70"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="69"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="68"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="67"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="66"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="65"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="64"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="63"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="62"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="61"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="60"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="59"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="58"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="57"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="56"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="55"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="20"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="19"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="18"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="17"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="16"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="15"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="14"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="13"/>
-    <tableColumn id="4" name="[order]" dataDxfId="12"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="11"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="10"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="9"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
+    <tableColumn id="4" name="[order]" dataDxfId="4"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5365,8 +5365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AV7" sqref="AA7:AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5417,35 +5417,35 @@
       <c r="T1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="114" t="s">
+      <c r="AA1" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="114"/>
+      <c r="AB1" s="146"/>
       <c r="AC1" s="32"/>
-      <c r="AD1" s="115" t="s">
+      <c r="AD1" s="147" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" s="115"/>
-      <c r="AF1" s="115"/>
-      <c r="AG1" s="115"/>
-      <c r="AH1" s="115"/>
-      <c r="AI1" s="115"/>
-      <c r="AJ1" s="115"/>
-      <c r="AK1" s="115"/>
-      <c r="AL1" s="115"/>
-      <c r="AM1" s="115"/>
-      <c r="AN1" s="115"/>
-      <c r="AO1" s="115"/>
-      <c r="AP1" s="115"/>
-      <c r="AQ1" s="115"/>
-      <c r="AR1" s="115"/>
-      <c r="AS1" s="115"/>
-      <c r="AT1" s="115"/>
-      <c r="AU1" s="115"/>
-      <c r="AV1" s="115"/>
-      <c r="AW1" s="115"/>
-      <c r="AX1" s="115"/>
-      <c r="AY1" s="115"/>
+      <c r="AE1" s="147"/>
+      <c r="AF1" s="147"/>
+      <c r="AG1" s="147"/>
+      <c r="AH1" s="147"/>
+      <c r="AI1" s="147"/>
+      <c r="AJ1" s="147"/>
+      <c r="AK1" s="147"/>
+      <c r="AL1" s="147"/>
+      <c r="AM1" s="147"/>
+      <c r="AN1" s="147"/>
+      <c r="AO1" s="147"/>
+      <c r="AP1" s="147"/>
+      <c r="AQ1" s="147"/>
+      <c r="AR1" s="147"/>
+      <c r="AS1" s="147"/>
+      <c r="AT1" s="147"/>
+      <c r="AU1" s="147"/>
+      <c r="AV1" s="147"/>
+      <c r="AW1" s="147"/>
+      <c r="AX1" s="147"/>
+      <c r="AY1" s="147"/>
     </row>
     <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5634,7 +5634,7 @@
         <v>27</v>
       </c>
       <c r="M3" s="45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" s="45" t="s">
         <v>250</v>
@@ -5649,7 +5649,7 @@
         <v>151</v>
       </c>
       <c r="R3" s="47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S3" s="48" t="s">
         <v>126</v>
@@ -5739,7 +5739,7 @@
         <v>151</v>
       </c>
       <c r="AV3" s="34" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AW3" s="27" t="s">
         <v>151</v>
@@ -5813,7 +5813,7 @@
         <v>107</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W4" s="35" t="b">
         <v>1</v>
@@ -5891,7 +5891,7 @@
         <v>151</v>
       </c>
       <c r="AV4" s="34" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AW4" s="27" t="s">
         <v>151</v>
@@ -6191,7 +6191,7 @@
         <v>151</v>
       </c>
       <c r="AV6" s="34" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AW6" s="27" t="s">
         <v>151</v>
@@ -6253,7 +6253,7 @@
         <v>151</v>
       </c>
       <c r="R7" s="47">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="S7" s="48" t="s">
         <v>99</v>
@@ -6415,7 +6415,7 @@
         <v>182</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="W8" s="35" t="b">
         <v>1</v>
@@ -6489,7 +6489,7 @@
         <v>151</v>
       </c>
       <c r="AV8" s="34" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AW8" s="27" t="s">
         <v>151</v>
@@ -6551,7 +6551,7 @@
         <v>151</v>
       </c>
       <c r="R9" s="47">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="S9" s="48" t="s">
         <v>126</v>
@@ -6652,150 +6652,150 @@
       </c>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="133" t="s">
+      <c r="C10" s="130" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="134" t="s">
+      <c r="D10" s="131" t="s">
         <v>173</v>
       </c>
-      <c r="E10" s="135" t="s">
+      <c r="E10" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="F10" s="136" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="136">
-        <v>1</v>
-      </c>
-      <c r="H10" s="137" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="137" t="s">
+      <c r="F10" s="133" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="133">
+        <v>1</v>
+      </c>
+      <c r="H10" s="134" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="137">
+      <c r="J10" s="134">
         <v>900</v>
       </c>
-      <c r="K10" s="137" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" s="138" t="s">
+      <c r="K10" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="L10" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="138">
+      <c r="M10" s="135">
         <v>300000</v>
       </c>
-      <c r="N10" s="138" t="s">
-        <v>151</v>
-      </c>
-      <c r="O10" s="139" t="s">
-        <v>151</v>
-      </c>
-      <c r="P10" s="139" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q10" s="139" t="s">
-        <v>151</v>
-      </c>
-      <c r="R10" s="140">
-        <v>8</v>
-      </c>
-      <c r="S10" s="141" t="s">
+      <c r="N10" s="135" t="s">
+        <v>151</v>
+      </c>
+      <c r="O10" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="P10" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q10" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="R10" s="137">
+        <v>9</v>
+      </c>
+      <c r="S10" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="T10" s="142">
+      <c r="T10" s="139">
         <v>-1</v>
       </c>
-      <c r="U10" s="143" t="s">
+      <c r="U10" s="140" t="s">
         <v>186</v>
       </c>
-      <c r="V10" s="144" t="s">
-        <v>320</v>
-      </c>
-      <c r="W10" s="145" t="b">
-        <v>1</v>
-      </c>
-      <c r="X10" s="145">
+      <c r="V10" s="141" t="s">
+        <v>319</v>
+      </c>
+      <c r="W10" s="142" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" s="142">
         <v>0</v>
       </c>
-      <c r="Y10" s="145" t="s">
+      <c r="Y10" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="Z10" s="145">
+      <c r="Z10" s="142">
         <v>10</v>
       </c>
-      <c r="AA10" s="146"/>
-      <c r="AB10" s="146" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC10" s="146">
+      <c r="AA10" s="143"/>
+      <c r="AB10" s="143" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC10" s="143">
         <v>2880</v>
       </c>
-      <c r="AD10" s="147" t="s">
+      <c r="AD10" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="AE10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG10" s="147">
+      <c r="AE10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG10" s="144">
         <v>4</v>
       </c>
-      <c r="AH10" s="147" t="s">
+      <c r="AH10" s="144" t="s">
         <v>190</v>
       </c>
-      <c r="AI10" s="147"/>
-      <c r="AJ10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV10" s="148" t="s">
-        <v>319</v>
-      </c>
-      <c r="AW10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX10" s="147" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY10" s="147" t="s">
+      <c r="AI10" s="144"/>
+      <c r="AJ10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV10" s="145" t="s">
+        <v>318</v>
+      </c>
+      <c r="AW10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX10" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY10" s="144" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6803,7 +6803,7 @@
       <c r="B11" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="128" t="s">
         <v>214</v>
       </c>
       <c r="D11" s="56" t="s">
@@ -6843,7 +6843,7 @@
       <c r="P11" s="60"/>
       <c r="Q11" s="60"/>
       <c r="R11" s="61">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S11" s="62" t="s">
         <v>99</v>
@@ -6982,8 +6982,8 @@
       <c r="O12" s="46"/>
       <c r="P12" s="46"/>
       <c r="Q12" s="46"/>
-      <c r="R12" s="47">
-        <v>10</v>
+      <c r="R12" s="61">
+        <v>20</v>
       </c>
       <c r="S12" s="48" t="s">
         <v>99</v>
@@ -7122,8 +7122,8 @@
       <c r="O13" s="46"/>
       <c r="P13" s="46"/>
       <c r="Q13" s="46"/>
-      <c r="R13" s="47">
-        <v>10</v>
+      <c r="R13" s="61">
+        <v>20</v>
       </c>
       <c r="S13" s="48" t="s">
         <v>126</v>
@@ -7262,8 +7262,8 @@
       <c r="O14" s="46"/>
       <c r="P14" s="46"/>
       <c r="Q14" s="46"/>
-      <c r="R14" s="47">
-        <v>10</v>
+      <c r="R14" s="61">
+        <v>20</v>
       </c>
       <c r="S14" s="48" t="s">
         <v>99</v>
@@ -7402,8 +7402,8 @@
       <c r="O15" s="46"/>
       <c r="P15" s="46"/>
       <c r="Q15" s="46"/>
-      <c r="R15" s="47">
-        <v>10</v>
+      <c r="R15" s="61">
+        <v>20</v>
       </c>
       <c r="S15" s="48" t="s">
         <v>125</v>
@@ -7542,8 +7542,8 @@
       <c r="O16" s="46"/>
       <c r="P16" s="46"/>
       <c r="Q16" s="46"/>
-      <c r="R16" s="47">
-        <v>10</v>
+      <c r="R16" s="61">
+        <v>20</v>
       </c>
       <c r="S16" s="48" t="s">
         <v>126</v>
@@ -7692,8 +7692,8 @@
         <v>100</v>
       </c>
       <c r="Q17" s="46"/>
-      <c r="R17" s="47">
-        <v>10</v>
+      <c r="R17" s="61">
+        <v>20</v>
       </c>
       <c r="S17" s="48" t="s">
         <v>99</v>
@@ -7836,8 +7836,8 @@
       <c r="O18" s="46"/>
       <c r="P18" s="46"/>
       <c r="Q18" s="46"/>
-      <c r="R18" s="47">
-        <v>10</v>
+      <c r="R18" s="61">
+        <v>20</v>
       </c>
       <c r="S18" s="48" t="s">
         <v>126</v>
@@ -7980,8 +7980,8 @@
       <c r="O19" s="46"/>
       <c r="P19" s="46"/>
       <c r="Q19" s="46"/>
-      <c r="R19" s="47">
-        <v>10</v>
+      <c r="R19" s="61">
+        <v>20</v>
       </c>
       <c r="S19" s="48" t="s">
         <v>99</v>
@@ -8124,8 +8124,8 @@
       <c r="O20" s="46"/>
       <c r="P20" s="46"/>
       <c r="Q20" s="46"/>
-      <c r="R20" s="47">
-        <v>10</v>
+      <c r="R20" s="61">
+        <v>20</v>
       </c>
       <c r="S20" s="48" t="s">
         <v>125</v>
@@ -8268,8 +8268,8 @@
       <c r="O21" s="46"/>
       <c r="P21" s="46"/>
       <c r="Q21" s="46"/>
-      <c r="R21" s="47">
-        <v>10</v>
+      <c r="R21" s="61">
+        <v>20</v>
       </c>
       <c r="S21" s="48" t="s">
         <v>99</v>
@@ -8412,8 +8412,8 @@
       <c r="O22" s="46"/>
       <c r="P22" s="46"/>
       <c r="Q22" s="46"/>
-      <c r="R22" s="47">
-        <v>10</v>
+      <c r="R22" s="61">
+        <v>20</v>
       </c>
       <c r="S22" s="48" t="s">
         <v>126</v>
@@ -8519,7 +8519,7 @@
       <c r="B23" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="119" t="s">
+      <c r="C23" s="116" t="s">
         <v>226</v>
       </c>
       <c r="D23" s="40" t="s">
@@ -8558,8 +8558,8 @@
       <c r="O23" s="46"/>
       <c r="P23" s="46"/>
       <c r="Q23" s="46"/>
-      <c r="R23" s="47">
-        <v>10</v>
+      <c r="R23" s="61">
+        <v>20</v>
       </c>
       <c r="S23" s="48" t="s">
         <v>99</v>
@@ -8665,7 +8665,7 @@
       <c r="B24" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="119" t="s">
+      <c r="C24" s="116" t="s">
         <v>227</v>
       </c>
       <c r="D24" s="40" t="s">
@@ -8698,8 +8698,8 @@
       <c r="O24" s="46"/>
       <c r="P24" s="46"/>
       <c r="Q24" s="46"/>
-      <c r="R24" s="47">
-        <v>10</v>
+      <c r="R24" s="61">
+        <v>20</v>
       </c>
       <c r="S24" s="48" t="s">
         <v>99</v>
@@ -8805,7 +8805,7 @@
       <c r="B25" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="119" t="s">
+      <c r="C25" s="116" t="s">
         <v>228</v>
       </c>
       <c r="D25" s="40" t="s">
@@ -8838,8 +8838,8 @@
       <c r="O25" s="46"/>
       <c r="P25" s="46"/>
       <c r="Q25" s="46"/>
-      <c r="R25" s="47">
-        <v>10</v>
+      <c r="R25" s="61">
+        <v>20</v>
       </c>
       <c r="S25" s="48" t="s">
         <v>126</v>
@@ -8945,7 +8945,7 @@
       <c r="B26" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="119" t="s">
+      <c r="C26" s="116" t="s">
         <v>229</v>
       </c>
       <c r="D26" s="40" t="s">
@@ -8978,8 +8978,8 @@
       <c r="O26" s="46"/>
       <c r="P26" s="46"/>
       <c r="Q26" s="46"/>
-      <c r="R26" s="47">
-        <v>10</v>
+      <c r="R26" s="61">
+        <v>20</v>
       </c>
       <c r="S26" s="48" t="s">
         <v>99</v>
@@ -9085,7 +9085,7 @@
       <c r="B27" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="119" t="s">
+      <c r="C27" s="116" t="s">
         <v>230</v>
       </c>
       <c r="D27" s="40" t="s">
@@ -9118,8 +9118,8 @@
       <c r="O27" s="46"/>
       <c r="P27" s="46"/>
       <c r="Q27" s="46"/>
-      <c r="R27" s="47">
-        <v>10</v>
+      <c r="R27" s="61">
+        <v>20</v>
       </c>
       <c r="S27" s="48" t="s">
         <v>126</v>
@@ -9225,7 +9225,7 @@
       <c r="B28" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="119" t="s">
+      <c r="C28" s="116" t="s">
         <v>231</v>
       </c>
       <c r="D28" s="40" t="s">
@@ -9258,8 +9258,8 @@
       <c r="O28" s="46"/>
       <c r="P28" s="46"/>
       <c r="Q28" s="46"/>
-      <c r="R28" s="47">
-        <v>10</v>
+      <c r="R28" s="61">
+        <v>20</v>
       </c>
       <c r="S28" s="48" t="s">
         <v>252</v>
@@ -9365,7 +9365,7 @@
       <c r="B29" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="119" t="s">
+      <c r="C29" s="116" t="s">
         <v>232</v>
       </c>
       <c r="D29" s="40" t="s">
@@ -9404,8 +9404,8 @@
       <c r="O29" s="46"/>
       <c r="P29" s="46"/>
       <c r="Q29" s="46"/>
-      <c r="R29" s="47">
-        <v>10</v>
+      <c r="R29" s="61">
+        <v>20</v>
       </c>
       <c r="S29" s="48" t="s">
         <v>126</v>
@@ -9511,7 +9511,7 @@
       <c r="B30" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="119" t="s">
+      <c r="C30" s="116" t="s">
         <v>233</v>
       </c>
       <c r="D30" s="40" t="s">
@@ -9550,8 +9550,8 @@
       <c r="O30" s="46"/>
       <c r="P30" s="46"/>
       <c r="Q30" s="46"/>
-      <c r="R30" s="47">
-        <v>10</v>
+      <c r="R30" s="61">
+        <v>20</v>
       </c>
       <c r="S30" s="48" t="s">
         <v>127</v>
@@ -9657,7 +9657,7 @@
       <c r="B31" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="119" t="s">
+      <c r="C31" s="116" t="s">
         <v>234</v>
       </c>
       <c r="D31" s="40" t="s">
@@ -9690,8 +9690,8 @@
       <c r="O31" s="46"/>
       <c r="P31" s="46"/>
       <c r="Q31" s="46"/>
-      <c r="R31" s="47">
-        <v>10</v>
+      <c r="R31" s="61">
+        <v>20</v>
       </c>
       <c r="S31" s="48" t="s">
         <v>252</v>
@@ -9797,7 +9797,7 @@
       <c r="B32" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="119" t="s">
+      <c r="C32" s="116" t="s">
         <v>235</v>
       </c>
       <c r="D32" s="40" t="s">
@@ -9834,8 +9834,8 @@
       <c r="O32" s="46"/>
       <c r="P32" s="46"/>
       <c r="Q32" s="46"/>
-      <c r="R32" s="47">
-        <v>10</v>
+      <c r="R32" s="61">
+        <v>20</v>
       </c>
       <c r="S32" s="48" t="s">
         <v>252</v>
@@ -9941,7 +9941,7 @@
       <c r="B33" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="119" t="s">
+      <c r="C33" s="116" t="s">
         <v>236</v>
       </c>
       <c r="D33" s="40" t="s">
@@ -9974,8 +9974,8 @@
       <c r="O33" s="46"/>
       <c r="P33" s="46"/>
       <c r="Q33" s="46"/>
-      <c r="R33" s="47">
-        <v>10</v>
+      <c r="R33" s="61">
+        <v>20</v>
       </c>
       <c r="S33" s="48" t="s">
         <v>99</v>
@@ -10118,252 +10118,252 @@
       <c r="O34" s="88"/>
       <c r="P34" s="88"/>
       <c r="Q34" s="88"/>
-      <c r="R34" s="89">
+      <c r="R34" s="61">
+        <v>20</v>
+      </c>
+      <c r="S34" s="89" t="s">
+        <v>126</v>
+      </c>
+      <c r="T34" s="113">
+        <v>-1</v>
+      </c>
+      <c r="U34" s="90" t="s">
+        <v>278</v>
+      </c>
+      <c r="V34" s="91" t="s">
+        <v>254</v>
+      </c>
+      <c r="W34" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="X34" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z34" s="92">
         <v>10</v>
       </c>
-      <c r="S34" s="90" t="s">
-        <v>126</v>
-      </c>
-      <c r="T34" s="116">
-        <v>-1</v>
-      </c>
-      <c r="U34" s="91" t="s">
-        <v>278</v>
-      </c>
-      <c r="V34" s="92" t="s">
-        <v>254</v>
-      </c>
-      <c r="W34" s="93" t="b">
-        <v>1</v>
-      </c>
-      <c r="X34" s="93">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="93" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z34" s="93">
-        <v>10</v>
-      </c>
-      <c r="AA34" s="94" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB34" s="94" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC34" s="94">
+      <c r="AA34" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB34" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC34" s="93">
         <v>2880</v>
       </c>
-      <c r="AD34" s="95" t="s">
+      <c r="AD34" s="94" t="s">
         <v>212</v>
       </c>
-      <c r="AE34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG34" s="95">
+      <c r="AE34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG34" s="94">
         <v>4</v>
       </c>
-      <c r="AH34" s="95" t="s">
+      <c r="AH34" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="AI34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ34" s="95" t="s">
+      <c r="AI34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ34" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="AK34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV34" s="117" t="s">
+      <c r="AK34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV34" s="114" t="s">
         <v>201</v>
       </c>
-      <c r="AW34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX34" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY34" s="95" t="s">
+      <c r="AW34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX34" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY34" s="94" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="35" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B35" s="98" t="s">
+      <c r="B35" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="126" t="s">
+      <c r="C35" s="123" t="s">
         <v>238</v>
       </c>
-      <c r="D35" s="98" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="98" t="s">
+      <c r="D35" s="97" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="97" t="s">
         <v>211</v>
       </c>
-      <c r="F35" s="99" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="99">
+      <c r="F35" s="98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="98">
         <v>-1</v>
       </c>
-      <c r="H35" s="100" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="100" t="s">
+      <c r="H35" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="100">
+      <c r="J35" s="99">
         <v>3</v>
       </c>
-      <c r="K35" s="100" t="s">
+      <c r="K35" s="99" t="s">
         <v>250</v>
       </c>
-      <c r="L35" s="101" t="s">
+      <c r="L35" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="M35" s="101">
+      <c r="M35" s="100">
         <v>3</v>
       </c>
-      <c r="N35" s="101" t="s">
+      <c r="N35" s="100" t="s">
         <v>188</v>
       </c>
-      <c r="O35" s="102"/>
-      <c r="P35" s="102"/>
-      <c r="Q35" s="102"/>
-      <c r="R35" s="103">
+      <c r="O35" s="101"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="101"/>
+      <c r="R35" s="61">
+        <v>20</v>
+      </c>
+      <c r="S35" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="T35" s="95">
+        <v>-1</v>
+      </c>
+      <c r="U35" s="104" t="s">
+        <v>279</v>
+      </c>
+      <c r="V35" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="W35" s="106" t="b">
+        <v>1</v>
+      </c>
+      <c r="X35" s="106">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="106" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z35" s="106">
         <v>10</v>
       </c>
-      <c r="S35" s="104" t="s">
-        <v>126</v>
-      </c>
-      <c r="T35" s="96">
-        <v>-1</v>
-      </c>
-      <c r="U35" s="105" t="s">
-        <v>279</v>
-      </c>
-      <c r="V35" s="106" t="s">
-        <v>254</v>
-      </c>
-      <c r="W35" s="107" t="b">
-        <v>1</v>
-      </c>
-      <c r="X35" s="107">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="107" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z35" s="107">
-        <v>10</v>
-      </c>
-      <c r="AA35" s="108" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB35" s="108" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC35" s="108">
+      <c r="AA35" s="107" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB35" s="107" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC35" s="107">
         <v>2880</v>
       </c>
-      <c r="AD35" s="109" t="s">
+      <c r="AD35" s="108" t="s">
         <v>212</v>
       </c>
-      <c r="AE35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG35" s="109">
+      <c r="AE35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG35" s="108">
         <v>4</v>
       </c>
-      <c r="AH35" s="109" t="s">
+      <c r="AH35" s="108" t="s">
         <v>190</v>
       </c>
-      <c r="AI35" s="109">
+      <c r="AI35" s="108">
         <v>20</v>
       </c>
-      <c r="AJ35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV35" s="97" t="s">
+      <c r="AJ35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV35" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="AW35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX35" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY35" s="109" t="s">
+      <c r="AW35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX35" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY35" s="108" t="s">
         <v>151</v>
       </c>
     </row>
@@ -10371,7 +10371,7 @@
       <c r="B36" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="119" t="s">
+      <c r="C36" s="116" t="s">
         <v>239</v>
       </c>
       <c r="D36" s="40" t="s">
@@ -10410,13 +10410,13 @@
       <c r="O36" s="46"/>
       <c r="P36" s="46"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="47">
-        <v>10</v>
+      <c r="R36" s="61">
+        <v>20</v>
       </c>
       <c r="S36" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T36" s="96">
+      <c r="T36" s="95">
         <v>-1</v>
       </c>
       <c r="U36" s="50" t="s">
@@ -10517,7 +10517,7 @@
       <c r="B37" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="119" t="s">
+      <c r="C37" s="116" t="s">
         <v>240</v>
       </c>
       <c r="D37" s="40" t="s">
@@ -10562,13 +10562,13 @@
       <c r="Q37" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="R37" s="47">
-        <v>10</v>
+      <c r="R37" s="61">
+        <v>20</v>
       </c>
       <c r="S37" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T37" s="96">
+      <c r="T37" s="95">
         <v>-1</v>
       </c>
       <c r="U37" s="50" t="s">
@@ -10669,7 +10669,7 @@
       <c r="B38" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="119" t="s">
+      <c r="C38" s="116" t="s">
         <v>241</v>
       </c>
       <c r="D38" s="40" t="s">
@@ -10702,13 +10702,13 @@
       <c r="O38" s="46"/>
       <c r="P38" s="46"/>
       <c r="Q38" s="46"/>
-      <c r="R38" s="47">
-        <v>10</v>
+      <c r="R38" s="61">
+        <v>20</v>
       </c>
       <c r="S38" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T38" s="96">
+      <c r="T38" s="95">
         <v>-1</v>
       </c>
       <c r="U38" s="50" t="s">
@@ -10809,7 +10809,7 @@
       <c r="B39" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="119" t="s">
+      <c r="C39" s="116" t="s">
         <v>242</v>
       </c>
       <c r="D39" s="40" t="s">
@@ -10842,13 +10842,13 @@
       <c r="O39" s="46"/>
       <c r="P39" s="46"/>
       <c r="Q39" s="46"/>
-      <c r="R39" s="47">
-        <v>10</v>
+      <c r="R39" s="61">
+        <v>20</v>
       </c>
       <c r="S39" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="T39" s="96">
+      <c r="T39" s="95">
         <v>-1</v>
       </c>
       <c r="U39" s="50" t="s">
@@ -10949,7 +10949,7 @@
       <c r="B40" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="119" t="s">
+      <c r="C40" s="116" t="s">
         <v>243</v>
       </c>
       <c r="D40" s="40" t="s">
@@ -10982,13 +10982,13 @@
       <c r="O40" s="46"/>
       <c r="P40" s="46"/>
       <c r="Q40" s="46"/>
-      <c r="R40" s="47">
-        <v>10</v>
+      <c r="R40" s="61">
+        <v>20</v>
       </c>
       <c r="S40" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T40" s="96">
+      <c r="T40" s="95">
         <v>-1</v>
       </c>
       <c r="U40" s="50" t="s">
@@ -11089,7 +11089,7 @@
       <c r="B41" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="119" t="s">
+      <c r="C41" s="116" t="s">
         <v>244</v>
       </c>
       <c r="D41" s="40" t="s">
@@ -11132,13 +11132,13 @@
         <v>100</v>
       </c>
       <c r="Q41" s="46"/>
-      <c r="R41" s="47">
-        <v>10</v>
+      <c r="R41" s="61">
+        <v>20</v>
       </c>
       <c r="S41" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T41" s="96">
+      <c r="T41" s="95">
         <v>-1</v>
       </c>
       <c r="U41" s="50" t="s">
@@ -11239,7 +11239,7 @@
       <c r="B42" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="119" t="s">
+      <c r="C42" s="116" t="s">
         <v>245</v>
       </c>
       <c r="D42" s="40" t="s">
@@ -11282,13 +11282,13 @@
         <v>250</v>
       </c>
       <c r="Q42" s="46"/>
-      <c r="R42" s="47">
-        <v>10</v>
+      <c r="R42" s="61">
+        <v>20</v>
       </c>
       <c r="S42" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="T42" s="96">
+      <c r="T42" s="95">
         <v>-1</v>
       </c>
       <c r="U42" s="50" t="s">
@@ -11389,7 +11389,7 @@
       <c r="B43" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="119" t="s">
+      <c r="C43" s="116" t="s">
         <v>246</v>
       </c>
       <c r="D43" s="40" t="s">
@@ -11432,13 +11432,13 @@
         <v>500</v>
       </c>
       <c r="Q43" s="46"/>
-      <c r="R43" s="47">
-        <v>10</v>
+      <c r="R43" s="61">
+        <v>20</v>
       </c>
       <c r="S43" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="T43" s="96">
+      <c r="T43" s="95">
         <v>-1</v>
       </c>
       <c r="U43" s="50" t="s">
@@ -11539,7 +11539,7 @@
       <c r="B44" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="119" t="s">
+      <c r="C44" s="116" t="s">
         <v>247</v>
       </c>
       <c r="D44" s="40" t="s">
@@ -11576,13 +11576,13 @@
       <c r="O44" s="46"/>
       <c r="P44" s="46"/>
       <c r="Q44" s="46"/>
-      <c r="R44" s="47">
-        <v>10</v>
+      <c r="R44" s="61">
+        <v>20</v>
       </c>
       <c r="S44" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T44" s="96">
+      <c r="T44" s="95">
         <v>-1</v>
       </c>
       <c r="U44" s="50" t="s">
@@ -11683,7 +11683,7 @@
       <c r="B45" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="119" t="s">
+      <c r="C45" s="116" t="s">
         <v>248</v>
       </c>
       <c r="D45" s="40" t="s">
@@ -11716,13 +11716,13 @@
       <c r="O45" s="46"/>
       <c r="P45" s="46"/>
       <c r="Q45" s="46"/>
-      <c r="R45" s="47">
-        <v>10</v>
+      <c r="R45" s="61">
+        <v>20</v>
       </c>
       <c r="S45" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T45" s="96">
+      <c r="T45" s="95">
         <v>-1</v>
       </c>
       <c r="U45" s="50" t="s">
@@ -11823,7 +11823,7 @@
       <c r="B46" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="110" t="s">
+      <c r="C46" s="109" t="s">
         <v>249</v>
       </c>
       <c r="D46" s="70" t="s">
@@ -11860,13 +11860,13 @@
       <c r="O46" s="74"/>
       <c r="P46" s="74"/>
       <c r="Q46" s="74"/>
-      <c r="R46" s="75">
-        <v>10</v>
+      <c r="R46" s="61">
+        <v>20</v>
       </c>
       <c r="S46" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="T46" s="96">
+      <c r="T46" s="95">
         <v>-1</v>
       </c>
       <c r="U46" s="77" t="s">
@@ -11964,154 +11964,154 @@
       </c>
     </row>
     <row r="47" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B47" s="118" t="s">
+      <c r="B47" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="129" t="s">
+      <c r="C47" s="126" t="s">
         <v>170</v>
       </c>
-      <c r="D47" s="130" t="s">
+      <c r="D47" s="127" t="s">
         <v>196</v>
       </c>
-      <c r="E47" s="98" t="s">
+      <c r="E47" s="97" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="99" t="b">
+      <c r="F47" s="98" t="b">
         <v>0</v>
       </c>
-      <c r="G47" s="99">
-        <v>1</v>
-      </c>
-      <c r="H47" s="100" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="100" t="s">
+      <c r="G47" s="98">
+        <v>1</v>
+      </c>
+      <c r="H47" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J47" s="100">
+      <c r="J47" s="99">
         <v>100</v>
       </c>
-      <c r="K47" s="100" t="s">
-        <v>151</v>
-      </c>
-      <c r="L47" s="101" t="s">
+      <c r="K47" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="L47" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="M47" s="101">
+      <c r="M47" s="100">
         <v>100000</v>
       </c>
-      <c r="N47" s="101" t="s">
-        <v>151</v>
-      </c>
-      <c r="O47" s="102" t="s">
-        <v>151</v>
-      </c>
-      <c r="P47" s="102" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q47" s="102" t="s">
-        <v>151</v>
-      </c>
-      <c r="R47" s="103">
+      <c r="N47" s="100" t="s">
+        <v>151</v>
+      </c>
+      <c r="O47" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="P47" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q47" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="R47" s="102">
         <v>2</v>
       </c>
-      <c r="S47" s="104" t="s">
+      <c r="S47" s="103" t="s">
         <v>99</v>
       </c>
-      <c r="T47" s="96" t="s">
+      <c r="T47" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="U47" s="105" t="s">
+      <c r="U47" s="104" t="s">
         <v>183</v>
       </c>
-      <c r="V47" s="106" t="s">
+      <c r="V47" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="W47" s="107" t="b">
-        <v>1</v>
-      </c>
-      <c r="X47" s="107">
+      <c r="W47" s="106" t="b">
+        <v>1</v>
+      </c>
+      <c r="X47" s="106">
         <v>0</v>
       </c>
-      <c r="Y47" s="107" t="s">
+      <c r="Y47" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="Z47" s="107">
+      <c r="Z47" s="106">
         <v>10</v>
       </c>
-      <c r="AA47" s="108">
+      <c r="AA47" s="107">
         <v>1526342400</v>
       </c>
-      <c r="AB47" s="108" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC47" s="108">
+      <c r="AB47" s="107" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC47" s="107">
         <v>1440</v>
       </c>
-      <c r="AD47" s="109" t="s">
+      <c r="AD47" s="108" t="s">
         <v>197</v>
       </c>
-      <c r="AE47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG47" s="109">
+      <c r="AE47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG47" s="108">
         <v>4</v>
       </c>
-      <c r="AH47" s="109" t="s">
+      <c r="AH47" s="108" t="s">
         <v>190</v>
       </c>
-      <c r="AI47" s="109">
+      <c r="AI47" s="108">
         <v>5</v>
       </c>
-      <c r="AJ47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV47" s="97" t="s">
+      <c r="AJ47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV47" s="96" t="s">
         <v>193</v>
       </c>
-      <c r="AW47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX47" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY47" s="109" t="s">
+      <c r="AW47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX47" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY47" s="108" t="s">
         <v>151</v>
       </c>
     </row>
@@ -12119,7 +12119,7 @@
       <c r="B48" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="120" t="s">
+      <c r="C48" s="117" t="s">
         <v>130</v>
       </c>
       <c r="D48" s="38" t="s">
@@ -12143,7 +12143,7 @@
       <c r="J48" s="44">
         <v>3</v>
       </c>
-      <c r="K48" s="100" t="s">
+      <c r="K48" s="99" t="s">
         <v>188</v>
       </c>
       <c r="L48" s="45" t="s">
@@ -12170,7 +12170,7 @@
       <c r="S48" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T48" s="96">
+      <c r="T48" s="95">
         <v>0.85</v>
       </c>
       <c r="U48" s="50" t="s">
@@ -12271,7 +12271,7 @@
       <c r="B49" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="120" t="s">
+      <c r="C49" s="117" t="s">
         <v>134</v>
       </c>
       <c r="D49" s="38" t="s">
@@ -12322,7 +12322,7 @@
       <c r="S49" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T49" s="96">
+      <c r="T49" s="95">
         <v>0.7</v>
       </c>
       <c r="U49" s="50" t="s">
@@ -12421,7 +12421,7 @@
       <c r="B50" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="120" t="s">
+      <c r="C50" s="117" t="s">
         <v>136</v>
       </c>
       <c r="D50" s="38" t="s">
@@ -12472,7 +12472,7 @@
       <c r="S50" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T50" s="96">
+      <c r="T50" s="95">
         <v>0.5</v>
       </c>
       <c r="U50" s="50" t="s">
@@ -12573,7 +12573,7 @@
       <c r="B51" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="120" t="s">
+      <c r="C51" s="117" t="s">
         <v>137</v>
       </c>
       <c r="D51" s="38" t="s">
@@ -12624,7 +12624,7 @@
       <c r="S51" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T51" s="96">
+      <c r="T51" s="95">
         <v>0.5</v>
       </c>
       <c r="U51" s="50" t="s">
@@ -12725,7 +12725,7 @@
       <c r="B52" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="120" t="s">
+      <c r="C52" s="117" t="s">
         <v>138</v>
       </c>
       <c r="D52" s="38" t="s">
@@ -12776,7 +12776,7 @@
       <c r="S52" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T52" s="96">
+      <c r="T52" s="95">
         <v>0.5</v>
       </c>
       <c r="U52" s="50" t="s">
@@ -12877,7 +12877,7 @@
       <c r="B53" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="120" t="s">
+      <c r="C53" s="117" t="s">
         <v>139</v>
       </c>
       <c r="D53" s="38" t="s">
@@ -12928,7 +12928,7 @@
       <c r="S53" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T53" s="96">
+      <c r="T53" s="95">
         <v>0.5</v>
       </c>
       <c r="U53" s="50" t="s">
@@ -13029,7 +13029,7 @@
       <c r="B54" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="120" t="s">
+      <c r="C54" s="117" t="s">
         <v>140</v>
       </c>
       <c r="D54" s="38" t="s">
@@ -13080,7 +13080,7 @@
       <c r="S54" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T54" s="96">
+      <c r="T54" s="95">
         <v>0.5</v>
       </c>
       <c r="U54" s="50" t="s">
@@ -13181,7 +13181,7 @@
       <c r="B55" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="120" t="s">
+      <c r="C55" s="117" t="s">
         <v>141</v>
       </c>
       <c r="D55" s="38" t="s">
@@ -13232,7 +13232,7 @@
       <c r="S55" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T55" s="96">
+      <c r="T55" s="95">
         <v>0.5</v>
       </c>
       <c r="U55" s="50" t="s">
@@ -13333,7 +13333,7 @@
       <c r="B56" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="120" t="s">
+      <c r="C56" s="117" t="s">
         <v>142</v>
       </c>
       <c r="D56" s="38" t="s">
@@ -13384,7 +13384,7 @@
       <c r="S56" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T56" s="96">
+      <c r="T56" s="95">
         <v>0.5</v>
       </c>
       <c r="U56" s="50" t="s">
@@ -13485,7 +13485,7 @@
       <c r="B57" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="120" t="s">
+      <c r="C57" s="117" t="s">
         <v>143</v>
       </c>
       <c r="D57" s="38" t="s">
@@ -13536,7 +13536,7 @@
       <c r="S57" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T57" s="96">
+      <c r="T57" s="95">
         <v>0.5</v>
       </c>
       <c r="U57" s="50" t="s">
@@ -13634,13 +13634,13 @@
       </c>
     </row>
     <row r="58" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B58" s="121" t="s">
+      <c r="B58" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="123" t="s">
+      <c r="C58" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="127" t="s">
+      <c r="D58" s="124" t="s">
         <v>151</v>
       </c>
       <c r="E58" s="70" t="s">
@@ -13688,7 +13688,7 @@
       <c r="S58" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="T58" s="96">
+      <c r="T58" s="95">
         <v>0.5</v>
       </c>
       <c r="U58" s="77" t="s">
@@ -13786,13 +13786,13 @@
       </c>
     </row>
     <row r="59" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B59" s="122" t="s">
+      <c r="B59" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="125" t="s">
+      <c r="C59" s="122" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="128" t="s">
+      <c r="D59" s="125" t="s">
         <v>151</v>
       </c>
       <c r="E59" s="56" t="s">
@@ -13840,7 +13840,7 @@
       <c r="S59" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="T59" s="96">
+      <c r="T59" s="95">
         <v>0.5</v>
       </c>
       <c r="U59" s="64" t="s">
@@ -13941,7 +13941,7 @@
       <c r="B60" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="120" t="s">
+      <c r="C60" s="117" t="s">
         <v>146</v>
       </c>
       <c r="D60" s="38" t="s">
@@ -13992,7 +13992,7 @@
       <c r="S60" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T60" s="96">
+      <c r="T60" s="95">
         <v>0.5</v>
       </c>
       <c r="U60" s="50" t="s">
@@ -14093,7 +14093,7 @@
       <c r="B61" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="120" t="s">
+      <c r="C61" s="117" t="s">
         <v>147</v>
       </c>
       <c r="D61" s="38" t="s">
@@ -14144,7 +14144,7 @@
       <c r="S61" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T61" s="96">
+      <c r="T61" s="95">
         <v>0.5</v>
       </c>
       <c r="U61" s="50" t="s">
@@ -14245,7 +14245,7 @@
       <c r="B62" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="120" t="s">
+      <c r="C62" s="117" t="s">
         <v>148</v>
       </c>
       <c r="D62" s="38" t="s">
@@ -14296,7 +14296,7 @@
       <c r="S62" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="T62" s="96">
+      <c r="T62" s="95">
         <v>0.5</v>
       </c>
       <c r="U62" s="50" t="s">
@@ -14397,7 +14397,7 @@
       <c r="B63" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="120" t="s">
+      <c r="C63" s="117" t="s">
         <v>149</v>
       </c>
       <c r="D63" s="38" t="s">
@@ -14448,7 +14448,7 @@
       <c r="S63" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T63" s="96">
+      <c r="T63" s="95">
         <v>0.5</v>
       </c>
       <c r="U63" s="50" t="s">
@@ -14549,7 +14549,7 @@
       <c r="B64" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="124" t="s">
+      <c r="C64" s="121" t="s">
         <v>150</v>
       </c>
       <c r="D64" s="38" t="s">
@@ -14600,7 +14600,7 @@
       <c r="S64" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="T64" s="96">
+      <c r="T64" s="95">
         <v>0.5</v>
       </c>
       <c r="U64" s="50" t="s">
@@ -14701,7 +14701,7 @@
       <c r="B65" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="124" t="s">
+      <c r="C65" s="121" t="s">
         <v>165</v>
       </c>
       <c r="D65" s="38" t="s">
@@ -14752,7 +14752,7 @@
       <c r="S65" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T65" s="96" t="s">
+      <c r="T65" s="95" t="s">
         <v>174</v>
       </c>
       <c r="U65" s="50" t="s">
@@ -14851,7 +14851,7 @@
       <c r="B66" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="124" t="s">
+      <c r="C66" s="121" t="s">
         <v>167</v>
       </c>
       <c r="D66" s="39" t="s">
@@ -14902,7 +14902,7 @@
       <c r="S66" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T66" s="96" t="s">
+      <c r="T66" s="95" t="s">
         <v>177</v>
       </c>
       <c r="U66" s="50" t="s">
@@ -15003,7 +15003,7 @@
       <c r="B67" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="124" t="s">
+      <c r="C67" s="121" t="s">
         <v>168</v>
       </c>
       <c r="D67" s="39" t="s">
@@ -15050,7 +15050,7 @@
       <c r="S67" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T67" s="96">
+      <c r="T67" s="95">
         <v>-1</v>
       </c>
       <c r="U67" s="50" t="s">
@@ -15151,7 +15151,7 @@
       <c r="B68" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="124" t="s">
+      <c r="C68" s="121" t="s">
         <v>171</v>
       </c>
       <c r="D68" s="39" t="s">
@@ -15202,7 +15202,7 @@
       <c r="S68" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T68" s="96" t="s">
+      <c r="T68" s="95" t="s">
         <v>174</v>
       </c>
       <c r="U68" s="50" t="s">
@@ -15303,7 +15303,7 @@
       <c r="B69" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="124" t="s">
+      <c r="C69" s="121" t="s">
         <v>203</v>
       </c>
       <c r="D69" s="38" t="s">
@@ -15346,7 +15346,7 @@
       <c r="S69" s="48">
         <v>4.99</v>
       </c>
-      <c r="T69" s="96" t="s">
+      <c r="T69" s="95" t="s">
         <v>175</v>
       </c>
       <c r="U69" s="50" t="s">
@@ -15480,7 +15480,7 @@
       <c r="S70" s="48">
         <v>1.99</v>
       </c>
-      <c r="T70" s="96" t="s">
+      <c r="T70" s="95" t="s">
         <v>175</v>
       </c>
       <c r="U70" s="50" t="s">
@@ -15581,13 +15581,13 @@
       <c r="B71" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="111" t="s">
+      <c r="C71" s="110" t="s">
         <v>298</v>
       </c>
       <c r="D71" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E71" s="112" t="s">
+      <c r="E71" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F71" s="43" t="b">
@@ -15733,13 +15733,13 @@
       <c r="B72" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="111" t="s">
+      <c r="C72" s="110" t="s">
         <v>299</v>
       </c>
       <c r="D72" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="112" t="s">
+      <c r="E72" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F72" s="43" t="b">
@@ -15885,13 +15885,13 @@
       <c r="B73" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="111" t="s">
+      <c r="C73" s="110" t="s">
         <v>300</v>
       </c>
       <c r="D73" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E73" s="112" t="s">
+      <c r="E73" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F73" s="43" t="b">
@@ -16037,13 +16037,13 @@
       <c r="B74" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="111" t="s">
+      <c r="C74" s="110" t="s">
         <v>301</v>
       </c>
       <c r="D74" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E74" s="112" t="s">
+      <c r="E74" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F74" s="43" t="b">
@@ -16189,13 +16189,13 @@
       <c r="B75" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="111" t="s">
+      <c r="C75" s="110" t="s">
         <v>302</v>
       </c>
       <c r="D75" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E75" s="112" t="s">
+      <c r="E75" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F75" s="43" t="b">
@@ -16341,13 +16341,13 @@
       <c r="B76" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="113" t="s">
+      <c r="C76" s="112" t="s">
         <v>303</v>
       </c>
       <c r="D76" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E76" s="112" t="s">
+      <c r="E76" s="111" t="s">
         <v>210</v>
       </c>
       <c r="F76" s="43" t="b">
@@ -16389,16 +16389,16 @@
       <c r="R76" s="47">
         <v>10</v>
       </c>
-      <c r="S76" s="90" t="s">
+      <c r="S76" s="89" t="s">
         <v>252</v>
       </c>
       <c r="T76" s="49">
         <v>0.5</v>
       </c>
-      <c r="U76" s="91" t="s">
+      <c r="U76" s="90" t="s">
         <v>296</v>
       </c>
-      <c r="V76" s="92" t="s">
+      <c r="V76" s="91" t="s">
         <v>309</v>
       </c>
       <c r="W76" s="35" t="b">
@@ -16495,10 +16495,10 @@
     <mergeCell ref="AD1:AY1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F76">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="96" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17539,127 +17539,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="41" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="48" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="46" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="45" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="44" priority="20">
+    <cfRule type="expression" dxfId="36" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="43" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="42" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="41" priority="17">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="40" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="39" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="38" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="36" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="35" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="34" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="33" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="31" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="29" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix in some offers
Former-commit-id: d2fb88bc8c7de5d8d53c93a65e318304463b6147
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="325">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -991,9 +991,6 @@
   </si>
   <si>
     <t>28:999</t>
-  </si>
-  <si>
-    <t>dragon_devil</t>
   </si>
   <si>
     <t>dragon_helicopter</t>
@@ -1892,245 +1889,245 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5623,8 +5620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="J43" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5675,35 +5672,35 @@
       <c r="T1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="135" t="s">
+      <c r="AA1" s="213" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="135"/>
+      <c r="AB1" s="213"/>
       <c r="AC1" s="32"/>
-      <c r="AD1" s="136" t="s">
+      <c r="AD1" s="214" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" s="136"/>
-      <c r="AF1" s="136"/>
-      <c r="AG1" s="136"/>
-      <c r="AH1" s="136"/>
-      <c r="AI1" s="136"/>
-      <c r="AJ1" s="136"/>
-      <c r="AK1" s="136"/>
-      <c r="AL1" s="136"/>
-      <c r="AM1" s="136"/>
-      <c r="AN1" s="136"/>
-      <c r="AO1" s="136"/>
-      <c r="AP1" s="136"/>
-      <c r="AQ1" s="136"/>
-      <c r="AR1" s="136"/>
-      <c r="AS1" s="136"/>
-      <c r="AT1" s="136"/>
-      <c r="AU1" s="136"/>
-      <c r="AV1" s="136"/>
-      <c r="AW1" s="136"/>
-      <c r="AX1" s="136"/>
-      <c r="AY1" s="136"/>
+      <c r="AE1" s="214"/>
+      <c r="AF1" s="214"/>
+      <c r="AG1" s="214"/>
+      <c r="AH1" s="214"/>
+      <c r="AI1" s="214"/>
+      <c r="AJ1" s="214"/>
+      <c r="AK1" s="214"/>
+      <c r="AL1" s="214"/>
+      <c r="AM1" s="214"/>
+      <c r="AN1" s="214"/>
+      <c r="AO1" s="214"/>
+      <c r="AP1" s="214"/>
+      <c r="AQ1" s="214"/>
+      <c r="AR1" s="214"/>
+      <c r="AS1" s="214"/>
+      <c r="AT1" s="214"/>
+      <c r="AU1" s="214"/>
+      <c r="AV1" s="214"/>
+      <c r="AW1" s="214"/>
+      <c r="AX1" s="214"/>
+      <c r="AY1" s="214"/>
     </row>
     <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -6884,7 +6881,7 @@
       <c r="AQ9" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="AR9" s="155" t="s">
+      <c r="AR9" s="153" t="s">
         <v>151</v>
       </c>
       <c r="AS9" s="27" t="s">
@@ -6893,7 +6890,7 @@
       <c r="AT9" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="AU9" s="155" t="s">
+      <c r="AU9" s="153" t="s">
         <v>151</v>
       </c>
       <c r="AV9" s="34" t="s">
@@ -6913,7 +6910,7 @@
       <c r="B10" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="175" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="120" t="s">
@@ -7065,7 +7062,7 @@
       <c r="B11" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="138" t="s">
+      <c r="C11" s="136" t="s">
         <v>137</v>
       </c>
       <c r="D11" s="118" t="s">
@@ -7974,154 +7971,154 @@
       </c>
     </row>
     <row r="17" spans="2:51" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="139" t="s">
+      <c r="B17" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="182" t="s">
+      <c r="C17" s="180" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="185" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="140" t="s">
+      <c r="D17" s="183" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="F17" s="141" t="b">
+      <c r="F17" s="139" t="b">
         <v>0</v>
       </c>
-      <c r="G17" s="141">
+      <c r="G17" s="139">
         <v>1</v>
       </c>
-      <c r="H17" s="142" t="b">
+      <c r="H17" s="140" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="142" t="s">
-        <v>151</v>
-      </c>
-      <c r="J17" s="142" t="s">
-        <v>151</v>
-      </c>
-      <c r="K17" s="142" t="s">
-        <v>151</v>
-      </c>
-      <c r="L17" s="143" t="s">
-        <v>151</v>
-      </c>
-      <c r="M17" s="143" t="s">
-        <v>151</v>
-      </c>
-      <c r="N17" s="143" t="s">
-        <v>151</v>
-      </c>
-      <c r="O17" s="144" t="s">
-        <v>151</v>
-      </c>
-      <c r="P17" s="144" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q17" s="144" t="s">
-        <v>151</v>
-      </c>
-      <c r="R17" s="145">
+      <c r="I17" s="140" t="s">
+        <v>151</v>
+      </c>
+      <c r="J17" s="140" t="s">
+        <v>151</v>
+      </c>
+      <c r="K17" s="140" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="141" t="s">
+        <v>151</v>
+      </c>
+      <c r="M17" s="141" t="s">
+        <v>151</v>
+      </c>
+      <c r="N17" s="141" t="s">
+        <v>151</v>
+      </c>
+      <c r="O17" s="142" t="s">
+        <v>151</v>
+      </c>
+      <c r="P17" s="142" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q17" s="142" t="s">
+        <v>151</v>
+      </c>
+      <c r="R17" s="143">
         <v>0</v>
       </c>
-      <c r="S17" s="146" t="s">
+      <c r="S17" s="144" t="s">
         <v>128</v>
       </c>
-      <c r="T17" s="147">
+      <c r="T17" s="145">
         <v>0.5</v>
       </c>
-      <c r="U17" s="148" t="s">
+      <c r="U17" s="146" t="s">
         <v>117</v>
       </c>
-      <c r="V17" s="149" t="s">
+      <c r="V17" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="W17" s="150" t="s">
-        <v>151</v>
-      </c>
-      <c r="X17" s="150" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y17" s="150" t="s">
+      <c r="W17" s="148" t="s">
+        <v>151</v>
+      </c>
+      <c r="X17" s="148" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y17" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="Z17" s="150" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA17" s="151" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB17" s="151" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC17" s="151" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD17" s="152" t="s">
+      <c r="Z17" s="148" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA17" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB17" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC17" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD17" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="AE17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV17" s="153" t="s">
-        <v>151</v>
-      </c>
-      <c r="AW17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX17" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY17" s="152" t="s">
+      <c r="AE17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV17" s="151" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX17" s="150" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY17" s="150" t="s">
         <v>151</v>
       </c>
     </row>
@@ -8129,7 +8126,7 @@
       <c r="B18" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="138" t="s">
+      <c r="C18" s="136" t="s">
         <v>144</v>
       </c>
       <c r="D18" s="118" t="s">
@@ -10523,7 +10520,7 @@
       <c r="B34" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="178" t="s">
+      <c r="C34" s="176" t="s">
         <v>218</v>
       </c>
       <c r="D34" s="82" t="s">
@@ -10663,7 +10660,7 @@
       <c r="B35" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="179" t="s">
+      <c r="C35" s="177" t="s">
         <v>220</v>
       </c>
       <c r="D35" s="96" t="s">
@@ -11418,13 +11415,13 @@
       <c r="O40" s="87"/>
       <c r="P40" s="87"/>
       <c r="Q40" s="87"/>
-      <c r="R40" s="159">
+      <c r="R40" s="157">
         <v>20</v>
       </c>
       <c r="S40" s="88" t="s">
         <v>126</v>
       </c>
-      <c r="T40" s="160">
+      <c r="T40" s="158">
         <v>-1</v>
       </c>
       <c r="U40" s="89" t="s">
@@ -11522,148 +11519,148 @@
       </c>
     </row>
     <row r="41" spans="2:51" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="161" t="s">
+      <c r="B41" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="183" t="s">
+      <c r="C41" s="181" t="s">
         <v>232</v>
       </c>
-      <c r="D41" s="161" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="161" t="s">
+      <c r="D41" s="159" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="159" t="s">
         <v>210</v>
       </c>
-      <c r="F41" s="162" t="b">
+      <c r="F41" s="160" t="b">
         <v>0</v>
       </c>
-      <c r="G41" s="162">
+      <c r="G41" s="160">
         <v>-1</v>
       </c>
-      <c r="H41" s="163" t="b">
+      <c r="H41" s="161" t="b">
         <v>1</v>
       </c>
-      <c r="I41" s="163" t="s">
+      <c r="I41" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="J41" s="163">
+      <c r="J41" s="161">
         <v>5</v>
       </c>
-      <c r="K41" s="163" t="s">
+      <c r="K41" s="161" t="s">
         <v>249</v>
       </c>
-      <c r="L41" s="164" t="s">
+      <c r="L41" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="M41" s="164">
+      <c r="M41" s="162">
         <v>10</v>
       </c>
-      <c r="N41" s="164" t="s">
+      <c r="N41" s="162" t="s">
         <v>188</v>
       </c>
-      <c r="O41" s="165"/>
-      <c r="P41" s="165"/>
-      <c r="Q41" s="165"/>
-      <c r="R41" s="166">
+      <c r="O41" s="163"/>
+      <c r="P41" s="163"/>
+      <c r="Q41" s="163"/>
+      <c r="R41" s="164">
         <v>20</v>
       </c>
-      <c r="S41" s="167" t="s">
+      <c r="S41" s="165" t="s">
         <v>127</v>
       </c>
-      <c r="T41" s="168">
+      <c r="T41" s="166">
         <v>-1</v>
       </c>
-      <c r="U41" s="169" t="s">
+      <c r="U41" s="167" t="s">
         <v>273</v>
       </c>
-      <c r="V41" s="170" t="s">
+      <c r="V41" s="168" t="s">
         <v>253</v>
       </c>
-      <c r="W41" s="171" t="b">
+      <c r="W41" s="169" t="b">
         <v>1</v>
       </c>
-      <c r="X41" s="171">
+      <c r="X41" s="169">
         <v>0</v>
       </c>
-      <c r="Y41" s="171" t="s">
+      <c r="Y41" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="Z41" s="171">
+      <c r="Z41" s="169">
         <v>10</v>
       </c>
-      <c r="AA41" s="172" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB41" s="172" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC41" s="172">
+      <c r="AA41" s="170" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB41" s="170" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC41" s="170">
         <v>2880</v>
       </c>
-      <c r="AD41" s="173" t="s">
+      <c r="AD41" s="171" t="s">
         <v>211</v>
       </c>
-      <c r="AE41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG41" s="173">
+      <c r="AE41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG41" s="171">
         <v>4</v>
       </c>
-      <c r="AH41" s="173" t="s">
+      <c r="AH41" s="171" t="s">
         <v>190</v>
       </c>
-      <c r="AI41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ41" s="173" t="s">
+      <c r="AI41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ41" s="171" t="s">
         <v>127</v>
       </c>
-      <c r="AK41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV41" s="174" t="s">
+      <c r="AK41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV41" s="172" t="s">
         <v>200</v>
       </c>
-      <c r="AW41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX41" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY41" s="173" t="s">
+      <c r="AW41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX41" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY41" s="171" t="s">
         <v>151</v>
       </c>
     </row>
@@ -12385,7 +12382,7 @@
       <c r="B47" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="176" t="s">
+      <c r="C47" s="174" t="s">
         <v>240</v>
       </c>
       <c r="D47" s="96" t="s">
@@ -13138,13 +13135,13 @@
       <c r="O52" s="87"/>
       <c r="P52" s="87"/>
       <c r="Q52" s="87"/>
-      <c r="R52" s="187">
+      <c r="R52" s="185">
         <v>20</v>
       </c>
       <c r="S52" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="T52" s="160">
+      <c r="T52" s="158">
         <v>-1</v>
       </c>
       <c r="U52" s="89" t="s">
@@ -13242,154 +13239,154 @@
       </c>
     </row>
     <row r="53" spans="2:51" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="188" t="s">
+      <c r="B53" s="186" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="189" t="s">
+      <c r="C53" s="187" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="190" t="s">
-        <v>151</v>
-      </c>
-      <c r="E53" s="161" t="s">
+      <c r="D53" s="188" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="159" t="s">
         <v>208</v>
       </c>
-      <c r="F53" s="162" t="b">
+      <c r="F53" s="160" t="b">
         <v>1</v>
       </c>
-      <c r="G53" s="162">
+      <c r="G53" s="160">
         <v>1</v>
       </c>
-      <c r="H53" s="163" t="b">
+      <c r="H53" s="161" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="163" t="s">
+      <c r="I53" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="J53" s="163">
+      <c r="J53" s="161">
         <v>1</v>
       </c>
-      <c r="K53" s="163" t="s">
-        <v>323</v>
-      </c>
-      <c r="L53" s="164" t="s">
+      <c r="K53" s="161" t="s">
+        <v>322</v>
+      </c>
+      <c r="L53" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="M53" s="164">
+      <c r="M53" s="162">
         <v>2</v>
       </c>
-      <c r="N53" s="164" t="s">
+      <c r="N53" s="162" t="s">
         <v>250</v>
       </c>
-      <c r="O53" s="165" t="s">
+      <c r="O53" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="P53" s="165">
+      <c r="P53" s="163">
         <v>2</v>
       </c>
-      <c r="Q53" s="165" t="s">
+      <c r="Q53" s="163" t="s">
         <v>188</v>
       </c>
-      <c r="R53" s="166">
+      <c r="R53" s="164">
         <v>8</v>
       </c>
-      <c r="S53" s="167" t="s">
+      <c r="S53" s="165" t="s">
         <v>125</v>
       </c>
-      <c r="T53" s="168">
+      <c r="T53" s="166">
         <v>-1</v>
       </c>
-      <c r="U53" s="169" t="s">
+      <c r="U53" s="167" t="s">
         <v>107</v>
       </c>
-      <c r="V53" s="170" t="s">
+      <c r="V53" s="168" t="s">
         <v>316</v>
       </c>
-      <c r="W53" s="171" t="b">
+      <c r="W53" s="169" t="b">
         <v>1</v>
       </c>
-      <c r="X53" s="171">
+      <c r="X53" s="169">
         <v>0</v>
       </c>
-      <c r="Y53" s="171" t="s">
+      <c r="Y53" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="Z53" s="171">
+      <c r="Z53" s="169">
         <v>20</v>
       </c>
-      <c r="AA53" s="172" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB53" s="172" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC53" s="172">
+      <c r="AA53" s="170" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB53" s="170" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC53" s="170">
         <v>2880</v>
       </c>
-      <c r="AD53" s="173" t="s">
+      <c r="AD53" s="171" t="s">
         <v>314</v>
       </c>
-      <c r="AE53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG53" s="173">
+      <c r="AE53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG53" s="171">
         <v>4</v>
       </c>
-      <c r="AH53" s="191" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV53" s="174" t="s">
+      <c r="AH53" s="189" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV53" s="172" t="s">
         <v>191</v>
       </c>
-      <c r="AW53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX53" s="173" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY53" s="173" t="s">
+      <c r="AW53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX53" s="171" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY53" s="171" t="s">
         <v>151</v>
       </c>
     </row>
@@ -13422,7 +13419,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L54" s="45" t="s">
         <v>65</v>
@@ -13430,7 +13427,7 @@
       <c r="M54" s="45">
         <v>100</v>
       </c>
-      <c r="N54" s="154" t="s">
+      <c r="N54" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O54" s="46" t="s">
@@ -13474,7 +13471,7 @@
         <v>151</v>
       </c>
       <c r="AC54" s="51">
-        <v>2880</v>
+        <v>4320</v>
       </c>
       <c r="AD54" s="27" t="s">
         <v>314</v>
@@ -13488,7 +13485,7 @@
       <c r="AG54" s="27">
         <v>4</v>
       </c>
-      <c r="AH54" s="155" t="s">
+      <c r="AH54" s="153" t="s">
         <v>151</v>
       </c>
       <c r="AI54" s="27" t="s">
@@ -13510,7 +13507,7 @@
         <v>151</v>
       </c>
       <c r="AO54" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AP54" s="27" t="s">
         <v>151</v>
@@ -13572,10 +13569,10 @@
       <c r="K55" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="L55" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="M55" s="154" t="s">
+      <c r="L55" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="M55" s="152" t="s">
         <v>151</v>
       </c>
       <c r="N55" s="45" t="s">
@@ -13624,7 +13621,7 @@
         <v>151</v>
       </c>
       <c r="AC55" s="51">
-        <v>1440</v>
+        <v>2880</v>
       </c>
       <c r="AD55" s="27" t="s">
         <v>196</v>
@@ -13638,10 +13635,10 @@
       <c r="AG55" s="27">
         <v>4</v>
       </c>
-      <c r="AH55" s="155" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI55" s="155" t="s">
+      <c r="AH55" s="153" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI55" s="153" t="s">
         <v>151</v>
       </c>
       <c r="AJ55" s="27" t="s">
@@ -13721,13 +13718,13 @@
       <c r="J56" s="44">
         <v>40000</v>
       </c>
-      <c r="K56" s="156" t="s">
-        <v>151</v>
-      </c>
-      <c r="L56" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="M56" s="154" t="s">
+      <c r="K56" s="154" t="s">
+        <v>151</v>
+      </c>
+      <c r="L56" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="M56" s="152" t="s">
         <v>151</v>
       </c>
       <c r="N56" s="45" t="s">
@@ -13776,7 +13773,7 @@
         <v>151</v>
       </c>
       <c r="AC56" s="51">
-        <v>1440</v>
+        <v>2880</v>
       </c>
       <c r="AD56" s="27" t="s">
         <v>196</v>
@@ -13926,7 +13923,7 @@
         <v>151</v>
       </c>
       <c r="AC57" s="51">
-        <v>1440</v>
+        <v>4320</v>
       </c>
       <c r="AD57" s="27" t="s">
         <v>196</v>
@@ -13962,7 +13959,7 @@
         <v>151</v>
       </c>
       <c r="AO57" s="27" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="AP57" s="27" t="s">
         <v>151</v>
@@ -13999,10 +13996,10 @@
       <c r="B58" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="180" t="s">
+      <c r="C58" s="178" t="s">
         <v>167</v>
       </c>
-      <c r="D58" s="184" t="s">
+      <c r="D58" s="182" t="s">
         <v>195</v>
       </c>
       <c r="E58" s="69" t="s">
@@ -14024,7 +14021,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="71" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L58" s="72" t="s">
         <v>27</v>
@@ -14077,8 +14074,8 @@
       <c r="AB58" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="AC58" s="79">
-        <v>1440</v>
+      <c r="AC58" s="51">
+        <v>2880</v>
       </c>
       <c r="AD58" s="80" t="s">
         <v>196</v>
@@ -14092,7 +14089,7 @@
       <c r="AG58" s="80">
         <v>4</v>
       </c>
-      <c r="AH58" s="186" t="s">
+      <c r="AH58" s="184" t="s">
         <v>151</v>
       </c>
       <c r="AI58" s="80" t="s">
@@ -14122,7 +14119,7 @@
       <c r="AQ58" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="AR58" s="186" t="s">
+      <c r="AR58" s="184" t="s">
         <v>151</v>
       </c>
       <c r="AS58" s="80" t="s">
@@ -14135,7 +14132,7 @@
         <v>151</v>
       </c>
       <c r="AV58" s="81" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AW58" s="80" t="s">
         <v>151</v>
@@ -14151,10 +14148,10 @@
       <c r="B59" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="181" t="s">
+      <c r="C59" s="179" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="137" t="s">
+      <c r="D59" s="135" t="s">
         <v>195</v>
       </c>
       <c r="E59" s="55" t="s">
@@ -14178,10 +14175,10 @@
       <c r="K59" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="L59" s="157" t="s">
-        <v>151</v>
-      </c>
-      <c r="M59" s="157" t="s">
+      <c r="L59" s="155" t="s">
+        <v>151</v>
+      </c>
+      <c r="M59" s="155" t="s">
         <v>151</v>
       </c>
       <c r="N59" s="58" t="s">
@@ -14229,8 +14226,8 @@
       <c r="AB59" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="AC59" s="66">
-        <v>1440</v>
+      <c r="AC59" s="51">
+        <v>2880</v>
       </c>
       <c r="AD59" s="67" t="s">
         <v>196</v>
@@ -14244,7 +14241,7 @@
       <c r="AG59" s="67">
         <v>4</v>
       </c>
-      <c r="AH59" s="158" t="s">
+      <c r="AH59" s="156" t="s">
         <v>151</v>
       </c>
       <c r="AI59" s="67" t="s">
@@ -14300,13 +14297,13 @@
       </c>
     </row>
     <row r="60" spans="2:51" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="192" t="s">
+      <c r="B60" s="190" t="s">
         <v>3</v>
       </c>
       <c r="C60" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="D60" s="193" t="s">
+      <c r="D60" s="191" t="s">
         <v>195</v>
       </c>
       <c r="E60" s="82" t="s">
@@ -14327,8 +14324,8 @@
       <c r="J60" s="85">
         <v>2</v>
       </c>
-      <c r="K60" s="194" t="s">
-        <v>323</v>
+      <c r="K60" s="192" t="s">
+        <v>322</v>
       </c>
       <c r="L60" s="86" t="s">
         <v>27</v>
@@ -14336,7 +14333,7 @@
       <c r="M60" s="86">
         <v>5</v>
       </c>
-      <c r="N60" s="195" t="s">
+      <c r="N60" s="193" t="s">
         <v>250</v>
       </c>
       <c r="O60" s="87" t="s">
@@ -14348,13 +14345,13 @@
       <c r="Q60" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="R60" s="187">
+      <c r="R60" s="185">
         <v>1</v>
       </c>
       <c r="S60" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="T60" s="160" t="s">
+      <c r="T60" s="158" t="s">
         <v>174</v>
       </c>
       <c r="U60" s="89" t="s">
@@ -14381,8 +14378,8 @@
       <c r="AB60" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="AC60" s="92">
-        <v>1440</v>
+      <c r="AC60" s="51">
+        <v>2880</v>
       </c>
       <c r="AD60" s="93" t="s">
         <v>196</v>
@@ -14396,10 +14393,10 @@
       <c r="AG60" s="93">
         <v>4</v>
       </c>
-      <c r="AH60" s="196" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI60" s="197" t="s">
+      <c r="AH60" s="194" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI60" s="195" t="s">
         <v>151</v>
       </c>
       <c r="AJ60" s="93" t="s">
@@ -14426,7 +14423,7 @@
       <c r="AQ60" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="AR60" s="196" t="s">
+      <c r="AR60" s="194" t="s">
         <v>151</v>
       </c>
       <c r="AS60" s="93" t="s">
@@ -14439,7 +14436,7 @@
         <v>151</v>
       </c>
       <c r="AV60" s="112" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AW60" s="93" t="s">
         <v>151</v>
@@ -14452,148 +14449,148 @@
       </c>
     </row>
     <row r="61" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B61" s="198" t="s">
+      <c r="B61" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="199" t="s">
+      <c r="C61" s="197" t="s">
         <v>213</v>
       </c>
-      <c r="D61" s="198" t="s">
-        <v>151</v>
-      </c>
-      <c r="E61" s="198" t="s">
+      <c r="D61" s="196" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="196" t="s">
         <v>210</v>
       </c>
-      <c r="F61" s="200" t="b">
+      <c r="F61" s="198" t="b">
         <v>1</v>
       </c>
-      <c r="G61" s="200">
+      <c r="G61" s="198">
         <v>-1</v>
       </c>
-      <c r="H61" s="201" t="b">
+      <c r="H61" s="199" t="b">
         <v>1</v>
       </c>
-      <c r="I61" s="201" t="s">
+      <c r="I61" s="199" t="s">
         <v>19</v>
       </c>
-      <c r="J61" s="201">
+      <c r="J61" s="199">
         <v>300</v>
       </c>
-      <c r="K61" s="202" t="s">
-        <v>151</v>
-      </c>
-      <c r="L61" s="203" t="s">
+      <c r="K61" s="200" t="s">
+        <v>151</v>
+      </c>
+      <c r="L61" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="M61" s="203">
+      <c r="M61" s="201">
         <v>300000</v>
       </c>
-      <c r="N61" s="204" t="s">
-        <v>151</v>
-      </c>
-      <c r="O61" s="205"/>
-      <c r="P61" s="205"/>
-      <c r="Q61" s="205"/>
-      <c r="R61" s="206">
+      <c r="N61" s="202" t="s">
+        <v>151</v>
+      </c>
+      <c r="O61" s="203"/>
+      <c r="P61" s="203"/>
+      <c r="Q61" s="203"/>
+      <c r="R61" s="204">
         <v>20</v>
       </c>
-      <c r="S61" s="207" t="s">
+      <c r="S61" s="205" t="s">
         <v>99</v>
       </c>
-      <c r="T61" s="208">
+      <c r="T61" s="206">
         <v>-1</v>
       </c>
-      <c r="U61" s="209" t="s">
+      <c r="U61" s="207" t="s">
         <v>254</v>
       </c>
-      <c r="V61" s="210" t="s">
+      <c r="V61" s="208" t="s">
         <v>253</v>
       </c>
-      <c r="W61" s="211" t="b">
+      <c r="W61" s="209" t="b">
         <v>1</v>
       </c>
-      <c r="X61" s="211">
+      <c r="X61" s="209">
         <v>0</v>
       </c>
-      <c r="Y61" s="211" t="s">
+      <c r="Y61" s="209" t="s">
         <v>26</v>
       </c>
-      <c r="Z61" s="211">
+      <c r="Z61" s="209">
         <v>10</v>
       </c>
-      <c r="AA61" s="212" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB61" s="212" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC61" s="212">
+      <c r="AA61" s="210" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB61" s="210" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC61" s="210">
         <v>2880</v>
       </c>
-      <c r="AD61" s="213" t="s">
+      <c r="AD61" s="211" t="s">
         <v>211</v>
       </c>
-      <c r="AE61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG61" s="213">
+      <c r="AE61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG61" s="211">
         <v>4</v>
       </c>
-      <c r="AH61" s="213" t="s">
+      <c r="AH61" s="211" t="s">
         <v>189</v>
       </c>
-      <c r="AI61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV61" s="214" t="s">
+      <c r="AI61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV61" s="212" t="s">
         <v>200</v>
       </c>
-      <c r="AW61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX61" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="AY61" s="213" t="s">
+      <c r="AW61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX61" s="211" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY61" s="211" t="s">
         <v>151</v>
       </c>
     </row>
@@ -14634,7 +14631,7 @@
       <c r="M62" s="45">
         <v>300</v>
       </c>
-      <c r="N62" s="154" t="s">
+      <c r="N62" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O62" s="46"/>
@@ -14771,7 +14768,7 @@
       <c r="J63" s="44">
         <v>200</v>
       </c>
-      <c r="K63" s="156" t="s">
+      <c r="K63" s="154" t="s">
         <v>151</v>
       </c>
       <c r="L63" s="45" t="s">
@@ -14780,7 +14777,7 @@
       <c r="M63" s="45">
         <v>200</v>
       </c>
-      <c r="N63" s="154" t="s">
+      <c r="N63" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O63" s="46"/>
@@ -14926,7 +14923,7 @@
       <c r="M64" s="45">
         <v>150000</v>
       </c>
-      <c r="N64" s="154" t="s">
+      <c r="N64" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O64" s="46"/>
@@ -15370,7 +15367,7 @@
       <c r="M67" s="45">
         <v>100</v>
       </c>
-      <c r="N67" s="154" t="s">
+      <c r="N67" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O67" s="46"/>
@@ -15507,7 +15504,7 @@
       <c r="J68" s="44">
         <v>100</v>
       </c>
-      <c r="K68" s="156" t="s">
+      <c r="K68" s="154" t="s">
         <v>151</v>
       </c>
       <c r="L68" s="45" t="s">
@@ -15516,7 +15513,7 @@
       <c r="M68" s="45">
         <v>100</v>
       </c>
-      <c r="N68" s="154" t="s">
+      <c r="N68" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O68" s="46" t="s">
@@ -15657,7 +15654,7 @@
       <c r="J69" s="44">
         <v>350</v>
       </c>
-      <c r="K69" s="156" t="s">
+      <c r="K69" s="154" t="s">
         <v>151</v>
       </c>
       <c r="L69" s="45"/>
@@ -15806,7 +15803,7 @@
       <c r="M70" s="45">
         <v>150000</v>
       </c>
-      <c r="N70" s="154" t="s">
+      <c r="N70" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O70" s="46"/>
@@ -15952,7 +15949,7 @@
       <c r="M71" s="45">
         <v>200000</v>
       </c>
-      <c r="N71" s="154" t="s">
+      <c r="N71" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O71" s="46"/>
@@ -16089,16 +16086,16 @@
       <c r="J72" s="44">
         <v>250</v>
       </c>
-      <c r="K72" s="156" t="s">
-        <v>151</v>
-      </c>
-      <c r="L72" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="M72" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="N72" s="154" t="s">
+      <c r="K72" s="154" t="s">
+        <v>151</v>
+      </c>
+      <c r="L72" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="M72" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="N72" s="152" t="s">
         <v>151</v>
       </c>
       <c r="O72" s="46"/>
@@ -16235,25 +16232,25 @@
       <c r="J73" s="44">
         <v>1200</v>
       </c>
-      <c r="K73" s="156" t="s">
-        <v>151</v>
-      </c>
-      <c r="L73" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="M73" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="N73" s="154" t="s">
-        <v>151</v>
-      </c>
-      <c r="O73" s="175" t="s">
-        <v>151</v>
-      </c>
-      <c r="P73" s="175" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q73" s="175" t="s">
+      <c r="K73" s="154" t="s">
+        <v>151</v>
+      </c>
+      <c r="L73" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="M73" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="N73" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="O73" s="173" t="s">
+        <v>151</v>
+      </c>
+      <c r="P73" s="173" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q73" s="173" t="s">
         <v>151</v>
       </c>
       <c r="R73" s="47">

</xml_diff>

<commit_message>
Progression offers packs texts updated
Former-commit-id: bb43c759f662811e53129fa79a46450f6589bed7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="329">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -1000,6 +1000,21 @@
   </si>
   <si>
     <t>55:999</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_31</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_CAMPAIGN2PROMO60</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_PROGRESSIONPACK1</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_VALUEGATCHAPACK</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_CURRENCYCATCHUPPACK1</t>
   </si>
 </sst>
 </file>
@@ -2127,32 +2142,32 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5645,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5697,35 +5712,35 @@
       <c r="T1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="213" t="s">
+      <c r="AA1" s="220" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="213"/>
+      <c r="AB1" s="220"/>
       <c r="AC1" s="32"/>
-      <c r="AD1" s="214" t="s">
+      <c r="AD1" s="221" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" s="214"/>
-      <c r="AF1" s="214"/>
-      <c r="AG1" s="214"/>
-      <c r="AH1" s="214"/>
-      <c r="AI1" s="214"/>
-      <c r="AJ1" s="214"/>
-      <c r="AK1" s="214"/>
-      <c r="AL1" s="214"/>
-      <c r="AM1" s="214"/>
-      <c r="AN1" s="214"/>
-      <c r="AO1" s="214"/>
-      <c r="AP1" s="214"/>
-      <c r="AQ1" s="214"/>
-      <c r="AR1" s="214"/>
-      <c r="AS1" s="214"/>
-      <c r="AT1" s="214"/>
-      <c r="AU1" s="214"/>
-      <c r="AV1" s="214"/>
-      <c r="AW1" s="214"/>
-      <c r="AX1" s="214"/>
-      <c r="AY1" s="214"/>
+      <c r="AE1" s="221"/>
+      <c r="AF1" s="221"/>
+      <c r="AG1" s="221"/>
+      <c r="AH1" s="221"/>
+      <c r="AI1" s="221"/>
+      <c r="AJ1" s="221"/>
+      <c r="AK1" s="221"/>
+      <c r="AL1" s="221"/>
+      <c r="AM1" s="221"/>
+      <c r="AN1" s="221"/>
+      <c r="AO1" s="221"/>
+      <c r="AP1" s="221"/>
+      <c r="AQ1" s="221"/>
+      <c r="AR1" s="221"/>
+      <c r="AS1" s="221"/>
+      <c r="AT1" s="221"/>
+      <c r="AU1" s="221"/>
+      <c r="AV1" s="221"/>
+      <c r="AW1" s="221"/>
+      <c r="AX1" s="221"/>
+      <c r="AY1" s="221"/>
     </row>
     <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -13318,14 +13333,14 @@
       <c r="S53" s="165" t="s">
         <v>125</v>
       </c>
-      <c r="T53" s="215">
+      <c r="T53" s="213">
         <v>-1</v>
       </c>
       <c r="U53" s="167" t="s">
         <v>107</v>
       </c>
       <c r="V53" s="168" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="W53" s="169" t="b">
         <v>1</v>
@@ -13470,14 +13485,14 @@
       <c r="S54" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T54" s="216">
+      <c r="T54" s="214">
         <v>-1</v>
       </c>
       <c r="U54" s="50" t="s">
         <v>181</v>
       </c>
       <c r="V54" s="11" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="W54" s="35" t="b">
         <v>1</v>
@@ -13618,14 +13633,14 @@
       <c r="S55" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T55" s="216">
+      <c r="T55" s="214">
         <v>-1</v>
       </c>
       <c r="U55" s="50" t="s">
         <v>182</v>
       </c>
       <c r="V55" s="11" t="s">
-        <v>45</v>
+        <v>328</v>
       </c>
       <c r="W55" s="35" t="b">
         <v>1</v>
@@ -13639,7 +13654,7 @@
       <c r="Z55" s="35">
         <v>10</v>
       </c>
-      <c r="AA55" s="218" t="s">
+      <c r="AA55" s="216" t="s">
         <v>151</v>
       </c>
       <c r="AB55" s="51" t="s">
@@ -13770,14 +13785,14 @@
       <c r="S56" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T56" s="216">
+      <c r="T56" s="214">
         <v>-1</v>
       </c>
       <c r="U56" s="50" t="s">
         <v>104</v>
       </c>
       <c r="V56" s="11" t="s">
-        <v>198</v>
+        <v>326</v>
       </c>
       <c r="W56" s="35" t="b">
         <v>1</v>
@@ -13922,14 +13937,14 @@
       <c r="S57" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T57" s="216">
+      <c r="T57" s="214">
         <v>-1</v>
       </c>
       <c r="U57" s="50" t="s">
         <v>108</v>
       </c>
       <c r="V57" s="11" t="s">
-        <v>198</v>
+        <v>324</v>
       </c>
       <c r="W57" s="35" t="b">
         <v>1</v>
@@ -14072,14 +14087,14 @@
       <c r="S58" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="T58" s="216">
+      <c r="T58" s="214">
         <v>-1</v>
       </c>
       <c r="U58" s="76" t="s">
         <v>179</v>
       </c>
       <c r="V58" s="77" t="s">
-        <v>45</v>
+        <v>314</v>
       </c>
       <c r="W58" s="78" t="b">
         <v>1</v>
@@ -14093,7 +14108,7 @@
       <c r="Z58" s="78">
         <v>10</v>
       </c>
-      <c r="AA58" s="219" t="s">
+      <c r="AA58" s="217" t="s">
         <v>151</v>
       </c>
       <c r="AB58" s="79" t="s">
@@ -14224,14 +14239,14 @@
       <c r="S59" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="T59" s="216">
+      <c r="T59" s="214">
         <v>-1</v>
       </c>
       <c r="U59" s="63" t="s">
         <v>180</v>
       </c>
       <c r="V59" s="64" t="s">
-        <v>44</v>
+        <v>315</v>
       </c>
       <c r="W59" s="65" t="b">
         <v>1</v>
@@ -14245,7 +14260,7 @@
       <c r="Z59" s="65">
         <v>10</v>
       </c>
-      <c r="AA59" s="220" t="s">
+      <c r="AA59" s="218" t="s">
         <v>151</v>
       </c>
       <c r="AB59" s="66" t="s">
@@ -14376,14 +14391,14 @@
       <c r="S60" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="T60" s="217">
+      <c r="T60" s="215">
         <v>-1</v>
       </c>
       <c r="U60" s="89" t="s">
         <v>183</v>
       </c>
       <c r="V60" s="90" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
       <c r="W60" s="91" t="b">
         <v>1</v>
@@ -14397,7 +14412,7 @@
       <c r="Z60" s="91">
         <v>10</v>
       </c>
-      <c r="AA60" s="221" t="s">
+      <c r="AA60" s="219" t="s">
         <v>151</v>
       </c>
       <c r="AB60" s="92" t="s">

</xml_diff>

<commit_message>
Removed the duration for the Push offers
Former-commit-id: 5663aacd7c6704b534664af9d1afa609144a86fa
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="329">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -5660,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="V60" sqref="V60"/>
+    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9586,8 +9586,8 @@
       <c r="AB27" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC27" s="51">
-        <v>2880</v>
+      <c r="AC27" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="AD27" s="27" t="s">
         <v>210</v>
@@ -9738,8 +9738,8 @@
       <c r="AB28" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC28" s="51">
-        <v>2880</v>
+      <c r="AC28" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="AD28" s="27" t="s">
         <v>210</v>
@@ -9890,8 +9890,8 @@
       <c r="AB29" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC29" s="51">
-        <v>2880</v>
+      <c r="AC29" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="AD29" s="27" t="s">
         <v>210</v>
@@ -10042,8 +10042,8 @@
       <c r="AB30" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC30" s="51">
-        <v>2880</v>
+      <c r="AC30" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="AD30" s="27" t="s">
         <v>210</v>
@@ -10194,8 +10194,8 @@
       <c r="AB31" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC31" s="51">
-        <v>2880</v>
+      <c r="AC31" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="AD31" s="27" t="s">
         <v>210</v>
@@ -10346,8 +10346,9 @@
       <c r="AB32" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AC32" s="51">
-        <v>2880</v>
+      <c r="AC32" s="51" t="str">
+        <f>AC26</f>
+        <v>-</v>
       </c>
       <c r="AD32" s="27" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
Bug fixing rotational offers min app version
Former-commit-id: 7e6c5a852288d2bd66b274d20e30b292d6721099
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="330">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -1015,6 +1015,9 @@
   </si>
   <si>
     <t>TID_STORE_PACK_CURRENCYCATCHUPPACK1</t>
+  </si>
+  <si>
+    <t>1.32</t>
   </si>
 </sst>
 </file>
@@ -5660,8 +5663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="V60" sqref="V60"/>
+    <sheetView tabSelected="1" topLeftCell="R16" workbookViewId="0">
+      <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10490,7 +10493,7 @@
         <v>2880</v>
       </c>
       <c r="AD33" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE33" s="27" t="s">
         <v>151</v>
@@ -10629,8 +10632,8 @@
       <c r="AC34" s="92">
         <v>2880</v>
       </c>
-      <c r="AD34" s="93" t="s">
-        <v>210</v>
+      <c r="AD34" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE34" s="93" t="s">
         <v>151</v>
@@ -10773,8 +10776,8 @@
       <c r="AC35" s="106">
         <v>2880</v>
       </c>
-      <c r="AD35" s="107" t="s">
-        <v>210</v>
+      <c r="AD35" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE35" s="107" t="s">
         <v>151</v>
@@ -10918,7 +10921,7 @@
         <v>2880</v>
       </c>
       <c r="AD36" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE36" s="27" t="s">
         <v>151</v>
@@ -11062,7 +11065,7 @@
         <v>2880</v>
       </c>
       <c r="AD37" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE37" s="27" t="s">
         <v>151</v>
@@ -11206,7 +11209,7 @@
         <v>2880</v>
       </c>
       <c r="AD38" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE38" s="27" t="s">
         <v>151</v>
@@ -11346,7 +11349,7 @@
         <v>2880</v>
       </c>
       <c r="AD39" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE39" s="27" t="s">
         <v>151</v>
@@ -11491,8 +11494,8 @@
       <c r="AC40" s="92">
         <v>2880</v>
       </c>
-      <c r="AD40" s="93" t="s">
-        <v>210</v>
+      <c r="AD40" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE40" s="93" t="s">
         <v>151</v>
@@ -11637,8 +11640,8 @@
       <c r="AC41" s="170">
         <v>2880</v>
       </c>
-      <c r="AD41" s="171" t="s">
-        <v>210</v>
+      <c r="AD41" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE41" s="171" t="s">
         <v>151</v>
@@ -11778,7 +11781,7 @@
         <v>2880</v>
       </c>
       <c r="AD42" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE42" s="27" t="s">
         <v>151</v>
@@ -11922,7 +11925,7 @@
         <v>2880</v>
       </c>
       <c r="AD43" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE43" s="27" t="s">
         <v>151</v>
@@ -12062,7 +12065,7 @@
         <v>2880</v>
       </c>
       <c r="AD44" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE44" s="27" t="s">
         <v>151</v>
@@ -12206,7 +12209,7 @@
         <v>2880</v>
       </c>
       <c r="AD45" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE45" s="27" t="s">
         <v>151</v>
@@ -12351,8 +12354,8 @@
       <c r="AC46" s="79">
         <v>2880</v>
       </c>
-      <c r="AD46" s="80" t="s">
-        <v>210</v>
+      <c r="AD46" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE46" s="80" t="s">
         <v>151</v>
@@ -12491,8 +12494,8 @@
       <c r="AC47" s="106">
         <v>2880</v>
       </c>
-      <c r="AD47" s="107" t="s">
-        <v>210</v>
+      <c r="AD47" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE47" s="107" t="s">
         <v>151</v>
@@ -12632,7 +12635,7 @@
         <v>2880</v>
       </c>
       <c r="AD48" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE48" s="27" t="s">
         <v>151</v>
@@ -12772,7 +12775,7 @@
         <v>2880</v>
       </c>
       <c r="AD49" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE49" s="27" t="s">
         <v>151</v>
@@ -12922,7 +12925,7 @@
         <v>2880</v>
       </c>
       <c r="AD50" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE50" s="27" t="s">
         <v>151</v>
@@ -13072,7 +13075,7 @@
         <v>2880</v>
       </c>
       <c r="AD51" s="27" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="AE51" s="27" t="s">
         <v>151</v>
@@ -13211,8 +13214,8 @@
       <c r="AC52" s="92">
         <v>2880</v>
       </c>
-      <c r="AD52" s="93" t="s">
-        <v>210</v>
+      <c r="AD52" s="27" t="s">
+        <v>329</v>
       </c>
       <c r="AE52" s="93" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Small tweak on the order for progression offers
Former-commit-id: eb33f9cd3e78febd12f5427a232219c7dd0baa1f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5660,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
-      <selection activeCell="AC32" sqref="AC32"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13933,7 +13933,7 @@
         <v>151</v>
       </c>
       <c r="R57" s="47">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="S57" s="48" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Starter pack modified: instead of 4 eggs -> 2 eggs + 100 gems. Also, instead of 3 days duration -> 1 week duration
Former-commit-id: c6db7ee46f29a4245b2222d0693560f76b6fc2f1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="OLD" sheetId="1" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="329">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -5660,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="R57" sqref="R57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13918,22 +13918,22 @@
         <v>27</v>
       </c>
       <c r="M57" s="45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N57" s="45" t="s">
         <v>248</v>
       </c>
       <c r="O57" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="P57" s="46" t="s">
-        <v>151</v>
+        <v>19</v>
+      </c>
+      <c r="P57" s="46">
+        <v>100</v>
       </c>
       <c r="Q57" s="46" t="s">
         <v>151</v>
       </c>
       <c r="R57" s="47">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="S57" s="48" t="s">
         <v>99</v>
@@ -13964,7 +13964,7 @@
         <v>151</v>
       </c>
       <c r="AC57" s="51">
-        <v>4320</v>
+        <v>10080</v>
       </c>
       <c r="AD57" s="27" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
We will show the discount in the starter pack. 80%
Former-commit-id: 0905643d16e2efd7a5ab560b352595a1c1a09d9e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="329">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -5661,7 +5661,7 @@
   <dimension ref="B1:AY76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="T57" sqref="T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13938,8 +13938,8 @@
       <c r="S57" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="T57" s="214">
-        <v>-1</v>
+      <c r="T57" s="214" t="s">
+        <v>174</v>
       </c>
       <c r="U57" s="50" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Changed priority for the Blaze starter Pack
Former-commit-id: 78e2eea356f161b8a92bb8db0453e365faa6b639
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5660,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="T57" sqref="T57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Z58" sqref="Z58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13353,7 +13353,7 @@
         <v>26</v>
       </c>
       <c r="Z53" s="169">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA53" s="170" t="s">
         <v>151</v>
@@ -13505,7 +13505,7 @@
         <v>26</v>
       </c>
       <c r="Z54" s="35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA54" s="51"/>
       <c r="AB54" s="51" t="s">
@@ -13805,7 +13805,7 @@
         <v>26</v>
       </c>
       <c r="Z56" s="35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA56" s="51" t="s">
         <v>151</v>
@@ -13933,7 +13933,7 @@
         <v>151</v>
       </c>
       <c r="R57" s="47">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="S57" s="48" t="s">
         <v>99</v>
@@ -13957,7 +13957,7 @@
         <v>26</v>
       </c>
       <c r="Z57" s="35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA57" s="51"/>
       <c r="AB57" s="51" t="s">

</xml_diff>

<commit_message>
Happy Hour Table added in content!
Former-commit-id: a6cfb5effa7b340a70f6b2313e4ce37770b0fe2e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3049" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3062" uniqueCount="343">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -1027,15 +1027,52 @@
   </si>
   <si>
     <t>8:999</t>
+  </si>
+  <si>
+    <t>{happyHourDefinitions}</t>
+  </si>
+  <si>
+    <t>happy_hour</t>
+  </si>
+  <si>
+    <t>[triggerRunNumber]</t>
+  </si>
+  <si>
+    <t>[happyHourTimer]</t>
+  </si>
+  <si>
+    <t>[percentageMinExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageMaxExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageIncrement]</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>HAPPY HOUR DEFINITIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1170,8 +1207,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1304,8 +1348,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1586,114 +1636,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1701,606 +1765,933 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2831,281 +3222,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5365,26 +5481,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5413,88 +5509,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY76" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AY76" totalsRowShown="0" headerRowDxfId="99" headerRowBorderDxfId="98" tableBorderDxfId="97">
   <autoFilter ref="B2:AY76">
     <filterColumn colId="4">
-      <colorFilter dxfId="92"/>
+      <colorFilter dxfId="96"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="B26:AY76">
     <sortCondition descending="1" ref="E2:E76"/>
   </sortState>
   <tableColumns count="50">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="91"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="89"/>
-    <tableColumn id="49" name="[type]" dataDxfId="88"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="87"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="86"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="85"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="84"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="83"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="82"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="81"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="80"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="79"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="78"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="77"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="76"/>
-    <tableColumn id="7" name="[order]" dataDxfId="75"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="74"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="73"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="72"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="71"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="70"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="69"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="68"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="67"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="66"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="65"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="64"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="63"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="62"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="61"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="60"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="59"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="58"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="57"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="56"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="55"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="54"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="53"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="52"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="51"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="50"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="49"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="48"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="47"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="46"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="45"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="44"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="43"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="42"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="95"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="94"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="93"/>
+    <tableColumn id="49" name="[type]" dataDxfId="92"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="91"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="90"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="89"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="88"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="87"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="86"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="85"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="84"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="83"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="82"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="81"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="80"/>
+    <tableColumn id="7" name="[order]" dataDxfId="79"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="78"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="77"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="76"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="75"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="74"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="73"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="72"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="71"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="70"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="69"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="68"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="67"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="66"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="65"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="64"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="63"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="62"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="61"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="60"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="59"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="58"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="57"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="56"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="55"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="54"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="53"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="52"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="51"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="50"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="49"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="48"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="47"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
   <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="10"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="9"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="8"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="7"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="6"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="5"/>
-    <tableColumn id="4" name="[order]" dataDxfId="4"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="3"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="2"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="39"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="38"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="37"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="36"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="35"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="34"/>
+    <tableColumn id="4" name="[order]" dataDxfId="33"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="32"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="31"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="30"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5797,10 +5893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AY76"/>
+  <dimension ref="B1:AY83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17052,17 +17148,86 @@
         <v>151</v>
       </c>
     </row>
+    <row r="80" spans="2:51" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B80" s="243" t="s">
+        <v>342</v>
+      </c>
+      <c r="C80" s="243"/>
+      <c r="D80" s="243"/>
+      <c r="E80" s="243"/>
+    </row>
+    <row r="82" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B82" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="C82" s="240" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" s="241" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="F82" s="241" t="s">
+        <v>336</v>
+      </c>
+      <c r="G82" s="242" t="s">
+        <v>337</v>
+      </c>
+      <c r="H82" s="242" t="s">
+        <v>338</v>
+      </c>
+      <c r="I82" s="242" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="239" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="239" t="s">
+        <v>334</v>
+      </c>
+      <c r="D83" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="239">
+        <v>0</v>
+      </c>
+      <c r="F83" s="239">
+        <v>120</v>
+      </c>
+      <c r="G83" s="239">
+        <v>1</v>
+      </c>
+      <c r="H83" s="239" t="s">
+        <v>340</v>
+      </c>
+      <c r="I83" s="239" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
+    <mergeCell ref="B80:E80"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F76">
-    <cfRule type="containsText" dxfId="97" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="28" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D83">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18102,127 +18267,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="39" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="23" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="22" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="36" priority="20">
+    <cfRule type="expression" dxfId="21" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="35" priority="19">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="18" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="16" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="26" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding Happy Hour table, as it seems it was 'lost' in some merges since 2.0
Former-commit-id: b0bbb005d2b69bdb82c1cbd12abb919eb8dfc325
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3126" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3139" uniqueCount="348">
   <si>
     <t>OFFER PACKS DEFINITIONS</t>
   </si>
@@ -1042,15 +1042,52 @@
   </si>
   <si>
     <t>real</t>
+  </si>
+  <si>
+    <t>HAPPY HOUR DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{happyHourDefinitions}</t>
+  </si>
+  <si>
+    <t>[triggerRunNumber]</t>
+  </si>
+  <si>
+    <t>[happyHourTimer]</t>
+  </si>
+  <si>
+    <t>[percentageMinExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageMaxExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageIncrement]</t>
+  </si>
+  <si>
+    <t>happy_hour</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1192,8 +1229,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1326,8 +1370,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1621,114 +1671,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1736,942 +1800,630 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="101">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3222,6 +2974,281 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -4641,6 +4668,47 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5415,6 +5483,14 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -5473,6 +5549,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5504,86 +5600,86 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="97" tableBorderDxfId="96">
   <autoFilter ref="B2:AZ76">
     <filterColumn colId="4">
-      <colorFilter dxfId="0"/>
+      <colorFilter dxfId="95"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="B26:AY76">
     <sortCondition descending="1" ref="E2:E76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="95"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="94"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="93"/>
-    <tableColumn id="49" name="[type]" dataDxfId="92"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="91"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="90"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="89"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="88"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="87"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="86"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="85"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="84"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="83"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="82"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="81"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="80"/>
-    <tableColumn id="7" name="[order]" dataDxfId="79"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="78"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="1"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="77"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="76"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="75"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="74"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="73"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="72"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="71"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="70"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="69"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="68"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="67"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="66"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="65"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="64"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="63"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="62"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="61"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="60"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="59"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="58"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="57"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="56"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="55"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="54"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="53"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="52"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="51"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="50"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="49"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="48"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="47"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="46"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="94"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="93"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="92"/>
+    <tableColumn id="49" name="[type]" dataDxfId="91"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="90"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="89"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="88"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="87"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="86"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="85"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="84"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="83"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="82"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="81"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="80"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="79"/>
+    <tableColumn id="7" name="[order]" dataDxfId="78"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="77"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="76"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="75"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="74"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="73"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="72"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="71"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="70"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="69"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="68"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="67"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="66"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="65"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="64"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="63"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="62"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="61"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="60"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="59"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="58"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="57"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="56"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="55"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="54"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="53"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="52"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="51"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="50"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="49"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="48"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="47"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="46"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="45"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions_OLD" displayName="offerPacksDefinitions_OLD" ref="B4:N44" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
   <autoFilter ref="B4:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="15" name="[paramValue]" dataDxfId="39"/>
-    <tableColumn id="7" name="[itemType]" dataDxfId="38"/>
-    <tableColumn id="8" name="[itemAmount]" dataDxfId="37"/>
-    <tableColumn id="9" name="[itemSku]" dataDxfId="36"/>
-    <tableColumn id="23" name="[itemFeatured]" dataDxfId="35"/>
-    <tableColumn id="22" name="[minAppVersion]" dataDxfId="34"/>
-    <tableColumn id="4" name="[order]" dataDxfId="33"/>
-    <tableColumn id="24" name="[refPrice]" dataDxfId="32"/>
-    <tableColumn id="6" name="[discount]" dataDxfId="31"/>
-    <tableColumn id="3" name="[iapSku]" dataDxfId="30"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="offerPacksDefinitions_OLD" dataDxfId="14"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="15" name="[paramValue]" dataDxfId="12"/>
+    <tableColumn id="7" name="[itemType]" dataDxfId="11"/>
+    <tableColumn id="8" name="[itemAmount]" dataDxfId="10"/>
+    <tableColumn id="9" name="[itemSku]" dataDxfId="9"/>
+    <tableColumn id="23" name="[itemFeatured]" dataDxfId="8"/>
+    <tableColumn id="22" name="[minAppVersion]" dataDxfId="7"/>
+    <tableColumn id="4" name="[order]" dataDxfId="6"/>
+    <tableColumn id="24" name="[refPrice]" dataDxfId="5"/>
+    <tableColumn id="6" name="[discount]" dataDxfId="4"/>
+    <tableColumn id="3" name="[iapSku]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5886,10 +5982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AZ76"/>
+  <dimension ref="B1:AZ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T74" sqref="T74"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5942,41 +6038,41 @@
       <c r="T1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="242" t="s">
+      <c r="U1" s="240" t="s">
         <v>335</v>
       </c>
-      <c r="V1" s="242" t="s">
+      <c r="V1" s="240" t="s">
         <v>336</v>
       </c>
-      <c r="AA1" s="238" t="s">
+      <c r="AA1" s="241" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="238"/>
+      <c r="AB1" s="241"/>
       <c r="AC1" s="32"/>
-      <c r="AD1" s="239" t="s">
+      <c r="AD1" s="242" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" s="239"/>
-      <c r="AF1" s="239"/>
-      <c r="AG1" s="239"/>
-      <c r="AH1" s="239"/>
-      <c r="AI1" s="239"/>
-      <c r="AJ1" s="239"/>
-      <c r="AK1" s="239"/>
-      <c r="AL1" s="239"/>
-      <c r="AM1" s="239"/>
-      <c r="AN1" s="239"/>
-      <c r="AO1" s="239"/>
-      <c r="AP1" s="239"/>
-      <c r="AQ1" s="239"/>
-      <c r="AR1" s="239"/>
-      <c r="AS1" s="239"/>
-      <c r="AT1" s="239"/>
-      <c r="AU1" s="239"/>
-      <c r="AV1" s="239"/>
-      <c r="AW1" s="239"/>
-      <c r="AX1" s="239"/>
-      <c r="AY1" s="239"/>
+      <c r="AE1" s="242"/>
+      <c r="AF1" s="242"/>
+      <c r="AG1" s="242"/>
+      <c r="AH1" s="242"/>
+      <c r="AI1" s="242"/>
+      <c r="AJ1" s="242"/>
+      <c r="AK1" s="242"/>
+      <c r="AL1" s="242"/>
+      <c r="AM1" s="242"/>
+      <c r="AN1" s="242"/>
+      <c r="AO1" s="242"/>
+      <c r="AP1" s="242"/>
+      <c r="AQ1" s="242"/>
+      <c r="AR1" s="242"/>
+      <c r="AS1" s="242"/>
+      <c r="AT1" s="242"/>
+      <c r="AU1" s="242"/>
+      <c r="AV1" s="242"/>
+      <c r="AW1" s="242"/>
+      <c r="AX1" s="242"/>
+      <c r="AY1" s="242"/>
     </row>
     <row r="2" spans="2:52" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -11834,7 +11930,7 @@
       <c r="S40" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="T40" s="240" t="s">
+      <c r="T40" s="238" t="s">
         <v>337</v>
       </c>
       <c r="U40" s="152">
@@ -13650,7 +13746,7 @@
       <c r="S52" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="T52" s="240" t="s">
+      <c r="T52" s="238" t="s">
         <v>337</v>
       </c>
       <c r="U52" s="93">
@@ -14399,7 +14495,7 @@
       <c r="S57" s="227" t="s">
         <v>99</v>
       </c>
-      <c r="T57" s="241" t="s">
+      <c r="T57" s="239" t="s">
         <v>337</v>
       </c>
       <c r="U57" s="228">
@@ -14550,7 +14646,7 @@
       <c r="S58" s="213" t="s">
         <v>125</v>
       </c>
-      <c r="T58" s="240" t="s">
+      <c r="T58" s="238" t="s">
         <v>337</v>
       </c>
       <c r="U58" s="62">
@@ -14844,7 +14940,7 @@
       <c r="S60" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="T60" s="240" t="s">
+      <c r="T60" s="238" t="s">
         <v>337</v>
       </c>
       <c r="U60" s="152">
@@ -17372,17 +17468,86 @@
         <v>151</v>
       </c>
     </row>
+    <row r="80" spans="2:52" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B80" s="244" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" s="244"/>
+      <c r="D80" s="244"/>
+      <c r="E80" s="244"/>
+    </row>
+    <row r="82" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B82" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="C82" s="245" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" s="246" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="F82" s="246" t="s">
+        <v>341</v>
+      </c>
+      <c r="G82" s="247" t="s">
+        <v>342</v>
+      </c>
+      <c r="H82" s="247" t="s">
+        <v>343</v>
+      </c>
+      <c r="I82" s="247" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="243" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="243" t="s">
+        <v>345</v>
+      </c>
+      <c r="D83" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="243">
+        <v>0</v>
+      </c>
+      <c r="F83" s="243">
+        <v>120</v>
+      </c>
+      <c r="G83" s="243">
+        <v>1</v>
+      </c>
+      <c r="H83" s="243" t="s">
+        <v>346</v>
+      </c>
+      <c r="I83" s="243" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
+    <mergeCell ref="B80:E80"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F76">
-    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="100" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="99" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D83">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18422,127 +18587,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:N13 I15:N25 I38:N44">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="43" priority="27">
       <formula>$B5&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:H13 F24:H24 E15:H23 E25:H25 E38:H44">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="42" priority="26">
       <formula>$B5&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13 D15 D38:D44">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>$B5&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="40" priority="22">
       <formula>$B16&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24 F24:L24 B5:N13 B15:L23 B25:L25 M15:N25 B38:N44">
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="39" priority="21">
       <formula>$B5="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="21" priority="20">
+    <cfRule type="expression" dxfId="38" priority="20">
       <formula>$B24&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="37" priority="19">
       <formula>$B24="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:N14">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="36" priority="18">
       <formula>$B14&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="18" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>$B14&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="34" priority="16">
       <formula>$B14&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:N14">
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="33" priority="15">
       <formula>$B14="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:N34 I37:N37">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>$B26&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34 E26:H33 E37:H37">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>$B26&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D34 D37">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="30" priority="12">
       <formula>$B26&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 F34:L34 B26:L33 M26:N34 B37:N37">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>$B26="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>$B34&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>$B34="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:N35">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>$B35&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:H35">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>$B35&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>$B35&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:N35">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>$B35="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:N36">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>$B36&lt;&gt;"&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$B36&lt;&gt;"&lt;Item&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$B36&lt;&gt;"&lt;Param&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:N36">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$B36="&lt;Definition&gt;"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Offers: Content - Merge conflict resolution.
Former-commit-id: 9f1f4dc3f2b4b260d4e12015c53bc434ace08249
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B31C280-7988-B647-BCDA-4F07F18FFFAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="32700" windowHeight="20535"/>
+    <workbookView xWindow="9800" yWindow="1340" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="Settings" sheetId="4" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="181029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3227" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3240" uniqueCount="341">
   <si>
     <t>[sku]</t>
   </si>
@@ -1020,13 +1021,43 @@
   </si>
   <si>
     <t>AdOffer4</t>
+  </si>
+  <si>
+    <t>HAPPY HOUR DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{happyHourDefinitions}</t>
+  </si>
+  <si>
+    <t>[triggerRunNumber]</t>
+  </si>
+  <si>
+    <t>[happyHourTimer]</t>
+  </si>
+  <si>
+    <t>[percentageMinExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageMaxExtraGems]</t>
+  </si>
+  <si>
+    <t>[percentageIncrement]</t>
+  </si>
+  <si>
+    <t>happy_hour</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1174,8 +1205,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1296,8 +1334,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1556,11 +1600,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="245">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2184,12 +2265,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2281,12 +2356,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="69">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2657,13 +2750,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -2673,6 +2759,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -5006,6 +5099,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5034,80 +5147,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B2:AZ76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="B2:AZ76" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="63"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="62"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="61"/>
-    <tableColumn id="49" name="[type]" dataDxfId="60"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="59"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="58"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="57"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="56"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="55"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="54"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="53"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="52"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="51"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="50"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="49"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[order]" dataDxfId="47"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="46"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="45"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="44"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="43"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="42"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="41"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="40"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="39"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="38"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="37"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="36"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="35"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="34"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="33"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="32"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="31"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="30"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="29"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="28"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="27"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="26"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="25"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="24"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="23"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="22"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="21"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="20"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="19"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="18"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="17"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="16"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="15"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="14"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="62"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[uniqueId]" dataDxfId="61"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[type]" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="59"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[purchaseLimit]" dataDxfId="58"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[item1Featured]" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="56"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[item1Amount]" dataDxfId="55"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[item1Sku]" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="53"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[item2Amount]" dataDxfId="52"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[item2Sku]" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="50"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[item3Amount]" dataDxfId="49"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[item3Sku]" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="46"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[currency]" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="39"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="38"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="37"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="36"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[durationMinutes]" dataDxfId="35"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="34"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="33"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="32"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="31"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="30"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="29"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[maxSpent]" dataDxfId="28"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[minNumberOfPurchases]" dataDxfId="27"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[minutesSinceLastPurchase]" dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="24"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="23"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="22"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="21"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="20"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="19"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="18"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="17"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="16"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="15"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="14"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11">
-  <autoFilter ref="B2:I3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="9"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="7"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="6"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="5"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="4"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="3"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{offerSettings}" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="[refreshFrequency]" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[rotationalActiveOffers]" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[rotationalHistorySize]" dataDxfId="5"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="[freeHistorySize]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[freeCooldownMinutes]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[emptyValue]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5409,56 +5522,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AZ81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:AZ87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+      <pane ySplit="2" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.875" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" customWidth="1"/>
-    <col min="22" max="22" width="42.75" customWidth="1"/>
-    <col min="23" max="23" width="42.25" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" customWidth="1"/>
+    <col min="22" max="22" width="42.6640625" customWidth="1"/>
+    <col min="23" max="23" width="42.1640625" customWidth="1"/>
     <col min="24" max="24" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.25" customWidth="1"/>
-    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" customWidth="1"/>
+    <col min="27" max="27" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="32" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" customWidth="1"/>
-    <col min="34" max="34" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="19.375" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="19.33203125" customWidth="1"/>
     <col min="37" max="38" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.75" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" customWidth="1"/>
     <col min="40" max="40" width="15" customWidth="1"/>
     <col min="41" max="41" width="19" customWidth="1"/>
-    <col min="42" max="42" width="16.875" customWidth="1"/>
-    <col min="43" max="43" width="16.125" customWidth="1"/>
-    <col min="44" max="44" width="14.625" customWidth="1"/>
-    <col min="45" max="45" width="20.125" customWidth="1"/>
+    <col min="42" max="42" width="16.83203125" customWidth="1"/>
+    <col min="43" max="43" width="16.1640625" customWidth="1"/>
+    <col min="44" max="44" width="14.6640625" customWidth="1"/>
+    <col min="45" max="45" width="20.1640625" customWidth="1"/>
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:52" s="10" customFormat="1" ht="135" x14ac:dyDescent="0.2">
       <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
@@ -5474,37 +5587,37 @@
       <c r="V1" s="210" t="s">
         <v>311</v>
       </c>
-      <c r="AA1" s="211" t="s">
+      <c r="AA1" s="243" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="211"/>
+      <c r="AB1" s="243"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="212" t="s">
+      <c r="AD1" s="244" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="212"/>
-      <c r="AF1" s="212"/>
-      <c r="AG1" s="212"/>
-      <c r="AH1" s="212"/>
-      <c r="AI1" s="212"/>
-      <c r="AJ1" s="212"/>
-      <c r="AK1" s="212"/>
-      <c r="AL1" s="212"/>
-      <c r="AM1" s="212"/>
-      <c r="AN1" s="212"/>
-      <c r="AO1" s="212"/>
-      <c r="AP1" s="212"/>
-      <c r="AQ1" s="212"/>
-      <c r="AR1" s="212"/>
-      <c r="AS1" s="212"/>
-      <c r="AT1" s="212"/>
-      <c r="AU1" s="212"/>
-      <c r="AV1" s="212"/>
-      <c r="AW1" s="212"/>
-      <c r="AX1" s="212"/>
-      <c r="AY1" s="212"/>
+      <c r="AE1" s="244"/>
+      <c r="AF1" s="244"/>
+      <c r="AG1" s="244"/>
+      <c r="AH1" s="244"/>
+      <c r="AI1" s="244"/>
+      <c r="AJ1" s="244"/>
+      <c r="AK1" s="244"/>
+      <c r="AL1" s="244"/>
+      <c r="AM1" s="244"/>
+      <c r="AN1" s="244"/>
+      <c r="AO1" s="244"/>
+      <c r="AP1" s="244"/>
+      <c r="AQ1" s="244"/>
+      <c r="AR1" s="244"/>
+      <c r="AS1" s="244"/>
+      <c r="AT1" s="244"/>
+      <c r="AU1" s="244"/>
+      <c r="AV1" s="244"/>
+      <c r="AW1" s="244"/>
+      <c r="AX1" s="244"/>
+      <c r="AY1" s="244"/>
     </row>
-    <row r="2" spans="2:52" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:52" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5659,7 +5772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -5814,7 +5927,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
@@ -5969,7 +6082,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -6124,7 +6237,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
@@ -6279,7 +6392,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -6434,7 +6547,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -6589,7 +6702,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
@@ -6744,7 +6857,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
@@ -6899,7 +7012,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B11" s="99" t="s">
         <v>2</v>
       </c>
@@ -7054,7 +7167,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
@@ -7209,7 +7322,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -7364,7 +7477,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B14" s="26" t="s">
         <v>2</v>
       </c>
@@ -7520,7 +7633,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B15" s="27" t="s">
         <v>2</v>
       </c>
@@ -7675,7 +7788,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B16" s="27" t="s">
         <v>2</v>
       </c>
@@ -7830,7 +7943,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="118" t="s">
         <v>2</v>
       </c>
@@ -7985,7 +8098,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B18" s="41" t="s">
         <v>2</v>
       </c>
@@ -8140,7 +8253,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -8295,7 +8408,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
@@ -8450,7 +8563,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B21" s="27" t="s">
         <v>2</v>
       </c>
@@ -8605,7 +8718,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>2</v>
       </c>
@@ -8758,7 +8871,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>2</v>
       </c>
@@ -8911,7 +9024,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B24" s="27" t="s">
         <v>2</v>
       </c>
@@ -9062,7 +9175,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -9217,7 +9330,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B26" s="27" t="s">
         <v>2</v>
       </c>
@@ -9368,7 +9481,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B27" s="27" t="s">
         <v>2</v>
       </c>
@@ -9523,7 +9636,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -9660,7 +9773,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B29" s="27" t="s">
         <v>2</v>
       </c>
@@ -9807,7 +9920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>2</v>
       </c>
@@ -9954,7 +10067,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
         <v>2</v>
       </c>
@@ -10097,7 +10210,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
@@ -10246,7 +10359,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>2</v>
       </c>
@@ -10389,7 +10502,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B34" s="67" t="s">
         <v>2</v>
       </c>
@@ -10532,7 +10645,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B35" s="81" t="s">
         <v>2</v>
       </c>
@@ -10675,7 +10788,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
@@ -10828,7 +10941,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
@@ -10981,7 +11094,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B38" s="26" t="s">
         <v>2</v>
       </c>
@@ -11128,7 +11241,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B39" s="26" t="s">
         <v>2</v>
       </c>
@@ -11271,7 +11384,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="67" t="s">
         <v>2</v>
       </c>
@@ -11418,7 +11531,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B41" s="138" t="s">
         <v>2</v>
       </c>
@@ -11561,7 +11674,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B42" s="26" t="s">
         <v>2</v>
       </c>
@@ -11710,7 +11823,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
@@ -11859,7 +11972,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
@@ -12010,7 +12123,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B45" s="26" t="s">
         <v>2</v>
       </c>
@@ -12157,11 +12270,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="218" t="s">
+      <c r="C46" s="216" t="s">
         <v>199</v>
       </c>
       <c r="D46" s="55" t="s">
@@ -12304,14 +12417,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B47" s="216" t="s">
+    <row r="47" spans="2:52" x14ac:dyDescent="0.2">
+      <c r="B47" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="219" t="s">
+      <c r="C47" s="217" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="226" t="s">
+      <c r="D47" s="224" t="s">
         <v>127</v>
       </c>
       <c r="E47" s="81" t="s">
@@ -12362,7 +12475,7 @@
       <c r="T47" s="47" t="s">
         <v>312</v>
       </c>
-      <c r="U47" s="234">
+      <c r="U47" s="232">
         <v>-1</v>
       </c>
       <c r="V47" s="88" t="s">
@@ -12383,7 +12496,7 @@
       <c r="AA47" s="90">
         <v>10</v>
       </c>
-      <c r="AB47" s="236" t="s">
+      <c r="AB47" s="234" t="s">
         <v>127</v>
       </c>
       <c r="AC47" s="91" t="s">
@@ -12404,10 +12517,10 @@
       <c r="AH47" s="92">
         <v>4</v>
       </c>
-      <c r="AI47" s="237" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ47" s="237" t="s">
+      <c r="AI47" s="235" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ47" s="235" t="s">
         <v>127</v>
       </c>
       <c r="AK47" s="92" t="s">
@@ -12434,7 +12547,7 @@
       <c r="AR47" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="AS47" s="237" t="s">
+      <c r="AS47" s="235" t="s">
         <v>127</v>
       </c>
       <c r="AT47" s="92" t="s">
@@ -12459,7 +12572,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
@@ -12602,7 +12715,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B49" s="26" t="s">
         <v>2</v>
       </c>
@@ -12751,7 +12864,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
@@ -12894,7 +13007,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B51" s="26" t="s">
         <v>2</v>
       </c>
@@ -13041,7 +13154,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="67" t="s">
         <v>2</v>
       </c>
@@ -13188,14 +13301,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="217" t="s">
+    <row r="53" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="215" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="222" t="s">
+      <c r="C53" s="220" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="227" t="s">
+      <c r="D53" s="225" t="s">
         <v>127</v>
       </c>
       <c r="E53" s="138" t="s">
@@ -13343,7 +13456,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B54" s="27" t="s">
         <v>2</v>
       </c>
@@ -13498,7 +13611,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
@@ -13653,11 +13766,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B56" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="223" t="s">
+      <c r="C56" s="221" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="25" t="s">
@@ -13711,7 +13824,7 @@
       <c r="T56" s="47" t="s">
         <v>312</v>
       </c>
-      <c r="U56" s="234" t="s">
+      <c r="U56" s="232" t="s">
         <v>301</v>
       </c>
       <c r="V56" s="36" t="s">
@@ -13808,11 +13921,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:52" s="205" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B57" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="221" t="s">
+      <c r="C57" s="219" t="s">
         <v>212</v>
       </c>
       <c r="D57" s="192" t="s">
@@ -13836,16 +13949,16 @@
       <c r="J57" s="194">
         <v>250</v>
       </c>
-      <c r="K57" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="L57" s="230" t="s">
-        <v>127</v>
-      </c>
-      <c r="M57" s="230" t="s">
-        <v>127</v>
-      </c>
-      <c r="N57" s="230" t="s">
+      <c r="K57" s="226" t="s">
+        <v>127</v>
+      </c>
+      <c r="L57" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="N57" s="228" t="s">
         <v>127</v>
       </c>
       <c r="O57" s="195" t="s">
@@ -13963,11 +14076,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B58" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="225" t="s">
+      <c r="C58" s="223" t="s">
         <v>223</v>
       </c>
       <c r="D58" s="179" t="s">
@@ -14118,11 +14231,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B59" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="224" t="s">
+      <c r="C59" s="222" t="s">
         <v>214</v>
       </c>
       <c r="D59" s="41" t="s">
@@ -14146,25 +14259,25 @@
       <c r="J59" s="43">
         <v>1200</v>
       </c>
-      <c r="K59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="L59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="M59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="N59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="O59" s="233" t="s">
-        <v>127</v>
-      </c>
-      <c r="P59" s="233" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q59" s="233" t="s">
+      <c r="K59" s="227" t="s">
+        <v>127</v>
+      </c>
+      <c r="L59" s="229" t="s">
+        <v>127</v>
+      </c>
+      <c r="M59" s="229" t="s">
+        <v>127</v>
+      </c>
+      <c r="N59" s="229" t="s">
+        <v>127</v>
+      </c>
+      <c r="O59" s="231" t="s">
+        <v>127</v>
+      </c>
+      <c r="P59" s="231" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q59" s="231" t="s">
         <v>127</v>
       </c>
       <c r="R59" s="46">
@@ -14273,7 +14386,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="67" t="s">
         <v>2</v>
       </c>
@@ -14426,11 +14539,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B61" s="158" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="220" t="s">
+      <c r="C61" s="218" t="s">
         <v>200</v>
       </c>
       <c r="D61" s="158" t="s">
@@ -14463,7 +14576,7 @@
       <c r="M61" s="161">
         <v>100</v>
       </c>
-      <c r="N61" s="232" t="s">
+      <c r="N61" s="230" t="s">
         <v>127</v>
       </c>
       <c r="O61" s="162" t="s">
@@ -14484,7 +14597,7 @@
       <c r="T61" s="164" t="s">
         <v>312</v>
       </c>
-      <c r="U61" s="235">
+      <c r="U61" s="233">
         <v>-1</v>
       </c>
       <c r="V61" s="165" t="s">
@@ -14581,7 +14694,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B62" s="26" t="s">
         <v>2</v>
       </c>
@@ -14736,7 +14849,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B63" s="26" t="s">
         <v>2</v>
       </c>
@@ -14891,7 +15004,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B64" s="26" t="s">
         <v>2</v>
       </c>
@@ -15046,7 +15159,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B65" s="26" t="s">
         <v>2</v>
       </c>
@@ -15201,7 +15314,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B66" s="26" t="s">
         <v>2</v>
       </c>
@@ -15356,7 +15469,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B67" s="26" t="s">
         <v>2</v>
       </c>
@@ -15511,7 +15624,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B68" s="26" t="s">
         <v>2</v>
       </c>
@@ -15666,7 +15779,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B69" s="26" t="s">
         <v>2</v>
       </c>
@@ -15819,7 +15932,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B70" s="26" t="s">
         <v>2</v>
       </c>
@@ -15974,7 +16087,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B71" s="27" t="s">
         <v>2</v>
       </c>
@@ -16129,7 +16242,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B72" s="27" t="s">
         <v>2</v>
       </c>
@@ -16282,7 +16395,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B73" s="27" t="s">
         <v>2</v>
       </c>
@@ -16437,7 +16550,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B74" s="27" t="s">
         <v>2</v>
       </c>
@@ -16588,7 +16701,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B75" s="27" t="s">
         <v>2</v>
       </c>
@@ -16743,7 +16856,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B76" s="27" t="s">
         <v>2</v>
       </c>
@@ -16898,17 +17011,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="214" t="s">
+      <c r="C77" s="212" t="s">
         <v>325</v>
       </c>
       <c r="D77" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E77" s="213" t="s">
+      <c r="E77" s="211" t="s">
         <v>313</v>
       </c>
       <c r="F77" s="29" t="b">
@@ -16956,13 +17069,13 @@
       <c r="T77" s="47" t="s">
         <v>323</v>
       </c>
-      <c r="U77" s="215" t="s">
+      <c r="U77" s="213" t="s">
         <v>127</v>
       </c>
       <c r="V77" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="W77" s="244" t="s">
+      <c r="W77" s="242" t="s">
         <v>326</v>
       </c>
       <c r="X77" s="21" t="b">
@@ -17053,17 +17166,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B78" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="214" t="s">
+      <c r="C78" s="212" t="s">
         <v>327</v>
       </c>
       <c r="D78" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E78" s="213" t="s">
+      <c r="E78" s="211" t="s">
         <v>313</v>
       </c>
       <c r="F78" s="29" t="b">
@@ -17111,13 +17224,13 @@
       <c r="T78" s="47" t="s">
         <v>323</v>
       </c>
-      <c r="U78" s="215" t="s">
+      <c r="U78" s="213" t="s">
         <v>127</v>
       </c>
       <c r="V78" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="W78" s="244" t="s">
+      <c r="W78" s="242" t="s">
         <v>326</v>
       </c>
       <c r="X78" s="21" t="b">
@@ -17208,17 +17321,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B79" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="214" t="s">
+      <c r="C79" s="212" t="s">
         <v>328</v>
       </c>
       <c r="D79" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E79" s="213" t="s">
+      <c r="E79" s="211" t="s">
         <v>313</v>
       </c>
       <c r="F79" s="29" t="b">
@@ -17266,13 +17379,13 @@
       <c r="T79" s="47" t="s">
         <v>323</v>
       </c>
-      <c r="U79" s="215" t="s">
+      <c r="U79" s="213" t="s">
         <v>127</v>
       </c>
       <c r="V79" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="W79" s="244" t="s">
+      <c r="W79" s="242" t="s">
         <v>326</v>
       </c>
       <c r="X79" s="21" t="b">
@@ -17363,17 +17476,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B80" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="214" t="s">
+      <c r="C80" s="212" t="s">
         <v>329</v>
       </c>
       <c r="D80" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E80" s="213" t="s">
+      <c r="E80" s="211" t="s">
         <v>313</v>
       </c>
       <c r="F80" s="29" t="b">
@@ -17421,13 +17534,13 @@
       <c r="T80" s="47" t="s">
         <v>323</v>
       </c>
-      <c r="U80" s="215" t="s">
+      <c r="U80" s="213" t="s">
         <v>127</v>
       </c>
       <c r="V80" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="W80" s="244" t="s">
+      <c r="W80" s="242" t="s">
         <v>326</v>
       </c>
       <c r="X80" s="21" t="b">
@@ -17518,17 +17631,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B81" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="214" t="s">
+      <c r="C81" s="212" t="s">
         <v>330</v>
       </c>
       <c r="D81" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E81" s="213" t="s">
+      <c r="E81" s="211" t="s">
         <v>313</v>
       </c>
       <c r="F81" s="29" t="b">
@@ -17576,13 +17689,13 @@
       <c r="T81" s="47" t="s">
         <v>323</v>
       </c>
-      <c r="U81" s="215" t="s">
+      <c r="U81" s="213" t="s">
         <v>127</v>
       </c>
       <c r="V81" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="W81" s="244" t="s">
+      <c r="W81" s="242" t="s">
         <v>326</v>
       </c>
       <c r="X81" s="21" t="b">
@@ -17673,17 +17786,86 @@
         <v>127</v>
       </c>
     </row>
+    <row r="84" spans="2:52" ht="26" x14ac:dyDescent="0.3">
+      <c r="B84" s="245" t="s">
+        <v>331</v>
+      </c>
+      <c r="C84" s="245"/>
+      <c r="D84" s="245"/>
+      <c r="E84" s="245"/>
+    </row>
+    <row r="86" spans="2:52" ht="133" x14ac:dyDescent="0.2">
+      <c r="B86" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="C86" s="246" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="247" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="F86" s="247" t="s">
+        <v>334</v>
+      </c>
+      <c r="G86" s="248" t="s">
+        <v>335</v>
+      </c>
+      <c r="H86" s="248" t="s">
+        <v>336</v>
+      </c>
+      <c r="I86" s="248" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="87" spans="2:52" x14ac:dyDescent="0.2">
+      <c r="B87" s="211" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="211" t="s">
+        <v>338</v>
+      </c>
+      <c r="D87" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="211">
+        <v>0</v>
+      </c>
+      <c r="F87" s="211">
+        <v>120</v>
+      </c>
+      <c r="G87" s="211">
+        <v>1</v>
+      </c>
+      <c r="H87" s="211" t="s">
+        <v>339</v>
+      </c>
+      <c r="I87" s="211" t="s">
+        <v>340</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
+    <mergeCell ref="B84:E84"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F81">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D87)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",D87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17695,7 +17877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:GA57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17703,80 +17885,80 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="8" width="13.875" customWidth="1"/>
-    <col min="9" max="9" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
     <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.875" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" customWidth="1"/>
-    <col min="22" max="22" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" customWidth="1"/>
+    <col min="22" max="22" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="32" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" customWidth="1"/>
-    <col min="34" max="34" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="19.375" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="19.33203125" customWidth="1"/>
     <col min="37" max="38" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.75" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" customWidth="1"/>
     <col min="40" max="40" width="15" customWidth="1"/>
     <col min="41" max="41" width="19" customWidth="1"/>
-    <col min="42" max="42" width="16.875" customWidth="1"/>
-    <col min="43" max="43" width="16.125" customWidth="1"/>
-    <col min="44" max="44" width="14.625" customWidth="1"/>
-    <col min="45" max="45" width="20.125" customWidth="1"/>
+    <col min="42" max="42" width="16.83203125" customWidth="1"/>
+    <col min="43" max="43" width="16.1640625" customWidth="1"/>
+    <col min="44" max="44" width="14.6640625" customWidth="1"/>
+    <col min="45" max="45" width="20.1640625" customWidth="1"/>
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="211"/>
-      <c r="AB1" s="211"/>
+      <c r="AA1" s="243"/>
+      <c r="AB1" s="243"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="212"/>
-      <c r="AE1" s="212"/>
-      <c r="AF1" s="212"/>
-      <c r="AG1" s="212"/>
-      <c r="AH1" s="212"/>
-      <c r="AI1" s="212"/>
-      <c r="AJ1" s="212"/>
-      <c r="AK1" s="212"/>
-      <c r="AL1" s="212"/>
-      <c r="AM1" s="212"/>
-      <c r="AN1" s="212"/>
-      <c r="AO1" s="212"/>
-      <c r="AP1" s="212"/>
-      <c r="AQ1" s="212"/>
-      <c r="AR1" s="212"/>
-      <c r="AS1" s="212"/>
-      <c r="AT1" s="212"/>
-      <c r="AU1" s="212"/>
-      <c r="AV1" s="212"/>
-      <c r="AW1" s="212"/>
-      <c r="AX1" s="212"/>
-      <c r="AY1" s="212"/>
+      <c r="AD1" s="244"/>
+      <c r="AE1" s="244"/>
+      <c r="AF1" s="244"/>
+      <c r="AG1" s="244"/>
+      <c r="AH1" s="244"/>
+      <c r="AI1" s="244"/>
+      <c r="AJ1" s="244"/>
+      <c r="AK1" s="244"/>
+      <c r="AL1" s="244"/>
+      <c r="AM1" s="244"/>
+      <c r="AN1" s="244"/>
+      <c r="AO1" s="244"/>
+      <c r="AP1" s="244"/>
+      <c r="AQ1" s="244"/>
+      <c r="AR1" s="244"/>
+      <c r="AS1" s="244"/>
+      <c r="AT1" s="244"/>
+      <c r="AU1" s="244"/>
+      <c r="AV1" s="244"/>
+      <c r="AW1" s="244"/>
+      <c r="AX1" s="244"/>
+      <c r="AY1" s="244"/>
     </row>
-    <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:51" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>314</v>
       </c>
@@ -17795,19 +17977,19 @@
       <c r="G2" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="H2" s="241" t="s">
+      <c r="H2" s="239" t="s">
         <v>320</v>
       </c>
-      <c r="I2" s="242" t="s">
+      <c r="I2" s="240" t="s">
         <v>321</v>
       </c>
-      <c r="J2" s="243"/>
+      <c r="J2" s="241"/>
     </row>
-    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="214" t="s">
+      <c r="C3" s="212" t="s">
         <v>315</v>
       </c>
       <c r="D3" s="24">
@@ -17822,197 +18004,197 @@
       <c r="G3" s="26">
         <v>2</v>
       </c>
-      <c r="H3" s="239">
+      <c r="H3" s="237">
         <v>360</v>
       </c>
-      <c r="I3" s="240" t="s">
+      <c r="I3" s="238" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="238"/>
-      <c r="B57" s="238"/>
-      <c r="C57" s="238"/>
-      <c r="D57" s="238"/>
-      <c r="E57" s="238"/>
-      <c r="F57" s="238"/>
-      <c r="G57" s="238"/>
-      <c r="H57" s="238"/>
-      <c r="I57" s="238"/>
-      <c r="J57" s="238"/>
-      <c r="K57" s="238"/>
-      <c r="L57" s="238"/>
-      <c r="M57" s="238"/>
-      <c r="N57" s="238"/>
-      <c r="O57" s="238"/>
-      <c r="P57" s="238"/>
-      <c r="Q57" s="238"/>
-      <c r="R57" s="238"/>
-      <c r="S57" s="238"/>
-      <c r="T57" s="238"/>
-      <c r="U57" s="238"/>
-      <c r="V57" s="238"/>
-      <c r="W57" s="238"/>
-      <c r="X57" s="238"/>
-      <c r="Y57" s="238"/>
-      <c r="Z57" s="238"/>
-      <c r="AA57" s="238"/>
-      <c r="AB57" s="238"/>
-      <c r="AC57" s="238"/>
-      <c r="AD57" s="238"/>
-      <c r="AE57" s="238"/>
-      <c r="AF57" s="238"/>
-      <c r="AG57" s="238"/>
-      <c r="AH57" s="238"/>
-      <c r="AI57" s="238"/>
-      <c r="AJ57" s="238"/>
-      <c r="AK57" s="238"/>
-      <c r="AL57" s="238"/>
-      <c r="AM57" s="238"/>
-      <c r="AN57" s="238"/>
-      <c r="AO57" s="238"/>
-      <c r="AP57" s="238"/>
-      <c r="AQ57" s="238"/>
-      <c r="AR57" s="238"/>
-      <c r="AS57" s="238"/>
-      <c r="AT57" s="238"/>
-      <c r="AU57" s="238"/>
-      <c r="AV57" s="238"/>
-      <c r="AW57" s="238"/>
-      <c r="AX57" s="238"/>
-      <c r="AY57" s="238"/>
-      <c r="AZ57" s="238"/>
-      <c r="BA57" s="238"/>
-      <c r="BB57" s="238"/>
-      <c r="BC57" s="238"/>
-      <c r="BD57" s="238"/>
-      <c r="BE57" s="238"/>
-      <c r="BF57" s="238"/>
-      <c r="BG57" s="238"/>
-      <c r="BH57" s="238"/>
-      <c r="BI57" s="238"/>
-      <c r="BJ57" s="238"/>
-      <c r="BK57" s="238"/>
-      <c r="BL57" s="238"/>
-      <c r="BM57" s="238"/>
-      <c r="BN57" s="238"/>
-      <c r="BO57" s="238"/>
-      <c r="BP57" s="238"/>
-      <c r="BQ57" s="238"/>
-      <c r="BR57" s="238"/>
-      <c r="BS57" s="238"/>
-      <c r="BT57" s="238"/>
-      <c r="BU57" s="238"/>
-      <c r="BV57" s="238"/>
-      <c r="BW57" s="238"/>
-      <c r="BX57" s="238"/>
-      <c r="BY57" s="238"/>
-      <c r="BZ57" s="238"/>
-      <c r="CA57" s="238"/>
-      <c r="CB57" s="238"/>
-      <c r="CC57" s="238"/>
-      <c r="CD57" s="238"/>
-      <c r="CE57" s="238"/>
-      <c r="CF57" s="238"/>
-      <c r="CG57" s="238"/>
-      <c r="CH57" s="238"/>
-      <c r="CI57" s="238"/>
-      <c r="CJ57" s="238"/>
-      <c r="CK57" s="238"/>
-      <c r="CL57" s="238"/>
-      <c r="CM57" s="238"/>
-      <c r="CN57" s="238"/>
-      <c r="CO57" s="238"/>
-      <c r="CP57" s="238"/>
-      <c r="CQ57" s="238"/>
-      <c r="CR57" s="238"/>
-      <c r="CS57" s="238"/>
-      <c r="CT57" s="238"/>
-      <c r="CU57" s="238"/>
-      <c r="CV57" s="238"/>
-      <c r="CW57" s="238"/>
-      <c r="CX57" s="238"/>
-      <c r="CY57" s="238"/>
-      <c r="CZ57" s="238"/>
-      <c r="DA57" s="238"/>
-      <c r="DB57" s="238"/>
-      <c r="DC57" s="238"/>
-      <c r="DD57" s="238"/>
-      <c r="DE57" s="238"/>
-      <c r="DF57" s="238"/>
-      <c r="DG57" s="238"/>
-      <c r="DH57" s="238"/>
-      <c r="DI57" s="238"/>
-      <c r="DJ57" s="238"/>
-      <c r="DK57" s="238"/>
-      <c r="DL57" s="238"/>
-      <c r="DM57" s="238"/>
-      <c r="DN57" s="238"/>
-      <c r="DO57" s="238"/>
-      <c r="DP57" s="238"/>
-      <c r="DQ57" s="238"/>
-      <c r="DR57" s="238"/>
-      <c r="DS57" s="238"/>
-      <c r="DT57" s="238"/>
-      <c r="DU57" s="238"/>
-      <c r="DV57" s="238"/>
-      <c r="DW57" s="238"/>
-      <c r="DX57" s="238"/>
-      <c r="DY57" s="238"/>
-      <c r="DZ57" s="238"/>
-      <c r="EA57" s="238"/>
-      <c r="EB57" s="238"/>
-      <c r="EC57" s="238"/>
-      <c r="ED57" s="238"/>
-      <c r="EE57" s="238"/>
-      <c r="EF57" s="238"/>
-      <c r="EG57" s="238"/>
-      <c r="EH57" s="238"/>
-      <c r="EI57" s="238"/>
-      <c r="EJ57" s="238"/>
-      <c r="EK57" s="238"/>
-      <c r="EL57" s="238"/>
-      <c r="EM57" s="238"/>
-      <c r="EN57" s="238"/>
-      <c r="EO57" s="238"/>
-      <c r="EP57" s="238"/>
-      <c r="EQ57" s="238"/>
-      <c r="ER57" s="238"/>
-      <c r="ES57" s="238"/>
-      <c r="ET57" s="238"/>
-      <c r="EU57" s="238"/>
-      <c r="EV57" s="238"/>
-      <c r="EW57" s="238"/>
-      <c r="EX57" s="238"/>
-      <c r="EY57" s="238"/>
-      <c r="EZ57" s="238"/>
-      <c r="FA57" s="238"/>
-      <c r="FB57" s="238"/>
-      <c r="FC57" s="238"/>
-      <c r="FD57" s="238"/>
-      <c r="FE57" s="238"/>
-      <c r="FF57" s="238"/>
-      <c r="FG57" s="238"/>
-      <c r="FH57" s="238"/>
-      <c r="FI57" s="238"/>
-      <c r="FJ57" s="238"/>
-      <c r="FK57" s="238"/>
-      <c r="FL57" s="238"/>
-      <c r="FM57" s="238"/>
-      <c r="FN57" s="238"/>
-      <c r="FO57" s="238"/>
-      <c r="FP57" s="238"/>
-      <c r="FQ57" s="238"/>
-      <c r="FR57" s="238"/>
-      <c r="FS57" s="238"/>
-      <c r="FT57" s="238"/>
-      <c r="FU57" s="238"/>
-      <c r="FV57" s="238"/>
-      <c r="FW57" s="238"/>
-      <c r="FX57" s="238"/>
-      <c r="FY57" s="238"/>
-      <c r="FZ57" s="238"/>
-      <c r="GA57" s="238"/>
+    <row r="57" spans="1:183" s="205" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="236"/>
+      <c r="B57" s="236"/>
+      <c r="C57" s="236"/>
+      <c r="D57" s="236"/>
+      <c r="E57" s="236"/>
+      <c r="F57" s="236"/>
+      <c r="G57" s="236"/>
+      <c r="H57" s="236"/>
+      <c r="I57" s="236"/>
+      <c r="J57" s="236"/>
+      <c r="K57" s="236"/>
+      <c r="L57" s="236"/>
+      <c r="M57" s="236"/>
+      <c r="N57" s="236"/>
+      <c r="O57" s="236"/>
+      <c r="P57" s="236"/>
+      <c r="Q57" s="236"/>
+      <c r="R57" s="236"/>
+      <c r="S57" s="236"/>
+      <c r="T57" s="236"/>
+      <c r="U57" s="236"/>
+      <c r="V57" s="236"/>
+      <c r="W57" s="236"/>
+      <c r="X57" s="236"/>
+      <c r="Y57" s="236"/>
+      <c r="Z57" s="236"/>
+      <c r="AA57" s="236"/>
+      <c r="AB57" s="236"/>
+      <c r="AC57" s="236"/>
+      <c r="AD57" s="236"/>
+      <c r="AE57" s="236"/>
+      <c r="AF57" s="236"/>
+      <c r="AG57" s="236"/>
+      <c r="AH57" s="236"/>
+      <c r="AI57" s="236"/>
+      <c r="AJ57" s="236"/>
+      <c r="AK57" s="236"/>
+      <c r="AL57" s="236"/>
+      <c r="AM57" s="236"/>
+      <c r="AN57" s="236"/>
+      <c r="AO57" s="236"/>
+      <c r="AP57" s="236"/>
+      <c r="AQ57" s="236"/>
+      <c r="AR57" s="236"/>
+      <c r="AS57" s="236"/>
+      <c r="AT57" s="236"/>
+      <c r="AU57" s="236"/>
+      <c r="AV57" s="236"/>
+      <c r="AW57" s="236"/>
+      <c r="AX57" s="236"/>
+      <c r="AY57" s="236"/>
+      <c r="AZ57" s="236"/>
+      <c r="BA57" s="236"/>
+      <c r="BB57" s="236"/>
+      <c r="BC57" s="236"/>
+      <c r="BD57" s="236"/>
+      <c r="BE57" s="236"/>
+      <c r="BF57" s="236"/>
+      <c r="BG57" s="236"/>
+      <c r="BH57" s="236"/>
+      <c r="BI57" s="236"/>
+      <c r="BJ57" s="236"/>
+      <c r="BK57" s="236"/>
+      <c r="BL57" s="236"/>
+      <c r="BM57" s="236"/>
+      <c r="BN57" s="236"/>
+      <c r="BO57" s="236"/>
+      <c r="BP57" s="236"/>
+      <c r="BQ57" s="236"/>
+      <c r="BR57" s="236"/>
+      <c r="BS57" s="236"/>
+      <c r="BT57" s="236"/>
+      <c r="BU57" s="236"/>
+      <c r="BV57" s="236"/>
+      <c r="BW57" s="236"/>
+      <c r="BX57" s="236"/>
+      <c r="BY57" s="236"/>
+      <c r="BZ57" s="236"/>
+      <c r="CA57" s="236"/>
+      <c r="CB57" s="236"/>
+      <c r="CC57" s="236"/>
+      <c r="CD57" s="236"/>
+      <c r="CE57" s="236"/>
+      <c r="CF57" s="236"/>
+      <c r="CG57" s="236"/>
+      <c r="CH57" s="236"/>
+      <c r="CI57" s="236"/>
+      <c r="CJ57" s="236"/>
+      <c r="CK57" s="236"/>
+      <c r="CL57" s="236"/>
+      <c r="CM57" s="236"/>
+      <c r="CN57" s="236"/>
+      <c r="CO57" s="236"/>
+      <c r="CP57" s="236"/>
+      <c r="CQ57" s="236"/>
+      <c r="CR57" s="236"/>
+      <c r="CS57" s="236"/>
+      <c r="CT57" s="236"/>
+      <c r="CU57" s="236"/>
+      <c r="CV57" s="236"/>
+      <c r="CW57" s="236"/>
+      <c r="CX57" s="236"/>
+      <c r="CY57" s="236"/>
+      <c r="CZ57" s="236"/>
+      <c r="DA57" s="236"/>
+      <c r="DB57" s="236"/>
+      <c r="DC57" s="236"/>
+      <c r="DD57" s="236"/>
+      <c r="DE57" s="236"/>
+      <c r="DF57" s="236"/>
+      <c r="DG57" s="236"/>
+      <c r="DH57" s="236"/>
+      <c r="DI57" s="236"/>
+      <c r="DJ57" s="236"/>
+      <c r="DK57" s="236"/>
+      <c r="DL57" s="236"/>
+      <c r="DM57" s="236"/>
+      <c r="DN57" s="236"/>
+      <c r="DO57" s="236"/>
+      <c r="DP57" s="236"/>
+      <c r="DQ57" s="236"/>
+      <c r="DR57" s="236"/>
+      <c r="DS57" s="236"/>
+      <c r="DT57" s="236"/>
+      <c r="DU57" s="236"/>
+      <c r="DV57" s="236"/>
+      <c r="DW57" s="236"/>
+      <c r="DX57" s="236"/>
+      <c r="DY57" s="236"/>
+      <c r="DZ57" s="236"/>
+      <c r="EA57" s="236"/>
+      <c r="EB57" s="236"/>
+      <c r="EC57" s="236"/>
+      <c r="ED57" s="236"/>
+      <c r="EE57" s="236"/>
+      <c r="EF57" s="236"/>
+      <c r="EG57" s="236"/>
+      <c r="EH57" s="236"/>
+      <c r="EI57" s="236"/>
+      <c r="EJ57" s="236"/>
+      <c r="EK57" s="236"/>
+      <c r="EL57" s="236"/>
+      <c r="EM57" s="236"/>
+      <c r="EN57" s="236"/>
+      <c r="EO57" s="236"/>
+      <c r="EP57" s="236"/>
+      <c r="EQ57" s="236"/>
+      <c r="ER57" s="236"/>
+      <c r="ES57" s="236"/>
+      <c r="ET57" s="236"/>
+      <c r="EU57" s="236"/>
+      <c r="EV57" s="236"/>
+      <c r="EW57" s="236"/>
+      <c r="EX57" s="236"/>
+      <c r="EY57" s="236"/>
+      <c r="EZ57" s="236"/>
+      <c r="FA57" s="236"/>
+      <c r="FB57" s="236"/>
+      <c r="FC57" s="236"/>
+      <c r="FD57" s="236"/>
+      <c r="FE57" s="236"/>
+      <c r="FF57" s="236"/>
+      <c r="FG57" s="236"/>
+      <c r="FH57" s="236"/>
+      <c r="FI57" s="236"/>
+      <c r="FJ57" s="236"/>
+      <c r="FK57" s="236"/>
+      <c r="FL57" s="236"/>
+      <c r="FM57" s="236"/>
+      <c r="FN57" s="236"/>
+      <c r="FO57" s="236"/>
+      <c r="FP57" s="236"/>
+      <c r="FQ57" s="236"/>
+      <c r="FR57" s="236"/>
+      <c r="FS57" s="236"/>
+      <c r="FT57" s="236"/>
+      <c r="FU57" s="236"/>
+      <c r="FV57" s="236"/>
+      <c r="FW57" s="236"/>
+      <c r="FX57" s="236"/>
+      <c r="FY57" s="236"/>
+      <c r="FZ57" s="236"/>
+      <c r="GA57" s="236"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -18028,19 +18210,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
@@ -18049,10 +18231,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -18060,7 +18242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -18068,7 +18250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -18076,13 +18258,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -18090,7 +18272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -18098,7 +18280,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>127</v>
       </c>
@@ -18106,107 +18288,107 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
All offers set with real money!
Former-commit-id: 2be0c8b35da16e433e4745b2ed1e4fbfaddbb56f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B31C280-7988-B647-BCDA-4F07F18FFFAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="1340" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -1056,7 +1055,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2357,6 +2356,15 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2365,41 +2373,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5119,6 +5098,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5147,80 +5146,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B2:AZ76" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
+  <autoFilter ref="B2:AZ76"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{offerPacksDefinitions}" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="62"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[uniqueId]" dataDxfId="61"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[type]" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="59"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[purchaseLimit]" dataDxfId="58"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[item1Featured]" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[item1Type]" dataDxfId="56"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[item1Amount]" dataDxfId="55"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[item1Sku]" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[item2Type]" dataDxfId="53"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[item2Amount]" dataDxfId="52"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[item2Sku]" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[item3Type]" dataDxfId="50"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[item3Amount]" dataDxfId="49"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[item3Sku]" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[refPrice]" dataDxfId="46"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[currency]" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[discount]" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[iapSku]" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[tidName]" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[featured]" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[maxViews]" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[zone]" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[frequency]" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[startDate]" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[endDate]" dataDxfId="36"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[durationMinutes]" dataDxfId="35"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[minAppVersion]" dataDxfId="34"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[countriesAllowed]" dataDxfId="33"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[countriesExcluded]" dataDxfId="32"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[gamesPlayed]" dataDxfId="31"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[payerType]" dataDxfId="30"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[minSpent]" dataDxfId="29"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[maxSpent]" dataDxfId="28"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[minNumberOfPurchases]" dataDxfId="27"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[minutesSinceLastPurchase]" dataDxfId="26"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[dragonUnlocked]" dataDxfId="25"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[dragonOwned]" dataDxfId="24"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[dragonNotOwned]" dataDxfId="23"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[scBalanceRange]" dataDxfId="22"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[hcBalanceRange]" dataDxfId="21"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[openedEggs]" dataDxfId="20"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[petsOwnedCount]" dataDxfId="19"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[petsOwned]" dataDxfId="18"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[petsNotOwned]" dataDxfId="17"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[progressionRange]" dataDxfId="16"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[skinsUnlocked]" dataDxfId="15"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[skinsOwned]" dataDxfId="14"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[skinsNotOwned]" dataDxfId="13"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="61"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="59"/>
+    <tableColumn id="49" name="[type]" dataDxfId="58"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="57"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="56"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="55"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="54"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="53"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="52"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="51"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="50"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="49"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="48"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="47"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="46"/>
+    <tableColumn id="7" name="[order]" dataDxfId="45"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="44"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="43"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="42"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="41"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="40"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="39"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="38"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="37"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="36"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="35"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="34"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="33"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="32"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="31"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="30"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="29"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="28"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="27"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="26"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="25"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="24"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="23"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="22"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="21"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="20"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="19"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="18"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="17"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="16"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="15"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="14"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="13"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="12"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B2:I3"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{offerSettings}" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="8"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="[refreshFrequency]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[rotationalActiveOffers]" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[rotationalHistorySize]" dataDxfId="5"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="[freeHistorySize]" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[freeCooldownMinutes]" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[emptyValue]" dataDxfId="2"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="7"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="5"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="4"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="3"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="2"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5522,56 +5521,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
     <col min="6" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
     <col min="9" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.83203125" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" customWidth="1"/>
-    <col min="22" max="22" width="42.6640625" customWidth="1"/>
-    <col min="23" max="23" width="42.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.875" customWidth="1"/>
+    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.625" customWidth="1"/>
+    <col min="22" max="22" width="42.625" customWidth="1"/>
+    <col min="23" max="23" width="42.125" customWidth="1"/>
     <col min="24" max="24" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.1640625" customWidth="1"/>
-    <col min="27" max="27" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.125" customWidth="1"/>
+    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
     <col min="28" max="32" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.1640625" customWidth="1"/>
-    <col min="34" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="19.33203125" customWidth="1"/>
+    <col min="33" max="33" width="20.125" customWidth="1"/>
+    <col min="34" max="34" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="19.375" customWidth="1"/>
     <col min="37" max="38" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.6640625" customWidth="1"/>
+    <col min="39" max="39" width="15.625" customWidth="1"/>
     <col min="40" max="40" width="15" customWidth="1"/>
     <col min="41" max="41" width="19" customWidth="1"/>
-    <col min="42" max="42" width="16.83203125" customWidth="1"/>
-    <col min="43" max="43" width="16.1640625" customWidth="1"/>
-    <col min="44" max="44" width="14.6640625" customWidth="1"/>
-    <col min="45" max="45" width="20.1640625" customWidth="1"/>
+    <col min="42" max="42" width="16.875" customWidth="1"/>
+    <col min="43" max="43" width="16.125" customWidth="1"/>
+    <col min="44" max="44" width="14.625" customWidth="1"/>
+    <col min="45" max="45" width="20.125" customWidth="1"/>
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:52" s="10" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
       <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
@@ -5587,37 +5586,37 @@
       <c r="V1" s="210" t="s">
         <v>311</v>
       </c>
-      <c r="AA1" s="243" t="s">
+      <c r="AA1" s="246" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="243"/>
+      <c r="AB1" s="246"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="244" t="s">
+      <c r="AD1" s="247" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="244"/>
-      <c r="AF1" s="244"/>
-      <c r="AG1" s="244"/>
-      <c r="AH1" s="244"/>
-      <c r="AI1" s="244"/>
-      <c r="AJ1" s="244"/>
-      <c r="AK1" s="244"/>
-      <c r="AL1" s="244"/>
-      <c r="AM1" s="244"/>
-      <c r="AN1" s="244"/>
-      <c r="AO1" s="244"/>
-      <c r="AP1" s="244"/>
-      <c r="AQ1" s="244"/>
-      <c r="AR1" s="244"/>
-      <c r="AS1" s="244"/>
-      <c r="AT1" s="244"/>
-      <c r="AU1" s="244"/>
-      <c r="AV1" s="244"/>
-      <c r="AW1" s="244"/>
-      <c r="AX1" s="244"/>
-      <c r="AY1" s="244"/>
+      <c r="AE1" s="247"/>
+      <c r="AF1" s="247"/>
+      <c r="AG1" s="247"/>
+      <c r="AH1" s="247"/>
+      <c r="AI1" s="247"/>
+      <c r="AJ1" s="247"/>
+      <c r="AK1" s="247"/>
+      <c r="AL1" s="247"/>
+      <c r="AM1" s="247"/>
+      <c r="AN1" s="247"/>
+      <c r="AO1" s="247"/>
+      <c r="AP1" s="247"/>
+      <c r="AQ1" s="247"/>
+      <c r="AR1" s="247"/>
+      <c r="AS1" s="247"/>
+      <c r="AT1" s="247"/>
+      <c r="AU1" s="247"/>
+      <c r="AV1" s="247"/>
+      <c r="AW1" s="247"/>
+      <c r="AX1" s="247"/>
+      <c r="AY1" s="247"/>
     </row>
-    <row r="2" spans="2:52" ht="149" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:52" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5772,7 +5771,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -5927,7 +5926,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
@@ -6082,7 +6081,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -6237,7 +6236,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
@@ -6392,7 +6391,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -6702,7 +6701,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
@@ -6857,7 +6856,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
@@ -7012,7 +7011,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B11" s="99" t="s">
         <v>2</v>
       </c>
@@ -7167,7 +7166,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
@@ -7322,7 +7321,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -7477,7 +7476,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>2</v>
       </c>
@@ -7633,7 +7632,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
         <v>2</v>
       </c>
@@ -7788,7 +7787,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B16" s="27" t="s">
         <v>2</v>
       </c>
@@ -7943,7 +7942,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="118" t="s">
         <v>2</v>
       </c>
@@ -8098,7 +8097,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41" t="s">
         <v>2</v>
       </c>
@@ -8253,7 +8252,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -8408,7 +8407,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
@@ -8563,7 +8562,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
         <v>2</v>
       </c>
@@ -8718,7 +8717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>2</v>
       </c>
@@ -8871,7 +8870,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>2</v>
       </c>
@@ -9024,7 +9023,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>2</v>
       </c>
@@ -9175,7 +9174,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -9330,7 +9329,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>2</v>
       </c>
@@ -9481,7 +9480,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>2</v>
       </c>
@@ -9636,7 +9635,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -9773,7 +9772,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>2</v>
       </c>
@@ -9920,7 +9919,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
         <v>2</v>
       </c>
@@ -10067,7 +10066,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
         <v>2</v>
       </c>
@@ -10210,7 +10209,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
@@ -10359,7 +10358,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B33" s="26" t="s">
         <v>2</v>
       </c>
@@ -10502,7 +10501,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B34" s="67" t="s">
         <v>2</v>
       </c>
@@ -10645,7 +10644,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B35" s="81" t="s">
         <v>2</v>
       </c>
@@ -10788,7 +10787,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
@@ -10941,7 +10940,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
@@ -11094,7 +11093,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B38" s="26" t="s">
         <v>2</v>
       </c>
@@ -11241,7 +11240,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
         <v>2</v>
       </c>
@@ -11384,7 +11383,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="67" t="s">
         <v>2</v>
       </c>
@@ -11531,7 +11530,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B41" s="138" t="s">
         <v>2</v>
       </c>
@@ -11674,7 +11673,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
         <v>2</v>
       </c>
@@ -11823,7 +11822,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
@@ -11972,7 +11971,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
@@ -12123,7 +12122,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
         <v>2</v>
       </c>
@@ -12270,7 +12269,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B46" s="55" t="s">
         <v>2</v>
       </c>
@@ -12417,7 +12416,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B47" s="214" t="s">
         <v>2</v>
       </c>
@@ -12572,7 +12571,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
@@ -12715,7 +12714,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B49" s="26" t="s">
         <v>2</v>
       </c>
@@ -12864,7 +12863,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
@@ -13007,7 +13006,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B51" s="26" t="s">
         <v>2</v>
       </c>
@@ -13154,7 +13153,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="67" t="s">
         <v>2</v>
       </c>
@@ -13301,7 +13300,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:52" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B53" s="215" t="s">
         <v>2</v>
       </c>
@@ -13456,7 +13455,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B54" s="27" t="s">
         <v>2</v>
       </c>
@@ -13611,7 +13610,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
@@ -13766,7 +13765,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B56" s="27" t="s">
         <v>2</v>
       </c>
@@ -13921,7 +13920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="2:52" s="205" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="192" t="s">
         <v>2</v>
       </c>
@@ -14076,7 +14075,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B58" s="179" t="s">
         <v>2</v>
       </c>
@@ -14231,7 +14230,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B59" s="41" t="s">
         <v>2</v>
       </c>
@@ -14386,7 +14385,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="2:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="67" t="s">
         <v>2</v>
       </c>
@@ -14539,7 +14538,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B61" s="158" t="s">
         <v>2</v>
       </c>
@@ -14694,7 +14693,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
         <v>2</v>
       </c>
@@ -14849,7 +14848,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
         <v>2</v>
       </c>
@@ -15004,7 +15003,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B64" s="26" t="s">
         <v>2</v>
       </c>
@@ -15159,7 +15158,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
         <v>2</v>
       </c>
@@ -15314,7 +15313,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B66" s="26" t="s">
         <v>2</v>
       </c>
@@ -15469,7 +15468,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
         <v>2</v>
       </c>
@@ -15624,7 +15623,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B68" s="26" t="s">
         <v>2</v>
       </c>
@@ -15779,7 +15778,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B69" s="26" t="s">
         <v>2</v>
       </c>
@@ -15932,7 +15931,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B70" s="26" t="s">
         <v>2</v>
       </c>
@@ -16087,7 +16086,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B71" s="27" t="s">
         <v>2</v>
       </c>
@@ -16143,7 +16142,7 @@
         <v>101</v>
       </c>
       <c r="T71" s="47" t="s">
-        <v>12</v>
+        <v>312</v>
       </c>
       <c r="U71" s="206" t="s">
         <v>306</v>
@@ -16242,7 +16241,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B72" s="27" t="s">
         <v>2</v>
       </c>
@@ -16395,7 +16394,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B73" s="27" t="s">
         <v>2</v>
       </c>
@@ -16451,7 +16450,7 @@
         <v>75</v>
       </c>
       <c r="T73" s="47" t="s">
-        <v>10</v>
+        <v>312</v>
       </c>
       <c r="U73" s="206" t="s">
         <v>301</v>
@@ -16550,7 +16549,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B74" s="27" t="s">
         <v>2</v>
       </c>
@@ -16606,7 +16605,7 @@
         <v>101</v>
       </c>
       <c r="T74" s="47" t="s">
-        <v>10</v>
+        <v>312</v>
       </c>
       <c r="U74" s="206" t="s">
         <v>301</v>
@@ -16701,7 +16700,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
         <v>2</v>
       </c>
@@ -16757,7 +16756,7 @@
         <v>101</v>
       </c>
       <c r="T75" s="47" t="s">
-        <v>12</v>
+        <v>312</v>
       </c>
       <c r="U75" s="206" t="s">
         <v>301</v>
@@ -16856,7 +16855,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
         <v>2</v>
       </c>
@@ -17011,7 +17010,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B77" s="27" t="s">
         <v>2</v>
       </c>
@@ -17166,7 +17165,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B78" s="27" t="s">
         <v>2</v>
       </c>
@@ -17321,7 +17320,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B79" s="27" t="s">
         <v>2</v>
       </c>
@@ -17476,7 +17475,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B80" s="27" t="s">
         <v>2</v>
       </c>
@@ -17631,7 +17630,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B81" s="27" t="s">
         <v>2</v>
       </c>
@@ -17786,41 +17785,41 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="2:52" ht="26" x14ac:dyDescent="0.3">
-      <c r="B84" s="245" t="s">
+    <row r="84" spans="2:52" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B84" s="248" t="s">
         <v>331</v>
       </c>
-      <c r="C84" s="245"/>
-      <c r="D84" s="245"/>
-      <c r="E84" s="245"/>
+      <c r="C84" s="248"/>
+      <c r="D84" s="248"/>
+      <c r="E84" s="248"/>
     </row>
-    <row r="86" spans="2:52" ht="133" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:52" ht="135" x14ac:dyDescent="0.25">
       <c r="B86" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="C86" s="246" t="s">
+      <c r="C86" s="243" t="s">
         <v>0</v>
       </c>
-      <c r="D86" s="247" t="s">
+      <c r="D86" s="244" t="s">
         <v>52</v>
       </c>
       <c r="E86" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="F86" s="247" t="s">
+      <c r="F86" s="244" t="s">
         <v>334</v>
       </c>
-      <c r="G86" s="248" t="s">
+      <c r="G86" s="245" t="s">
         <v>335</v>
       </c>
-      <c r="H86" s="248" t="s">
+      <c r="H86" s="245" t="s">
         <v>336</v>
       </c>
-      <c r="I86" s="248" t="s">
+      <c r="I86" s="245" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="87" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B87" s="211" t="s">
         <v>2</v>
       </c>
@@ -17861,10 +17860,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D87)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17877,7 +17876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GA57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17885,80 +17884,80 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="8" width="13.875" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
     <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.83203125" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" customWidth="1"/>
-    <col min="22" max="22" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.875" customWidth="1"/>
+    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.625" customWidth="1"/>
+    <col min="22" max="22" width="32.875" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
     <col min="28" max="32" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.1640625" customWidth="1"/>
-    <col min="34" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="19.33203125" customWidth="1"/>
+    <col min="33" max="33" width="20.125" customWidth="1"/>
+    <col min="34" max="34" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="19.375" customWidth="1"/>
     <col min="37" max="38" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.6640625" customWidth="1"/>
+    <col min="39" max="39" width="15.625" customWidth="1"/>
     <col min="40" max="40" width="15" customWidth="1"/>
     <col min="41" max="41" width="19" customWidth="1"/>
-    <col min="42" max="42" width="16.83203125" customWidth="1"/>
-    <col min="43" max="43" width="16.1640625" customWidth="1"/>
-    <col min="44" max="44" width="14.6640625" customWidth="1"/>
-    <col min="45" max="45" width="20.1640625" customWidth="1"/>
+    <col min="42" max="42" width="16.875" customWidth="1"/>
+    <col min="43" max="43" width="16.125" customWidth="1"/>
+    <col min="44" max="44" width="14.625" customWidth="1"/>
+    <col min="45" max="45" width="20.125" customWidth="1"/>
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="243"/>
-      <c r="AB1" s="243"/>
+      <c r="AA1" s="246"/>
+      <c r="AB1" s="246"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="244"/>
-      <c r="AE1" s="244"/>
-      <c r="AF1" s="244"/>
-      <c r="AG1" s="244"/>
-      <c r="AH1" s="244"/>
-      <c r="AI1" s="244"/>
-      <c r="AJ1" s="244"/>
-      <c r="AK1" s="244"/>
-      <c r="AL1" s="244"/>
-      <c r="AM1" s="244"/>
-      <c r="AN1" s="244"/>
-      <c r="AO1" s="244"/>
-      <c r="AP1" s="244"/>
-      <c r="AQ1" s="244"/>
-      <c r="AR1" s="244"/>
-      <c r="AS1" s="244"/>
-      <c r="AT1" s="244"/>
-      <c r="AU1" s="244"/>
-      <c r="AV1" s="244"/>
-      <c r="AW1" s="244"/>
-      <c r="AX1" s="244"/>
-      <c r="AY1" s="244"/>
+      <c r="AD1" s="247"/>
+      <c r="AE1" s="247"/>
+      <c r="AF1" s="247"/>
+      <c r="AG1" s="247"/>
+      <c r="AH1" s="247"/>
+      <c r="AI1" s="247"/>
+      <c r="AJ1" s="247"/>
+      <c r="AK1" s="247"/>
+      <c r="AL1" s="247"/>
+      <c r="AM1" s="247"/>
+      <c r="AN1" s="247"/>
+      <c r="AO1" s="247"/>
+      <c r="AP1" s="247"/>
+      <c r="AQ1" s="247"/>
+      <c r="AR1" s="247"/>
+      <c r="AS1" s="247"/>
+      <c r="AT1" s="247"/>
+      <c r="AU1" s="247"/>
+      <c r="AV1" s="247"/>
+      <c r="AW1" s="247"/>
+      <c r="AX1" s="247"/>
+      <c r="AY1" s="247"/>
     </row>
-    <row r="2" spans="2:51" ht="149" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>314</v>
       </c>
@@ -17985,7 +17984,7 @@
       </c>
       <c r="J2" s="241"/>
     </row>
-    <row r="3" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -18011,7 +18010,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:183" s="205" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="236"/>
       <c r="B57" s="236"/>
       <c r="C57" s="236"/>
@@ -18210,19 +18209,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
@@ -18231,10 +18230,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -18242,7 +18241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -18250,7 +18249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -18258,13 +18257,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -18272,7 +18271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -18280,7 +18279,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>127</v>
       </c>
@@ -18288,107 +18287,107 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Updated rotational offers number active
Former-commit-id: 36f18ac470b9d116f0ec27ca8c4ce5eb4a6f6134
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535"/>
+    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
     <sheet name="Settings" sheetId="4" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5524,7 +5524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
@@ -17879,9 +17879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17995,7 +17995,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="24">
         <v>2</v>

</xml_diff>

<commit_message>
Updated the range progression for rotational offers!
Former-commit-id: 7366aba6121dd29573468c1fdc6a7d1bfc231934
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535" activeTab="1"/>
+    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -953,9 +953,6 @@
     <t>0.65</t>
   </si>
   <si>
-    <t>8:999</t>
-  </si>
-  <si>
     <t>dragon_electric;dragon_chinese</t>
   </si>
   <si>
@@ -1050,6 +1047,9 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>2:999</t>
   </si>
 </sst>
 </file>
@@ -5524,8 +5524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
@@ -5581,10 +5581,10 @@
         <v>18</v>
       </c>
       <c r="U1" s="210" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="V1" s="210" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AA1" s="246" t="s">
         <v>77</v>
@@ -5672,7 +5672,7 @@
         <v>20</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>4</v>
@@ -5827,7 +5827,7 @@
         <v>102</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U3" s="35">
         <v>-1</v>
@@ -5982,7 +5982,7 @@
         <v>102</v>
       </c>
       <c r="T4" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U4" s="35">
         <v>0.5</v>
@@ -6137,7 +6137,7 @@
         <v>226</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U5" s="35">
         <v>0.5</v>
@@ -6292,7 +6292,7 @@
         <v>101</v>
       </c>
       <c r="T6" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U6" s="35">
         <v>0.5</v>
@@ -6447,7 +6447,7 @@
         <v>103</v>
       </c>
       <c r="T7" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U7" s="35">
         <v>0.5</v>
@@ -6602,7 +6602,7 @@
         <v>271</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U8" s="35">
         <v>0.5</v>
@@ -6757,7 +6757,7 @@
         <v>227</v>
       </c>
       <c r="T9" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U9" s="35">
         <v>0.5</v>
@@ -6912,7 +6912,7 @@
         <v>104</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U10" s="110">
         <v>0.5</v>
@@ -7067,7 +7067,7 @@
         <v>75</v>
       </c>
       <c r="T11" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U11" s="48">
         <v>0.5</v>
@@ -7222,7 +7222,7 @@
         <v>105</v>
       </c>
       <c r="T12" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U12" s="35">
         <v>0.5</v>
@@ -7377,7 +7377,7 @@
         <v>102</v>
       </c>
       <c r="T13" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U13" s="35">
         <v>0.5</v>
@@ -7532,7 +7532,7 @@
         <v>226</v>
       </c>
       <c r="T14" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U14" s="35">
         <v>0.5</v>
@@ -7688,7 +7688,7 @@
         <v>101</v>
       </c>
       <c r="T15" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U15" s="35">
         <v>0.5</v>
@@ -7843,7 +7843,7 @@
         <v>103</v>
       </c>
       <c r="T16" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U16" s="35">
         <v>0.5</v>
@@ -7998,7 +7998,7 @@
         <v>271</v>
       </c>
       <c r="T17" s="124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U17" s="125">
         <v>0.5</v>
@@ -8153,7 +8153,7 @@
         <v>227</v>
       </c>
       <c r="T18" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U18" s="48">
         <v>0.5</v>
@@ -8308,7 +8308,7 @@
         <v>104</v>
       </c>
       <c r="T19" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U19" s="35">
         <v>0.5</v>
@@ -8463,7 +8463,7 @@
         <v>75</v>
       </c>
       <c r="T20" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U20" s="35">
         <v>0.5</v>
@@ -8618,7 +8618,7 @@
         <v>105</v>
       </c>
       <c r="T21" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U21" s="35">
         <v>0.5</v>
@@ -8773,7 +8773,7 @@
         <v>75</v>
       </c>
       <c r="T22" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U22" s="35" t="s">
         <v>152</v>
@@ -8926,7 +8926,7 @@
         <v>102</v>
       </c>
       <c r="T23" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U23" s="35" t="s">
         <v>152</v>
@@ -9075,7 +9075,7 @@
         <v>75</v>
       </c>
       <c r="T24" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U24" s="35">
         <v>-1</v>
@@ -9230,7 +9230,7 @@
         <v>75</v>
       </c>
       <c r="T25" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U25" s="35" t="s">
         <v>150</v>
@@ -9385,7 +9385,7 @@
         <v>103</v>
       </c>
       <c r="T26" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U26" s="35">
         <v>-1</v>
@@ -9536,7 +9536,7 @@
         <v>102</v>
       </c>
       <c r="T27" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U27" s="35">
         <v>-1</v>
@@ -9673,7 +9673,7 @@
         <v>1.99</v>
       </c>
       <c r="T28" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U28" s="35" t="s">
         <v>151</v>
@@ -9820,7 +9820,7 @@
         <v>4.99</v>
       </c>
       <c r="T29" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U29" s="35" t="s">
         <v>151</v>
@@ -9967,7 +9967,7 @@
         <v>103</v>
       </c>
       <c r="T30" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U30" s="35">
         <v>-1</v>
@@ -10110,7 +10110,7 @@
         <v>104</v>
       </c>
       <c r="T31" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U31" s="35">
         <v>-1</v>
@@ -10259,7 +10259,7 @@
         <v>103</v>
       </c>
       <c r="T32" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U32" s="35">
         <v>-1</v>
@@ -10402,7 +10402,7 @@
         <v>104</v>
       </c>
       <c r="T33" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U33" s="35">
         <v>-1</v>
@@ -10545,7 +10545,7 @@
         <v>105</v>
       </c>
       <c r="T34" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U34" s="95">
         <v>-1</v>
@@ -10688,7 +10688,7 @@
         <v>103</v>
       </c>
       <c r="T35" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U35" s="79">
         <v>-1</v>
@@ -10841,7 +10841,7 @@
         <v>103</v>
       </c>
       <c r="T36" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U36" s="79">
         <v>-1</v>
@@ -10994,7 +10994,7 @@
         <v>105</v>
       </c>
       <c r="T37" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U37" s="79">
         <v>-1</v>
@@ -11141,7 +11141,7 @@
         <v>226</v>
       </c>
       <c r="T38" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U38" s="79">
         <v>-1</v>
@@ -11284,7 +11284,7 @@
         <v>75</v>
       </c>
       <c r="T39" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U39" s="79">
         <v>-1</v>
@@ -11431,7 +11431,7 @@
         <v>102</v>
       </c>
       <c r="T40" s="208" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U40" s="137">
         <v>-1</v>
@@ -11574,7 +11574,7 @@
         <v>226</v>
       </c>
       <c r="T41" s="144" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U41" s="145">
         <v>-1</v>
@@ -11723,7 +11723,7 @@
         <v>102</v>
       </c>
       <c r="T42" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U42" s="79">
         <v>-1</v>
@@ -11872,7 +11872,7 @@
         <v>103</v>
       </c>
       <c r="T43" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U43" s="79">
         <v>-1</v>
@@ -12023,7 +12023,7 @@
         <v>101</v>
       </c>
       <c r="T44" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U44" s="79">
         <v>-1</v>
@@ -12170,7 +12170,7 @@
         <v>75</v>
       </c>
       <c r="T45" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U45" s="79">
         <v>-1</v>
@@ -12317,7 +12317,7 @@
         <v>102</v>
       </c>
       <c r="T46" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U46" s="79">
         <v>-1</v>
@@ -12472,7 +12472,7 @@
         <v>75</v>
       </c>
       <c r="T47" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U47" s="232">
         <v>-1</v>
@@ -12615,7 +12615,7 @@
         <v>102</v>
       </c>
       <c r="T48" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U48" s="79">
         <v>-1</v>
@@ -12764,7 +12764,7 @@
         <v>75</v>
       </c>
       <c r="T49" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U49" s="79">
         <v>-1</v>
@@ -12907,7 +12907,7 @@
         <v>102</v>
       </c>
       <c r="T50" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U50" s="79">
         <v>-1</v>
@@ -13054,7 +13054,7 @@
         <v>102</v>
       </c>
       <c r="T51" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U51" s="79">
         <v>-1</v>
@@ -13201,7 +13201,7 @@
         <v>75</v>
       </c>
       <c r="T52" s="208" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U52" s="79">
         <v>-1</v>
@@ -13356,7 +13356,7 @@
         <v>101</v>
       </c>
       <c r="T53" s="144" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U53" s="145">
         <v>0.5</v>
@@ -13511,7 +13511,7 @@
         <v>75</v>
       </c>
       <c r="T54" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U54" s="79">
         <v>0.5</v>
@@ -13666,7 +13666,7 @@
         <v>102</v>
       </c>
       <c r="T55" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U55" s="79">
         <v>0.5</v>
@@ -13821,7 +13821,7 @@
         <v>101</v>
       </c>
       <c r="T56" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U56" s="232" t="s">
         <v>301</v>
@@ -13976,7 +13976,7 @@
         <v>102</v>
       </c>
       <c r="T57" s="209" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U57" s="198">
         <v>-1</v>
@@ -14063,7 +14063,7 @@
         <v>127</v>
       </c>
       <c r="AW57" s="204" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX57" s="203" t="s">
         <v>127</v>
@@ -14131,7 +14131,7 @@
         <v>227</v>
       </c>
       <c r="T58" s="208" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U58" s="48">
         <v>-1</v>
@@ -14218,7 +14218,7 @@
         <v>127</v>
       </c>
       <c r="AW58" s="191" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX58" s="190" t="s">
         <v>127</v>
@@ -14286,7 +14286,7 @@
         <v>104</v>
       </c>
       <c r="T59" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U59" s="79">
         <v>-1</v>
@@ -14373,7 +14373,7 @@
         <v>127</v>
       </c>
       <c r="AW59" s="54" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX59" s="53" t="s">
         <v>127</v>
@@ -14439,7 +14439,7 @@
         <v>227</v>
       </c>
       <c r="T60" s="208" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U60" s="137">
         <v>-1</v>
@@ -14526,7 +14526,7 @@
         <v>127</v>
       </c>
       <c r="AW60" s="96" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX60" s="78" t="s">
         <v>127</v>
@@ -14594,7 +14594,7 @@
         <v>75</v>
       </c>
       <c r="T61" s="164" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U61" s="233">
         <v>-1</v>
@@ -14681,7 +14681,7 @@
         <v>127</v>
       </c>
       <c r="AW61" s="170" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX61" s="169" t="s">
         <v>127</v>
@@ -14749,7 +14749,7 @@
         <v>75</v>
       </c>
       <c r="T62" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U62" s="79">
         <v>-1</v>
@@ -14836,7 +14836,7 @@
         <v>127</v>
       </c>
       <c r="AW62" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX62" s="13" t="s">
         <v>127</v>
@@ -14904,7 +14904,7 @@
         <v>102</v>
       </c>
       <c r="T63" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U63" s="79">
         <v>-1</v>
@@ -14991,7 +14991,7 @@
         <v>127</v>
       </c>
       <c r="AW63" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX63" s="13" t="s">
         <v>127</v>
@@ -15059,7 +15059,7 @@
         <v>75</v>
       </c>
       <c r="T64" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U64" s="79">
         <v>-1</v>
@@ -15146,7 +15146,7 @@
         <v>127</v>
       </c>
       <c r="AW64" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX64" s="13" t="s">
         <v>127</v>
@@ -15214,7 +15214,7 @@
         <v>102</v>
       </c>
       <c r="T65" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U65" s="79">
         <v>-1</v>
@@ -15301,7 +15301,7 @@
         <v>127</v>
       </c>
       <c r="AW65" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX65" s="13" t="s">
         <v>127</v>
@@ -15369,7 +15369,7 @@
         <v>226</v>
       </c>
       <c r="T66" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U66" s="79">
         <v>-1</v>
@@ -15456,7 +15456,7 @@
         <v>127</v>
       </c>
       <c r="AW66" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX66" s="13" t="s">
         <v>127</v>
@@ -15524,7 +15524,7 @@
         <v>75</v>
       </c>
       <c r="T67" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U67" s="79">
         <v>-1</v>
@@ -15611,7 +15611,7 @@
         <v>127</v>
       </c>
       <c r="AW67" s="20" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="AX67" s="13" t="s">
         <v>127</v>
@@ -15679,7 +15679,7 @@
         <v>75</v>
       </c>
       <c r="T68" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U68" s="79">
         <v>-1</v>
@@ -15766,7 +15766,7 @@
         <v>127</v>
       </c>
       <c r="AW68" s="20" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="AX68" s="13" t="s">
         <v>127</v>
@@ -15832,7 +15832,7 @@
         <v>101</v>
       </c>
       <c r="T69" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U69" s="79">
         <v>-1</v>
@@ -15919,7 +15919,7 @@
         <v>127</v>
       </c>
       <c r="AW69" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX69" s="13" t="s">
         <v>127</v>
@@ -15987,7 +15987,7 @@
         <v>75</v>
       </c>
       <c r="T70" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U70" s="79">
         <v>-1</v>
@@ -16074,7 +16074,7 @@
         <v>127</v>
       </c>
       <c r="AW70" s="20" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="AX70" s="13" t="s">
         <v>127</v>
@@ -16142,7 +16142,7 @@
         <v>101</v>
       </c>
       <c r="T71" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U71" s="206" t="s">
         <v>306</v>
@@ -16297,7 +16297,7 @@
         <v>75</v>
       </c>
       <c r="T72" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U72" s="206" t="s">
         <v>150</v>
@@ -16450,7 +16450,7 @@
         <v>75</v>
       </c>
       <c r="T73" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U73" s="206" t="s">
         <v>301</v>
@@ -16513,7 +16513,7 @@
         <v>127</v>
       </c>
       <c r="AO73" s="13" t="s">
-        <v>302</v>
+        <v>127</v>
       </c>
       <c r="AP73" s="13" t="s">
         <v>127</v>
@@ -16605,7 +16605,7 @@
         <v>101</v>
       </c>
       <c r="T74" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U74" s="206" t="s">
         <v>301</v>
@@ -16669,7 +16669,7 @@
         <v>127</v>
       </c>
       <c r="AP74" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AQ74" s="13" t="s">
         <v>127</v>
@@ -16756,7 +16756,7 @@
         <v>101</v>
       </c>
       <c r="T75" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U75" s="206" t="s">
         <v>301</v>
@@ -16843,7 +16843,7 @@
         <v>127</v>
       </c>
       <c r="AW75" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX75" s="13" t="s">
         <v>127</v>
@@ -16911,7 +16911,7 @@
         <v>75</v>
       </c>
       <c r="T76" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U76" s="206" t="s">
         <v>307</v>
@@ -17015,13 +17015,13 @@
         <v>2</v>
       </c>
       <c r="C77" s="212" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D77" s="24" t="s">
         <v>127</v>
       </c>
       <c r="E77" s="211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F77" s="29" t="b">
         <v>1</v>
@@ -17066,7 +17066,7 @@
         <v>127</v>
       </c>
       <c r="T77" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U77" s="213" t="s">
         <v>127</v>
@@ -17075,7 +17075,7 @@
         <v>127</v>
       </c>
       <c r="W77" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X77" s="21" t="b">
         <v>0</v>
@@ -17099,7 +17099,7 @@
         <v>127</v>
       </c>
       <c r="AE77" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF77" s="13" t="s">
         <v>127</v>
@@ -17153,7 +17153,7 @@
         <v>127</v>
       </c>
       <c r="AW77" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX77" s="13" t="s">
         <v>127</v>
@@ -17170,13 +17170,13 @@
         <v>2</v>
       </c>
       <c r="C78" s="212" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D78" s="24" t="s">
         <v>127</v>
       </c>
       <c r="E78" s="211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F78" s="29" t="b">
         <v>1</v>
@@ -17221,7 +17221,7 @@
         <v>127</v>
       </c>
       <c r="T78" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U78" s="213" t="s">
         <v>127</v>
@@ -17230,7 +17230,7 @@
         <v>127</v>
       </c>
       <c r="W78" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X78" s="21" t="b">
         <v>0</v>
@@ -17254,7 +17254,7 @@
         <v>127</v>
       </c>
       <c r="AE78" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF78" s="13" t="s">
         <v>127</v>
@@ -17308,7 +17308,7 @@
         <v>127</v>
       </c>
       <c r="AW78" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX78" s="13" t="s">
         <v>127</v>
@@ -17325,13 +17325,13 @@
         <v>2</v>
       </c>
       <c r="C79" s="212" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D79" s="24" t="s">
         <v>127</v>
       </c>
       <c r="E79" s="211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F79" s="29" t="b">
         <v>1</v>
@@ -17376,7 +17376,7 @@
         <v>127</v>
       </c>
       <c r="T79" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U79" s="213" t="s">
         <v>127</v>
@@ -17385,7 +17385,7 @@
         <v>127</v>
       </c>
       <c r="W79" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X79" s="21" t="b">
         <v>0</v>
@@ -17409,7 +17409,7 @@
         <v>127</v>
       </c>
       <c r="AE79" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF79" s="13" t="s">
         <v>127</v>
@@ -17463,7 +17463,7 @@
         <v>127</v>
       </c>
       <c r="AW79" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX79" s="13" t="s">
         <v>127</v>
@@ -17480,13 +17480,13 @@
         <v>2</v>
       </c>
       <c r="C80" s="212" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D80" s="24" t="s">
         <v>127</v>
       </c>
       <c r="E80" s="211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F80" s="29" t="b">
         <v>1</v>
@@ -17531,7 +17531,7 @@
         <v>127</v>
       </c>
       <c r="T80" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U80" s="213" t="s">
         <v>127</v>
@@ -17540,7 +17540,7 @@
         <v>127</v>
       </c>
       <c r="W80" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X80" s="21" t="b">
         <v>0</v>
@@ -17564,7 +17564,7 @@
         <v>127</v>
       </c>
       <c r="AE80" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF80" s="13" t="s">
         <v>127</v>
@@ -17618,7 +17618,7 @@
         <v>127</v>
       </c>
       <c r="AW80" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX80" s="13" t="s">
         <v>127</v>
@@ -17635,13 +17635,13 @@
         <v>2</v>
       </c>
       <c r="C81" s="212" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D81" s="24" t="s">
         <v>127</v>
       </c>
       <c r="E81" s="211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F81" s="29" t="b">
         <v>1</v>
@@ -17686,7 +17686,7 @@
         <v>127</v>
       </c>
       <c r="T81" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U81" s="213" t="s">
         <v>127</v>
@@ -17695,7 +17695,7 @@
         <v>127</v>
       </c>
       <c r="W81" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X81" s="21" t="b">
         <v>0</v>
@@ -17719,7 +17719,7 @@
         <v>127</v>
       </c>
       <c r="AE81" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF81" s="13" t="s">
         <v>127</v>
@@ -17773,7 +17773,7 @@
         <v>127</v>
       </c>
       <c r="AW81" s="20" t="s">
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AX81" s="13" t="s">
         <v>127</v>
@@ -17787,7 +17787,7 @@
     </row>
     <row r="84" spans="2:52" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B84" s="248" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C84" s="248"/>
       <c r="D84" s="248"/>
@@ -17795,7 +17795,7 @@
     </row>
     <row r="86" spans="2:52" ht="135" x14ac:dyDescent="0.25">
       <c r="B86" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C86" s="243" t="s">
         <v>0</v>
@@ -17804,19 +17804,19 @@
         <v>52</v>
       </c>
       <c r="E86" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="F86" s="244" t="s">
         <v>333</v>
       </c>
-      <c r="F86" s="244" t="s">
+      <c r="G86" s="245" t="s">
         <v>334</v>
       </c>
-      <c r="G86" s="245" t="s">
+      <c r="H86" s="245" t="s">
         <v>335</v>
       </c>
-      <c r="H86" s="245" t="s">
+      <c r="I86" s="245" t="s">
         <v>336</v>
-      </c>
-      <c r="I86" s="245" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="87" spans="2:52" x14ac:dyDescent="0.25">
@@ -17824,7 +17824,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="211" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D87" s="29" t="b">
         <v>1</v>
@@ -17839,10 +17839,10 @@
         <v>1</v>
       </c>
       <c r="H87" s="211" t="s">
+        <v>338</v>
+      </c>
+      <c r="I87" s="211" t="s">
         <v>339</v>
-      </c>
-      <c r="I87" s="211" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -17879,7 +17879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
@@ -17959,28 +17959,28 @@
     </row>
     <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="H2" s="239" t="s">
         <v>319</v>
       </c>
-      <c r="H2" s="239" t="s">
+      <c r="I2" s="240" t="s">
         <v>320</v>
-      </c>
-      <c r="I2" s="240" t="s">
-        <v>321</v>
       </c>
       <c r="J2" s="241"/>
     </row>
@@ -17989,7 +17989,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="212" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D3" s="24">
         <v>1</v>

</xml_diff>

<commit_message>
Progression offers now appear after the second run played!
Former-commit-id: e2c6891258208460e3a0b2808066995d840ec219
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3240" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="341">
   <si>
     <t>[sku]</t>
   </si>
@@ -2381,6 +2381,46 @@
   <dxfs count="69">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5078,46 +5118,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5146,80 +5146,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B2:AZ76"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="61"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="59"/>
-    <tableColumn id="49" name="[type]" dataDxfId="58"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="57"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="56"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="55"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="54"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="53"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="52"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="51"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="50"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="49"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="48"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="47"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="46"/>
-    <tableColumn id="7" name="[order]" dataDxfId="45"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="44"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="43"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="42"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="41"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="40"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="39"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="38"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="37"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="36"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="35"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="34"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="33"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="32"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="31"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="30"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="29"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="28"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="27"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="26"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="25"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="24"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="23"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="22"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="21"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="20"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="19"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="18"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="17"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="16"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="15"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="14"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="13"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="12"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="11"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="65"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="63"/>
+    <tableColumn id="49" name="[type]" dataDxfId="62"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="61"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="60"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="59"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="58"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="57"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="56"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="55"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="54"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="53"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="52"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="51"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[order]" dataDxfId="49"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="48"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="47"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="46"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="45"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="44"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="43"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="42"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="41"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="40"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="39"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="38"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="37"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="36"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="35"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="34"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="33"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="32"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="31"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="30"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="29"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="28"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="27"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="26"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="25"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="24"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="23"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="22"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="21"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="20"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="19"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="18"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="17"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="16"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B2:I3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="7"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="5"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="4"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="3"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="2"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="0"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="11"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="9"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="8"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="7"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="6"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="5"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5525,8 +5525,8 @@
   <dimension ref="B1:AZ87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5869,7 +5869,7 @@
         <v>127</v>
       </c>
       <c r="AH3" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI3" s="13" t="s">
         <v>165</v>
@@ -6023,8 +6023,8 @@
       <c r="AG4" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH4" s="13" t="s">
-        <v>127</v>
+      <c r="AH4" s="13">
+        <v>2</v>
       </c>
       <c r="AI4" s="13" t="s">
         <v>127</v>
@@ -6179,7 +6179,7 @@
         <v>127</v>
       </c>
       <c r="AH5" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI5" s="13" t="s">
         <v>127</v>
@@ -6333,8 +6333,8 @@
       <c r="AG6" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH6" s="13" t="s">
-        <v>127</v>
+      <c r="AH6" s="13">
+        <v>2</v>
       </c>
       <c r="AI6" s="13" t="s">
         <v>127</v>
@@ -6488,8 +6488,8 @@
       <c r="AG7" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH7" s="13" t="s">
-        <v>127</v>
+      <c r="AH7" s="13">
+        <v>2</v>
       </c>
       <c r="AI7" s="13" t="s">
         <v>127</v>
@@ -6644,7 +6644,7 @@
         <v>127</v>
       </c>
       <c r="AH8" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI8" s="13" t="s">
         <v>127</v>
@@ -6799,7 +6799,7 @@
         <v>127</v>
       </c>
       <c r="AH9" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI9" s="13" t="s">
         <v>127</v>
@@ -6953,8 +6953,8 @@
       <c r="AG10" s="115" t="s">
         <v>127</v>
       </c>
-      <c r="AH10" s="115" t="s">
-        <v>127</v>
+      <c r="AH10" s="13">
+        <v>2</v>
       </c>
       <c r="AI10" s="115" t="s">
         <v>127</v>
@@ -7108,8 +7108,8 @@
       <c r="AG11" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="AH11" s="53" t="s">
-        <v>127</v>
+      <c r="AH11" s="13">
+        <v>2</v>
       </c>
       <c r="AI11" s="53" t="s">
         <v>127</v>
@@ -7263,8 +7263,8 @@
       <c r="AG12" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH12" s="13" t="s">
-        <v>127</v>
+      <c r="AH12" s="13">
+        <v>2</v>
       </c>
       <c r="AI12" s="13" t="s">
         <v>127</v>
@@ -7418,8 +7418,8 @@
       <c r="AG13" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH13" s="13" t="s">
-        <v>127</v>
+      <c r="AH13" s="13">
+        <v>2</v>
       </c>
       <c r="AI13" s="13" t="s">
         <v>127</v>
@@ -7575,7 +7575,7 @@
         <v>127</v>
       </c>
       <c r="AH14" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI14" s="13" t="s">
         <v>127</v>
@@ -7729,8 +7729,8 @@
       <c r="AG15" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH15" s="13" t="s">
-        <v>127</v>
+      <c r="AH15" s="13">
+        <v>2</v>
       </c>
       <c r="AI15" s="13" t="s">
         <v>127</v>
@@ -7884,8 +7884,8 @@
       <c r="AG16" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH16" s="13" t="s">
-        <v>127</v>
+      <c r="AH16" s="13">
+        <v>2</v>
       </c>
       <c r="AI16" s="13" t="s">
         <v>127</v>
@@ -8039,8 +8039,8 @@
       <c r="AG17" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="AH17" s="130">
-        <v>4</v>
+      <c r="AH17" s="13">
+        <v>2</v>
       </c>
       <c r="AI17" s="130" t="s">
         <v>127</v>
@@ -8194,8 +8194,8 @@
       <c r="AG18" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="AH18" s="53">
-        <v>4</v>
+      <c r="AH18" s="13">
+        <v>2</v>
       </c>
       <c r="AI18" s="53" t="s">
         <v>127</v>
@@ -8349,8 +8349,8 @@
       <c r="AG19" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH19" s="13" t="s">
-        <v>127</v>
+      <c r="AH19" s="13">
+        <v>2</v>
       </c>
       <c r="AI19" s="13" t="s">
         <v>127</v>
@@ -8504,8 +8504,8 @@
       <c r="AG20" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH20" s="13" t="s">
-        <v>127</v>
+      <c r="AH20" s="13">
+        <v>2</v>
       </c>
       <c r="AI20" s="13" t="s">
         <v>127</v>
@@ -8659,8 +8659,8 @@
       <c r="AG21" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH21" s="13" t="s">
-        <v>127</v>
+      <c r="AH21" s="13">
+        <v>2</v>
       </c>
       <c r="AI21" s="13" t="s">
         <v>127</v>
@@ -8815,7 +8815,7 @@
         <v>127</v>
       </c>
       <c r="AH22" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI22" s="13"/>
       <c r="AJ22" s="13" t="s">
@@ -8968,7 +8968,7 @@
         <v>127</v>
       </c>
       <c r="AH23" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI23" s="13" t="s">
         <v>127</v>
@@ -9117,7 +9117,7 @@
         <v>127</v>
       </c>
       <c r="AH24" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI24" s="13" t="s">
         <v>164</v>
@@ -9272,7 +9272,7 @@
         <v>127</v>
       </c>
       <c r="AH25" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI25" s="13" t="s">
         <v>127</v>
@@ -9425,7 +9425,7 @@
         <v>127</v>
       </c>
       <c r="AH26" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI26" s="13" t="s">
         <v>165</v>
@@ -9578,7 +9578,7 @@
         <v>127</v>
       </c>
       <c r="AH27" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI27" s="13" t="s">
         <v>127</v>
@@ -9715,7 +9715,7 @@
         <v>127</v>
       </c>
       <c r="AH28" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI28" s="13" t="s">
         <v>127</v>
@@ -9862,7 +9862,7 @@
         <v>127</v>
       </c>
       <c r="AH29" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI29" s="13" t="s">
         <v>127</v>
@@ -10009,7 +10009,7 @@
         <v>127</v>
       </c>
       <c r="AH30" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI30" s="13" t="s">
         <v>165</v>
@@ -10152,7 +10152,7 @@
         <v>127</v>
       </c>
       <c r="AH31" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI31" s="13" t="s">
         <v>165</v>
@@ -10301,7 +10301,7 @@
         <v>127</v>
       </c>
       <c r="AH32" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI32" s="13" t="s">
         <v>165</v>
@@ -10444,7 +10444,7 @@
         <v>127</v>
       </c>
       <c r="AH33" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI33" s="13" t="s">
         <v>165</v>
@@ -10586,8 +10586,8 @@
       <c r="AG34" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="AH34" s="78">
-        <v>4</v>
+      <c r="AH34" s="13">
+        <v>2</v>
       </c>
       <c r="AI34" s="78" t="s">
         <v>165</v>
@@ -10729,8 +10729,8 @@
       <c r="AG35" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="AH35" s="92">
-        <v>4</v>
+      <c r="AH35" s="13">
+        <v>2</v>
       </c>
       <c r="AI35" s="92" t="s">
         <v>165</v>
@@ -10883,7 +10883,7 @@
         <v>127</v>
       </c>
       <c r="AH36" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI36" s="13" t="s">
         <v>165</v>
@@ -11036,7 +11036,7 @@
         <v>127</v>
       </c>
       <c r="AH37" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI37" s="13" t="s">
         <v>165</v>
@@ -11183,7 +11183,7 @@
         <v>127</v>
       </c>
       <c r="AH38" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI38" s="13" t="s">
         <v>165</v>
@@ -11326,7 +11326,7 @@
         <v>127</v>
       </c>
       <c r="AH39" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI39" s="13" t="s">
         <v>165</v>
@@ -11472,8 +11472,8 @@
       <c r="AG40" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="AH40" s="78">
-        <v>4</v>
+      <c r="AH40" s="13">
+        <v>2</v>
       </c>
       <c r="AI40" s="78" t="s">
         <v>165</v>
@@ -11615,8 +11615,8 @@
       <c r="AG41" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="AH41" s="150">
-        <v>4</v>
+      <c r="AH41" s="13">
+        <v>2</v>
       </c>
       <c r="AI41" s="150" t="s">
         <v>165</v>
@@ -11765,7 +11765,7 @@
         <v>127</v>
       </c>
       <c r="AH42" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI42" s="13" t="s">
         <v>165</v>
@@ -11914,7 +11914,7 @@
         <v>127</v>
       </c>
       <c r="AH43" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI43" s="13" t="s">
         <v>165</v>
@@ -12065,7 +12065,7 @@
         <v>127</v>
       </c>
       <c r="AH44" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI44" s="13" t="s">
         <v>164</v>
@@ -12212,7 +12212,7 @@
         <v>127</v>
       </c>
       <c r="AH45" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI45" s="13" t="s">
         <v>164</v>
@@ -12358,8 +12358,8 @@
       <c r="AG46" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="AH46" s="65">
-        <v>4</v>
+      <c r="AH46" s="13">
+        <v>2</v>
       </c>
       <c r="AI46" s="13" t="s">
         <v>164</v>
@@ -12513,8 +12513,8 @@
       <c r="AG47" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="AH47" s="92">
-        <v>4</v>
+      <c r="AH47" s="13">
+        <v>2</v>
       </c>
       <c r="AI47" s="235" t="s">
         <v>127</v>
@@ -12657,7 +12657,7 @@
         <v>127</v>
       </c>
       <c r="AH48" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI48" s="13" t="s">
         <v>164</v>
@@ -12806,7 +12806,7 @@
         <v>127</v>
       </c>
       <c r="AH49" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI49" s="13" t="s">
         <v>164</v>
@@ -12949,7 +12949,7 @@
         <v>127</v>
       </c>
       <c r="AH50" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI50" s="13" t="s">
         <v>164</v>
@@ -13096,7 +13096,7 @@
         <v>127</v>
       </c>
       <c r="AH51" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI51" s="13" t="s">
         <v>164</v>
@@ -13242,8 +13242,8 @@
       <c r="AG52" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="AH52" s="78">
-        <v>4</v>
+      <c r="AH52" s="13">
+        <v>2</v>
       </c>
       <c r="AI52" s="78" t="s">
         <v>164</v>
@@ -13397,8 +13397,8 @@
       <c r="AG53" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="AH53" s="150" t="s">
-        <v>127</v>
+      <c r="AH53" s="13">
+        <v>2</v>
       </c>
       <c r="AI53" s="150" t="s">
         <v>127</v>
@@ -13552,8 +13552,8 @@
       <c r="AG54" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH54" s="13" t="s">
-        <v>127</v>
+      <c r="AH54" s="13">
+        <v>2</v>
       </c>
       <c r="AI54" s="13" t="s">
         <v>127</v>
@@ -13707,8 +13707,8 @@
       <c r="AG55" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AH55" s="13" t="s">
-        <v>127</v>
+      <c r="AH55" s="13">
+        <v>2</v>
       </c>
       <c r="AI55" s="13" t="s">
         <v>127</v>
@@ -13863,7 +13863,7 @@
         <v>127</v>
       </c>
       <c r="AH56" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI56" s="133" t="s">
         <v>127</v>
@@ -14017,8 +14017,8 @@
       <c r="AG57" s="203" t="s">
         <v>127</v>
       </c>
-      <c r="AH57" s="203">
-        <v>4</v>
+      <c r="AH57" s="13">
+        <v>2</v>
       </c>
       <c r="AI57" s="203" t="s">
         <v>165</v>
@@ -14172,8 +14172,8 @@
       <c r="AG58" s="190" t="s">
         <v>127</v>
       </c>
-      <c r="AH58" s="190">
-        <v>4</v>
+      <c r="AH58" s="13">
+        <v>2</v>
       </c>
       <c r="AI58" s="190" t="s">
         <v>165</v>
@@ -14327,8 +14327,8 @@
       <c r="AG59" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="AH59" s="53">
-        <v>4</v>
+      <c r="AH59" s="13">
+        <v>2</v>
       </c>
       <c r="AI59" s="53" t="s">
         <v>165</v>
@@ -14480,8 +14480,8 @@
       <c r="AG60" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="AH60" s="78">
-        <v>4</v>
+      <c r="AH60" s="13">
+        <v>2</v>
       </c>
       <c r="AI60" s="78" t="s">
         <v>165</v>
@@ -14635,8 +14635,8 @@
       <c r="AG61" s="169" t="s">
         <v>127</v>
       </c>
-      <c r="AH61" s="169">
-        <v>4</v>
+      <c r="AH61" s="13">
+        <v>2</v>
       </c>
       <c r="AI61" s="169" t="s">
         <v>165</v>
@@ -14791,7 +14791,7 @@
         <v>127</v>
       </c>
       <c r="AH62" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI62" s="13" t="s">
         <v>165</v>
@@ -14946,7 +14946,7 @@
         <v>127</v>
       </c>
       <c r="AH63" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI63" s="13" t="s">
         <v>165</v>
@@ -15101,7 +15101,7 @@
         <v>127</v>
       </c>
       <c r="AH64" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI64" s="13" t="s">
         <v>165</v>
@@ -15256,7 +15256,7 @@
         <v>127</v>
       </c>
       <c r="AH65" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI65" s="13" t="s">
         <v>165</v>
@@ -15411,7 +15411,7 @@
         <v>127</v>
       </c>
       <c r="AH66" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI66" s="13" t="s">
         <v>165</v>
@@ -15566,7 +15566,7 @@
         <v>127</v>
       </c>
       <c r="AH67" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI67" s="13" t="s">
         <v>164</v>
@@ -15721,7 +15721,7 @@
         <v>127</v>
       </c>
       <c r="AH68" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI68" s="13" t="s">
         <v>164</v>
@@ -15874,7 +15874,7 @@
         <v>127</v>
       </c>
       <c r="AH69" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI69" s="13" t="s">
         <v>164</v>
@@ -16029,7 +16029,7 @@
         <v>127</v>
       </c>
       <c r="AH70" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI70" s="13" t="s">
         <v>164</v>
@@ -16184,7 +16184,7 @@
         <v>127</v>
       </c>
       <c r="AH71" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI71" s="133" t="s">
         <v>127</v>
@@ -16337,7 +16337,7 @@
         <v>127</v>
       </c>
       <c r="AH72" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI72" s="13" t="s">
         <v>127</v>
@@ -16492,7 +16492,7 @@
         <v>127</v>
       </c>
       <c r="AH73" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI73" s="133" t="s">
         <v>127</v>
@@ -16645,7 +16645,7 @@
         <v>127</v>
       </c>
       <c r="AH74" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI74" s="133" t="s">
         <v>127</v>
@@ -16798,7 +16798,7 @@
         <v>127</v>
       </c>
       <c r="AH75" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI75" s="13" t="s">
         <v>127</v>
@@ -16953,7 +16953,7 @@
         <v>127</v>
       </c>
       <c r="AH76" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI76" s="133" t="s">
         <v>127</v>
@@ -17108,7 +17108,7 @@
         <v>127</v>
       </c>
       <c r="AH77" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI77" s="133" t="s">
         <v>127</v>
@@ -17263,7 +17263,7 @@
         <v>127</v>
       </c>
       <c r="AH78" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI78" s="133" t="s">
         <v>127</v>
@@ -17418,7 +17418,7 @@
         <v>127</v>
       </c>
       <c r="AH79" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI79" s="133" t="s">
         <v>127</v>
@@ -17573,7 +17573,7 @@
         <v>127</v>
       </c>
       <c r="AH80" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI80" s="133" t="s">
         <v>127</v>
@@ -17728,7 +17728,7 @@
         <v>127</v>
       </c>
       <c r="AH81" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI81" s="133" t="s">
         <v>127</v>
@@ -17852,18 +17852,18 @@
     <mergeCell ref="B84:E84"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F81">
-    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D87)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reduced the amount of coins given by the Ad offer.
Former-commit-id: 88815d67ede1c8f83f9e2e55bf4a1ea30fb3b8f9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -2381,46 +2381,6 @@
   <dxfs count="69">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5118,6 +5078,46 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5146,80 +5146,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="B2:AZ76"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="65"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="63"/>
-    <tableColumn id="49" name="[type]" dataDxfId="62"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="61"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="60"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="59"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="58"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="57"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="56"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="55"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="54"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="53"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="52"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="51"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[order]" dataDxfId="49"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="48"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="47"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="46"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="45"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="44"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="43"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="42"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="41"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="40"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="39"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="38"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="37"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="36"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="35"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="34"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="33"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="32"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="31"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="30"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="29"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="28"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="27"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="26"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="25"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="24"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="23"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="22"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="21"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="20"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="19"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="18"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="17"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="16"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="15"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="61"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="59"/>
+    <tableColumn id="49" name="[type]" dataDxfId="58"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="57"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="56"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="55"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="54"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="53"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="52"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="51"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="50"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="49"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="48"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="47"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="46"/>
+    <tableColumn id="7" name="[order]" dataDxfId="45"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="44"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="43"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="42"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="41"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="40"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="39"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="38"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="37"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="36"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="35"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="34"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="33"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="32"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="31"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="30"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="29"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="28"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="27"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="26"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="25"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="24"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="23"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="22"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="21"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="20"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="19"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="18"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="17"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="16"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="15"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="14"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="13"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="12"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="B2:I3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="9"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="8"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="7"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="6"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="5"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="4"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="7"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="5"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="4"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="3"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="2"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5526,7 +5526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17191,7 +17191,7 @@
         <v>12</v>
       </c>
       <c r="J78" s="30">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K78" s="30" t="s">
         <v>127</v>
@@ -17656,7 +17656,7 @@
         <v>12</v>
       </c>
       <c r="J81" s="30">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="K81" s="30" t="s">
         <v>127</v>
@@ -17852,18 +17852,18 @@
     <mergeCell ref="B84:E84"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F81">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D87)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding the offer. I don't export now, we already have an excel for testing
Former-commit-id: 18033ae2981791023b102ab6ec32df9390d83097
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3271" uniqueCount="346">
   <si>
     <t>[sku]</t>
   </si>
@@ -1050,13 +1050,28 @@
   </si>
   <si>
     <t>2:999</t>
+  </si>
+  <si>
+    <t>removeAdsOffer</t>
+  </si>
+  <si>
+    <t>removeAds</t>
+  </si>
+  <si>
+    <t>5.99</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.remove_ads_offer</t>
+  </si>
+  <si>
+    <t>TID_REMOVE_ADS_OFFER_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1209,6 +1224,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1640,7 +1666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="280">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2270,9 +2296,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2353,9 +2376,6 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -2373,12 +2393,151 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5078,46 +5237,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5146,80 +5265,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
-  <autoFilter ref="B2:AZ76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+  <autoFilter ref="B2:AZ82"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="61"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="59"/>
-    <tableColumn id="49" name="[type]" dataDxfId="58"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="57"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="56"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="55"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="54"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="53"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="52"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="51"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="50"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="49"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="48"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="47"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="46"/>
-    <tableColumn id="7" name="[order]" dataDxfId="45"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="44"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="43"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="42"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="41"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="40"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="39"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="38"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="37"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="36"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="35"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="34"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="33"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="32"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="31"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="30"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="29"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="28"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="27"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="26"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="25"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="24"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="23"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="22"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="21"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="20"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="19"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="18"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="17"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="16"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="15"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="14"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="13"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="12"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="11"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="65"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="63"/>
+    <tableColumn id="49" name="[type]" dataDxfId="62"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="61"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="60"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="59"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="58"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="57"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="56"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="55"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="54"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="53"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="52"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="51"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[order]" dataDxfId="49"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="48"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="47"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="46"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="45"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="44"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="43"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="42"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="41"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="40"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="39"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="38"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="37"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="36"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="35"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="34"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="33"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="32"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="31"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="30"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="29"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="28"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="27"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="26"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="25"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="24"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="23"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="22"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="21"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="20"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="19"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="18"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="17"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="16"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B2:I3"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="7"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="5"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="4"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="3"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="2"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="0"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="11"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="9"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="8"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="7"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="6"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="5"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5522,14 +5641,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AZ87"/>
+  <dimension ref="B1:AZ88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AW84" sqref="AW84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
@@ -5570,7 +5689,7 @@
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5">
       <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
@@ -5586,37 +5705,37 @@
       <c r="V1" s="210" t="s">
         <v>310</v>
       </c>
-      <c r="AA1" s="246" t="s">
+      <c r="AA1" s="244" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="246"/>
+      <c r="AB1" s="244"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="247" t="s">
+      <c r="AD1" s="245" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="247"/>
-      <c r="AF1" s="247"/>
-      <c r="AG1" s="247"/>
-      <c r="AH1" s="247"/>
-      <c r="AI1" s="247"/>
-      <c r="AJ1" s="247"/>
-      <c r="AK1" s="247"/>
-      <c r="AL1" s="247"/>
-      <c r="AM1" s="247"/>
-      <c r="AN1" s="247"/>
-      <c r="AO1" s="247"/>
-      <c r="AP1" s="247"/>
-      <c r="AQ1" s="247"/>
-      <c r="AR1" s="247"/>
-      <c r="AS1" s="247"/>
-      <c r="AT1" s="247"/>
-      <c r="AU1" s="247"/>
-      <c r="AV1" s="247"/>
-      <c r="AW1" s="247"/>
-      <c r="AX1" s="247"/>
-      <c r="AY1" s="247"/>
+      <c r="AE1" s="245"/>
+      <c r="AF1" s="245"/>
+      <c r="AG1" s="245"/>
+      <c r="AH1" s="245"/>
+      <c r="AI1" s="245"/>
+      <c r="AJ1" s="245"/>
+      <c r="AK1" s="245"/>
+      <c r="AL1" s="245"/>
+      <c r="AM1" s="245"/>
+      <c r="AN1" s="245"/>
+      <c r="AO1" s="245"/>
+      <c r="AP1" s="245"/>
+      <c r="AQ1" s="245"/>
+      <c r="AR1" s="245"/>
+      <c r="AS1" s="245"/>
+      <c r="AT1" s="245"/>
+      <c r="AU1" s="245"/>
+      <c r="AV1" s="245"/>
+      <c r="AW1" s="245"/>
+      <c r="AX1" s="245"/>
+      <c r="AY1" s="245"/>
     </row>
-    <row r="2" spans="2:52" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:52" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5771,7 +5890,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:52">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -5926,7 +6045,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:52">
       <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
@@ -6081,7 +6200,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:52">
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -6236,7 +6355,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:52">
       <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
@@ -6391,7 +6510,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:52">
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -6546,7 +6665,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:52">
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -6701,7 +6820,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:52">
       <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
@@ -6856,7 +6975,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:52">
       <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
@@ -7011,7 +7130,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:52">
       <c r="B11" s="99" t="s">
         <v>2</v>
       </c>
@@ -7166,7 +7285,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:52">
       <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
@@ -7321,7 +7440,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:52">
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -7476,7 +7595,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:52">
       <c r="B14" s="26" t="s">
         <v>2</v>
       </c>
@@ -7632,7 +7751,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:52">
       <c r="B15" s="27" t="s">
         <v>2</v>
       </c>
@@ -7787,7 +7906,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:52">
       <c r="B16" s="27" t="s">
         <v>2</v>
       </c>
@@ -7942,7 +8061,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:52" ht="16.5" thickBot="1">
       <c r="B17" s="118" t="s">
         <v>2</v>
       </c>
@@ -8097,7 +8216,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:52" ht="16.5" thickTop="1">
       <c r="B18" s="41" t="s">
         <v>2</v>
       </c>
@@ -8252,7 +8371,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:52">
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -8407,7 +8526,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:52">
       <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
@@ -8562,7 +8681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:52">
       <c r="B21" s="27" t="s">
         <v>2</v>
       </c>
@@ -8717,7 +8836,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:52">
       <c r="B22" s="27" t="s">
         <v>2</v>
       </c>
@@ -8870,7 +8989,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:52">
       <c r="B23" s="27" t="s">
         <v>2</v>
       </c>
@@ -9023,7 +9142,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:52">
       <c r="B24" s="27" t="s">
         <v>2</v>
       </c>
@@ -9174,7 +9293,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:52">
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -9329,7 +9448,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:52">
       <c r="B26" s="27" t="s">
         <v>2</v>
       </c>
@@ -9480,7 +9599,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:52">
       <c r="B27" s="27" t="s">
         <v>2</v>
       </c>
@@ -9635,7 +9754,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:52">
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -9772,7 +9891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:52">
       <c r="B29" s="27" t="s">
         <v>2</v>
       </c>
@@ -9919,7 +10038,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:52">
       <c r="B30" s="26" t="s">
         <v>2</v>
       </c>
@@ -10066,7 +10185,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:52">
       <c r="B31" s="26" t="s">
         <v>2</v>
       </c>
@@ -10209,7 +10328,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:52">
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
@@ -10358,7 +10477,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:52">
       <c r="B33" s="26" t="s">
         <v>2</v>
       </c>
@@ -10501,7 +10620,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:52">
       <c r="B34" s="67" t="s">
         <v>2</v>
       </c>
@@ -10644,7 +10763,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:52">
       <c r="B35" s="81" t="s">
         <v>2</v>
       </c>
@@ -10787,7 +10906,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:52">
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
@@ -10940,7 +11059,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:52">
       <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
@@ -11093,7 +11212,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:52">
       <c r="B38" s="26" t="s">
         <v>2</v>
       </c>
@@ -11240,7 +11359,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:52">
       <c r="B39" s="26" t="s">
         <v>2</v>
       </c>
@@ -11383,7 +11502,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:52" ht="16.5" thickBot="1">
       <c r="B40" s="67" t="s">
         <v>2</v>
       </c>
@@ -11530,7 +11649,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:52" ht="16.5" thickTop="1">
       <c r="B41" s="138" t="s">
         <v>2</v>
       </c>
@@ -11673,7 +11792,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:52">
       <c r="B42" s="26" t="s">
         <v>2</v>
       </c>
@@ -11822,7 +11941,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:52">
       <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
@@ -11971,7 +12090,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:52">
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
@@ -12122,7 +12241,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:52">
       <c r="B45" s="26" t="s">
         <v>2</v>
       </c>
@@ -12269,11 +12388,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:52">
       <c r="B46" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="216" t="s">
+      <c r="C46" s="215" t="s">
         <v>199</v>
       </c>
       <c r="D46" s="55" t="s">
@@ -12416,14 +12535,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B47" s="214" t="s">
+    <row r="47" spans="2:52">
+      <c r="B47" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="217" t="s">
+      <c r="C47" s="216" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="224" t="s">
+      <c r="D47" s="223" t="s">
         <v>127</v>
       </c>
       <c r="E47" s="81" t="s">
@@ -12474,7 +12593,7 @@
       <c r="T47" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="U47" s="232">
+      <c r="U47" s="231">
         <v>-1</v>
       </c>
       <c r="V47" s="88" t="s">
@@ -12495,7 +12614,7 @@
       <c r="AA47" s="90">
         <v>10</v>
       </c>
-      <c r="AB47" s="234" t="s">
+      <c r="AB47" s="233" t="s">
         <v>127</v>
       </c>
       <c r="AC47" s="91" t="s">
@@ -12516,10 +12635,10 @@
       <c r="AH47" s="13">
         <v>2</v>
       </c>
-      <c r="AI47" s="235" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ47" s="235" t="s">
+      <c r="AI47" s="234" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ47" s="234" t="s">
         <v>127</v>
       </c>
       <c r="AK47" s="92" t="s">
@@ -12546,7 +12665,7 @@
       <c r="AR47" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="AS47" s="235" t="s">
+      <c r="AS47" s="234" t="s">
         <v>127</v>
       </c>
       <c r="AT47" s="92" t="s">
@@ -12571,7 +12690,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:52">
       <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
@@ -12714,7 +12833,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:52">
       <c r="B49" s="26" t="s">
         <v>2</v>
       </c>
@@ -12863,7 +12982,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:52">
       <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
@@ -13006,7 +13125,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:52">
       <c r="B51" s="26" t="s">
         <v>2</v>
       </c>
@@ -13153,7 +13272,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:52" ht="16.5" thickBot="1">
       <c r="B52" s="67" t="s">
         <v>2</v>
       </c>
@@ -13300,14 +13419,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="215" t="s">
+    <row r="53" spans="2:52" ht="16.5" thickTop="1">
+      <c r="B53" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="220" t="s">
+      <c r="C53" s="219" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="225" t="s">
+      <c r="D53" s="224" t="s">
         <v>127</v>
       </c>
       <c r="E53" s="138" t="s">
@@ -13455,7 +13574,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:52">
       <c r="B54" s="27" t="s">
         <v>2</v>
       </c>
@@ -13610,7 +13729,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:52">
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
@@ -13765,11 +13884,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:52">
       <c r="B56" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="221" t="s">
+      <c r="C56" s="220" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="25" t="s">
@@ -13823,7 +13942,7 @@
       <c r="T56" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="U56" s="232" t="s">
+      <c r="U56" s="231" t="s">
         <v>301</v>
       </c>
       <c r="V56" s="36" t="s">
@@ -13920,11 +14039,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1">
       <c r="B57" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="219" t="s">
+      <c r="C57" s="218" t="s">
         <v>212</v>
       </c>
       <c r="D57" s="192" t="s">
@@ -13948,16 +14067,16 @@
       <c r="J57" s="194">
         <v>250</v>
       </c>
-      <c r="K57" s="226" t="s">
-        <v>127</v>
-      </c>
-      <c r="L57" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="M57" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="N57" s="228" t="s">
+      <c r="K57" s="225" t="s">
+        <v>127</v>
+      </c>
+      <c r="L57" s="227" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" s="227" t="s">
+        <v>127</v>
+      </c>
+      <c r="N57" s="227" t="s">
         <v>127</v>
       </c>
       <c r="O57" s="195" t="s">
@@ -14075,11 +14194,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:52">
       <c r="B58" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="223" t="s">
+      <c r="C58" s="222" t="s">
         <v>223</v>
       </c>
       <c r="D58" s="179" t="s">
@@ -14230,11 +14349,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:52">
       <c r="B59" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="222" t="s">
+      <c r="C59" s="221" t="s">
         <v>214</v>
       </c>
       <c r="D59" s="41" t="s">
@@ -14258,25 +14377,25 @@
       <c r="J59" s="43">
         <v>1200</v>
       </c>
-      <c r="K59" s="227" t="s">
-        <v>127</v>
-      </c>
-      <c r="L59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="M59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="N59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="O59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="P59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q59" s="231" t="s">
+      <c r="K59" s="226" t="s">
+        <v>127</v>
+      </c>
+      <c r="L59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="M59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="N59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="O59" s="230" t="s">
+        <v>127</v>
+      </c>
+      <c r="P59" s="230" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q59" s="230" t="s">
         <v>127</v>
       </c>
       <c r="R59" s="46">
@@ -14385,7 +14504,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:52" ht="16.5" thickBot="1">
       <c r="B60" s="67" t="s">
         <v>2</v>
       </c>
@@ -14538,11 +14657,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:52">
       <c r="B61" s="158" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="218" t="s">
+      <c r="C61" s="217" t="s">
         <v>200</v>
       </c>
       <c r="D61" s="158" t="s">
@@ -14575,7 +14694,7 @@
       <c r="M61" s="161">
         <v>100</v>
       </c>
-      <c r="N61" s="230" t="s">
+      <c r="N61" s="229" t="s">
         <v>127</v>
       </c>
       <c r="O61" s="162" t="s">
@@ -14596,7 +14715,7 @@
       <c r="T61" s="164" t="s">
         <v>311</v>
       </c>
-      <c r="U61" s="233">
+      <c r="U61" s="232">
         <v>-1</v>
       </c>
       <c r="V61" s="165" t="s">
@@ -14693,7 +14812,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:52">
       <c r="B62" s="26" t="s">
         <v>2</v>
       </c>
@@ -14848,7 +14967,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:52">
       <c r="B63" s="26" t="s">
         <v>2</v>
       </c>
@@ -15003,7 +15122,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:52">
       <c r="B64" s="26" t="s">
         <v>2</v>
       </c>
@@ -15158,7 +15277,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:52">
       <c r="B65" s="26" t="s">
         <v>2</v>
       </c>
@@ -15313,7 +15432,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:52">
       <c r="B66" s="26" t="s">
         <v>2</v>
       </c>
@@ -15468,7 +15587,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:52">
       <c r="B67" s="26" t="s">
         <v>2</v>
       </c>
@@ -15623,7 +15742,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:52">
       <c r="B68" s="26" t="s">
         <v>2</v>
       </c>
@@ -15778,7 +15897,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:52">
       <c r="B69" s="26" t="s">
         <v>2</v>
       </c>
@@ -15931,7 +16050,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:52">
       <c r="B70" s="26" t="s">
         <v>2</v>
       </c>
@@ -16086,7 +16205,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:52">
       <c r="B71" s="27" t="s">
         <v>2</v>
       </c>
@@ -16241,7 +16360,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:52">
       <c r="B72" s="27" t="s">
         <v>2</v>
       </c>
@@ -16394,7 +16513,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:52">
       <c r="B73" s="27" t="s">
         <v>2</v>
       </c>
@@ -16549,7 +16668,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:52">
       <c r="B74" s="27" t="s">
         <v>2</v>
       </c>
@@ -16700,7 +16819,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:52">
       <c r="B75" s="27" t="s">
         <v>2</v>
       </c>
@@ -16855,7 +16974,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:52">
       <c r="B76" s="27" t="s">
         <v>2</v>
       </c>
@@ -17010,838 +17129,993 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B77" s="27" t="s">
+    <row r="77" spans="2:52">
+      <c r="B77" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="212" t="s">
+      <c r="C77" s="247" t="s">
         <v>324</v>
       </c>
-      <c r="D77" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E77" s="211" t="s">
+      <c r="D77" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F77" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="69">
-        <v>1</v>
-      </c>
-      <c r="H77" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I77" s="30" t="s">
+      <c r="F77" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="248">
+        <v>1</v>
+      </c>
+      <c r="H77" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I77" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="J77" s="30">
-        <v>1</v>
-      </c>
-      <c r="K77" s="30" t="s">
+      <c r="J77" s="249">
+        <v>1</v>
+      </c>
+      <c r="K77" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="L77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R77" s="33">
+      <c r="L77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R77" s="252">
         <v>-25</v>
       </c>
-      <c r="S77" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T77" s="47" t="s">
+      <c r="S77" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T77" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U77" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V77" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W77" s="242" t="s">
+      <c r="U77" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V77" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W77" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X77" s="21" t="b">
+      <c r="X77" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y77" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z77" s="21" t="s">
+      <c r="Y77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z77" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA77" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB77" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC77" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD77" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE77" s="13" t="s">
+      <c r="AA77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB77" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC77" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD77" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE77" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH77" s="13">
+      <c r="AF77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH77" s="260">
         <v>2</v>
       </c>
-      <c r="AI77" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ77" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS77" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW77" s="20" t="s">
+      <c r="AI77" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS77" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW77" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ77" s="13" t="s">
+      <c r="AX77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ77" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B78" s="27" t="s">
+    <row r="78" spans="2:52">
+      <c r="B78" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="212" t="s">
+      <c r="C78" s="247" t="s">
         <v>326</v>
       </c>
-      <c r="D78" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E78" s="211" t="s">
+      <c r="D78" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E78" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="69">
+      <c r="F78" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="248">
         <v>-1</v>
       </c>
-      <c r="H78" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I78" s="30" t="s">
+      <c r="H78" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I78" s="249" t="s">
         <v>12</v>
       </c>
-      <c r="J78" s="30">
+      <c r="J78" s="249">
         <v>1000</v>
       </c>
-      <c r="K78" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R78" s="33">
+      <c r="K78" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="L78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R78" s="252">
         <v>-25</v>
       </c>
-      <c r="S78" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T78" s="47" t="s">
+      <c r="S78" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T78" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U78" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V78" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W78" s="242" t="s">
+      <c r="U78" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V78" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W78" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X78" s="21" t="b">
+      <c r="X78" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y78" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z78" s="21" t="s">
+      <c r="Y78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z78" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA78" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB78" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC78" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD78" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE78" s="13" t="s">
+      <c r="AA78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB78" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC78" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD78" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE78" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH78" s="13">
+      <c r="AF78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH78" s="260">
         <v>2</v>
       </c>
-      <c r="AI78" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ78" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS78" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW78" s="20" t="s">
+      <c r="AI78" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS78" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW78" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ78" s="13" t="s">
+      <c r="AX78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ78" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B79" s="27" t="s">
+    <row r="79" spans="2:52">
+      <c r="B79" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="212" t="s">
+      <c r="C79" s="247" t="s">
         <v>327</v>
       </c>
-      <c r="D79" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E79" s="211" t="s">
+      <c r="D79" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E79" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F79" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79" s="69">
+      <c r="F79" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="248">
         <v>-1</v>
       </c>
-      <c r="H79" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I79" s="30" t="s">
+      <c r="H79" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I79" s="249" t="s">
         <v>10</v>
       </c>
-      <c r="J79" s="30">
+      <c r="J79" s="249">
         <v>2</v>
       </c>
-      <c r="K79" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R79" s="33">
+      <c r="K79" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="L79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R79" s="252">
         <v>-25</v>
       </c>
-      <c r="S79" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T79" s="47" t="s">
+      <c r="S79" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T79" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U79" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V79" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W79" s="242" t="s">
+      <c r="U79" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V79" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W79" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X79" s="21" t="b">
+      <c r="X79" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y79" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z79" s="21" t="s">
+      <c r="Y79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z79" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA79" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB79" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC79" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD79" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE79" s="13" t="s">
+      <c r="AA79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB79" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC79" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD79" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE79" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH79" s="13">
+      <c r="AF79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH79" s="260">
         <v>2</v>
       </c>
-      <c r="AI79" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ79" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS79" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW79" s="20" t="s">
+      <c r="AI79" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS79" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW79" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ79" s="13" t="s">
+      <c r="AX79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ79" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B80" s="27" t="s">
+    <row r="80" spans="2:52">
+      <c r="B80" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="212" t="s">
+      <c r="C80" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="D80" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E80" s="211" t="s">
+      <c r="D80" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E80" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F80" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G80" s="69">
+      <c r="F80" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="248">
         <v>-1</v>
       </c>
-      <c r="H80" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I80" s="30" t="s">
+      <c r="H80" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I80" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="J80" s="30">
-        <v>1</v>
-      </c>
-      <c r="K80" s="30" t="s">
+      <c r="J80" s="249">
+        <v>1</v>
+      </c>
+      <c r="K80" s="249" t="s">
         <v>163</v>
       </c>
-      <c r="L80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R80" s="33">
+      <c r="L80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R80" s="252">
         <v>-25</v>
       </c>
-      <c r="S80" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T80" s="47" t="s">
+      <c r="S80" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T80" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U80" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V80" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W80" s="242" t="s">
+      <c r="U80" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V80" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W80" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X80" s="21" t="b">
+      <c r="X80" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y80" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z80" s="21" t="s">
+      <c r="Y80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z80" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA80" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB80" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC80" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD80" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE80" s="13" t="s">
+      <c r="AA80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB80" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC80" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD80" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE80" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH80" s="13">
+      <c r="AF80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH80" s="260">
         <v>2</v>
       </c>
-      <c r="AI80" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ80" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS80" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW80" s="20" t="s">
+      <c r="AI80" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS80" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW80" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ80" s="13" t="s">
+      <c r="AX80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ80" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B81" s="27" t="s">
+    <row r="81" spans="2:52">
+      <c r="B81" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="212" t="s">
+      <c r="C81" s="264" t="s">
         <v>329</v>
       </c>
-      <c r="D81" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E81" s="211" t="s">
+      <c r="D81" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="E81" s="263" t="s">
         <v>312</v>
       </c>
-      <c r="F81" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="69">
+      <c r="F81" s="265" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" s="265">
         <v>-1</v>
       </c>
-      <c r="H81" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I81" s="30" t="s">
+      <c r="H81" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="I81" s="266" t="s">
         <v>12</v>
       </c>
-      <c r="J81" s="30">
+      <c r="J81" s="266">
         <v>2000</v>
       </c>
-      <c r="K81" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R81" s="33">
+      <c r="K81" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="L81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="M81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="N81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="O81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="P81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="R81" s="269">
         <v>-25</v>
       </c>
-      <c r="S81" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T81" s="47" t="s">
+      <c r="S81" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="T81" s="270" t="s">
         <v>322</v>
       </c>
-      <c r="U81" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V81" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W81" s="242" t="s">
+      <c r="U81" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="V81" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="W81" s="273" t="s">
         <v>325</v>
       </c>
-      <c r="X81" s="21" t="b">
+      <c r="X81" s="274" t="b">
         <v>0</v>
       </c>
-      <c r="Y81" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z81" s="21" t="s">
+      <c r="Y81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z81" s="274" t="s">
         <v>16</v>
       </c>
-      <c r="AA81" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB81" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC81" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD81" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE81" s="13" t="s">
+      <c r="AA81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB81" s="275" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC81" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD81" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE81" s="277" t="s">
         <v>321</v>
       </c>
-      <c r="AF81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH81" s="13">
+      <c r="AF81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH81" s="277">
         <v>2</v>
       </c>
-      <c r="AI81" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ81" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS81" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW81" s="20" t="s">
+      <c r="AI81" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS81" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW81" s="279" t="s">
         <v>340</v>
       </c>
-      <c r="AX81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ81" s="13" t="s">
+      <c r="AX81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ81" s="277" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="2:52" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B84" s="248" t="s">
+    <row r="82" spans="2:52">
+      <c r="B82" s="263" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="264" t="s">
+        <v>341</v>
+      </c>
+      <c r="D82" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="E82" s="263" t="s">
+        <v>342</v>
+      </c>
+      <c r="F82" s="265" t="b">
+        <v>1</v>
+      </c>
+      <c r="G82" s="265">
+        <v>1</v>
+      </c>
+      <c r="H82" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="I82" s="266" t="s">
+        <v>342</v>
+      </c>
+      <c r="J82" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="K82" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="L82" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="M82" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="N82" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="O82" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="P82" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q82" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="R82" s="269">
+        <v>100</v>
+      </c>
+      <c r="S82" s="270" t="s">
+        <v>343</v>
+      </c>
+      <c r="T82" s="270" t="s">
+        <v>311</v>
+      </c>
+      <c r="U82" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="V82" s="272" t="s">
+        <v>344</v>
+      </c>
+      <c r="W82" s="273" t="s">
+        <v>345</v>
+      </c>
+      <c r="X82" s="274" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z82" s="274" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA82" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB82" s="275" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC82" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD82" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE82" s="277" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH82" s="277">
+        <v>1</v>
+      </c>
+      <c r="AI82" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS82" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY82" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ82" s="277" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="2:52" ht="26.25">
+      <c r="B85" s="246" t="s">
         <v>330</v>
       </c>
-      <c r="C84" s="248"/>
-      <c r="D84" s="248"/>
-      <c r="E84" s="248"/>
+      <c r="C85" s="246"/>
+      <c r="D85" s="246"/>
+      <c r="E85" s="246"/>
     </row>
-    <row r="86" spans="2:52" ht="135" x14ac:dyDescent="0.25">
-      <c r="B86" s="23" t="s">
+    <row r="87" spans="2:52" ht="135">
+      <c r="B87" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="C86" s="243" t="s">
+      <c r="C87" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="D86" s="244" t="s">
+      <c r="D87" s="242" t="s">
         <v>52</v>
       </c>
-      <c r="E86" s="23" t="s">
+      <c r="E87" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="F86" s="244" t="s">
+      <c r="F87" s="242" t="s">
         <v>333</v>
       </c>
-      <c r="G86" s="245" t="s">
+      <c r="G87" s="243" t="s">
         <v>334</v>
       </c>
-      <c r="H86" s="245" t="s">
+      <c r="H87" s="243" t="s">
         <v>335</v>
       </c>
-      <c r="I86" s="245" t="s">
+      <c r="I87" s="243" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="87" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B87" s="211" t="s">
+    <row r="88" spans="2:52">
+      <c r="B88" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="211" t="s">
+      <c r="C88" s="211" t="s">
         <v>337</v>
       </c>
-      <c r="D87" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="211">
+      <c r="D88" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="211">
         <v>0</v>
       </c>
-      <c r="F87" s="211">
+      <c r="F88" s="211">
         <v>120</v>
       </c>
-      <c r="G87" s="211">
-        <v>1</v>
-      </c>
-      <c r="H87" s="211" t="s">
+      <c r="G88" s="211">
+        <v>1</v>
+      </c>
+      <c r="H88" s="211" t="s">
         <v>338</v>
       </c>
-      <c r="I87" s="211" t="s">
+      <c r="I88" s="211" t="s">
         <v>339</v>
       </c>
     </row>
@@ -17849,22 +18123,22 @@
   <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
-    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F81">
-    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="F3:F82">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",D87)))</formula>
+  <conditionalFormatting sqref="D88">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",D87)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17884,7 +18158,7 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
@@ -17925,39 +18199,39 @@
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="10" customFormat="1">
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="246"/>
-      <c r="AB1" s="246"/>
+      <c r="AA1" s="244"/>
+      <c r="AB1" s="244"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="247"/>
-      <c r="AE1" s="247"/>
-      <c r="AF1" s="247"/>
-      <c r="AG1" s="247"/>
-      <c r="AH1" s="247"/>
-      <c r="AI1" s="247"/>
-      <c r="AJ1" s="247"/>
-      <c r="AK1" s="247"/>
-      <c r="AL1" s="247"/>
-      <c r="AM1" s="247"/>
-      <c r="AN1" s="247"/>
-      <c r="AO1" s="247"/>
-      <c r="AP1" s="247"/>
-      <c r="AQ1" s="247"/>
-      <c r="AR1" s="247"/>
-      <c r="AS1" s="247"/>
-      <c r="AT1" s="247"/>
-      <c r="AU1" s="247"/>
-      <c r="AV1" s="247"/>
-      <c r="AW1" s="247"/>
-      <c r="AX1" s="247"/>
-      <c r="AY1" s="247"/>
+      <c r="AD1" s="245"/>
+      <c r="AE1" s="245"/>
+      <c r="AF1" s="245"/>
+      <c r="AG1" s="245"/>
+      <c r="AH1" s="245"/>
+      <c r="AI1" s="245"/>
+      <c r="AJ1" s="245"/>
+      <c r="AK1" s="245"/>
+      <c r="AL1" s="245"/>
+      <c r="AM1" s="245"/>
+      <c r="AN1" s="245"/>
+      <c r="AO1" s="245"/>
+      <c r="AP1" s="245"/>
+      <c r="AQ1" s="245"/>
+      <c r="AR1" s="245"/>
+      <c r="AS1" s="245"/>
+      <c r="AT1" s="245"/>
+      <c r="AU1" s="245"/>
+      <c r="AV1" s="245"/>
+      <c r="AW1" s="245"/>
+      <c r="AX1" s="245"/>
+      <c r="AY1" s="245"/>
     </row>
-    <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:51" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>313</v>
       </c>
@@ -17976,15 +18250,15 @@
       <c r="G2" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="H2" s="239" t="s">
+      <c r="H2" s="238" t="s">
         <v>319</v>
       </c>
-      <c r="I2" s="240" t="s">
+      <c r="I2" s="239" t="s">
         <v>320</v>
       </c>
-      <c r="J2" s="241"/>
+      <c r="J2" s="240"/>
     </row>
-    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:51">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -18003,197 +18277,197 @@
       <c r="G3" s="26">
         <v>2</v>
       </c>
-      <c r="H3" s="237">
+      <c r="H3" s="236">
         <v>360</v>
       </c>
-      <c r="I3" s="238" t="s">
+      <c r="I3" s="237" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="236"/>
-      <c r="B57" s="236"/>
-      <c r="C57" s="236"/>
-      <c r="D57" s="236"/>
-      <c r="E57" s="236"/>
-      <c r="F57" s="236"/>
-      <c r="G57" s="236"/>
-      <c r="H57" s="236"/>
-      <c r="I57" s="236"/>
-      <c r="J57" s="236"/>
-      <c r="K57" s="236"/>
-      <c r="L57" s="236"/>
-      <c r="M57" s="236"/>
-      <c r="N57" s="236"/>
-      <c r="O57" s="236"/>
-      <c r="P57" s="236"/>
-      <c r="Q57" s="236"/>
-      <c r="R57" s="236"/>
-      <c r="S57" s="236"/>
-      <c r="T57" s="236"/>
-      <c r="U57" s="236"/>
-      <c r="V57" s="236"/>
-      <c r="W57" s="236"/>
-      <c r="X57" s="236"/>
-      <c r="Y57" s="236"/>
-      <c r="Z57" s="236"/>
-      <c r="AA57" s="236"/>
-      <c r="AB57" s="236"/>
-      <c r="AC57" s="236"/>
-      <c r="AD57" s="236"/>
-      <c r="AE57" s="236"/>
-      <c r="AF57" s="236"/>
-      <c r="AG57" s="236"/>
-      <c r="AH57" s="236"/>
-      <c r="AI57" s="236"/>
-      <c r="AJ57" s="236"/>
-      <c r="AK57" s="236"/>
-      <c r="AL57" s="236"/>
-      <c r="AM57" s="236"/>
-      <c r="AN57" s="236"/>
-      <c r="AO57" s="236"/>
-      <c r="AP57" s="236"/>
-      <c r="AQ57" s="236"/>
-      <c r="AR57" s="236"/>
-      <c r="AS57" s="236"/>
-      <c r="AT57" s="236"/>
-      <c r="AU57" s="236"/>
-      <c r="AV57" s="236"/>
-      <c r="AW57" s="236"/>
-      <c r="AX57" s="236"/>
-      <c r="AY57" s="236"/>
-      <c r="AZ57" s="236"/>
-      <c r="BA57" s="236"/>
-      <c r="BB57" s="236"/>
-      <c r="BC57" s="236"/>
-      <c r="BD57" s="236"/>
-      <c r="BE57" s="236"/>
-      <c r="BF57" s="236"/>
-      <c r="BG57" s="236"/>
-      <c r="BH57" s="236"/>
-      <c r="BI57" s="236"/>
-      <c r="BJ57" s="236"/>
-      <c r="BK57" s="236"/>
-      <c r="BL57" s="236"/>
-      <c r="BM57" s="236"/>
-      <c r="BN57" s="236"/>
-      <c r="BO57" s="236"/>
-      <c r="BP57" s="236"/>
-      <c r="BQ57" s="236"/>
-      <c r="BR57" s="236"/>
-      <c r="BS57" s="236"/>
-      <c r="BT57" s="236"/>
-      <c r="BU57" s="236"/>
-      <c r="BV57" s="236"/>
-      <c r="BW57" s="236"/>
-      <c r="BX57" s="236"/>
-      <c r="BY57" s="236"/>
-      <c r="BZ57" s="236"/>
-      <c r="CA57" s="236"/>
-      <c r="CB57" s="236"/>
-      <c r="CC57" s="236"/>
-      <c r="CD57" s="236"/>
-      <c r="CE57" s="236"/>
-      <c r="CF57" s="236"/>
-      <c r="CG57" s="236"/>
-      <c r="CH57" s="236"/>
-      <c r="CI57" s="236"/>
-      <c r="CJ57" s="236"/>
-      <c r="CK57" s="236"/>
-      <c r="CL57" s="236"/>
-      <c r="CM57" s="236"/>
-      <c r="CN57" s="236"/>
-      <c r="CO57" s="236"/>
-      <c r="CP57" s="236"/>
-      <c r="CQ57" s="236"/>
-      <c r="CR57" s="236"/>
-      <c r="CS57" s="236"/>
-      <c r="CT57" s="236"/>
-      <c r="CU57" s="236"/>
-      <c r="CV57" s="236"/>
-      <c r="CW57" s="236"/>
-      <c r="CX57" s="236"/>
-      <c r="CY57" s="236"/>
-      <c r="CZ57" s="236"/>
-      <c r="DA57" s="236"/>
-      <c r="DB57" s="236"/>
-      <c r="DC57" s="236"/>
-      <c r="DD57" s="236"/>
-      <c r="DE57" s="236"/>
-      <c r="DF57" s="236"/>
-      <c r="DG57" s="236"/>
-      <c r="DH57" s="236"/>
-      <c r="DI57" s="236"/>
-      <c r="DJ57" s="236"/>
-      <c r="DK57" s="236"/>
-      <c r="DL57" s="236"/>
-      <c r="DM57" s="236"/>
-      <c r="DN57" s="236"/>
-      <c r="DO57" s="236"/>
-      <c r="DP57" s="236"/>
-      <c r="DQ57" s="236"/>
-      <c r="DR57" s="236"/>
-      <c r="DS57" s="236"/>
-      <c r="DT57" s="236"/>
-      <c r="DU57" s="236"/>
-      <c r="DV57" s="236"/>
-      <c r="DW57" s="236"/>
-      <c r="DX57" s="236"/>
-      <c r="DY57" s="236"/>
-      <c r="DZ57" s="236"/>
-      <c r="EA57" s="236"/>
-      <c r="EB57" s="236"/>
-      <c r="EC57" s="236"/>
-      <c r="ED57" s="236"/>
-      <c r="EE57" s="236"/>
-      <c r="EF57" s="236"/>
-      <c r="EG57" s="236"/>
-      <c r="EH57" s="236"/>
-      <c r="EI57" s="236"/>
-      <c r="EJ57" s="236"/>
-      <c r="EK57" s="236"/>
-      <c r="EL57" s="236"/>
-      <c r="EM57" s="236"/>
-      <c r="EN57" s="236"/>
-      <c r="EO57" s="236"/>
-      <c r="EP57" s="236"/>
-      <c r="EQ57" s="236"/>
-      <c r="ER57" s="236"/>
-      <c r="ES57" s="236"/>
-      <c r="ET57" s="236"/>
-      <c r="EU57" s="236"/>
-      <c r="EV57" s="236"/>
-      <c r="EW57" s="236"/>
-      <c r="EX57" s="236"/>
-      <c r="EY57" s="236"/>
-      <c r="EZ57" s="236"/>
-      <c r="FA57" s="236"/>
-      <c r="FB57" s="236"/>
-      <c r="FC57" s="236"/>
-      <c r="FD57" s="236"/>
-      <c r="FE57" s="236"/>
-      <c r="FF57" s="236"/>
-      <c r="FG57" s="236"/>
-      <c r="FH57" s="236"/>
-      <c r="FI57" s="236"/>
-      <c r="FJ57" s="236"/>
-      <c r="FK57" s="236"/>
-      <c r="FL57" s="236"/>
-      <c r="FM57" s="236"/>
-      <c r="FN57" s="236"/>
-      <c r="FO57" s="236"/>
-      <c r="FP57" s="236"/>
-      <c r="FQ57" s="236"/>
-      <c r="FR57" s="236"/>
-      <c r="FS57" s="236"/>
-      <c r="FT57" s="236"/>
-      <c r="FU57" s="236"/>
-      <c r="FV57" s="236"/>
-      <c r="FW57" s="236"/>
-      <c r="FX57" s="236"/>
-      <c r="FY57" s="236"/>
-      <c r="FZ57" s="236"/>
-      <c r="GA57" s="236"/>
+    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A57" s="235"/>
+      <c r="B57" s="235"/>
+      <c r="C57" s="235"/>
+      <c r="D57" s="235"/>
+      <c r="E57" s="235"/>
+      <c r="F57" s="235"/>
+      <c r="G57" s="235"/>
+      <c r="H57" s="235"/>
+      <c r="I57" s="235"/>
+      <c r="J57" s="235"/>
+      <c r="K57" s="235"/>
+      <c r="L57" s="235"/>
+      <c r="M57" s="235"/>
+      <c r="N57" s="235"/>
+      <c r="O57" s="235"/>
+      <c r="P57" s="235"/>
+      <c r="Q57" s="235"/>
+      <c r="R57" s="235"/>
+      <c r="S57" s="235"/>
+      <c r="T57" s="235"/>
+      <c r="U57" s="235"/>
+      <c r="V57" s="235"/>
+      <c r="W57" s="235"/>
+      <c r="X57" s="235"/>
+      <c r="Y57" s="235"/>
+      <c r="Z57" s="235"/>
+      <c r="AA57" s="235"/>
+      <c r="AB57" s="235"/>
+      <c r="AC57" s="235"/>
+      <c r="AD57" s="235"/>
+      <c r="AE57" s="235"/>
+      <c r="AF57" s="235"/>
+      <c r="AG57" s="235"/>
+      <c r="AH57" s="235"/>
+      <c r="AI57" s="235"/>
+      <c r="AJ57" s="235"/>
+      <c r="AK57" s="235"/>
+      <c r="AL57" s="235"/>
+      <c r="AM57" s="235"/>
+      <c r="AN57" s="235"/>
+      <c r="AO57" s="235"/>
+      <c r="AP57" s="235"/>
+      <c r="AQ57" s="235"/>
+      <c r="AR57" s="235"/>
+      <c r="AS57" s="235"/>
+      <c r="AT57" s="235"/>
+      <c r="AU57" s="235"/>
+      <c r="AV57" s="235"/>
+      <c r="AW57" s="235"/>
+      <c r="AX57" s="235"/>
+      <c r="AY57" s="235"/>
+      <c r="AZ57" s="235"/>
+      <c r="BA57" s="235"/>
+      <c r="BB57" s="235"/>
+      <c r="BC57" s="235"/>
+      <c r="BD57" s="235"/>
+      <c r="BE57" s="235"/>
+      <c r="BF57" s="235"/>
+      <c r="BG57" s="235"/>
+      <c r="BH57" s="235"/>
+      <c r="BI57" s="235"/>
+      <c r="BJ57" s="235"/>
+      <c r="BK57" s="235"/>
+      <c r="BL57" s="235"/>
+      <c r="BM57" s="235"/>
+      <c r="BN57" s="235"/>
+      <c r="BO57" s="235"/>
+      <c r="BP57" s="235"/>
+      <c r="BQ57" s="235"/>
+      <c r="BR57" s="235"/>
+      <c r="BS57" s="235"/>
+      <c r="BT57" s="235"/>
+      <c r="BU57" s="235"/>
+      <c r="BV57" s="235"/>
+      <c r="BW57" s="235"/>
+      <c r="BX57" s="235"/>
+      <c r="BY57" s="235"/>
+      <c r="BZ57" s="235"/>
+      <c r="CA57" s="235"/>
+      <c r="CB57" s="235"/>
+      <c r="CC57" s="235"/>
+      <c r="CD57" s="235"/>
+      <c r="CE57" s="235"/>
+      <c r="CF57" s="235"/>
+      <c r="CG57" s="235"/>
+      <c r="CH57" s="235"/>
+      <c r="CI57" s="235"/>
+      <c r="CJ57" s="235"/>
+      <c r="CK57" s="235"/>
+      <c r="CL57" s="235"/>
+      <c r="CM57" s="235"/>
+      <c r="CN57" s="235"/>
+      <c r="CO57" s="235"/>
+      <c r="CP57" s="235"/>
+      <c r="CQ57" s="235"/>
+      <c r="CR57" s="235"/>
+      <c r="CS57" s="235"/>
+      <c r="CT57" s="235"/>
+      <c r="CU57" s="235"/>
+      <c r="CV57" s="235"/>
+      <c r="CW57" s="235"/>
+      <c r="CX57" s="235"/>
+      <c r="CY57" s="235"/>
+      <c r="CZ57" s="235"/>
+      <c r="DA57" s="235"/>
+      <c r="DB57" s="235"/>
+      <c r="DC57" s="235"/>
+      <c r="DD57" s="235"/>
+      <c r="DE57" s="235"/>
+      <c r="DF57" s="235"/>
+      <c r="DG57" s="235"/>
+      <c r="DH57" s="235"/>
+      <c r="DI57" s="235"/>
+      <c r="DJ57" s="235"/>
+      <c r="DK57" s="235"/>
+      <c r="DL57" s="235"/>
+      <c r="DM57" s="235"/>
+      <c r="DN57" s="235"/>
+      <c r="DO57" s="235"/>
+      <c r="DP57" s="235"/>
+      <c r="DQ57" s="235"/>
+      <c r="DR57" s="235"/>
+      <c r="DS57" s="235"/>
+      <c r="DT57" s="235"/>
+      <c r="DU57" s="235"/>
+      <c r="DV57" s="235"/>
+      <c r="DW57" s="235"/>
+      <c r="DX57" s="235"/>
+      <c r="DY57" s="235"/>
+      <c r="DZ57" s="235"/>
+      <c r="EA57" s="235"/>
+      <c r="EB57" s="235"/>
+      <c r="EC57" s="235"/>
+      <c r="ED57" s="235"/>
+      <c r="EE57" s="235"/>
+      <c r="EF57" s="235"/>
+      <c r="EG57" s="235"/>
+      <c r="EH57" s="235"/>
+      <c r="EI57" s="235"/>
+      <c r="EJ57" s="235"/>
+      <c r="EK57" s="235"/>
+      <c r="EL57" s="235"/>
+      <c r="EM57" s="235"/>
+      <c r="EN57" s="235"/>
+      <c r="EO57" s="235"/>
+      <c r="EP57" s="235"/>
+      <c r="EQ57" s="235"/>
+      <c r="ER57" s="235"/>
+      <c r="ES57" s="235"/>
+      <c r="ET57" s="235"/>
+      <c r="EU57" s="235"/>
+      <c r="EV57" s="235"/>
+      <c r="EW57" s="235"/>
+      <c r="EX57" s="235"/>
+      <c r="EY57" s="235"/>
+      <c r="EZ57" s="235"/>
+      <c r="FA57" s="235"/>
+      <c r="FB57" s="235"/>
+      <c r="FC57" s="235"/>
+      <c r="FD57" s="235"/>
+      <c r="FE57" s="235"/>
+      <c r="FF57" s="235"/>
+      <c r="FG57" s="235"/>
+      <c r="FH57" s="235"/>
+      <c r="FI57" s="235"/>
+      <c r="FJ57" s="235"/>
+      <c r="FK57" s="235"/>
+      <c r="FL57" s="235"/>
+      <c r="FM57" s="235"/>
+      <c r="FN57" s="235"/>
+      <c r="FO57" s="235"/>
+      <c r="FP57" s="235"/>
+      <c r="FQ57" s="235"/>
+      <c r="FR57" s="235"/>
+      <c r="FS57" s="235"/>
+      <c r="FT57" s="235"/>
+      <c r="FU57" s="235"/>
+      <c r="FV57" s="235"/>
+      <c r="FW57" s="235"/>
+      <c r="FX57" s="235"/>
+      <c r="FY57" s="235"/>
+      <c r="FZ57" s="235"/>
+      <c r="GA57" s="235"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -18216,12 +18490,12 @@
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
@@ -18230,10 +18504,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -18241,7 +18515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -18249,7 +18523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -18257,13 +18531,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -18271,7 +18545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -18279,7 +18553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>127</v>
       </c>
@@ -18287,107 +18561,107 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="D11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="D12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="D14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4">
       <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Free rewards cooldown set to 12h instead of 6h
Former-commit-id: 69a2e6373ea04d6b60c4e023dfcc66c5aa5ca9be
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1056,7 +1056,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1209,6 +1209,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1640,7 +1651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="280">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2270,9 +2281,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2353,9 +2361,6 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -2373,6 +2378,105 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5146,8 +5250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ76" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
-  <autoFilter ref="B2:AZ76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ81" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
+  <autoFilter ref="B2:AZ81"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
@@ -5525,11 +5629,11 @@
   <dimension ref="B1:AZ87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
@@ -5570,7 +5674,7 @@
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:52" s="10" customFormat="1" ht="115.5">
       <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
@@ -5586,37 +5690,37 @@
       <c r="V1" s="210" t="s">
         <v>310</v>
       </c>
-      <c r="AA1" s="246" t="s">
+      <c r="AA1" s="244" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="246"/>
+      <c r="AB1" s="244"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="247" t="s">
+      <c r="AD1" s="245" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="247"/>
-      <c r="AF1" s="247"/>
-      <c r="AG1" s="247"/>
-      <c r="AH1" s="247"/>
-      <c r="AI1" s="247"/>
-      <c r="AJ1" s="247"/>
-      <c r="AK1" s="247"/>
-      <c r="AL1" s="247"/>
-      <c r="AM1" s="247"/>
-      <c r="AN1" s="247"/>
-      <c r="AO1" s="247"/>
-      <c r="AP1" s="247"/>
-      <c r="AQ1" s="247"/>
-      <c r="AR1" s="247"/>
-      <c r="AS1" s="247"/>
-      <c r="AT1" s="247"/>
-      <c r="AU1" s="247"/>
-      <c r="AV1" s="247"/>
-      <c r="AW1" s="247"/>
-      <c r="AX1" s="247"/>
-      <c r="AY1" s="247"/>
+      <c r="AE1" s="245"/>
+      <c r="AF1" s="245"/>
+      <c r="AG1" s="245"/>
+      <c r="AH1" s="245"/>
+      <c r="AI1" s="245"/>
+      <c r="AJ1" s="245"/>
+      <c r="AK1" s="245"/>
+      <c r="AL1" s="245"/>
+      <c r="AM1" s="245"/>
+      <c r="AN1" s="245"/>
+      <c r="AO1" s="245"/>
+      <c r="AP1" s="245"/>
+      <c r="AQ1" s="245"/>
+      <c r="AR1" s="245"/>
+      <c r="AS1" s="245"/>
+      <c r="AT1" s="245"/>
+      <c r="AU1" s="245"/>
+      <c r="AV1" s="245"/>
+      <c r="AW1" s="245"/>
+      <c r="AX1" s="245"/>
+      <c r="AY1" s="245"/>
     </row>
-    <row r="2" spans="2:52" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:52" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5771,7 +5875,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:52">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -5926,7 +6030,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:52">
       <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
@@ -6081,7 +6185,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:52">
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -6236,7 +6340,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:52">
       <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
@@ -6391,7 +6495,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:52">
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -6546,7 +6650,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:52">
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -6701,7 +6805,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:52">
       <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
@@ -6856,7 +6960,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:52">
       <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
@@ -7011,7 +7115,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:52">
       <c r="B11" s="99" t="s">
         <v>2</v>
       </c>
@@ -7166,7 +7270,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:52">
       <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
@@ -7321,7 +7425,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:52">
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -7476,7 +7580,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:52">
       <c r="B14" s="26" t="s">
         <v>2</v>
       </c>
@@ -7632,7 +7736,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:52">
       <c r="B15" s="27" t="s">
         <v>2</v>
       </c>
@@ -7787,7 +7891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:52">
       <c r="B16" s="27" t="s">
         <v>2</v>
       </c>
@@ -7942,7 +8046,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:52" ht="16.5" thickBot="1">
       <c r="B17" s="118" t="s">
         <v>2</v>
       </c>
@@ -8097,7 +8201,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:52" ht="16.5" thickTop="1">
       <c r="B18" s="41" t="s">
         <v>2</v>
       </c>
@@ -8252,7 +8356,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:52">
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -8407,7 +8511,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:52">
       <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
@@ -8562,7 +8666,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:52">
       <c r="B21" s="27" t="s">
         <v>2</v>
       </c>
@@ -8717,7 +8821,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:52">
       <c r="B22" s="27" t="s">
         <v>2</v>
       </c>
@@ -8870,7 +8974,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:52">
       <c r="B23" s="27" t="s">
         <v>2</v>
       </c>
@@ -9023,7 +9127,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:52">
       <c r="B24" s="27" t="s">
         <v>2</v>
       </c>
@@ -9174,7 +9278,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:52">
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -9329,7 +9433,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:52">
       <c r="B26" s="27" t="s">
         <v>2</v>
       </c>
@@ -9480,7 +9584,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:52">
       <c r="B27" s="27" t="s">
         <v>2</v>
       </c>
@@ -9635,7 +9739,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:52">
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -9772,7 +9876,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:52">
       <c r="B29" s="27" t="s">
         <v>2</v>
       </c>
@@ -9919,7 +10023,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:52">
       <c r="B30" s="26" t="s">
         <v>2</v>
       </c>
@@ -10066,7 +10170,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:52">
       <c r="B31" s="26" t="s">
         <v>2</v>
       </c>
@@ -10209,7 +10313,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:52">
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
@@ -10358,7 +10462,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:52">
       <c r="B33" s="26" t="s">
         <v>2</v>
       </c>
@@ -10501,7 +10605,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:52">
       <c r="B34" s="67" t="s">
         <v>2</v>
       </c>
@@ -10644,7 +10748,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:52">
       <c r="B35" s="81" t="s">
         <v>2</v>
       </c>
@@ -10787,7 +10891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:52">
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
@@ -10940,7 +11044,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:52">
       <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
@@ -11093,7 +11197,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:52">
       <c r="B38" s="26" t="s">
         <v>2</v>
       </c>
@@ -11240,7 +11344,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:52">
       <c r="B39" s="26" t="s">
         <v>2</v>
       </c>
@@ -11383,7 +11487,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:52" ht="16.5" thickBot="1">
       <c r="B40" s="67" t="s">
         <v>2</v>
       </c>
@@ -11530,7 +11634,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:52" ht="16.5" thickTop="1">
       <c r="B41" s="138" t="s">
         <v>2</v>
       </c>
@@ -11673,7 +11777,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:52">
       <c r="B42" s="26" t="s">
         <v>2</v>
       </c>
@@ -11822,7 +11926,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:52">
       <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
@@ -11971,7 +12075,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:52">
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
@@ -12122,7 +12226,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:52">
       <c r="B45" s="26" t="s">
         <v>2</v>
       </c>
@@ -12269,11 +12373,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:52">
       <c r="B46" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="216" t="s">
+      <c r="C46" s="215" t="s">
         <v>199</v>
       </c>
       <c r="D46" s="55" t="s">
@@ -12416,14 +12520,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B47" s="214" t="s">
+    <row r="47" spans="2:52">
+      <c r="B47" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="217" t="s">
+      <c r="C47" s="216" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="224" t="s">
+      <c r="D47" s="223" t="s">
         <v>127</v>
       </c>
       <c r="E47" s="81" t="s">
@@ -12474,7 +12578,7 @@
       <c r="T47" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="U47" s="232">
+      <c r="U47" s="231">
         <v>-1</v>
       </c>
       <c r="V47" s="88" t="s">
@@ -12495,7 +12599,7 @@
       <c r="AA47" s="90">
         <v>10</v>
       </c>
-      <c r="AB47" s="234" t="s">
+      <c r="AB47" s="233" t="s">
         <v>127</v>
       </c>
       <c r="AC47" s="91" t="s">
@@ -12516,10 +12620,10 @@
       <c r="AH47" s="13">
         <v>2</v>
       </c>
-      <c r="AI47" s="235" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ47" s="235" t="s">
+      <c r="AI47" s="234" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ47" s="234" t="s">
         <v>127</v>
       </c>
       <c r="AK47" s="92" t="s">
@@ -12546,7 +12650,7 @@
       <c r="AR47" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="AS47" s="235" t="s">
+      <c r="AS47" s="234" t="s">
         <v>127</v>
       </c>
       <c r="AT47" s="92" t="s">
@@ -12571,7 +12675,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:52">
       <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
@@ -12714,7 +12818,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:52">
       <c r="B49" s="26" t="s">
         <v>2</v>
       </c>
@@ -12863,7 +12967,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:52">
       <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
@@ -13006,7 +13110,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:52">
       <c r="B51" s="26" t="s">
         <v>2</v>
       </c>
@@ -13153,7 +13257,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:52" ht="16.5" thickBot="1">
       <c r="B52" s="67" t="s">
         <v>2</v>
       </c>
@@ -13300,14 +13404,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:52" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="215" t="s">
+    <row r="53" spans="2:52" ht="16.5" thickTop="1">
+      <c r="B53" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="220" t="s">
+      <c r="C53" s="219" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="225" t="s">
+      <c r="D53" s="224" t="s">
         <v>127</v>
       </c>
       <c r="E53" s="138" t="s">
@@ -13455,7 +13559,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:52">
       <c r="B54" s="27" t="s">
         <v>2</v>
       </c>
@@ -13610,7 +13714,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:52">
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
@@ -13765,11 +13869,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:52">
       <c r="B56" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="221" t="s">
+      <c r="C56" s="220" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="25" t="s">
@@ -13823,7 +13927,7 @@
       <c r="T56" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="U56" s="232" t="s">
+      <c r="U56" s="231" t="s">
         <v>301</v>
       </c>
       <c r="V56" s="36" t="s">
@@ -13920,11 +14024,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:52" s="205" customFormat="1" ht="16.5" thickBot="1">
       <c r="B57" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="219" t="s">
+      <c r="C57" s="218" t="s">
         <v>212</v>
       </c>
       <c r="D57" s="192" t="s">
@@ -13948,16 +14052,16 @@
       <c r="J57" s="194">
         <v>250</v>
       </c>
-      <c r="K57" s="226" t="s">
-        <v>127</v>
-      </c>
-      <c r="L57" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="M57" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="N57" s="228" t="s">
+      <c r="K57" s="225" t="s">
+        <v>127</v>
+      </c>
+      <c r="L57" s="227" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" s="227" t="s">
+        <v>127</v>
+      </c>
+      <c r="N57" s="227" t="s">
         <v>127</v>
       </c>
       <c r="O57" s="195" t="s">
@@ -14075,11 +14179,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:52">
       <c r="B58" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="223" t="s">
+      <c r="C58" s="222" t="s">
         <v>223</v>
       </c>
       <c r="D58" s="179" t="s">
@@ -14230,11 +14334,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:52">
       <c r="B59" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="222" t="s">
+      <c r="C59" s="221" t="s">
         <v>214</v>
       </c>
       <c r="D59" s="41" t="s">
@@ -14258,25 +14362,25 @@
       <c r="J59" s="43">
         <v>1200</v>
       </c>
-      <c r="K59" s="227" t="s">
-        <v>127</v>
-      </c>
-      <c r="L59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="M59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="N59" s="229" t="s">
-        <v>127</v>
-      </c>
-      <c r="O59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="P59" s="231" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q59" s="231" t="s">
+      <c r="K59" s="226" t="s">
+        <v>127</v>
+      </c>
+      <c r="L59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="M59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="N59" s="228" t="s">
+        <v>127</v>
+      </c>
+      <c r="O59" s="230" t="s">
+        <v>127</v>
+      </c>
+      <c r="P59" s="230" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q59" s="230" t="s">
         <v>127</v>
       </c>
       <c r="R59" s="46">
@@ -14385,7 +14489,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="2:52" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:52" ht="16.5" thickBot="1">
       <c r="B60" s="67" t="s">
         <v>2</v>
       </c>
@@ -14538,11 +14642,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:52">
       <c r="B61" s="158" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="218" t="s">
+      <c r="C61" s="217" t="s">
         <v>200</v>
       </c>
       <c r="D61" s="158" t="s">
@@ -14575,7 +14679,7 @@
       <c r="M61" s="161">
         <v>100</v>
       </c>
-      <c r="N61" s="230" t="s">
+      <c r="N61" s="229" t="s">
         <v>127</v>
       </c>
       <c r="O61" s="162" t="s">
@@ -14596,7 +14700,7 @@
       <c r="T61" s="164" t="s">
         <v>311</v>
       </c>
-      <c r="U61" s="233">
+      <c r="U61" s="232">
         <v>-1</v>
       </c>
       <c r="V61" s="165" t="s">
@@ -14693,7 +14797,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:52">
       <c r="B62" s="26" t="s">
         <v>2</v>
       </c>
@@ -14848,7 +14952,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:52">
       <c r="B63" s="26" t="s">
         <v>2</v>
       </c>
@@ -15003,7 +15107,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:52">
       <c r="B64" s="26" t="s">
         <v>2</v>
       </c>
@@ -15158,7 +15262,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:52">
       <c r="B65" s="26" t="s">
         <v>2</v>
       </c>
@@ -15313,7 +15417,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:52">
       <c r="B66" s="26" t="s">
         <v>2</v>
       </c>
@@ -15468,7 +15572,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:52">
       <c r="B67" s="26" t="s">
         <v>2</v>
       </c>
@@ -15623,7 +15727,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:52">
       <c r="B68" s="26" t="s">
         <v>2</v>
       </c>
@@ -15778,7 +15882,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:52">
       <c r="B69" s="26" t="s">
         <v>2</v>
       </c>
@@ -15931,7 +16035,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:52">
       <c r="B70" s="26" t="s">
         <v>2</v>
       </c>
@@ -16086,7 +16190,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:52">
       <c r="B71" s="27" t="s">
         <v>2</v>
       </c>
@@ -16241,7 +16345,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:52">
       <c r="B72" s="27" t="s">
         <v>2</v>
       </c>
@@ -16394,7 +16498,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:52">
       <c r="B73" s="27" t="s">
         <v>2</v>
       </c>
@@ -16549,7 +16653,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:52">
       <c r="B74" s="27" t="s">
         <v>2</v>
       </c>
@@ -16700,7 +16804,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:52">
       <c r="B75" s="27" t="s">
         <v>2</v>
       </c>
@@ -16855,7 +16959,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:52">
       <c r="B76" s="27" t="s">
         <v>2</v>
       </c>
@@ -17010,816 +17114,816 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B77" s="27" t="s">
+    <row r="77" spans="2:52">
+      <c r="B77" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="212" t="s">
+      <c r="C77" s="247" t="s">
         <v>324</v>
       </c>
-      <c r="D77" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E77" s="211" t="s">
+      <c r="D77" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F77" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="69">
-        <v>1</v>
-      </c>
-      <c r="H77" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I77" s="30" t="s">
+      <c r="F77" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="248">
+        <v>1</v>
+      </c>
+      <c r="H77" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I77" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="J77" s="30">
-        <v>1</v>
-      </c>
-      <c r="K77" s="30" t="s">
+      <c r="J77" s="249">
+        <v>1</v>
+      </c>
+      <c r="K77" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="L77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q77" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R77" s="33">
+      <c r="L77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R77" s="252">
         <v>-25</v>
       </c>
-      <c r="S77" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T77" s="47" t="s">
+      <c r="S77" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T77" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U77" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V77" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W77" s="242" t="s">
+      <c r="U77" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V77" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W77" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X77" s="21" t="b">
+      <c r="X77" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y77" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z77" s="21" t="s">
+      <c r="Y77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z77" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA77" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB77" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC77" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD77" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE77" s="13" t="s">
+      <c r="AA77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB77" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC77" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD77" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE77" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH77" s="13">
+      <c r="AF77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH77" s="260">
         <v>2</v>
       </c>
-      <c r="AI77" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ77" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS77" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW77" s="20" t="s">
+      <c r="AI77" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS77" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW77" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY77" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ77" s="13" t="s">
+      <c r="AX77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY77" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ77" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B78" s="27" t="s">
+    <row r="78" spans="2:52">
+      <c r="B78" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="212" t="s">
+      <c r="C78" s="247" t="s">
         <v>326</v>
       </c>
-      <c r="D78" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E78" s="211" t="s">
+      <c r="D78" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E78" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="69">
+      <c r="F78" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="248">
         <v>-1</v>
       </c>
-      <c r="H78" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I78" s="30" t="s">
+      <c r="H78" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I78" s="249" t="s">
         <v>12</v>
       </c>
-      <c r="J78" s="30">
+      <c r="J78" s="249">
         <v>1000</v>
       </c>
-      <c r="K78" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R78" s="33">
+      <c r="K78" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="L78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R78" s="252">
         <v>-25</v>
       </c>
-      <c r="S78" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T78" s="47" t="s">
+      <c r="S78" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T78" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U78" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V78" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W78" s="242" t="s">
+      <c r="U78" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V78" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W78" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X78" s="21" t="b">
+      <c r="X78" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y78" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z78" s="21" t="s">
+      <c r="Y78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z78" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA78" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB78" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC78" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD78" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE78" s="13" t="s">
+      <c r="AA78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB78" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC78" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD78" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE78" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH78" s="13">
+      <c r="AF78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH78" s="260">
         <v>2</v>
       </c>
-      <c r="AI78" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ78" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS78" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW78" s="20" t="s">
+      <c r="AI78" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS78" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW78" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY78" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ78" s="13" t="s">
+      <c r="AX78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY78" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ78" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B79" s="27" t="s">
+    <row r="79" spans="2:52">
+      <c r="B79" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="212" t="s">
+      <c r="C79" s="247" t="s">
         <v>327</v>
       </c>
-      <c r="D79" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E79" s="211" t="s">
+      <c r="D79" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E79" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F79" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79" s="69">
+      <c r="F79" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="248">
         <v>-1</v>
       </c>
-      <c r="H79" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I79" s="30" t="s">
+      <c r="H79" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I79" s="249" t="s">
         <v>10</v>
       </c>
-      <c r="J79" s="30">
+      <c r="J79" s="249">
         <v>2</v>
       </c>
-      <c r="K79" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q79" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R79" s="33">
+      <c r="K79" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="L79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R79" s="252">
         <v>-25</v>
       </c>
-      <c r="S79" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T79" s="47" t="s">
+      <c r="S79" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T79" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U79" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V79" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W79" s="242" t="s">
+      <c r="U79" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V79" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W79" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X79" s="21" t="b">
+      <c r="X79" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y79" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z79" s="21" t="s">
+      <c r="Y79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z79" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA79" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB79" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC79" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD79" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE79" s="13" t="s">
+      <c r="AA79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB79" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC79" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD79" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE79" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH79" s="13">
+      <c r="AF79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH79" s="260">
         <v>2</v>
       </c>
-      <c r="AI79" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ79" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS79" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW79" s="20" t="s">
+      <c r="AI79" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS79" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW79" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY79" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ79" s="13" t="s">
+      <c r="AX79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY79" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ79" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B80" s="27" t="s">
+    <row r="80" spans="2:52">
+      <c r="B80" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="212" t="s">
+      <c r="C80" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="D80" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E80" s="211" t="s">
+      <c r="D80" s="236" t="s">
+        <v>127</v>
+      </c>
+      <c r="E80" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F80" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G80" s="69">
+      <c r="F80" s="248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="248">
         <v>-1</v>
       </c>
-      <c r="H80" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I80" s="30" t="s">
+      <c r="H80" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="I80" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="J80" s="30">
-        <v>1</v>
-      </c>
-      <c r="K80" s="30" t="s">
+      <c r="J80" s="249">
+        <v>1</v>
+      </c>
+      <c r="K80" s="249" t="s">
         <v>163</v>
       </c>
-      <c r="L80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q80" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R80" s="33">
+      <c r="L80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="M80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="N80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="O80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="P80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="R80" s="252">
         <v>-25</v>
       </c>
-      <c r="S80" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T80" s="47" t="s">
+      <c r="S80" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="T80" s="253" t="s">
         <v>322</v>
       </c>
-      <c r="U80" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V80" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W80" s="242" t="s">
+      <c r="U80" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="V80" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="W80" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="X80" s="21" t="b">
+      <c r="X80" s="257" t="b">
         <v>0</v>
       </c>
-      <c r="Y80" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z80" s="21" t="s">
+      <c r="Y80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z80" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="AA80" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB80" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC80" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD80" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE80" s="13" t="s">
+      <c r="AA80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB80" s="258" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC80" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD80" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE80" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="AF80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH80" s="13">
+      <c r="AF80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH80" s="260">
         <v>2</v>
       </c>
-      <c r="AI80" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ80" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS80" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW80" s="20" t="s">
+      <c r="AI80" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS80" s="261" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW80" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="AX80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY80" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ80" s="13" t="s">
+      <c r="AX80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY80" s="260" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ80" s="260" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="B81" s="27" t="s">
+    <row r="81" spans="2:52">
+      <c r="B81" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="212" t="s">
+      <c r="C81" s="264" t="s">
         <v>329</v>
       </c>
-      <c r="D81" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="E81" s="211" t="s">
+      <c r="D81" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="E81" s="263" t="s">
         <v>312</v>
       </c>
-      <c r="F81" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="69">
+      <c r="F81" s="265" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" s="265">
         <v>-1</v>
       </c>
-      <c r="H81" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I81" s="30" t="s">
+      <c r="H81" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="I81" s="266" t="s">
         <v>12</v>
       </c>
-      <c r="J81" s="30">
+      <c r="J81" s="266">
         <v>2000</v>
       </c>
-      <c r="K81" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="M81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="N81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="O81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q81" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="R81" s="33">
+      <c r="K81" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="L81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="M81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="N81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="O81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="P81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="R81" s="269">
         <v>-25</v>
       </c>
-      <c r="S81" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="T81" s="47" t="s">
+      <c r="S81" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="T81" s="270" t="s">
         <v>322</v>
       </c>
-      <c r="U81" s="213" t="s">
-        <v>127</v>
-      </c>
-      <c r="V81" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="W81" s="242" t="s">
+      <c r="U81" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="V81" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="W81" s="273" t="s">
         <v>325</v>
       </c>
-      <c r="X81" s="21" t="b">
+      <c r="X81" s="274" t="b">
         <v>0</v>
       </c>
-      <c r="Y81" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z81" s="21" t="s">
+      <c r="Y81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z81" s="274" t="s">
         <v>16</v>
       </c>
-      <c r="AA81" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB81" s="171" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC81" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD81" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE81" s="13" t="s">
+      <c r="AA81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB81" s="275" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC81" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD81" s="276" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE81" s="277" t="s">
         <v>321</v>
       </c>
-      <c r="AF81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH81" s="13">
+      <c r="AF81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH81" s="277">
         <v>2</v>
       </c>
-      <c r="AI81" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ81" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS81" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW81" s="20" t="s">
+      <c r="AI81" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS81" s="278" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW81" s="279" t="s">
         <v>340</v>
       </c>
-      <c r="AX81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY81" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ81" s="13" t="s">
+      <c r="AX81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY81" s="277" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ81" s="277" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="2:52" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B84" s="248" t="s">
+    <row r="84" spans="2:52" ht="26.25">
+      <c r="B84" s="246" t="s">
         <v>330</v>
       </c>
-      <c r="C84" s="248"/>
-      <c r="D84" s="248"/>
-      <c r="E84" s="248"/>
+      <c r="C84" s="246"/>
+      <c r="D84" s="246"/>
+      <c r="E84" s="246"/>
     </row>
-    <row r="86" spans="2:52" ht="135" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:52" ht="135">
       <c r="B86" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="C86" s="243" t="s">
+      <c r="C86" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="D86" s="244" t="s">
+      <c r="D86" s="242" t="s">
         <v>52</v>
       </c>
       <c r="E86" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="F86" s="244" t="s">
+      <c r="F86" s="242" t="s">
         <v>333</v>
       </c>
-      <c r="G86" s="245" t="s">
+      <c r="G86" s="243" t="s">
         <v>334</v>
       </c>
-      <c r="H86" s="245" t="s">
+      <c r="H86" s="243" t="s">
         <v>335</v>
       </c>
-      <c r="I86" s="245" t="s">
+      <c r="I86" s="243" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="87" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:52">
       <c r="B87" s="211" t="s">
         <v>2</v>
       </c>
@@ -17884,7 +17988,7 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
@@ -17925,39 +18029,39 @@
     <col min="46" max="49" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="10" customFormat="1">
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="246"/>
-      <c r="AB1" s="246"/>
+      <c r="AA1" s="244"/>
+      <c r="AB1" s="244"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="247"/>
-      <c r="AE1" s="247"/>
-      <c r="AF1" s="247"/>
-      <c r="AG1" s="247"/>
-      <c r="AH1" s="247"/>
-      <c r="AI1" s="247"/>
-      <c r="AJ1" s="247"/>
-      <c r="AK1" s="247"/>
-      <c r="AL1" s="247"/>
-      <c r="AM1" s="247"/>
-      <c r="AN1" s="247"/>
-      <c r="AO1" s="247"/>
-      <c r="AP1" s="247"/>
-      <c r="AQ1" s="247"/>
-      <c r="AR1" s="247"/>
-      <c r="AS1" s="247"/>
-      <c r="AT1" s="247"/>
-      <c r="AU1" s="247"/>
-      <c r="AV1" s="247"/>
-      <c r="AW1" s="247"/>
-      <c r="AX1" s="247"/>
-      <c r="AY1" s="247"/>
+      <c r="AD1" s="245"/>
+      <c r="AE1" s="245"/>
+      <c r="AF1" s="245"/>
+      <c r="AG1" s="245"/>
+      <c r="AH1" s="245"/>
+      <c r="AI1" s="245"/>
+      <c r="AJ1" s="245"/>
+      <c r="AK1" s="245"/>
+      <c r="AL1" s="245"/>
+      <c r="AM1" s="245"/>
+      <c r="AN1" s="245"/>
+      <c r="AO1" s="245"/>
+      <c r="AP1" s="245"/>
+      <c r="AQ1" s="245"/>
+      <c r="AR1" s="245"/>
+      <c r="AS1" s="245"/>
+      <c r="AT1" s="245"/>
+      <c r="AU1" s="245"/>
+      <c r="AV1" s="245"/>
+      <c r="AW1" s="245"/>
+      <c r="AX1" s="245"/>
+      <c r="AY1" s="245"/>
     </row>
-    <row r="2" spans="2:51" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:51" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>313</v>
       </c>
@@ -17976,15 +18080,15 @@
       <c r="G2" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="H2" s="239" t="s">
+      <c r="H2" s="238" t="s">
         <v>319</v>
       </c>
-      <c r="I2" s="240" t="s">
+      <c r="I2" s="239" t="s">
         <v>320</v>
       </c>
-      <c r="J2" s="241"/>
+      <c r="J2" s="240"/>
     </row>
-    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:51">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -18003,197 +18107,197 @@
       <c r="G3" s="26">
         <v>2</v>
       </c>
-      <c r="H3" s="237">
-        <v>360</v>
-      </c>
-      <c r="I3" s="238" t="s">
+      <c r="H3" s="236">
+        <v>720</v>
+      </c>
+      <c r="I3" s="237" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="236"/>
-      <c r="B57" s="236"/>
-      <c r="C57" s="236"/>
-      <c r="D57" s="236"/>
-      <c r="E57" s="236"/>
-      <c r="F57" s="236"/>
-      <c r="G57" s="236"/>
-      <c r="H57" s="236"/>
-      <c r="I57" s="236"/>
-      <c r="J57" s="236"/>
-      <c r="K57" s="236"/>
-      <c r="L57" s="236"/>
-      <c r="M57" s="236"/>
-      <c r="N57" s="236"/>
-      <c r="O57" s="236"/>
-      <c r="P57" s="236"/>
-      <c r="Q57" s="236"/>
-      <c r="R57" s="236"/>
-      <c r="S57" s="236"/>
-      <c r="T57" s="236"/>
-      <c r="U57" s="236"/>
-      <c r="V57" s="236"/>
-      <c r="W57" s="236"/>
-      <c r="X57" s="236"/>
-      <c r="Y57" s="236"/>
-      <c r="Z57" s="236"/>
-      <c r="AA57" s="236"/>
-      <c r="AB57" s="236"/>
-      <c r="AC57" s="236"/>
-      <c r="AD57" s="236"/>
-      <c r="AE57" s="236"/>
-      <c r="AF57" s="236"/>
-      <c r="AG57" s="236"/>
-      <c r="AH57" s="236"/>
-      <c r="AI57" s="236"/>
-      <c r="AJ57" s="236"/>
-      <c r="AK57" s="236"/>
-      <c r="AL57" s="236"/>
-      <c r="AM57" s="236"/>
-      <c r="AN57" s="236"/>
-      <c r="AO57" s="236"/>
-      <c r="AP57" s="236"/>
-      <c r="AQ57" s="236"/>
-      <c r="AR57" s="236"/>
-      <c r="AS57" s="236"/>
-      <c r="AT57" s="236"/>
-      <c r="AU57" s="236"/>
-      <c r="AV57" s="236"/>
-      <c r="AW57" s="236"/>
-      <c r="AX57" s="236"/>
-      <c r="AY57" s="236"/>
-      <c r="AZ57" s="236"/>
-      <c r="BA57" s="236"/>
-      <c r="BB57" s="236"/>
-      <c r="BC57" s="236"/>
-      <c r="BD57" s="236"/>
-      <c r="BE57" s="236"/>
-      <c r="BF57" s="236"/>
-      <c r="BG57" s="236"/>
-      <c r="BH57" s="236"/>
-      <c r="BI57" s="236"/>
-      <c r="BJ57" s="236"/>
-      <c r="BK57" s="236"/>
-      <c r="BL57" s="236"/>
-      <c r="BM57" s="236"/>
-      <c r="BN57" s="236"/>
-      <c r="BO57" s="236"/>
-      <c r="BP57" s="236"/>
-      <c r="BQ57" s="236"/>
-      <c r="BR57" s="236"/>
-      <c r="BS57" s="236"/>
-      <c r="BT57" s="236"/>
-      <c r="BU57" s="236"/>
-      <c r="BV57" s="236"/>
-      <c r="BW57" s="236"/>
-      <c r="BX57" s="236"/>
-      <c r="BY57" s="236"/>
-      <c r="BZ57" s="236"/>
-      <c r="CA57" s="236"/>
-      <c r="CB57" s="236"/>
-      <c r="CC57" s="236"/>
-      <c r="CD57" s="236"/>
-      <c r="CE57" s="236"/>
-      <c r="CF57" s="236"/>
-      <c r="CG57" s="236"/>
-      <c r="CH57" s="236"/>
-      <c r="CI57" s="236"/>
-      <c r="CJ57" s="236"/>
-      <c r="CK57" s="236"/>
-      <c r="CL57" s="236"/>
-      <c r="CM57" s="236"/>
-      <c r="CN57" s="236"/>
-      <c r="CO57" s="236"/>
-      <c r="CP57" s="236"/>
-      <c r="CQ57" s="236"/>
-      <c r="CR57" s="236"/>
-      <c r="CS57" s="236"/>
-      <c r="CT57" s="236"/>
-      <c r="CU57" s="236"/>
-      <c r="CV57" s="236"/>
-      <c r="CW57" s="236"/>
-      <c r="CX57" s="236"/>
-      <c r="CY57" s="236"/>
-      <c r="CZ57" s="236"/>
-      <c r="DA57" s="236"/>
-      <c r="DB57" s="236"/>
-      <c r="DC57" s="236"/>
-      <c r="DD57" s="236"/>
-      <c r="DE57" s="236"/>
-      <c r="DF57" s="236"/>
-      <c r="DG57" s="236"/>
-      <c r="DH57" s="236"/>
-      <c r="DI57" s="236"/>
-      <c r="DJ57" s="236"/>
-      <c r="DK57" s="236"/>
-      <c r="DL57" s="236"/>
-      <c r="DM57" s="236"/>
-      <c r="DN57" s="236"/>
-      <c r="DO57" s="236"/>
-      <c r="DP57" s="236"/>
-      <c r="DQ57" s="236"/>
-      <c r="DR57" s="236"/>
-      <c r="DS57" s="236"/>
-      <c r="DT57" s="236"/>
-      <c r="DU57" s="236"/>
-      <c r="DV57" s="236"/>
-      <c r="DW57" s="236"/>
-      <c r="DX57" s="236"/>
-      <c r="DY57" s="236"/>
-      <c r="DZ57" s="236"/>
-      <c r="EA57" s="236"/>
-      <c r="EB57" s="236"/>
-      <c r="EC57" s="236"/>
-      <c r="ED57" s="236"/>
-      <c r="EE57" s="236"/>
-      <c r="EF57" s="236"/>
-      <c r="EG57" s="236"/>
-      <c r="EH57" s="236"/>
-      <c r="EI57" s="236"/>
-      <c r="EJ57" s="236"/>
-      <c r="EK57" s="236"/>
-      <c r="EL57" s="236"/>
-      <c r="EM57" s="236"/>
-      <c r="EN57" s="236"/>
-      <c r="EO57" s="236"/>
-      <c r="EP57" s="236"/>
-      <c r="EQ57" s="236"/>
-      <c r="ER57" s="236"/>
-      <c r="ES57" s="236"/>
-      <c r="ET57" s="236"/>
-      <c r="EU57" s="236"/>
-      <c r="EV57" s="236"/>
-      <c r="EW57" s="236"/>
-      <c r="EX57" s="236"/>
-      <c r="EY57" s="236"/>
-      <c r="EZ57" s="236"/>
-      <c r="FA57" s="236"/>
-      <c r="FB57" s="236"/>
-      <c r="FC57" s="236"/>
-      <c r="FD57" s="236"/>
-      <c r="FE57" s="236"/>
-      <c r="FF57" s="236"/>
-      <c r="FG57" s="236"/>
-      <c r="FH57" s="236"/>
-      <c r="FI57" s="236"/>
-      <c r="FJ57" s="236"/>
-      <c r="FK57" s="236"/>
-      <c r="FL57" s="236"/>
-      <c r="FM57" s="236"/>
-      <c r="FN57" s="236"/>
-      <c r="FO57" s="236"/>
-      <c r="FP57" s="236"/>
-      <c r="FQ57" s="236"/>
-      <c r="FR57" s="236"/>
-      <c r="FS57" s="236"/>
-      <c r="FT57" s="236"/>
-      <c r="FU57" s="236"/>
-      <c r="FV57" s="236"/>
-      <c r="FW57" s="236"/>
-      <c r="FX57" s="236"/>
-      <c r="FY57" s="236"/>
-      <c r="FZ57" s="236"/>
-      <c r="GA57" s="236"/>
+    <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A57" s="235"/>
+      <c r="B57" s="235"/>
+      <c r="C57" s="235"/>
+      <c r="D57" s="235"/>
+      <c r="E57" s="235"/>
+      <c r="F57" s="235"/>
+      <c r="G57" s="235"/>
+      <c r="H57" s="235"/>
+      <c r="I57" s="235"/>
+      <c r="J57" s="235"/>
+      <c r="K57" s="235"/>
+      <c r="L57" s="235"/>
+      <c r="M57" s="235"/>
+      <c r="N57" s="235"/>
+      <c r="O57" s="235"/>
+      <c r="P57" s="235"/>
+      <c r="Q57" s="235"/>
+      <c r="R57" s="235"/>
+      <c r="S57" s="235"/>
+      <c r="T57" s="235"/>
+      <c r="U57" s="235"/>
+      <c r="V57" s="235"/>
+      <c r="W57" s="235"/>
+      <c r="X57" s="235"/>
+      <c r="Y57" s="235"/>
+      <c r="Z57" s="235"/>
+      <c r="AA57" s="235"/>
+      <c r="AB57" s="235"/>
+      <c r="AC57" s="235"/>
+      <c r="AD57" s="235"/>
+      <c r="AE57" s="235"/>
+      <c r="AF57" s="235"/>
+      <c r="AG57" s="235"/>
+      <c r="AH57" s="235"/>
+      <c r="AI57" s="235"/>
+      <c r="AJ57" s="235"/>
+      <c r="AK57" s="235"/>
+      <c r="AL57" s="235"/>
+      <c r="AM57" s="235"/>
+      <c r="AN57" s="235"/>
+      <c r="AO57" s="235"/>
+      <c r="AP57" s="235"/>
+      <c r="AQ57" s="235"/>
+      <c r="AR57" s="235"/>
+      <c r="AS57" s="235"/>
+      <c r="AT57" s="235"/>
+      <c r="AU57" s="235"/>
+      <c r="AV57" s="235"/>
+      <c r="AW57" s="235"/>
+      <c r="AX57" s="235"/>
+      <c r="AY57" s="235"/>
+      <c r="AZ57" s="235"/>
+      <c r="BA57" s="235"/>
+      <c r="BB57" s="235"/>
+      <c r="BC57" s="235"/>
+      <c r="BD57" s="235"/>
+      <c r="BE57" s="235"/>
+      <c r="BF57" s="235"/>
+      <c r="BG57" s="235"/>
+      <c r="BH57" s="235"/>
+      <c r="BI57" s="235"/>
+      <c r="BJ57" s="235"/>
+      <c r="BK57" s="235"/>
+      <c r="BL57" s="235"/>
+      <c r="BM57" s="235"/>
+      <c r="BN57" s="235"/>
+      <c r="BO57" s="235"/>
+      <c r="BP57" s="235"/>
+      <c r="BQ57" s="235"/>
+      <c r="BR57" s="235"/>
+      <c r="BS57" s="235"/>
+      <c r="BT57" s="235"/>
+      <c r="BU57" s="235"/>
+      <c r="BV57" s="235"/>
+      <c r="BW57" s="235"/>
+      <c r="BX57" s="235"/>
+      <c r="BY57" s="235"/>
+      <c r="BZ57" s="235"/>
+      <c r="CA57" s="235"/>
+      <c r="CB57" s="235"/>
+      <c r="CC57" s="235"/>
+      <c r="CD57" s="235"/>
+      <c r="CE57" s="235"/>
+      <c r="CF57" s="235"/>
+      <c r="CG57" s="235"/>
+      <c r="CH57" s="235"/>
+      <c r="CI57" s="235"/>
+      <c r="CJ57" s="235"/>
+      <c r="CK57" s="235"/>
+      <c r="CL57" s="235"/>
+      <c r="CM57" s="235"/>
+      <c r="CN57" s="235"/>
+      <c r="CO57" s="235"/>
+      <c r="CP57" s="235"/>
+      <c r="CQ57" s="235"/>
+      <c r="CR57" s="235"/>
+      <c r="CS57" s="235"/>
+      <c r="CT57" s="235"/>
+      <c r="CU57" s="235"/>
+      <c r="CV57" s="235"/>
+      <c r="CW57" s="235"/>
+      <c r="CX57" s="235"/>
+      <c r="CY57" s="235"/>
+      <c r="CZ57" s="235"/>
+      <c r="DA57" s="235"/>
+      <c r="DB57" s="235"/>
+      <c r="DC57" s="235"/>
+      <c r="DD57" s="235"/>
+      <c r="DE57" s="235"/>
+      <c r="DF57" s="235"/>
+      <c r="DG57" s="235"/>
+      <c r="DH57" s="235"/>
+      <c r="DI57" s="235"/>
+      <c r="DJ57" s="235"/>
+      <c r="DK57" s="235"/>
+      <c r="DL57" s="235"/>
+      <c r="DM57" s="235"/>
+      <c r="DN57" s="235"/>
+      <c r="DO57" s="235"/>
+      <c r="DP57" s="235"/>
+      <c r="DQ57" s="235"/>
+      <c r="DR57" s="235"/>
+      <c r="DS57" s="235"/>
+      <c r="DT57" s="235"/>
+      <c r="DU57" s="235"/>
+      <c r="DV57" s="235"/>
+      <c r="DW57" s="235"/>
+      <c r="DX57" s="235"/>
+      <c r="DY57" s="235"/>
+      <c r="DZ57" s="235"/>
+      <c r="EA57" s="235"/>
+      <c r="EB57" s="235"/>
+      <c r="EC57" s="235"/>
+      <c r="ED57" s="235"/>
+      <c r="EE57" s="235"/>
+      <c r="EF57" s="235"/>
+      <c r="EG57" s="235"/>
+      <c r="EH57" s="235"/>
+      <c r="EI57" s="235"/>
+      <c r="EJ57" s="235"/>
+      <c r="EK57" s="235"/>
+      <c r="EL57" s="235"/>
+      <c r="EM57" s="235"/>
+      <c r="EN57" s="235"/>
+      <c r="EO57" s="235"/>
+      <c r="EP57" s="235"/>
+      <c r="EQ57" s="235"/>
+      <c r="ER57" s="235"/>
+      <c r="ES57" s="235"/>
+      <c r="ET57" s="235"/>
+      <c r="EU57" s="235"/>
+      <c r="EV57" s="235"/>
+      <c r="EW57" s="235"/>
+      <c r="EX57" s="235"/>
+      <c r="EY57" s="235"/>
+      <c r="EZ57" s="235"/>
+      <c r="FA57" s="235"/>
+      <c r="FB57" s="235"/>
+      <c r="FC57" s="235"/>
+      <c r="FD57" s="235"/>
+      <c r="FE57" s="235"/>
+      <c r="FF57" s="235"/>
+      <c r="FG57" s="235"/>
+      <c r="FH57" s="235"/>
+      <c r="FI57" s="235"/>
+      <c r="FJ57" s="235"/>
+      <c r="FK57" s="235"/>
+      <c r="FL57" s="235"/>
+      <c r="FM57" s="235"/>
+      <c r="FN57" s="235"/>
+      <c r="FO57" s="235"/>
+      <c r="FP57" s="235"/>
+      <c r="FQ57" s="235"/>
+      <c r="FR57" s="235"/>
+      <c r="FS57" s="235"/>
+      <c r="FT57" s="235"/>
+      <c r="FU57" s="235"/>
+      <c r="FV57" s="235"/>
+      <c r="FW57" s="235"/>
+      <c r="FX57" s="235"/>
+      <c r="FY57" s="235"/>
+      <c r="FZ57" s="235"/>
+      <c r="GA57" s="235"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -18216,12 +18320,12 @@
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
@@ -18230,10 +18334,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -18241,7 +18345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -18249,7 +18353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -18257,13 +18361,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -18271,7 +18375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -18279,7 +18383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>127</v>
       </c>
@@ -18287,107 +18391,107 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="D11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="D12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="D14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4">
       <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Adding new column to set intersticials seen before launch popup offer to remove ads
Former-commit-id: be95cd763252175dc153a7f55573657bef496c4f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535"/>
+    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3271" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="347">
   <si>
     <t>[sku]</t>
   </si>
@@ -1065,6 +1065,9 @@
   </si>
   <si>
     <t>TID_REMOVE_ADS_OFFER_NAME</t>
+  </si>
+  <si>
+    <t>[interstitialsBeforeNoAdsPopup]</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="280">
+  <cellXfs count="279">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2375,7 +2378,6 @@
     <xf numFmtId="0" fontId="20" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -2385,6 +2387,105 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2393,150 +2494,55 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="70">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5237,6 +5243,46 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5265,80 +5311,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="B2:AZ82"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="65"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="63"/>
-    <tableColumn id="49" name="[type]" dataDxfId="62"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="61"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="60"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="59"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="58"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="57"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="56"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="55"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="54"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="53"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="52"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="51"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[order]" dataDxfId="49"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="48"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="47"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="46"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="45"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="44"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="43"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="42"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="41"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="40"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="39"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="38"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="37"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="36"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="35"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="34"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="33"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="32"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="31"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="30"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="29"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="28"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="27"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="26"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="25"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="24"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="23"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="22"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="21"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="20"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="19"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="18"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="17"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="16"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="15"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="62"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="61"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="60"/>
+    <tableColumn id="49" name="[type]" dataDxfId="59"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="58"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="57"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="56"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="55"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="54"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="53"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="52"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="51"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="50"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="49"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="48"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="47"/>
+    <tableColumn id="7" name="[order]" dataDxfId="46"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="45"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="44"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="43"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="42"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="41"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="40"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="39"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="38"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="37"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="36"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="35"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="34"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="33"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="32"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="31"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="30"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="29"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="28"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="27"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="26"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="25"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="24"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="23"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="22"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="21"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="20"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="19"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="18"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="17"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="16"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="15"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="14"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="13"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="B2:I3"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="9"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="8"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="7"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="6"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="5"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:J3" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="B2:J3"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="8"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="6"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="5"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="4"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="3"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="2"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="1"/>
+    <tableColumn id="7" name="[interstitialsBeforeNoAdsPopup]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5643,7 +5690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AW84" sqref="AW84"/>
     </sheetView>
@@ -5705,35 +5752,35 @@
       <c r="V1" s="210" t="s">
         <v>310</v>
       </c>
-      <c r="AA1" s="244" t="s">
+      <c r="AA1" s="276" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="244"/>
+      <c r="AB1" s="276"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="245" t="s">
+      <c r="AD1" s="277" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="245"/>
-      <c r="AF1" s="245"/>
-      <c r="AG1" s="245"/>
-      <c r="AH1" s="245"/>
-      <c r="AI1" s="245"/>
-      <c r="AJ1" s="245"/>
-      <c r="AK1" s="245"/>
-      <c r="AL1" s="245"/>
-      <c r="AM1" s="245"/>
-      <c r="AN1" s="245"/>
-      <c r="AO1" s="245"/>
-      <c r="AP1" s="245"/>
-      <c r="AQ1" s="245"/>
-      <c r="AR1" s="245"/>
-      <c r="AS1" s="245"/>
-      <c r="AT1" s="245"/>
-      <c r="AU1" s="245"/>
-      <c r="AV1" s="245"/>
-      <c r="AW1" s="245"/>
-      <c r="AX1" s="245"/>
-      <c r="AY1" s="245"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="277"/>
+      <c r="AH1" s="277"/>
+      <c r="AI1" s="277"/>
+      <c r="AJ1" s="277"/>
+      <c r="AK1" s="277"/>
+      <c r="AL1" s="277"/>
+      <c r="AM1" s="277"/>
+      <c r="AN1" s="277"/>
+      <c r="AO1" s="277"/>
+      <c r="AP1" s="277"/>
+      <c r="AQ1" s="277"/>
+      <c r="AR1" s="277"/>
+      <c r="AS1" s="277"/>
+      <c r="AT1" s="277"/>
+      <c r="AU1" s="277"/>
+      <c r="AV1" s="277"/>
+      <c r="AW1" s="277"/>
+      <c r="AX1" s="277"/>
+      <c r="AY1" s="277"/>
     </row>
     <row r="2" spans="2:52" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
@@ -17133,7 +17180,7 @@
       <c r="B77" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="247" t="s">
+      <c r="C77" s="243" t="s">
         <v>324</v>
       </c>
       <c r="D77" s="236" t="s">
@@ -17142,145 +17189,145 @@
       <c r="E77" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F77" s="248" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="248">
-        <v>1</v>
-      </c>
-      <c r="H77" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="I77" s="249" t="s">
+      <c r="F77" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="244">
+        <v>1</v>
+      </c>
+      <c r="H77" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="I77" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="J77" s="249">
-        <v>1</v>
-      </c>
-      <c r="K77" s="249" t="s">
+      <c r="J77" s="245">
+        <v>1</v>
+      </c>
+      <c r="K77" s="245" t="s">
         <v>224</v>
       </c>
-      <c r="L77" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="M77" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="N77" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="O77" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="P77" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q77" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="R77" s="252">
+      <c r="L77" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="M77" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="N77" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="O77" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="P77" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q77" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="R77" s="248">
         <v>-25</v>
       </c>
-      <c r="S77" s="253" t="s">
-        <v>127</v>
-      </c>
-      <c r="T77" s="253" t="s">
+      <c r="S77" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="T77" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="U77" s="254" t="s">
-        <v>127</v>
-      </c>
-      <c r="V77" s="255" t="s">
-        <v>127</v>
-      </c>
-      <c r="W77" s="256" t="s">
+      <c r="U77" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="V77" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="W77" s="252" t="s">
         <v>325</v>
       </c>
-      <c r="X77" s="257" t="b">
+      <c r="X77" s="253" t="b">
         <v>0</v>
       </c>
-      <c r="Y77" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z77" s="257" t="s">
+      <c r="Y77" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z77" s="253" t="s">
         <v>16</v>
       </c>
-      <c r="AA77" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB77" s="258" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC77" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD77" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE77" s="260" t="s">
+      <c r="AA77" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB77" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC77" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD77" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE77" s="256" t="s">
         <v>321</v>
       </c>
-      <c r="AF77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH77" s="260">
+      <c r="AF77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH77" s="256">
         <v>2</v>
       </c>
-      <c r="AI77" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS77" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW77" s="262" t="s">
+      <c r="AI77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS77" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW77" s="258" t="s">
         <v>340</v>
       </c>
-      <c r="AX77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY77" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ77" s="260" t="s">
+      <c r="AX77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY77" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ77" s="256" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17288,7 +17335,7 @@
       <c r="B78" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="247" t="s">
+      <c r="C78" s="243" t="s">
         <v>326</v>
       </c>
       <c r="D78" s="236" t="s">
@@ -17297,145 +17344,145 @@
       <c r="E78" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="248" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="248">
+      <c r="F78" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="244">
         <v>-1</v>
       </c>
-      <c r="H78" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="I78" s="249" t="s">
+      <c r="H78" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="I78" s="245" t="s">
         <v>12</v>
       </c>
-      <c r="J78" s="249">
+      <c r="J78" s="245">
         <v>1000</v>
       </c>
-      <c r="K78" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="L78" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="M78" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="N78" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="O78" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="P78" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q78" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="R78" s="252">
+      <c r="K78" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="L78" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="M78" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="N78" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="O78" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="P78" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q78" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="R78" s="248">
         <v>-25</v>
       </c>
-      <c r="S78" s="253" t="s">
-        <v>127</v>
-      </c>
-      <c r="T78" s="253" t="s">
+      <c r="S78" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="T78" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="U78" s="254" t="s">
-        <v>127</v>
-      </c>
-      <c r="V78" s="255" t="s">
-        <v>127</v>
-      </c>
-      <c r="W78" s="256" t="s">
+      <c r="U78" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="V78" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="W78" s="252" t="s">
         <v>325</v>
       </c>
-      <c r="X78" s="257" t="b">
+      <c r="X78" s="253" t="b">
         <v>0</v>
       </c>
-      <c r="Y78" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z78" s="257" t="s">
+      <c r="Y78" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z78" s="253" t="s">
         <v>16</v>
       </c>
-      <c r="AA78" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB78" s="258" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC78" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD78" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE78" s="260" t="s">
+      <c r="AA78" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB78" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC78" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD78" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE78" s="256" t="s">
         <v>321</v>
       </c>
-      <c r="AF78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH78" s="260">
+      <c r="AF78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH78" s="256">
         <v>2</v>
       </c>
-      <c r="AI78" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS78" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW78" s="262" t="s">
+      <c r="AI78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS78" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW78" s="258" t="s">
         <v>340</v>
       </c>
-      <c r="AX78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY78" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ78" s="260" t="s">
+      <c r="AX78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY78" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ78" s="256" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17443,7 +17490,7 @@
       <c r="B79" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="247" t="s">
+      <c r="C79" s="243" t="s">
         <v>327</v>
       </c>
       <c r="D79" s="236" t="s">
@@ -17452,145 +17499,145 @@
       <c r="E79" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F79" s="248" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79" s="248">
+      <c r="F79" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="244">
         <v>-1</v>
       </c>
-      <c r="H79" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="I79" s="249" t="s">
+      <c r="H79" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="I79" s="245" t="s">
         <v>10</v>
       </c>
-      <c r="J79" s="249">
+      <c r="J79" s="245">
         <v>2</v>
       </c>
-      <c r="K79" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="L79" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="M79" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="N79" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="O79" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="P79" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q79" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="R79" s="252">
+      <c r="K79" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="L79" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="M79" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="N79" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="O79" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="P79" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q79" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="R79" s="248">
         <v>-25</v>
       </c>
-      <c r="S79" s="253" t="s">
-        <v>127</v>
-      </c>
-      <c r="T79" s="253" t="s">
+      <c r="S79" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="T79" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="U79" s="254" t="s">
-        <v>127</v>
-      </c>
-      <c r="V79" s="255" t="s">
-        <v>127</v>
-      </c>
-      <c r="W79" s="256" t="s">
+      <c r="U79" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="V79" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="W79" s="252" t="s">
         <v>325</v>
       </c>
-      <c r="X79" s="257" t="b">
+      <c r="X79" s="253" t="b">
         <v>0</v>
       </c>
-      <c r="Y79" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z79" s="257" t="s">
+      <c r="Y79" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z79" s="253" t="s">
         <v>16</v>
       </c>
-      <c r="AA79" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB79" s="258" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC79" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD79" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE79" s="260" t="s">
+      <c r="AA79" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB79" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC79" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD79" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE79" s="256" t="s">
         <v>321</v>
       </c>
-      <c r="AF79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH79" s="260">
+      <c r="AF79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH79" s="256">
         <v>2</v>
       </c>
-      <c r="AI79" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS79" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW79" s="262" t="s">
+      <c r="AI79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS79" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW79" s="258" t="s">
         <v>340</v>
       </c>
-      <c r="AX79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY79" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ79" s="260" t="s">
+      <c r="AX79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY79" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ79" s="256" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17598,7 +17645,7 @@
       <c r="B80" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="247" t="s">
+      <c r="C80" s="243" t="s">
         <v>328</v>
       </c>
       <c r="D80" s="236" t="s">
@@ -17607,489 +17654,489 @@
       <c r="E80" s="236" t="s">
         <v>312</v>
       </c>
-      <c r="F80" s="248" t="b">
-        <v>1</v>
-      </c>
-      <c r="G80" s="248">
+      <c r="F80" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="244">
         <v>-1</v>
       </c>
-      <c r="H80" s="249" t="s">
-        <v>127</v>
-      </c>
-      <c r="I80" s="249" t="s">
+      <c r="H80" s="245" t="s">
+        <v>127</v>
+      </c>
+      <c r="I80" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="J80" s="249">
-        <v>1</v>
-      </c>
-      <c r="K80" s="249" t="s">
+      <c r="J80" s="245">
+        <v>1</v>
+      </c>
+      <c r="K80" s="245" t="s">
         <v>163</v>
       </c>
-      <c r="L80" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="M80" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="N80" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="O80" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="P80" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q80" s="251" t="s">
-        <v>127</v>
-      </c>
-      <c r="R80" s="252">
+      <c r="L80" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="M80" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="N80" s="246" t="s">
+        <v>127</v>
+      </c>
+      <c r="O80" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="P80" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q80" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="R80" s="248">
         <v>-25</v>
       </c>
-      <c r="S80" s="253" t="s">
-        <v>127</v>
-      </c>
-      <c r="T80" s="253" t="s">
+      <c r="S80" s="249" t="s">
+        <v>127</v>
+      </c>
+      <c r="T80" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="U80" s="254" t="s">
-        <v>127</v>
-      </c>
-      <c r="V80" s="255" t="s">
-        <v>127</v>
-      </c>
-      <c r="W80" s="256" t="s">
+      <c r="U80" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="V80" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="W80" s="252" t="s">
         <v>325</v>
       </c>
-      <c r="X80" s="257" t="b">
+      <c r="X80" s="253" t="b">
         <v>0</v>
       </c>
-      <c r="Y80" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z80" s="257" t="s">
+      <c r="Y80" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z80" s="253" t="s">
         <v>16</v>
       </c>
-      <c r="AA80" s="257" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB80" s="258" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC80" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD80" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE80" s="260" t="s">
+      <c r="AA80" s="253" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB80" s="254" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC80" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD80" s="255" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE80" s="256" t="s">
         <v>321</v>
       </c>
-      <c r="AF80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH80" s="260">
+      <c r="AF80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH80" s="256">
         <v>2</v>
       </c>
-      <c r="AI80" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS80" s="261" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW80" s="262" t="s">
+      <c r="AI80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS80" s="257" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW80" s="258" t="s">
         <v>340</v>
       </c>
-      <c r="AX80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY80" s="260" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ80" s="260" t="s">
+      <c r="AX80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY80" s="256" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ80" s="256" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="81" spans="2:52">
-      <c r="B81" s="263" t="s">
+      <c r="B81" s="259" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="264" t="s">
+      <c r="C81" s="260" t="s">
         <v>329</v>
       </c>
-      <c r="D81" s="263" t="s">
-        <v>127</v>
-      </c>
-      <c r="E81" s="263" t="s">
+      <c r="D81" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="E81" s="259" t="s">
         <v>312</v>
       </c>
-      <c r="F81" s="265" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="265">
+      <c r="F81" s="261" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" s="261">
         <v>-1</v>
       </c>
-      <c r="H81" s="266" t="s">
-        <v>127</v>
-      </c>
-      <c r="I81" s="266" t="s">
+      <c r="H81" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="I81" s="262" t="s">
         <v>12</v>
       </c>
-      <c r="J81" s="266">
+      <c r="J81" s="262">
         <v>2000</v>
       </c>
-      <c r="K81" s="266" t="s">
-        <v>127</v>
-      </c>
-      <c r="L81" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="M81" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="N81" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="O81" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="P81" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q81" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="R81" s="269">
+      <c r="K81" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="L81" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="M81" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="N81" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="O81" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="P81" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q81" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="R81" s="265">
         <v>-25</v>
       </c>
-      <c r="S81" s="270" t="s">
-        <v>127</v>
-      </c>
-      <c r="T81" s="270" t="s">
+      <c r="S81" s="266" t="s">
+        <v>127</v>
+      </c>
+      <c r="T81" s="266" t="s">
         <v>322</v>
       </c>
-      <c r="U81" s="271" t="s">
-        <v>127</v>
-      </c>
-      <c r="V81" s="272" t="s">
-        <v>127</v>
-      </c>
-      <c r="W81" s="273" t="s">
+      <c r="U81" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="V81" s="268" t="s">
+        <v>127</v>
+      </c>
+      <c r="W81" s="269" t="s">
         <v>325</v>
       </c>
-      <c r="X81" s="274" t="b">
+      <c r="X81" s="270" t="b">
         <v>0</v>
       </c>
-      <c r="Y81" s="274" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z81" s="274" t="s">
+      <c r="Y81" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z81" s="270" t="s">
         <v>16</v>
       </c>
-      <c r="AA81" s="274" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB81" s="275" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC81" s="276" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD81" s="276" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE81" s="277" t="s">
+      <c r="AA81" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB81" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC81" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD81" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE81" s="273" t="s">
         <v>321</v>
       </c>
-      <c r="AF81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH81" s="277">
+      <c r="AF81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH81" s="273">
         <v>2</v>
       </c>
-      <c r="AI81" s="278" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS81" s="278" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW81" s="279" t="s">
+      <c r="AI81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS81" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW81" s="275" t="s">
         <v>340</v>
       </c>
-      <c r="AX81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY81" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ81" s="277" t="s">
+      <c r="AX81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY81" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ81" s="273" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="82" spans="2:52">
-      <c r="B82" s="263" t="s">
+      <c r="B82" s="259" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="264" t="s">
+      <c r="C82" s="260" t="s">
         <v>341</v>
       </c>
-      <c r="D82" s="263" t="s">
-        <v>127</v>
-      </c>
-      <c r="E82" s="263" t="s">
+      <c r="D82" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="E82" s="259" t="s">
         <v>342</v>
       </c>
-      <c r="F82" s="265" t="b">
-        <v>1</v>
-      </c>
-      <c r="G82" s="265">
-        <v>1</v>
-      </c>
-      <c r="H82" s="266" t="s">
-        <v>127</v>
-      </c>
-      <c r="I82" s="266" t="s">
+      <c r="F82" s="261" t="b">
+        <v>1</v>
+      </c>
+      <c r="G82" s="261">
+        <v>1</v>
+      </c>
+      <c r="H82" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="I82" s="262" t="s">
         <v>342</v>
       </c>
-      <c r="J82" s="266" t="s">
-        <v>127</v>
-      </c>
-      <c r="K82" s="266" t="s">
-        <v>127</v>
-      </c>
-      <c r="L82" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="M82" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="N82" s="267" t="s">
-        <v>127</v>
-      </c>
-      <c r="O82" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="P82" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q82" s="268" t="s">
-        <v>127</v>
-      </c>
-      <c r="R82" s="269">
+      <c r="J82" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="K82" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="L82" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="M82" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="N82" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="O82" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="P82" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q82" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="R82" s="265">
         <v>100</v>
       </c>
-      <c r="S82" s="270" t="s">
+      <c r="S82" s="266" t="s">
         <v>343</v>
       </c>
-      <c r="T82" s="270" t="s">
+      <c r="T82" s="266" t="s">
         <v>311</v>
       </c>
-      <c r="U82" s="271" t="s">
-        <v>127</v>
-      </c>
-      <c r="V82" s="272" t="s">
+      <c r="U82" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="V82" s="268" t="s">
         <v>344</v>
       </c>
-      <c r="W82" s="273" t="s">
+      <c r="W82" s="269" t="s">
         <v>345</v>
       </c>
-      <c r="X82" s="274" t="b">
+      <c r="X82" s="270" t="b">
         <v>0</v>
       </c>
-      <c r="Y82" s="274" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z82" s="274" t="s">
+      <c r="Y82" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z82" s="270" t="s">
         <v>16</v>
       </c>
-      <c r="AA82" s="274" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB82" s="275" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC82" s="276" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD82" s="276" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE82" s="277" t="s">
+      <c r="AA82" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB82" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC82" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD82" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE82" s="273" t="s">
         <v>321</v>
       </c>
-      <c r="AF82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH82" s="277">
-        <v>1</v>
-      </c>
-      <c r="AI82" s="278" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS82" s="278" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY82" s="277" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ82" s="277" t="s">
+      <c r="AF82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH82" s="273">
+        <v>1</v>
+      </c>
+      <c r="AI82" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS82" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY82" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ82" s="273" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="85" spans="2:52" ht="26.25">
-      <c r="B85" s="246" t="s">
+      <c r="B85" s="278" t="s">
         <v>330</v>
       </c>
-      <c r="C85" s="246"/>
-      <c r="D85" s="246"/>
-      <c r="E85" s="246"/>
+      <c r="C85" s="278"/>
+      <c r="D85" s="278"/>
+      <c r="E85" s="278"/>
     </row>
     <row r="87" spans="2:52" ht="135">
       <c r="B87" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="C87" s="241" t="s">
+      <c r="C87" s="240" t="s">
         <v>0</v>
       </c>
-      <c r="D87" s="242" t="s">
+      <c r="D87" s="241" t="s">
         <v>52</v>
       </c>
       <c r="E87" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="F87" s="242" t="s">
+      <c r="F87" s="241" t="s">
         <v>333</v>
       </c>
-      <c r="G87" s="243" t="s">
+      <c r="G87" s="242" t="s">
         <v>334</v>
       </c>
-      <c r="H87" s="243" t="s">
+      <c r="H87" s="242" t="s">
         <v>335</v>
       </c>
-      <c r="I87" s="243" t="s">
+      <c r="I87" s="242" t="s">
         <v>336</v>
       </c>
     </row>
@@ -18126,18 +18173,18 @@
     <mergeCell ref="B85:E85"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F82">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="66" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D88)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18153,9 +18200,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -18205,31 +18252,31 @@
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="244"/>
-      <c r="AB1" s="244"/>
+      <c r="AA1" s="276"/>
+      <c r="AB1" s="276"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="245"/>
-      <c r="AE1" s="245"/>
-      <c r="AF1" s="245"/>
-      <c r="AG1" s="245"/>
-      <c r="AH1" s="245"/>
-      <c r="AI1" s="245"/>
-      <c r="AJ1" s="245"/>
-      <c r="AK1" s="245"/>
-      <c r="AL1" s="245"/>
-      <c r="AM1" s="245"/>
-      <c r="AN1" s="245"/>
-      <c r="AO1" s="245"/>
-      <c r="AP1" s="245"/>
-      <c r="AQ1" s="245"/>
-      <c r="AR1" s="245"/>
-      <c r="AS1" s="245"/>
-      <c r="AT1" s="245"/>
-      <c r="AU1" s="245"/>
-      <c r="AV1" s="245"/>
-      <c r="AW1" s="245"/>
-      <c r="AX1" s="245"/>
-      <c r="AY1" s="245"/>
+      <c r="AD1" s="277"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="277"/>
+      <c r="AH1" s="277"/>
+      <c r="AI1" s="277"/>
+      <c r="AJ1" s="277"/>
+      <c r="AK1" s="277"/>
+      <c r="AL1" s="277"/>
+      <c r="AM1" s="277"/>
+      <c r="AN1" s="277"/>
+      <c r="AO1" s="277"/>
+      <c r="AP1" s="277"/>
+      <c r="AQ1" s="277"/>
+      <c r="AR1" s="277"/>
+      <c r="AS1" s="277"/>
+      <c r="AT1" s="277"/>
+      <c r="AU1" s="277"/>
+      <c r="AV1" s="277"/>
+      <c r="AW1" s="277"/>
+      <c r="AX1" s="277"/>
+      <c r="AY1" s="277"/>
     </row>
     <row r="2" spans="2:51" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
@@ -18256,7 +18303,9 @@
       <c r="I2" s="239" t="s">
         <v>320</v>
       </c>
-      <c r="J2" s="240"/>
+      <c r="J2" s="239" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="3" spans="2:51">
       <c r="B3" s="27" t="s">
@@ -18282,6 +18331,9 @@
       </c>
       <c r="I3" s="237" t="s">
         <v>127</v>
+      </c>
+      <c r="J3" s="237">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1">

</xml_diff>

<commit_message>
Adding a new variable to show this popup in a loop (watching a number of ads)
Former-commit-id: 27443cbb1bbd916313d4d8c3037da01232fe52fd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="352">
   <si>
     <t>[sku]</t>
   </si>
@@ -1067,16 +1067,38 @@
     <t>TID_REMOVE_ADS_OFFER_NAME</t>
   </si>
   <si>
-    <t>[interstitialsBeforeNoAdsPopup]</t>
+    <t>[interstitialsBeforeFirstNoAdsPopup]</t>
+  </si>
+  <si>
+    <t>interstitialsBeforeFirstNoAdsPopup</t>
+  </si>
+  <si>
+    <t>Intersticials player see before first time we show the 'removeAds' offer</t>
+  </si>
+  <si>
+    <t>interstitialsBetweenNoAdsPopup</t>
+  </si>
+  <si>
+    <t>If &lt; 1 won't show anymore this popup. If &gt;= 1 will be a loop showing this popup</t>
+  </si>
+  <si>
+    <t>[interstitialsBetweenNoAdsPopup]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1239,6 +1261,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1669,70 +1697,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1740,766 +1771,856 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="71">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5243,46 +5364,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5311,81 +5392,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="B2:AZ82"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="62"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="61"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="60"/>
-    <tableColumn id="49" name="[type]" dataDxfId="59"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="58"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="57"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="56"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="55"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="54"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="53"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="52"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="51"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="50"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="49"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="48"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="47"/>
-    <tableColumn id="7" name="[order]" dataDxfId="46"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="45"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="44"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="43"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="42"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="41"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="40"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="39"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="38"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="37"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="36"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="35"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="34"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="33"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="32"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="31"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="30"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="29"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="28"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="27"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="26"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="25"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="24"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="23"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="22"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="21"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="20"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="19"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="18"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="17"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="16"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="15"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="14"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="13"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="12"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="65"/>
+    <tableColumn id="49" name="[type]" dataDxfId="64"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="63"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="62"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="61"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="60"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="59"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="58"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="57"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="56"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="55"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="54"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="53"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="52"/>
+    <tableColumn id="7" name="[order]" dataDxfId="51"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="50"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="49"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="48"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="47"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="46"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="45"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="44"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="43"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="42"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="41"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="40"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="39"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="38"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="37"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="36"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="35"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="34"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="33"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="32"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="31"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="30"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="29"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="28"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="27"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="26"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="25"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="24"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="23"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="22"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="21"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="20"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="19"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="18"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:J3" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="B2:J3"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="8"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="6"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="5"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="4"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="3"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="2"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="1"/>
-    <tableColumn id="7" name="[interstitialsBeforeNoAdsPopup]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="B2:K3"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="11"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="10"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="9"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="8"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="7"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="6"/>
+    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="5"/>
+    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5691,7 +5773,7 @@
   <dimension ref="B1:AZ88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AW84" sqref="AW84"/>
     </sheetView>
   </sheetViews>
@@ -18173,18 +18255,18 @@
     <mergeCell ref="B85:E85"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F82">
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D88)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18202,7 +18284,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -18216,8 +18298,8 @@
     <col min="7" max="8" width="13.875" customWidth="1"/>
     <col min="9" max="9" width="10.125" customWidth="1"/>
     <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="12" max="12" width="41.25" customWidth="1"/>
     <col min="13" max="13" width="9.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="16" width="7.5" bestFit="1" customWidth="1"/>
@@ -18278,7 +18360,7 @@
       <c r="AX1" s="277"/>
       <c r="AY1" s="277"/>
     </row>
-    <row r="2" spans="2:51" ht="149.1" customHeight="1">
+    <row r="2" spans="2:51" ht="190.5" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>313</v>
       </c>
@@ -18305,6 +18387,9 @@
       </c>
       <c r="J2" s="239" t="s">
         <v>346</v>
+      </c>
+      <c r="K2" s="239" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="2:51">
@@ -18334,6 +18419,26 @@
       </c>
       <c r="J3" s="237">
         <v>4</v>
+      </c>
+      <c r="K3" s="281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:51" ht="16.5">
+      <c r="L8" s="280" t="s">
+        <v>347</v>
+      </c>
+      <c r="M8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="2:51" ht="16.5">
+      <c r="D9" s="279"/>
+      <c r="L9" s="279" t="s">
+        <v>349</v>
+      </c>
+      <c r="M9" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1">

</xml_diff>

<commit_message>
Adding offers for the feature
Former-commit-id: 4fd9f3f432051914cd053fb76fe71e264be9a5e2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535" activeTab="1"/>
+    <workbookView xWindow="9795" yWindow="1335" windowWidth="32700" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Packs" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="357">
   <si>
     <t>[sku]</t>
   </si>
@@ -1052,9 +1052,6 @@
     <t>2:999</t>
   </si>
   <si>
-    <t>removeAdsOffer</t>
-  </si>
-  <si>
     <t>removeAds</t>
   </si>
   <si>
@@ -1083,6 +1080,24 @@
   </si>
   <si>
     <t>[interstitialsBetweenNoAdsPopup]</t>
+  </si>
+  <si>
+    <t>removeAdsOffer1</t>
+  </si>
+  <si>
+    <t>removeAdsOffer2</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.remove_ads_offer_4</t>
+  </si>
+  <si>
+    <t>removeAdsOffer3</t>
+  </si>
+  <si>
+    <t>com.ubisoft.hungrydragon.remove_ads_offer_2</t>
   </si>
 </sst>
 </file>
@@ -2514,6 +2529,15 @@
     <xf numFmtId="49" fontId="24" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2522,64 +2546,31 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="81">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2620,6 +2611,130 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5392,82 +5507,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ82" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68">
-  <autoFilter ref="B2:AZ82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ84" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78">
+  <autoFilter ref="B2:AZ84"/>
   <sortState ref="B3:AZ76">
     <sortCondition ref="F2:F76"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="67"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="65"/>
-    <tableColumn id="49" name="[type]" dataDxfId="64"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="63"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="62"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="61"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="60"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="59"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="58"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="57"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="56"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="55"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="54"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="53"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="52"/>
-    <tableColumn id="7" name="[order]" dataDxfId="51"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="50"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="49"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="48"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="47"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="46"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="45"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="44"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="43"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="42"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="41"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="40"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="39"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="38"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="37"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="36"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="35"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="34"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="33"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="32"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="31"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="30"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="29"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="28"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="27"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="26"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="25"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="24"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="23"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="22"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="21"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="20"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="19"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="18"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="17"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="75"/>
+    <tableColumn id="49" name="[type]" dataDxfId="74"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="73"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="72"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="71"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="70"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="69"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="68"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="67"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="66"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="65"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="64"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="63"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="62"/>
+    <tableColumn id="7" name="[order]" dataDxfId="61"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="60"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="59"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="58"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="57"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="55"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="54"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="53"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="52"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="51"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="50"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="49"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="48"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="47"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="46"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="45"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="44"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="43"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="42"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="41"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="40"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="39"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="38"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="37"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="36"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="35"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="34"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="33"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="32"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="31"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="30"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="29"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="28"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="B2:K3"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="11"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="10"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="9"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="8"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="7"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="6"/>
-    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="5"/>
-    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="0"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="23"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="22"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="21"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="20"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="19"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="18"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="17"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="16"/>
+    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="15"/>
+    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5770,11 +5885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AZ88"/>
+  <dimension ref="B1:AZ89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW84" sqref="AW84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5834,35 +5949,35 @@
       <c r="V1" s="210" t="s">
         <v>310</v>
       </c>
-      <c r="AA1" s="276" t="s">
+      <c r="AA1" s="279" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="276"/>
+      <c r="AB1" s="279"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="277" t="s">
+      <c r="AD1" s="280" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="277"/>
-      <c r="AF1" s="277"/>
-      <c r="AG1" s="277"/>
-      <c r="AH1" s="277"/>
-      <c r="AI1" s="277"/>
-      <c r="AJ1" s="277"/>
-      <c r="AK1" s="277"/>
-      <c r="AL1" s="277"/>
-      <c r="AM1" s="277"/>
-      <c r="AN1" s="277"/>
-      <c r="AO1" s="277"/>
-      <c r="AP1" s="277"/>
-      <c r="AQ1" s="277"/>
-      <c r="AR1" s="277"/>
-      <c r="AS1" s="277"/>
-      <c r="AT1" s="277"/>
-      <c r="AU1" s="277"/>
-      <c r="AV1" s="277"/>
-      <c r="AW1" s="277"/>
-      <c r="AX1" s="277"/>
-      <c r="AY1" s="277"/>
+      <c r="AE1" s="280"/>
+      <c r="AF1" s="280"/>
+      <c r="AG1" s="280"/>
+      <c r="AH1" s="280"/>
+      <c r="AI1" s="280"/>
+      <c r="AJ1" s="280"/>
+      <c r="AK1" s="280"/>
+      <c r="AL1" s="280"/>
+      <c r="AM1" s="280"/>
+      <c r="AN1" s="280"/>
+      <c r="AO1" s="280"/>
+      <c r="AP1" s="280"/>
+      <c r="AQ1" s="280"/>
+      <c r="AR1" s="280"/>
+      <c r="AS1" s="280"/>
+      <c r="AT1" s="280"/>
+      <c r="AU1" s="280"/>
+      <c r="AV1" s="280"/>
+      <c r="AW1" s="280"/>
+      <c r="AX1" s="280"/>
+      <c r="AY1" s="280"/>
     </row>
     <row r="2" spans="2:52" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
@@ -18038,14 +18153,14 @@
         <v>2</v>
       </c>
       <c r="C82" s="260" t="s">
+        <v>351</v>
+      </c>
+      <c r="D82" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="E82" s="259" t="s">
         <v>341</v>
       </c>
-      <c r="D82" s="259" t="s">
-        <v>127</v>
-      </c>
-      <c r="E82" s="259" t="s">
-        <v>342</v>
-      </c>
       <c r="F82" s="261" t="b">
         <v>1</v>
       </c>
@@ -18056,7 +18171,7 @@
         <v>127</v>
       </c>
       <c r="I82" s="262" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J82" s="262" t="s">
         <v>127</v>
@@ -18086,7 +18201,7 @@
         <v>100</v>
       </c>
       <c r="S82" s="266" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="T82" s="266" t="s">
         <v>311</v>
@@ -18095,10 +18210,10 @@
         <v>127</v>
       </c>
       <c r="V82" s="268" t="s">
+        <v>343</v>
+      </c>
+      <c r="W82" s="269" t="s">
         <v>344</v>
-      </c>
-      <c r="W82" s="269" t="s">
-        <v>345</v>
       </c>
       <c r="X82" s="270" t="b">
         <v>0</v>
@@ -18188,63 +18303,373 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="2:52" ht="26.25">
-      <c r="B85" s="278" t="s">
+    <row r="83" spans="2:52">
+      <c r="B83" s="259" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="260" t="s">
+        <v>352</v>
+      </c>
+      <c r="D83" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="E83" s="259" t="s">
+        <v>341</v>
+      </c>
+      <c r="F83" s="261" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="261">
+        <v>1</v>
+      </c>
+      <c r="H83" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="I83" s="262" t="s">
+        <v>341</v>
+      </c>
+      <c r="J83" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="K83" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="L83" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="M83" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="N83" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="O83" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="P83" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q83" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="R83" s="265">
+        <v>100</v>
+      </c>
+      <c r="S83" s="266" t="s">
+        <v>353</v>
+      </c>
+      <c r="T83" s="266" t="s">
+        <v>311</v>
+      </c>
+      <c r="U83" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="V83" s="268" t="s">
+        <v>354</v>
+      </c>
+      <c r="W83" s="269" t="s">
+        <v>344</v>
+      </c>
+      <c r="X83" s="270" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z83" s="270" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA83" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB83" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC83" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD83" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE83" s="273" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH83" s="273">
+        <v>1</v>
+      </c>
+      <c r="AI83" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS83" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW83" s="275" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY83" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ83" s="273" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="2:52">
+      <c r="B84" s="259" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="260" t="s">
+        <v>355</v>
+      </c>
+      <c r="D84" s="259" t="s">
+        <v>127</v>
+      </c>
+      <c r="E84" s="259" t="s">
+        <v>341</v>
+      </c>
+      <c r="F84" s="261" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" s="261">
+        <v>1</v>
+      </c>
+      <c r="H84" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="I84" s="262" t="s">
+        <v>341</v>
+      </c>
+      <c r="J84" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="K84" s="262" t="s">
+        <v>127</v>
+      </c>
+      <c r="L84" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="M84" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="N84" s="263" t="s">
+        <v>127</v>
+      </c>
+      <c r="O84" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="P84" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q84" s="264" t="s">
+        <v>127</v>
+      </c>
+      <c r="R84" s="265">
+        <v>100</v>
+      </c>
+      <c r="S84" s="266" t="s">
+        <v>101</v>
+      </c>
+      <c r="T84" s="266" t="s">
+        <v>311</v>
+      </c>
+      <c r="U84" s="267" t="s">
+        <v>127</v>
+      </c>
+      <c r="V84" s="268" t="s">
+        <v>356</v>
+      </c>
+      <c r="W84" s="269" t="s">
+        <v>344</v>
+      </c>
+      <c r="X84" s="270" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y84" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z84" s="270" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA84" s="270" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB84" s="271" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC84" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD84" s="272" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE84" s="273" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH84" s="273">
+        <v>1</v>
+      </c>
+      <c r="AI84" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS84" s="274" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW84" s="275" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY84" s="273" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ84" s="273" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="2:52" ht="26.25">
+      <c r="B86" s="281" t="s">
         <v>330</v>
       </c>
-      <c r="C85" s="278"/>
-      <c r="D85" s="278"/>
-      <c r="E85" s="278"/>
+      <c r="C86" s="281"/>
+      <c r="D86" s="281"/>
+      <c r="E86" s="281"/>
     </row>
-    <row r="87" spans="2:52" ht="135">
-      <c r="B87" s="23" t="s">
+    <row r="88" spans="2:52" ht="135">
+      <c r="B88" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="C87" s="240" t="s">
+      <c r="C88" s="240" t="s">
         <v>0</v>
       </c>
-      <c r="D87" s="241" t="s">
+      <c r="D88" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="E87" s="23" t="s">
+      <c r="E88" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="F87" s="241" t="s">
+      <c r="F88" s="241" t="s">
         <v>333</v>
       </c>
-      <c r="G87" s="242" t="s">
+      <c r="G88" s="242" t="s">
         <v>334</v>
       </c>
-      <c r="H87" s="242" t="s">
+      <c r="H88" s="242" t="s">
         <v>335</v>
       </c>
-      <c r="I87" s="242" t="s">
+      <c r="I88" s="242" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="88" spans="2:52">
-      <c r="B88" s="211" t="s">
+    <row r="89" spans="2:52">
+      <c r="B89" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="C88" s="211" t="s">
+      <c r="C89" s="211" t="s">
         <v>337</v>
       </c>
-      <c r="D88" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="211">
+      <c r="D89" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="211">
         <v>0</v>
       </c>
-      <c r="F88" s="211">
+      <c r="F89" s="211">
         <v>120</v>
       </c>
-      <c r="G88" s="211">
-        <v>1</v>
-      </c>
-      <c r="H88" s="211" t="s">
+      <c r="G89" s="211">
+        <v>1</v>
+      </c>
+      <c r="H89" s="211" t="s">
         <v>338</v>
       </c>
-      <c r="I88" s="211" t="s">
+      <c r="I89" s="211" t="s">
         <v>339</v>
       </c>
     </row>
@@ -18252,22 +18677,46 @@
   <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
-    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F82">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="F3:F84">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",D88)))</formula>
+  <conditionalFormatting sqref="D89">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",D88)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D89)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F84)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18282,7 +18731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
@@ -18334,31 +18783,31 @@
       <c r="T1" s="5"/>
       <c r="U1" s="210"/>
       <c r="V1" s="210"/>
-      <c r="AA1" s="276"/>
-      <c r="AB1" s="276"/>
+      <c r="AA1" s="279"/>
+      <c r="AB1" s="279"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="277"/>
-      <c r="AE1" s="277"/>
-      <c r="AF1" s="277"/>
-      <c r="AG1" s="277"/>
-      <c r="AH1" s="277"/>
-      <c r="AI1" s="277"/>
-      <c r="AJ1" s="277"/>
-      <c r="AK1" s="277"/>
-      <c r="AL1" s="277"/>
-      <c r="AM1" s="277"/>
-      <c r="AN1" s="277"/>
-      <c r="AO1" s="277"/>
-      <c r="AP1" s="277"/>
-      <c r="AQ1" s="277"/>
-      <c r="AR1" s="277"/>
-      <c r="AS1" s="277"/>
-      <c r="AT1" s="277"/>
-      <c r="AU1" s="277"/>
-      <c r="AV1" s="277"/>
-      <c r="AW1" s="277"/>
-      <c r="AX1" s="277"/>
-      <c r="AY1" s="277"/>
+      <c r="AD1" s="280"/>
+      <c r="AE1" s="280"/>
+      <c r="AF1" s="280"/>
+      <c r="AG1" s="280"/>
+      <c r="AH1" s="280"/>
+      <c r="AI1" s="280"/>
+      <c r="AJ1" s="280"/>
+      <c r="AK1" s="280"/>
+      <c r="AL1" s="280"/>
+      <c r="AM1" s="280"/>
+      <c r="AN1" s="280"/>
+      <c r="AO1" s="280"/>
+      <c r="AP1" s="280"/>
+      <c r="AQ1" s="280"/>
+      <c r="AR1" s="280"/>
+      <c r="AS1" s="280"/>
+      <c r="AT1" s="280"/>
+      <c r="AU1" s="280"/>
+      <c r="AV1" s="280"/>
+      <c r="AW1" s="280"/>
+      <c r="AX1" s="280"/>
+      <c r="AY1" s="280"/>
     </row>
     <row r="2" spans="2:51" ht="190.5" customHeight="1">
       <c r="B2" s="1" t="s">
@@ -18386,10 +18835,10 @@
         <v>320</v>
       </c>
       <c r="J2" s="239" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K2" s="239" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="2:51">
@@ -18420,25 +18869,25 @@
       <c r="J3" s="237">
         <v>4</v>
       </c>
-      <c r="K3" s="281">
+      <c r="K3" s="278">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="16.5">
-      <c r="L8" s="280" t="s">
+      <c r="L8" s="277" t="s">
+        <v>346</v>
+      </c>
+      <c r="M8" t="s">
         <v>347</v>
-      </c>
-      <c r="M8" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="16.5">
-      <c r="D9" s="279"/>
-      <c r="L9" s="279" t="s">
+      <c r="D9" s="276"/>
+      <c r="L9" s="276" t="s">
+        <v>348</v>
+      </c>
+      <c r="M9" t="s">
         <v>349</v>
-      </c>
-      <c r="M9" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:183" s="205" customFormat="1" ht="16.5" thickBot="1">

</xml_diff>

<commit_message>
Adding offers needed for the AB test
Former-commit-id: 761d71334629cb8e9727ad5e073b54a82685ecea
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="378">
   <si>
     <t>[sku]</t>
   </si>
@@ -2569,6 +2569,60 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2577,74 +2631,12 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="82">
     <dxf>
       <font>
         <b val="0"/>
@@ -5374,6 +5366,14 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -5532,6 +5532,46 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5560,86 +5600,86 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ88" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="B2:AZ88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ90" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B2:AZ90">
     <filterColumn colId="4">
-      <colorFilter dxfId="0"/>
+      <colorFilter dxfId="64"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="B24:AZ86">
     <sortCondition descending="1" ref="E2:E88"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="64"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="62"/>
-    <tableColumn id="49" name="[type]" dataDxfId="61"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="60"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="59"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="58"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="57"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="56"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="55"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="54"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="53"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="52"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="51"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="50"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[order]" dataDxfId="48"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="47"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="46"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="45"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="44"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="43"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="42"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="41"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="40"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="39"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="38"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="37"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="36"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="35"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="34"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="33"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="32"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="31"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="30"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="29"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="28"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="27"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="26"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="25"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="24"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="23"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="22"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="21"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="20"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="19"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="18"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="17"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="16"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="15"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="14"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="63"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="62"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="61"/>
+    <tableColumn id="49" name="[type]" dataDxfId="60"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="59"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="58"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="57"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="56"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="55"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="54"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="53"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="52"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="51"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="50"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="49"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[order]" dataDxfId="47"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="46"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="45"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="44"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="43"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="42"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="41"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="40"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="39"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="38"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="37"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="36"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="35"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="34"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="33"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="32"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="31"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="30"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="29"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="28"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="27"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="26"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="25"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="24"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="23"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="22"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="21"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="20"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="19"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="18"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="17"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="16"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="15"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="14"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B2:K3"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="10"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="8"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="7"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="6"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="5"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="4"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="3"/>
-    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="2"/>
-    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="1"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="9"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="7"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="6"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="5"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="4"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="3"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="2"/>
+    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="1"/>
+    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5942,11 +5982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AZ93"/>
+  <dimension ref="B1:AZ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V75" sqref="V75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6007,35 +6047,35 @@
       <c r="V1" s="204" t="s">
         <v>297</v>
       </c>
-      <c r="AA1" s="264" t="s">
+      <c r="AA1" s="282" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="264"/>
+      <c r="AB1" s="282"/>
       <c r="AC1" s="18"/>
-      <c r="AD1" s="265" t="s">
+      <c r="AD1" s="283" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="265"/>
-      <c r="AF1" s="265"/>
-      <c r="AG1" s="265"/>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
-      <c r="AK1" s="265"/>
-      <c r="AL1" s="265"/>
-      <c r="AM1" s="265"/>
-      <c r="AN1" s="265"/>
-      <c r="AO1" s="265"/>
-      <c r="AP1" s="265"/>
-      <c r="AQ1" s="265"/>
-      <c r="AR1" s="265"/>
-      <c r="AS1" s="265"/>
-      <c r="AT1" s="265"/>
-      <c r="AU1" s="265"/>
-      <c r="AV1" s="265"/>
-      <c r="AW1" s="265"/>
-      <c r="AX1" s="265"/>
-      <c r="AY1" s="265"/>
+      <c r="AE1" s="283"/>
+      <c r="AF1" s="283"/>
+      <c r="AG1" s="283"/>
+      <c r="AH1" s="283"/>
+      <c r="AI1" s="283"/>
+      <c r="AJ1" s="283"/>
+      <c r="AK1" s="283"/>
+      <c r="AL1" s="283"/>
+      <c r="AM1" s="283"/>
+      <c r="AN1" s="283"/>
+      <c r="AO1" s="283"/>
+      <c r="AP1" s="283"/>
+      <c r="AQ1" s="283"/>
+      <c r="AR1" s="283"/>
+      <c r="AS1" s="283"/>
+      <c r="AT1" s="283"/>
+      <c r="AU1" s="283"/>
+      <c r="AV1" s="283"/>
+      <c r="AW1" s="283"/>
+      <c r="AX1" s="283"/>
+      <c r="AY1" s="283"/>
     </row>
     <row r="2" spans="2:52" ht="149.1" customHeight="1">
       <c r="B2" s="1" t="s">
@@ -9132,7 +9172,7 @@
       <c r="V24" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="W24" s="280" t="s">
+      <c r="W24" s="277" t="s">
         <v>221</v>
       </c>
       <c r="X24" s="21" t="b">
@@ -10492,13 +10532,13 @@
       <c r="N34" s="129" t="s">
         <v>126</v>
       </c>
-      <c r="O34" s="276" t="s">
-        <v>126</v>
-      </c>
-      <c r="P34" s="276" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q34" s="276" t="s">
+      <c r="O34" s="273" t="s">
+        <v>126</v>
+      </c>
+      <c r="P34" s="273" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q34" s="273" t="s">
         <v>126</v>
       </c>
       <c r="R34" s="46">
@@ -12506,7 +12546,7 @@
       <c r="J48" s="30">
         <v>100</v>
       </c>
-      <c r="K48" s="274" t="s">
+      <c r="K48" s="271" t="s">
         <v>126</v>
       </c>
       <c r="L48" s="31" t="s">
@@ -12774,7 +12814,7 @@
       <c r="B50" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="271" t="s">
+      <c r="C50" s="268" t="s">
         <v>196</v>
       </c>
       <c r="D50" s="55" t="s">
@@ -13086,7 +13126,7 @@
       </c>
       <c r="I52" s="30"/>
       <c r="J52" s="30"/>
-      <c r="K52" s="272"/>
+      <c r="K52" s="269"/>
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
       <c r="N52" s="31"/>
@@ -14380,13 +14420,13 @@
       <c r="K61" s="189" t="s">
         <v>367</v>
       </c>
-      <c r="L61" s="267" t="s">
-        <v>126</v>
-      </c>
-      <c r="M61" s="267" t="s">
-        <v>126</v>
-      </c>
-      <c r="N61" s="267" t="s">
+      <c r="L61" s="264" t="s">
+        <v>126</v>
+      </c>
+      <c r="M61" s="264" t="s">
+        <v>126</v>
+      </c>
+      <c r="N61" s="264" t="s">
         <v>126</v>
       </c>
       <c r="O61" s="190" t="s">
@@ -14508,7 +14548,7 @@
       <c r="B62" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="281" t="s">
+      <c r="C62" s="278" t="s">
         <v>181</v>
       </c>
       <c r="D62" s="175" t="s">
@@ -14532,7 +14572,7 @@
       <c r="J62" s="177">
         <v>1</v>
       </c>
-      <c r="K62" s="274" t="s">
+      <c r="K62" s="271" t="s">
         <v>368</v>
       </c>
       <c r="L62" s="178" t="s">
@@ -14541,7 +14581,7 @@
       <c r="M62" s="178">
         <v>1</v>
       </c>
-      <c r="N62" s="275" t="s">
+      <c r="N62" s="272" t="s">
         <v>369</v>
       </c>
       <c r="O62" s="179" t="s">
@@ -14663,7 +14703,7 @@
       <c r="B63" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="269" t="s">
+      <c r="C63" s="266" t="s">
         <v>190</v>
       </c>
       <c r="D63" s="41" t="s">
@@ -14851,7 +14891,7 @@
       <c r="M64" s="70">
         <v>1</v>
       </c>
-      <c r="N64" s="282" t="s">
+      <c r="N64" s="279" t="s">
         <v>372</v>
       </c>
       <c r="O64" s="71" t="s">
@@ -14973,7 +15013,7 @@
       <c r="B65" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="270" t="s">
+      <c r="C65" s="267" t="s">
         <v>191</v>
       </c>
       <c r="D65" s="155" t="s">
@@ -16329,7 +16369,7 @@
       <c r="G74" s="227">
         <v>1</v>
       </c>
-      <c r="H74" s="273" t="s">
+      <c r="H74" s="270" t="s">
         <v>126</v>
       </c>
       <c r="I74" s="228" t="s">
@@ -16365,10 +16405,10 @@
       <c r="S74" s="232" t="s">
         <v>329</v>
       </c>
-      <c r="T74" s="277" t="s">
+      <c r="T74" s="274" t="s">
         <v>298</v>
       </c>
-      <c r="U74" s="278" t="s">
+      <c r="U74" s="275" t="s">
         <v>126</v>
       </c>
       <c r="V74" s="234" t="s">
@@ -16410,10 +16450,10 @@
       <c r="AH74" s="239">
         <v>4</v>
       </c>
-      <c r="AI74" s="283" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ74" s="284" t="s">
+      <c r="AI74" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ74" s="281" t="s">
         <v>126</v>
       </c>
       <c r="AK74" s="239" t="s">
@@ -16465,304 +16505,322 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="2:52" hidden="1">
-      <c r="B75" s="27" t="s">
+    <row r="75" spans="2:52">
+      <c r="B75" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="D75" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E75" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="F75" s="29" t="b">
+      <c r="C75" s="243" t="s">
+        <v>339</v>
+      </c>
+      <c r="D75" s="219" t="s">
+        <v>126</v>
+      </c>
+      <c r="E75" s="219" t="s">
+        <v>328</v>
+      </c>
+      <c r="F75" s="227" t="b">
         <v>0</v>
       </c>
-      <c r="G75" s="29">
-        <v>1</v>
-      </c>
-      <c r="H75" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="31"/>
-      <c r="M75" s="31"/>
-      <c r="N75" s="31"/>
-      <c r="O75" s="32"/>
-      <c r="P75" s="32"/>
-      <c r="Q75" s="32"/>
-      <c r="R75" s="33">
-        <v>0</v>
-      </c>
-      <c r="S75" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="T75" s="47" t="s">
+      <c r="G75" s="227">
+        <v>1</v>
+      </c>
+      <c r="H75" s="270" t="s">
+        <v>126</v>
+      </c>
+      <c r="I75" s="228" t="s">
+        <v>328</v>
+      </c>
+      <c r="J75" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="K75" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="L75" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="M75" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="N75" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="O75" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="P75" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q75" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="R75" s="231">
+        <v>-24</v>
+      </c>
+      <c r="S75" s="232" t="s">
+        <v>340</v>
+      </c>
+      <c r="T75" s="274" t="s">
         <v>298</v>
       </c>
-      <c r="U75" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="V75" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="W75" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="X75" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y75" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z75" s="21" t="s">
+      <c r="U75" s="275" t="s">
+        <v>126</v>
+      </c>
+      <c r="V75" s="234" t="s">
+        <v>341</v>
+      </c>
+      <c r="W75" s="235" t="s">
+        <v>331</v>
+      </c>
+      <c r="X75" s="236" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y75" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z75" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="AA75" s="21">
-        <v>10</v>
-      </c>
-      <c r="AB75" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC75" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD75" s="37">
-        <v>2880</v>
-      </c>
-      <c r="AE75" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="AF75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH75" s="13">
-        <v>2</v>
-      </c>
-      <c r="AI75" s="130" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ75" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW75" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY75" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ75" s="13" t="s">
+      <c r="AA75" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB75" s="237" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC75" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD75" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE75" s="239" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH75" s="239">
+        <v>4</v>
+      </c>
+      <c r="AI75" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ75" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS75" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY75" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ75" s="239" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="76" spans="2:52">
-      <c r="B76" s="27" t="s">
+      <c r="B76" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E76" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="F76" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G76" s="29">
-        <v>1</v>
-      </c>
-      <c r="H76" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I76" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="J76" s="30">
-        <v>1</v>
-      </c>
-      <c r="K76" s="30" t="s">
-        <v>293</v>
-      </c>
-      <c r="L76" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M76" s="31">
-        <v>1</v>
-      </c>
-      <c r="N76" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="O76" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="P76" s="32">
-        <v>10000</v>
-      </c>
-      <c r="Q76" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="R76" s="33">
-        <v>-15</v>
-      </c>
-      <c r="S76" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="T76" s="47" t="s">
+      <c r="C76" s="243" t="s">
+        <v>342</v>
+      </c>
+      <c r="D76" s="219" t="s">
+        <v>126</v>
+      </c>
+      <c r="E76" s="219" t="s">
+        <v>328</v>
+      </c>
+      <c r="F76" s="227" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" s="227">
+        <v>1</v>
+      </c>
+      <c r="H76" s="270" t="s">
+        <v>126</v>
+      </c>
+      <c r="I76" s="228" t="s">
+        <v>328</v>
+      </c>
+      <c r="J76" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="K76" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="L76" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="M76" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="N76" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="O76" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="P76" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q76" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="R76" s="231">
+        <v>-24</v>
+      </c>
+      <c r="S76" s="232" t="s">
+        <v>100</v>
+      </c>
+      <c r="T76" s="274" t="s">
         <v>298</v>
       </c>
-      <c r="U76" s="35" t="s">
-        <v>344</v>
-      </c>
-      <c r="V76" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="W76" s="279" t="s">
-        <v>289</v>
-      </c>
-      <c r="X76" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y76" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z76" s="21" t="s">
+      <c r="U76" s="275" t="s">
+        <v>126</v>
+      </c>
+      <c r="V76" s="234" t="s">
+        <v>343</v>
+      </c>
+      <c r="W76" s="235" t="s">
+        <v>331</v>
+      </c>
+      <c r="X76" s="236" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y76" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z76" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="AA76" s="21">
-        <v>10</v>
-      </c>
-      <c r="AB76" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC76" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD76" s="37">
-        <v>2880</v>
-      </c>
-      <c r="AE76" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="AF76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH76" s="13">
-        <v>2</v>
-      </c>
-      <c r="AI76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ76" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO76" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="AP76" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="AQ76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW76" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="AX76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY76" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ76" s="13" t="s">
+      <c r="AA76" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB76" s="237" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC76" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD76" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE76" s="239" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH76" s="239">
+        <v>4</v>
+      </c>
+      <c r="AI76" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ76" s="281" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS76" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY76" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ76" s="239" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="77" spans="2:52" hidden="1">
+    <row r="77" spans="2:52">
       <c r="B77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="38" t="s">
-        <v>145</v>
+      <c r="C77" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="D77" s="24" t="s">
         <v>126</v>
@@ -16782,8 +16840,8 @@
       <c r="I77" s="30"/>
       <c r="J77" s="30"/>
       <c r="K77" s="30"/>
-      <c r="L77" s="129"/>
-      <c r="M77" s="129"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
       <c r="N77" s="31"/>
       <c r="O77" s="32"/>
       <c r="P77" s="32"/>
@@ -16792,7 +16850,7 @@
         <v>0</v>
       </c>
       <c r="S77" s="34" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="T77" s="47" t="s">
         <v>298</v>
@@ -16801,10 +16859,10 @@
         <v>126</v>
       </c>
       <c r="V77" s="36" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="W77" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X77" s="21" t="b">
         <v>1</v>
@@ -16818,7 +16876,7 @@
       <c r="AA77" s="21">
         <v>10</v>
       </c>
-      <c r="AB77" s="167" t="s">
+      <c r="AB77" s="37" t="s">
         <v>126</v>
       </c>
       <c r="AC77" s="37" t="s">
@@ -16842,7 +16900,7 @@
       <c r="AI77" s="130" t="s">
         <v>126</v>
       </c>
-      <c r="AJ77" s="132" t="s">
+      <c r="AJ77" s="53" t="s">
         <v>126</v>
       </c>
       <c r="AK77" s="13" t="s">
@@ -16882,7 +16940,7 @@
         <v>126</v>
       </c>
       <c r="AW77" s="20" t="s">
-        <v>171</v>
+        <v>294</v>
       </c>
       <c r="AX77" s="13" t="s">
         <v>126</v>
@@ -16894,21 +16952,21 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="2:52" hidden="1">
+    <row r="78" spans="2:52">
       <c r="B78" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>177</v>
       </c>
       <c r="F78" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="29">
         <v>1</v>
@@ -16916,32 +16974,50 @@
       <c r="H78" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I78" s="30"/>
-      <c r="J78" s="30"/>
-      <c r="K78" s="153"/>
-      <c r="L78" s="129"/>
-      <c r="M78" s="129"/>
-      <c r="N78" s="154"/>
-      <c r="O78" s="32"/>
-      <c r="P78" s="32"/>
-      <c r="Q78" s="32"/>
+      <c r="I78" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="J78" s="30">
+        <v>1</v>
+      </c>
+      <c r="K78" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="L78" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="M78" s="31">
+        <v>1</v>
+      </c>
+      <c r="N78" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="O78" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="P78" s="32">
+        <v>10000</v>
+      </c>
+      <c r="Q78" s="32" t="s">
+        <v>126</v>
+      </c>
       <c r="R78" s="33">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="S78" s="34" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="T78" s="47" t="s">
         <v>298</v>
       </c>
       <c r="U78" s="35" t="s">
-        <v>126</v>
+        <v>344</v>
       </c>
       <c r="V78" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="W78" s="4" t="s">
-        <v>288</v>
+        <v>80</v>
+      </c>
+      <c r="W78" s="276" t="s">
+        <v>289</v>
       </c>
       <c r="X78" s="21" t="b">
         <v>1</v>
@@ -16955,7 +17031,9 @@
       <c r="AA78" s="21">
         <v>10</v>
       </c>
-      <c r="AB78" s="37"/>
+      <c r="AB78" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="AC78" s="37" t="s">
         <v>126</v>
       </c>
@@ -16974,7 +17052,7 @@
       <c r="AH78" s="13">
         <v>2</v>
       </c>
-      <c r="AI78" s="130" t="s">
+      <c r="AI78" s="13" t="s">
         <v>126</v>
       </c>
       <c r="AJ78" s="53" t="s">
@@ -16993,10 +17071,10 @@
         <v>126</v>
       </c>
       <c r="AO78" s="13" t="s">
-        <v>126</v>
+        <v>357</v>
       </c>
       <c r="AP78" s="13" t="s">
-        <v>126</v>
+        <v>356</v>
       </c>
       <c r="AQ78" s="13" t="s">
         <v>126</v>
@@ -17004,7 +17082,9 @@
       <c r="AR78" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AS78" s="13"/>
+      <c r="AS78" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="AT78" s="13" t="s">
         <v>126</v>
       </c>
@@ -17015,7 +17095,7 @@
         <v>126</v>
       </c>
       <c r="AW78" s="20" t="s">
-        <v>285</v>
+        <v>358</v>
       </c>
       <c r="AX78" s="13" t="s">
         <v>126</v>
@@ -17031,8 +17111,8 @@
       <c r="B79" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="28" t="s">
-        <v>109</v>
+      <c r="C79" s="38" t="s">
+        <v>145</v>
       </c>
       <c r="D79" s="24" t="s">
         <v>126</v>
@@ -17041,7 +17121,7 @@
         <v>177</v>
       </c>
       <c r="F79" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" s="29">
         <v>1</v>
@@ -17049,35 +17129,17 @@
       <c r="H79" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I79" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="J79" s="30">
-        <v>1</v>
-      </c>
-      <c r="K79" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="L79" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M79" s="31">
-        <v>1</v>
-      </c>
-      <c r="N79" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="O79" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="P79" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q79" s="32" t="s">
-        <v>126</v>
-      </c>
+      <c r="I79" s="30"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79" s="129"/>
+      <c r="M79" s="129"/>
+      <c r="N79" s="31"/>
+      <c r="O79" s="32"/>
+      <c r="P79" s="32"/>
+      <c r="Q79" s="32"/>
       <c r="R79" s="33">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="S79" s="34" t="s">
         <v>75</v>
@@ -17085,14 +17147,14 @@
       <c r="T79" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="U79" s="268" t="s">
-        <v>150</v>
+      <c r="U79" s="35" t="s">
+        <v>126</v>
       </c>
       <c r="V79" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="W79" s="280" t="s">
-        <v>287</v>
+        <v>156</v>
+      </c>
+      <c r="W79" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="X79" s="21" t="b">
         <v>1</v>
@@ -17106,7 +17168,9 @@
       <c r="AA79" s="21">
         <v>10</v>
       </c>
-      <c r="AB79" s="37"/>
+      <c r="AB79" s="167" t="s">
+        <v>126</v>
+      </c>
       <c r="AC79" s="37" t="s">
         <v>126</v>
       </c>
@@ -17125,10 +17189,10 @@
       <c r="AH79" s="13">
         <v>2</v>
       </c>
-      <c r="AI79" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ79" s="53" t="s">
+      <c r="AI79" s="130" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ79" s="132" t="s">
         <v>126</v>
       </c>
       <c r="AK79" s="13" t="s">
@@ -17147,7 +17211,7 @@
         <v>126</v>
       </c>
       <c r="AP79" s="13" t="s">
-        <v>278</v>
+        <v>126</v>
       </c>
       <c r="AQ79" s="13" t="s">
         <v>126</v>
@@ -17168,7 +17232,7 @@
         <v>126</v>
       </c>
       <c r="AW79" s="20" t="s">
-        <v>327</v>
+        <v>171</v>
       </c>
       <c r="AX79" s="13" t="s">
         <v>126</v>
@@ -17180,12 +17244,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="80" spans="2:52" hidden="1">
+    <row r="80" spans="2:52">
       <c r="B80" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="174" t="s">
-        <v>142</v>
+      <c r="C80" s="38" t="s">
+        <v>144</v>
       </c>
       <c r="D80" s="24" t="s">
         <v>126</v>
@@ -17196,7 +17260,7 @@
       <c r="F80" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="G80" s="68">
+      <c r="G80" s="29">
         <v>1</v>
       </c>
       <c r="H80" s="30" t="b">
@@ -17204,18 +17268,18 @@
       </c>
       <c r="I80" s="30"/>
       <c r="J80" s="30"/>
-      <c r="K80" s="30"/>
-      <c r="L80" s="31"/>
-      <c r="M80" s="31"/>
-      <c r="N80" s="31"/>
+      <c r="K80" s="153"/>
+      <c r="L80" s="129"/>
+      <c r="M80" s="129"/>
+      <c r="N80" s="154"/>
       <c r="O80" s="32"/>
       <c r="P80" s="32"/>
       <c r="Q80" s="32"/>
       <c r="R80" s="33">
         <v>0</v>
       </c>
-      <c r="S80" s="72" t="s">
-        <v>75</v>
+      <c r="S80" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="T80" s="47" t="s">
         <v>298</v>
@@ -17223,11 +17287,11 @@
       <c r="U80" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="V80" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="W80" s="74" t="s">
-        <v>281</v>
+      <c r="V80" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="W80" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="X80" s="21" t="b">
         <v>1</v>
@@ -17241,9 +17305,7 @@
       <c r="AA80" s="21">
         <v>10</v>
       </c>
-      <c r="AB80" s="167" t="s">
-        <v>126</v>
-      </c>
+      <c r="AB80" s="37"/>
       <c r="AC80" s="37" t="s">
         <v>126</v>
       </c>
@@ -17292,9 +17354,7 @@
       <c r="AR80" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AS80" s="130" t="s">
-        <v>126</v>
-      </c>
+      <c r="AS80" s="13"/>
       <c r="AT80" s="13" t="s">
         <v>126</v>
       </c>
@@ -17305,7 +17365,7 @@
         <v>126</v>
       </c>
       <c r="AW80" s="20" t="s">
-        <v>165</v>
+        <v>285</v>
       </c>
       <c r="AX80" s="13" t="s">
         <v>126</v>
@@ -17322,7 +17382,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D81" s="24" t="s">
         <v>126</v>
@@ -17345,44 +17405,44 @@
       <c r="J81" s="30">
         <v>1</v>
       </c>
-      <c r="K81" s="131" t="s">
-        <v>50</v>
-      </c>
-      <c r="L81" s="129" t="s">
+      <c r="K81" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="L81" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="M81" s="129">
+      <c r="M81" s="31">
         <v>1</v>
       </c>
       <c r="N81" s="31" t="s">
-        <v>286</v>
+        <v>218</v>
       </c>
       <c r="O81" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="P81" s="32">
-        <v>1</v>
+        <v>126</v>
+      </c>
+      <c r="P81" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="Q81" s="32" t="s">
-        <v>218</v>
+        <v>126</v>
       </c>
       <c r="R81" s="33">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="S81" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="T81" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="T81" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="U81" s="200" t="s">
-        <v>292</v>
+      <c r="U81" s="265" t="s">
+        <v>150</v>
       </c>
       <c r="V81" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="W81" s="279" t="s">
-        <v>359</v>
+        <v>83</v>
+      </c>
+      <c r="W81" s="277" t="s">
+        <v>287</v>
       </c>
       <c r="X81" s="21" t="b">
         <v>1</v>
@@ -17396,9 +17456,7 @@
       <c r="AA81" s="21">
         <v>10</v>
       </c>
-      <c r="AB81" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="AB81" s="37"/>
       <c r="AC81" s="37" t="s">
         <v>126</v>
       </c>
@@ -17415,12 +17473,12 @@
         <v>126</v>
       </c>
       <c r="AH81" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI81" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AJ81" s="13" t="s">
+      <c r="AJ81" s="53" t="s">
         <v>126</v>
       </c>
       <c r="AK81" s="13" t="s">
@@ -17439,7 +17497,7 @@
         <v>126</v>
       </c>
       <c r="AP81" s="13" t="s">
-        <v>360</v>
+        <v>278</v>
       </c>
       <c r="AQ81" s="13" t="s">
         <v>126</v>
@@ -17473,312 +17531,294 @@
       </c>
     </row>
     <row r="82" spans="2:52">
-      <c r="B82" s="219" t="s">
+      <c r="B82" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="226" t="s">
-        <v>311</v>
-      </c>
-      <c r="D82" s="219" t="s">
-        <v>126</v>
-      </c>
-      <c r="E82" s="219" t="s">
-        <v>299</v>
-      </c>
-      <c r="F82" s="227" t="b">
-        <v>1</v>
-      </c>
-      <c r="G82" s="227">
-        <v>1</v>
-      </c>
-      <c r="H82" s="228" t="s">
-        <v>126</v>
-      </c>
-      <c r="I82" s="228" t="s">
-        <v>17</v>
-      </c>
-      <c r="J82" s="228">
-        <v>1</v>
-      </c>
-      <c r="K82" s="228" t="s">
-        <v>217</v>
-      </c>
-      <c r="L82" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="M82" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="N82" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="O82" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="P82" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q82" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="R82" s="231">
-        <v>-25</v>
-      </c>
-      <c r="S82" s="232" t="s">
-        <v>126</v>
-      </c>
-      <c r="T82" s="232" t="s">
-        <v>309</v>
-      </c>
-      <c r="U82" s="233" t="s">
-        <v>126</v>
-      </c>
-      <c r="V82" s="234" t="s">
-        <v>126</v>
-      </c>
-      <c r="W82" s="235" t="s">
-        <v>312</v>
-      </c>
-      <c r="X82" s="236" t="b">
+      <c r="C82" s="174" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E82" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F82" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="Y82" s="236" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z82" s="236" t="s">
+      <c r="G82" s="68">
+        <v>1</v>
+      </c>
+      <c r="H82" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" s="30"/>
+      <c r="J82" s="30"/>
+      <c r="K82" s="30"/>
+      <c r="L82" s="31"/>
+      <c r="M82" s="31"/>
+      <c r="N82" s="31"/>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="32"/>
+      <c r="R82" s="33">
+        <v>0</v>
+      </c>
+      <c r="S82" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="T82" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="U82" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="V82" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="W82" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="X82" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y82" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AA82" s="236" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB82" s="237" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC82" s="238" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD82" s="238" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE82" s="239" t="s">
-        <v>308</v>
-      </c>
-      <c r="AF82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH82" s="239">
+      <c r="AA82" s="21">
+        <v>10</v>
+      </c>
+      <c r="AB82" s="167" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC82" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD82" s="37">
+        <v>2880</v>
+      </c>
+      <c r="AE82" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="AF82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH82" s="13">
         <v>2</v>
       </c>
-      <c r="AI82" s="240" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS82" s="240" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW82" s="241" t="s">
-        <v>327</v>
-      </c>
-      <c r="AX82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY82" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ82" s="239" t="s">
+      <c r="AI82" s="130" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ82" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS82" s="130" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW82" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="AX82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ82" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="83" spans="2:52">
-      <c r="B83" s="219" t="s">
+      <c r="B83" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C83" s="226" t="s">
-        <v>313</v>
-      </c>
-      <c r="D83" s="219" t="s">
-        <v>126</v>
-      </c>
-      <c r="E83" s="219" t="s">
-        <v>299</v>
-      </c>
-      <c r="F83" s="227" t="b">
-        <v>1</v>
-      </c>
-      <c r="G83" s="227">
-        <v>-1</v>
-      </c>
-      <c r="H83" s="228" t="s">
-        <v>126</v>
-      </c>
-      <c r="I83" s="228" t="s">
-        <v>12</v>
-      </c>
-      <c r="J83" s="228">
-        <v>1000</v>
-      </c>
-      <c r="K83" s="228" t="s">
-        <v>126</v>
-      </c>
-      <c r="L83" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="M83" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="N83" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="O83" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="P83" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q83" s="230" t="s">
-        <v>126</v>
-      </c>
-      <c r="R83" s="231">
-        <v>-25</v>
-      </c>
-      <c r="S83" s="232" t="s">
-        <v>126</v>
-      </c>
-      <c r="T83" s="232" t="s">
-        <v>309</v>
-      </c>
-      <c r="U83" s="233" t="s">
-        <v>126</v>
-      </c>
-      <c r="V83" s="234" t="s">
-        <v>126</v>
-      </c>
-      <c r="W83" s="235" t="s">
-        <v>312</v>
-      </c>
-      <c r="X83" s="236" t="b">
+      <c r="C83" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E83" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F83" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="29">
+        <v>1</v>
+      </c>
+      <c r="H83" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="J83" s="30">
+        <v>1</v>
+      </c>
+      <c r="K83" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="L83" s="129" t="s">
+        <v>17</v>
+      </c>
+      <c r="M83" s="129">
+        <v>1</v>
+      </c>
+      <c r="N83" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="O83" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="P83" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="R83" s="33">
+        <v>-16</v>
+      </c>
+      <c r="S83" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="T83" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="U83" s="200" t="s">
+        <v>292</v>
+      </c>
+      <c r="V83" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="W83" s="276" t="s">
+        <v>359</v>
+      </c>
+      <c r="X83" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y83" s="21">
         <v>0</v>
       </c>
-      <c r="Y83" s="236" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z83" s="236" t="s">
+      <c r="Z83" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AA83" s="236" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB83" s="237" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC83" s="238" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD83" s="238" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE83" s="239" t="s">
-        <v>308</v>
-      </c>
-      <c r="AF83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH83" s="239">
-        <v>2</v>
-      </c>
-      <c r="AI83" s="240" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS83" s="240" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW83" s="241" t="s">
+      <c r="AA83" s="21">
+        <v>10</v>
+      </c>
+      <c r="AB83" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC83" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD83" s="37">
+        <v>2880</v>
+      </c>
+      <c r="AE83" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="AF83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH83" s="13">
+        <v>3</v>
+      </c>
+      <c r="AI83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP83" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="AQ83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW83" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="AX83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY83" s="239" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ83" s="239" t="s">
+      <c r="AX83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ83" s="13" t="s">
         <v>126</v>
       </c>
     </row>
@@ -17787,7 +17827,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="226" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D84" s="219" t="s">
         <v>126</v>
@@ -17799,19 +17839,19 @@
         <v>1</v>
       </c>
       <c r="G84" s="227">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H84" s="228" t="s">
         <v>126</v>
       </c>
       <c r="I84" s="228" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J84" s="228">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K84" s="228" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="L84" s="229" t="s">
         <v>126</v>
@@ -17938,366 +17978,384 @@
       </c>
     </row>
     <row r="85" spans="2:52">
-      <c r="B85" s="242" t="s">
+      <c r="B85" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="C85" s="243" t="s">
-        <v>315</v>
-      </c>
-      <c r="D85" s="242" t="s">
-        <v>126</v>
-      </c>
-      <c r="E85" s="242" t="s">
+      <c r="C85" s="226" t="s">
+        <v>313</v>
+      </c>
+      <c r="D85" s="219" t="s">
+        <v>126</v>
+      </c>
+      <c r="E85" s="219" t="s">
         <v>299</v>
       </c>
-      <c r="F85" s="244" t="b">
-        <v>1</v>
-      </c>
-      <c r="G85" s="244">
+      <c r="F85" s="227" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" s="227">
         <v>-1</v>
       </c>
-      <c r="H85" s="245" t="s">
-        <v>126</v>
-      </c>
-      <c r="I85" s="245" t="s">
-        <v>17</v>
-      </c>
-      <c r="J85" s="245">
-        <v>1</v>
-      </c>
-      <c r="K85" s="245" t="s">
-        <v>160</v>
-      </c>
-      <c r="L85" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="M85" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="N85" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="O85" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="P85" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q85" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="R85" s="248">
+      <c r="H85" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="I85" s="228" t="s">
+        <v>12</v>
+      </c>
+      <c r="J85" s="228">
+        <v>1000</v>
+      </c>
+      <c r="K85" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="L85" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="M85" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="N85" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="O85" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="P85" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q85" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="R85" s="231">
         <v>-25</v>
       </c>
-      <c r="S85" s="249" t="s">
-        <v>126</v>
-      </c>
-      <c r="T85" s="249" t="s">
+      <c r="S85" s="232" t="s">
+        <v>126</v>
+      </c>
+      <c r="T85" s="232" t="s">
         <v>309</v>
       </c>
-      <c r="U85" s="250" t="s">
-        <v>126</v>
-      </c>
-      <c r="V85" s="251" t="s">
-        <v>126</v>
-      </c>
-      <c r="W85" s="252" t="s">
+      <c r="U85" s="233" t="s">
+        <v>126</v>
+      </c>
+      <c r="V85" s="234" t="s">
+        <v>126</v>
+      </c>
+      <c r="W85" s="235" t="s">
         <v>312</v>
       </c>
-      <c r="X85" s="253" t="b">
+      <c r="X85" s="236" t="b">
         <v>0</v>
       </c>
-      <c r="Y85" s="253" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z85" s="253" t="s">
+      <c r="Y85" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z85" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="AA85" s="253" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB85" s="254" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC85" s="255" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD85" s="255" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE85" s="256" t="s">
+      <c r="AA85" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB85" s="237" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC85" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD85" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE85" s="239" t="s">
         <v>308</v>
       </c>
-      <c r="AF85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH85" s="256">
+      <c r="AF85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH85" s="239">
         <v>2</v>
       </c>
-      <c r="AI85" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS85" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW85" s="258" t="s">
+      <c r="AI85" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS85" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW85" s="241" t="s">
         <v>327</v>
       </c>
-      <c r="AX85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY85" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ85" s="256" t="s">
+      <c r="AX85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY85" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ85" s="239" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="86" spans="2:52">
-      <c r="B86" s="242" t="s">
+      <c r="B86" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="243" t="s">
-        <v>316</v>
-      </c>
-      <c r="D86" s="242" t="s">
-        <v>126</v>
-      </c>
-      <c r="E86" s="242" t="s">
+      <c r="C86" s="226" t="s">
+        <v>314</v>
+      </c>
+      <c r="D86" s="219" t="s">
+        <v>126</v>
+      </c>
+      <c r="E86" s="219" t="s">
         <v>299</v>
       </c>
-      <c r="F86" s="244" t="b">
-        <v>1</v>
-      </c>
-      <c r="G86" s="244">
+      <c r="F86" s="227" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="227">
         <v>-1</v>
       </c>
-      <c r="H86" s="245" t="s">
-        <v>126</v>
-      </c>
-      <c r="I86" s="245" t="s">
-        <v>12</v>
-      </c>
-      <c r="J86" s="245">
-        <v>2000</v>
-      </c>
-      <c r="K86" s="245" t="s">
-        <v>126</v>
-      </c>
-      <c r="L86" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="M86" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="N86" s="246" t="s">
-        <v>126</v>
-      </c>
-      <c r="O86" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="P86" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q86" s="247" t="s">
-        <v>126</v>
-      </c>
-      <c r="R86" s="248">
+      <c r="H86" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="I86" s="228" t="s">
+        <v>10</v>
+      </c>
+      <c r="J86" s="228">
+        <v>2</v>
+      </c>
+      <c r="K86" s="228" t="s">
+        <v>126</v>
+      </c>
+      <c r="L86" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="M86" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="N86" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="O86" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="P86" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q86" s="230" t="s">
+        <v>126</v>
+      </c>
+      <c r="R86" s="231">
         <v>-25</v>
       </c>
-      <c r="S86" s="249" t="s">
-        <v>126</v>
-      </c>
-      <c r="T86" s="249" t="s">
+      <c r="S86" s="232" t="s">
+        <v>126</v>
+      </c>
+      <c r="T86" s="232" t="s">
         <v>309</v>
       </c>
-      <c r="U86" s="250" t="s">
-        <v>126</v>
-      </c>
-      <c r="V86" s="251" t="s">
-        <v>126</v>
-      </c>
-      <c r="W86" s="252" t="s">
+      <c r="U86" s="233" t="s">
+        <v>126</v>
+      </c>
+      <c r="V86" s="234" t="s">
+        <v>126</v>
+      </c>
+      <c r="W86" s="235" t="s">
         <v>312</v>
       </c>
-      <c r="X86" s="253" t="b">
+      <c r="X86" s="236" t="b">
         <v>0</v>
       </c>
-      <c r="Y86" s="253" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z86" s="253" t="s">
+      <c r="Y86" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z86" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="AA86" s="253" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB86" s="254" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC86" s="255" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD86" s="255" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE86" s="256" t="s">
+      <c r="AA86" s="236" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB86" s="237" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC86" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD86" s="238" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE86" s="239" t="s">
         <v>308</v>
       </c>
-      <c r="AF86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH86" s="256">
+      <c r="AF86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH86" s="239">
         <v>2</v>
       </c>
-      <c r="AI86" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS86" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW86" s="258" t="s">
+      <c r="AI86" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS86" s="240" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW86" s="241" t="s">
         <v>327</v>
       </c>
-      <c r="AX86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY86" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ86" s="256" t="s">
+      <c r="AX86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY86" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ86" s="239" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="2:52" hidden="1">
+    <row r="87" spans="2:52">
       <c r="B87" s="242" t="s">
         <v>2</v>
       </c>
       <c r="C87" s="243" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="D87" s="242" t="s">
         <v>126</v>
       </c>
       <c r="E87" s="242" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="F87" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="244">
+        <v>-1</v>
+      </c>
+      <c r="H87" s="245" t="s">
+        <v>126</v>
+      </c>
+      <c r="I87" s="245" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="245">
+        <v>1</v>
+      </c>
+      <c r="K87" s="245" t="s">
+        <v>160</v>
+      </c>
+      <c r="L87" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="M87" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="N87" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="O87" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="P87" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q87" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="R87" s="248">
+        <v>-25</v>
+      </c>
+      <c r="S87" s="249" t="s">
+        <v>126</v>
+      </c>
+      <c r="T87" s="249" t="s">
+        <v>309</v>
+      </c>
+      <c r="U87" s="250" t="s">
+        <v>126</v>
+      </c>
+      <c r="V87" s="251" t="s">
+        <v>126</v>
+      </c>
+      <c r="W87" s="252" t="s">
+        <v>312</v>
+      </c>
+      <c r="X87" s="253" t="b">
         <v>0</v>
-      </c>
-      <c r="G87" s="244">
-        <v>1</v>
-      </c>
-      <c r="H87" s="245" t="s">
-        <v>126</v>
-      </c>
-      <c r="I87" s="245"/>
-      <c r="J87" s="245"/>
-      <c r="K87" s="245"/>
-      <c r="L87" s="246"/>
-      <c r="M87" s="246"/>
-      <c r="N87" s="246"/>
-      <c r="O87" s="247"/>
-      <c r="P87" s="247"/>
-      <c r="Q87" s="247"/>
-      <c r="R87" s="33">
-        <v>0</v>
-      </c>
-      <c r="S87" s="249" t="s">
-        <v>340</v>
-      </c>
-      <c r="T87" s="249" t="s">
-        <v>298</v>
-      </c>
-      <c r="U87" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="V87" s="251" t="s">
-        <v>341</v>
-      </c>
-      <c r="W87" s="252" t="s">
-        <v>331</v>
-      </c>
-      <c r="X87" s="253" t="b">
-        <v>1</v>
       </c>
       <c r="Y87" s="253" t="s">
         <v>126</v>
@@ -18327,7 +18385,7 @@
         <v>126</v>
       </c>
       <c r="AH87" s="256">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI87" s="257" t="s">
         <v>126</v>
@@ -18372,7 +18430,7 @@
         <v>126</v>
       </c>
       <c r="AW87" s="258" t="s">
-        <v>126</v>
+        <v>327</v>
       </c>
       <c r="AX87" s="256" t="s">
         <v>126</v>
@@ -18384,57 +18442,75 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="2:52" hidden="1">
+    <row r="88" spans="2:52">
       <c r="B88" s="242" t="s">
         <v>2</v>
       </c>
       <c r="C88" s="243" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="D88" s="242" t="s">
         <v>126</v>
       </c>
       <c r="E88" s="242" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="F88" s="244" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" s="244">
+        <v>-1</v>
+      </c>
+      <c r="H88" s="245" t="s">
+        <v>126</v>
+      </c>
+      <c r="I88" s="245" t="s">
+        <v>12</v>
+      </c>
+      <c r="J88" s="245">
+        <v>2000</v>
+      </c>
+      <c r="K88" s="245" t="s">
+        <v>126</v>
+      </c>
+      <c r="L88" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="M88" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="N88" s="246" t="s">
+        <v>126</v>
+      </c>
+      <c r="O88" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="P88" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q88" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="R88" s="248">
+        <v>-25</v>
+      </c>
+      <c r="S88" s="249" t="s">
+        <v>126</v>
+      </c>
+      <c r="T88" s="249" t="s">
+        <v>309</v>
+      </c>
+      <c r="U88" s="250" t="s">
+        <v>126</v>
+      </c>
+      <c r="V88" s="251" t="s">
+        <v>126</v>
+      </c>
+      <c r="W88" s="252" t="s">
+        <v>312</v>
+      </c>
+      <c r="X88" s="253" t="b">
         <v>0</v>
-      </c>
-      <c r="G88" s="244">
-        <v>1</v>
-      </c>
-      <c r="H88" s="245" t="s">
-        <v>126</v>
-      </c>
-      <c r="I88" s="245"/>
-      <c r="J88" s="245"/>
-      <c r="K88" s="245"/>
-      <c r="L88" s="246"/>
-      <c r="M88" s="246"/>
-      <c r="N88" s="246"/>
-      <c r="O88" s="247"/>
-      <c r="P88" s="247"/>
-      <c r="Q88" s="247"/>
-      <c r="R88" s="33">
-        <v>0</v>
-      </c>
-      <c r="S88" s="249" t="s">
-        <v>100</v>
-      </c>
-      <c r="T88" s="249" t="s">
-        <v>298</v>
-      </c>
-      <c r="U88" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="V88" s="251" t="s">
-        <v>343</v>
-      </c>
-      <c r="W88" s="252" t="s">
-        <v>331</v>
-      </c>
-      <c r="X88" s="253" t="b">
-        <v>1</v>
       </c>
       <c r="Y88" s="253" t="s">
         <v>126</v>
@@ -18464,120 +18540,394 @@
         <v>126</v>
       </c>
       <c r="AH88" s="256">
+        <v>2</v>
+      </c>
+      <c r="AI88" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS88" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW88" s="258" t="s">
+        <v>327</v>
+      </c>
+      <c r="AX88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY88" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ88" s="256" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="2:52" hidden="1">
+      <c r="B89" s="242" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="243" t="s">
+        <v>339</v>
+      </c>
+      <c r="D89" s="242" t="s">
+        <v>126</v>
+      </c>
+      <c r="E89" s="242" t="s">
+        <v>328</v>
+      </c>
+      <c r="F89" s="244" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" s="244">
+        <v>1</v>
+      </c>
+      <c r="H89" s="245" t="s">
+        <v>126</v>
+      </c>
+      <c r="I89" s="245"/>
+      <c r="J89" s="245"/>
+      <c r="K89" s="245"/>
+      <c r="L89" s="246"/>
+      <c r="M89" s="246"/>
+      <c r="N89" s="246"/>
+      <c r="O89" s="247"/>
+      <c r="P89" s="247"/>
+      <c r="Q89" s="247"/>
+      <c r="R89" s="33">
+        <v>0</v>
+      </c>
+      <c r="S89" s="249" t="s">
+        <v>340</v>
+      </c>
+      <c r="T89" s="249" t="s">
+        <v>298</v>
+      </c>
+      <c r="U89" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="V89" s="251" t="s">
+        <v>341</v>
+      </c>
+      <c r="W89" s="252" t="s">
+        <v>331</v>
+      </c>
+      <c r="X89" s="253" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y89" s="253" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z89" s="253" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA89" s="253" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB89" s="254" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC89" s="255" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD89" s="255" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE89" s="256" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH89" s="256">
         <v>4</v>
       </c>
-      <c r="AI88" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS88" s="257" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW88" s="258" t="s">
-        <v>126</v>
-      </c>
-      <c r="AX88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY88" s="256" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ88" s="256" t="s">
+      <c r="AI89" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS89" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW89" s="258" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY89" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ89" s="256" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="2:52" ht="26.25">
-      <c r="B90" s="266" t="s">
+    <row r="90" spans="2:52" hidden="1">
+      <c r="B90" s="242" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="243" t="s">
+        <v>342</v>
+      </c>
+      <c r="D90" s="242" t="s">
+        <v>126</v>
+      </c>
+      <c r="E90" s="242" t="s">
+        <v>328</v>
+      </c>
+      <c r="F90" s="244" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="244">
+        <v>1</v>
+      </c>
+      <c r="H90" s="245" t="s">
+        <v>126</v>
+      </c>
+      <c r="I90" s="245"/>
+      <c r="J90" s="245"/>
+      <c r="K90" s="245"/>
+      <c r="L90" s="246"/>
+      <c r="M90" s="246"/>
+      <c r="N90" s="246"/>
+      <c r="O90" s="247"/>
+      <c r="P90" s="247"/>
+      <c r="Q90" s="247"/>
+      <c r="R90" s="33">
+        <v>0</v>
+      </c>
+      <c r="S90" s="249" t="s">
+        <v>100</v>
+      </c>
+      <c r="T90" s="249" t="s">
+        <v>298</v>
+      </c>
+      <c r="U90" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="V90" s="251" t="s">
+        <v>343</v>
+      </c>
+      <c r="W90" s="252" t="s">
+        <v>331</v>
+      </c>
+      <c r="X90" s="253" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y90" s="253" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z90" s="253" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA90" s="253" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB90" s="254" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC90" s="255" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD90" s="255" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE90" s="256" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH90" s="256">
+        <v>4</v>
+      </c>
+      <c r="AI90" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS90" s="257" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW90" s="258" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY90" s="256" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ90" s="256" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="2:52" ht="26.25">
+      <c r="B92" s="284" t="s">
         <v>317</v>
       </c>
-      <c r="C90" s="266"/>
-      <c r="D90" s="266"/>
-      <c r="E90" s="266"/>
+      <c r="C92" s="284"/>
+      <c r="D92" s="284"/>
+      <c r="E92" s="284"/>
     </row>
-    <row r="92" spans="2:52" ht="135">
-      <c r="B92" s="23" t="s">
+    <row r="94" spans="2:52" ht="135">
+      <c r="B94" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="C92" s="223" t="s">
+      <c r="C94" s="223" t="s">
         <v>0</v>
       </c>
-      <c r="D92" s="224" t="s">
+      <c r="D94" s="224" t="s">
         <v>52</v>
       </c>
-      <c r="E92" s="23" t="s">
+      <c r="E94" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="F92" s="224" t="s">
+      <c r="F94" s="224" t="s">
         <v>320</v>
       </c>
-      <c r="G92" s="225" t="s">
+      <c r="G94" s="225" t="s">
         <v>321</v>
       </c>
-      <c r="H92" s="225" t="s">
+      <c r="H94" s="225" t="s">
         <v>322</v>
       </c>
-      <c r="I92" s="225" t="s">
+      <c r="I94" s="225" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="93" spans="2:52">
-      <c r="B93" s="205" t="s">
+    <row r="95" spans="2:52">
+      <c r="B95" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="C93" s="205" t="s">
+      <c r="C95" s="205" t="s">
         <v>324</v>
       </c>
-      <c r="D93" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="205">
+      <c r="D95" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="205">
         <v>0</v>
       </c>
-      <c r="F93" s="205">
+      <c r="F95" s="205">
         <v>120</v>
       </c>
-      <c r="G93" s="205">
-        <v>1</v>
-      </c>
-      <c r="H93" s="205" t="s">
+      <c r="G95" s="205">
+        <v>1</v>
+      </c>
+      <c r="H95" s="205" t="s">
         <v>325</v>
       </c>
-      <c r="I93" s="205" t="s">
+      <c r="I95" s="205" t="s">
         <v>326</v>
       </c>
     </row>
@@ -18585,46 +18935,62 @@
   <mergeCells count="3">
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AD1:AY1"/>
-    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="B92:E92"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F88">
-    <cfRule type="containsText" dxfId="77" priority="9" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="F3:F74 F77:F90">
+    <cfRule type="containsText" dxfId="81" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="10" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="80" priority="14" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D93">
+  <conditionalFormatting sqref="D95">
+    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D95)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="12" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D95)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F89">
+    <cfRule type="containsText" dxfId="77" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F89)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="10" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F89)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F90">
     <cfRule type="containsText" dxfId="75" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",D93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F90)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",D93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F90)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87">
+  <conditionalFormatting sqref="F90">
     <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F87)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F90)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F87)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F90)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88">
+  <conditionalFormatting sqref="F75">
     <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F75)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="4" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F75)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88">
+  <conditionalFormatting sqref="F76">
     <cfRule type="containsText" dxfId="69" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F76)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18691,31 +19057,31 @@
       <c r="T1" s="5"/>
       <c r="U1" s="204"/>
       <c r="V1" s="204"/>
-      <c r="AA1" s="264"/>
-      <c r="AB1" s="264"/>
+      <c r="AA1" s="282"/>
+      <c r="AB1" s="282"/>
       <c r="AC1" s="201"/>
-      <c r="AD1" s="265"/>
-      <c r="AE1" s="265"/>
-      <c r="AF1" s="265"/>
-      <c r="AG1" s="265"/>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
-      <c r="AK1" s="265"/>
-      <c r="AL1" s="265"/>
-      <c r="AM1" s="265"/>
-      <c r="AN1" s="265"/>
-      <c r="AO1" s="265"/>
-      <c r="AP1" s="265"/>
-      <c r="AQ1" s="265"/>
-      <c r="AR1" s="265"/>
-      <c r="AS1" s="265"/>
-      <c r="AT1" s="265"/>
-      <c r="AU1" s="265"/>
-      <c r="AV1" s="265"/>
-      <c r="AW1" s="265"/>
-      <c r="AX1" s="265"/>
-      <c r="AY1" s="265"/>
+      <c r="AD1" s="283"/>
+      <c r="AE1" s="283"/>
+      <c r="AF1" s="283"/>
+      <c r="AG1" s="283"/>
+      <c r="AH1" s="283"/>
+      <c r="AI1" s="283"/>
+      <c r="AJ1" s="283"/>
+      <c r="AK1" s="283"/>
+      <c r="AL1" s="283"/>
+      <c r="AM1" s="283"/>
+      <c r="AN1" s="283"/>
+      <c r="AO1" s="283"/>
+      <c r="AP1" s="283"/>
+      <c r="AQ1" s="283"/>
+      <c r="AR1" s="283"/>
+      <c r="AS1" s="283"/>
+      <c r="AT1" s="283"/>
+      <c r="AU1" s="283"/>
+      <c r="AV1" s="283"/>
+      <c r="AW1" s="283"/>
+      <c r="AX1" s="283"/>
+      <c r="AY1" s="283"/>
     </row>
     <row r="2" spans="2:51" ht="190.5" customHeight="1">
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
changed remove ads offer title to "VIP OFFER"
Former-commit-id: 3b6b38cde6eb1d0a030ca256fadf0b45bfa9cd3d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="379">
   <si>
     <t>[sku]</t>
   </si>
@@ -1161,6 +1161,9 @@
   </si>
   <si>
     <t>0.01</t>
+  </si>
+  <si>
+    <t>TID_REMOVE_ADS_REWARD_TITLE</t>
   </si>
 </sst>
 </file>
@@ -5984,9 +5987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V75" sqref="V75"/>
+      <selection pane="bottomLeft" activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16415,7 +16418,7 @@
         <v>330</v>
       </c>
       <c r="W74" s="235" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="X74" s="236" t="b">
         <v>1</v>
@@ -16570,7 +16573,7 @@
         <v>341</v>
       </c>
       <c r="W75" s="235" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="X75" s="236" t="b">
         <v>1</v>
@@ -16725,7 +16728,7 @@
         <v>343</v>
       </c>
       <c r="W76" s="235" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="X76" s="236" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Featured column set on FALSE for the remove ads offer!
Former-commit-id: 36735c985ad543cb38c2a5b37803d5333c944290
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5987,9 +5987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W75" sqref="W75"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W82" sqref="W82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16421,7 +16421,7 @@
         <v>378</v>
       </c>
       <c r="X74" s="236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y74" s="236" t="s">
         <v>126</v>
@@ -16576,7 +16576,7 @@
         <v>378</v>
       </c>
       <c r="X75" s="236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y75" s="236" t="s">
         <v>126</v>
@@ -16731,7 +16731,7 @@
         <v>378</v>
       </c>
       <c r="X76" s="236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y76" s="236" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Setting minAppVersion to 2.4
Former-commit-id: 5553b549496bd7be3445236760dfceee50b57558
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="380">
   <si>
     <t>[sku]</t>
   </si>
@@ -1164,6 +1164,9 @@
   </si>
   <si>
     <t>TID_REMOVE_ADS_REWARD_TITLE</t>
+  </si>
+  <si>
+    <t>2.4</t>
   </si>
 </sst>
 </file>
@@ -5987,9 +5990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W82" sqref="W82"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE77" sqref="AE77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16442,7 +16445,7 @@
         <v>126</v>
       </c>
       <c r="AE74" s="239" t="s">
-        <v>308</v>
+        <v>379</v>
       </c>
       <c r="AF74" s="239" t="s">
         <v>126</v>
@@ -16597,7 +16600,7 @@
         <v>126</v>
       </c>
       <c r="AE75" s="239" t="s">
-        <v>308</v>
+        <v>379</v>
       </c>
       <c r="AF75" s="239" t="s">
         <v>126</v>
@@ -16752,7 +16755,7 @@
         <v>126</v>
       </c>
       <c r="AE76" s="239" t="s">
-        <v>308</v>
+        <v>379</v>
       </c>
       <c r="AF76" s="239" t="s">
         <v>126</v>
@@ -19010,7 +19013,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Removed filter to hide offers set to false
Former-commit-id: f071f067e8f9b87dc059b20007adc75f3867d4c0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -2639,147 +2639,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <font>
         <b val="0"/>
@@ -5575,6 +5435,86 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5603,86 +5543,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ88" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79">
-  <autoFilter ref="B2:AZ88">
-    <filterColumn colId="4">
-      <colorFilter dxfId="78"/>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="B24:AZ86">
-    <sortCondition descending="1" ref="E2:E88"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ88" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B2:AZ88"/>
   <tableColumns count="51">
-    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="77"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
-    <tableColumn id="45" name="[uniqueId]" dataDxfId="75"/>
-    <tableColumn id="49" name="[type]" dataDxfId="74"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="73"/>
-    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="72"/>
-    <tableColumn id="38" name="[item1Featured]" dataDxfId="71"/>
-    <tableColumn id="4" name="[item1Type]" dataDxfId="70"/>
-    <tableColumn id="37" name="[item1Amount]" dataDxfId="69"/>
-    <tableColumn id="40" name="[item1Sku]" dataDxfId="68"/>
-    <tableColumn id="5" name="[item2Type]" dataDxfId="67"/>
-    <tableColumn id="41" name="[item2Amount]" dataDxfId="66"/>
-    <tableColumn id="42" name="[item2Sku]" dataDxfId="65"/>
-    <tableColumn id="6" name="[item3Type]" dataDxfId="64"/>
-    <tableColumn id="43" name="[item3Amount]" dataDxfId="63"/>
-    <tableColumn id="44" name="[item3Sku]" dataDxfId="62"/>
-    <tableColumn id="7" name="[order]" dataDxfId="61"/>
-    <tableColumn id="8" name="[refPrice]" dataDxfId="60"/>
-    <tableColumn id="51" name="[currency]" dataDxfId="59"/>
-    <tableColumn id="9" name="[discount]" dataDxfId="58"/>
-    <tableColumn id="10" name="[iapSku]" dataDxfId="57"/>
-    <tableColumn id="11" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="12" name="[featured]" dataDxfId="55"/>
-    <tableColumn id="13" name="[maxViews]" dataDxfId="54"/>
-    <tableColumn id="14" name="[zone]" dataDxfId="53"/>
-    <tableColumn id="15" name="[frequency]" dataDxfId="52"/>
-    <tableColumn id="16" name="[startDate]" dataDxfId="51"/>
-    <tableColumn id="17" name="[endDate]" dataDxfId="50"/>
-    <tableColumn id="46" name="[durationMinutes]" dataDxfId="49"/>
-    <tableColumn id="18" name="[minAppVersion]" dataDxfId="48"/>
-    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="47"/>
-    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="46"/>
-    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="45"/>
-    <tableColumn id="22" name="[payerType]" dataDxfId="44"/>
-    <tableColumn id="23" name="[minSpent]" dataDxfId="43"/>
-    <tableColumn id="50" name="[maxSpent]" dataDxfId="42"/>
-    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="41"/>
-    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="40"/>
-    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="39"/>
-    <tableColumn id="25" name="[dragonOwned]" dataDxfId="38"/>
-    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="37"/>
-    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="36"/>
-    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="35"/>
-    <tableColumn id="29" name="[openedEggs]" dataDxfId="34"/>
-    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="33"/>
-    <tableColumn id="31" name="[petsOwned]" dataDxfId="32"/>
-    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="31"/>
-    <tableColumn id="33" name="[progressionRange]" dataDxfId="30"/>
-    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="29"/>
-    <tableColumn id="35" name="[skinsOwned]" dataDxfId="28"/>
-    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="27"/>
+    <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="63"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="62"/>
+    <tableColumn id="45" name="[uniqueId]" dataDxfId="61"/>
+    <tableColumn id="49" name="[type]" dataDxfId="60"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="59"/>
+    <tableColumn id="39" name="[purchaseLimit]" dataDxfId="58"/>
+    <tableColumn id="38" name="[item1Featured]" dataDxfId="57"/>
+    <tableColumn id="4" name="[item1Type]" dataDxfId="56"/>
+    <tableColumn id="37" name="[item1Amount]" dataDxfId="55"/>
+    <tableColumn id="40" name="[item1Sku]" dataDxfId="54"/>
+    <tableColumn id="5" name="[item2Type]" dataDxfId="53"/>
+    <tableColumn id="41" name="[item2Amount]" dataDxfId="52"/>
+    <tableColumn id="42" name="[item2Sku]" dataDxfId="51"/>
+    <tableColumn id="6" name="[item3Type]" dataDxfId="50"/>
+    <tableColumn id="43" name="[item3Amount]" dataDxfId="49"/>
+    <tableColumn id="44" name="[item3Sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[order]" dataDxfId="47"/>
+    <tableColumn id="8" name="[refPrice]" dataDxfId="46"/>
+    <tableColumn id="51" name="[currency]" dataDxfId="45"/>
+    <tableColumn id="9" name="[discount]" dataDxfId="44"/>
+    <tableColumn id="10" name="[iapSku]" dataDxfId="43"/>
+    <tableColumn id="11" name="[tidName]" dataDxfId="42"/>
+    <tableColumn id="12" name="[featured]" dataDxfId="41"/>
+    <tableColumn id="13" name="[maxViews]" dataDxfId="40"/>
+    <tableColumn id="14" name="[zone]" dataDxfId="39"/>
+    <tableColumn id="15" name="[frequency]" dataDxfId="38"/>
+    <tableColumn id="16" name="[startDate]" dataDxfId="37"/>
+    <tableColumn id="17" name="[endDate]" dataDxfId="36"/>
+    <tableColumn id="46" name="[durationMinutes]" dataDxfId="35"/>
+    <tableColumn id="18" name="[minAppVersion]" dataDxfId="34"/>
+    <tableColumn id="19" name="[countriesAllowed]" dataDxfId="33"/>
+    <tableColumn id="20" name="[countriesExcluded]" dataDxfId="32"/>
+    <tableColumn id="21" name="[gamesPlayed]" dataDxfId="31"/>
+    <tableColumn id="22" name="[payerType]" dataDxfId="30"/>
+    <tableColumn id="23" name="[minSpent]" dataDxfId="29"/>
+    <tableColumn id="50" name="[maxSpent]" dataDxfId="28"/>
+    <tableColumn id="47" name="[minNumberOfPurchases]" dataDxfId="27"/>
+    <tableColumn id="48" name="[minutesSinceLastPurchase]" dataDxfId="26"/>
+    <tableColumn id="24" name="[dragonUnlocked]" dataDxfId="25"/>
+    <tableColumn id="25" name="[dragonOwned]" dataDxfId="24"/>
+    <tableColumn id="26" name="[dragonNotOwned]" dataDxfId="23"/>
+    <tableColumn id="27" name="[scBalanceRange]" dataDxfId="22"/>
+    <tableColumn id="28" name="[hcBalanceRange]" dataDxfId="21"/>
+    <tableColumn id="29" name="[openedEggs]" dataDxfId="20"/>
+    <tableColumn id="30" name="[petsOwnedCount]" dataDxfId="19"/>
+    <tableColumn id="31" name="[petsOwned]" dataDxfId="18"/>
+    <tableColumn id="32" name="[petsNotOwned]" dataDxfId="17"/>
+    <tableColumn id="33" name="[progressionRange]" dataDxfId="16"/>
+    <tableColumn id="34" name="[skinsUnlocked]" dataDxfId="15"/>
+    <tableColumn id="35" name="[skinsOwned]" dataDxfId="14"/>
+    <tableColumn id="36" name="[skinsNotOwned]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="offerPacksDefinitions2" displayName="offerPacksDefinitions2" ref="B2:K3" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B2:K3"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{offerSettings}" dataDxfId="23"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="22"/>
-    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="21"/>
-    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="20"/>
-    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="19"/>
-    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="18"/>
-    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="17"/>
-    <tableColumn id="6" name="[emptyValue]" dataDxfId="16"/>
-    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="15"/>
-    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="14"/>
+    <tableColumn id="1" name="{offerSettings}" dataDxfId="9"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="45" name="[refreshFrequency]" dataDxfId="7"/>
+    <tableColumn id="4" name="[rotationalActiveOffers]" dataDxfId="6"/>
+    <tableColumn id="5" name="[rotationalHistorySize]" dataDxfId="5"/>
+    <tableColumn id="49" name="[freeHistorySize]" dataDxfId="4"/>
+    <tableColumn id="3" name="[freeCooldownMinutes]" dataDxfId="3"/>
+    <tableColumn id="6" name="[emptyValue]" dataDxfId="2"/>
+    <tableColumn id="7" name="[interstitialsBeforeFirstNoAdsPopup]" dataDxfId="1"/>
+    <tableColumn id="8" name="[interstitialsBetweenNoAdsPopup]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5987,9 +5920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6235,7 +6168,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:52" hidden="1">
+    <row r="3" spans="2:52">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -6372,7 +6305,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="2:52" hidden="1">
+    <row r="4" spans="2:52">
       <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
@@ -6509,7 +6442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:52" hidden="1">
+    <row r="5" spans="2:52">
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -6646,7 +6579,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="2:52" hidden="1">
+    <row r="6" spans="2:52">
       <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
@@ -6783,7 +6716,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="2:52" hidden="1">
+    <row r="7" spans="2:52">
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -6920,7 +6853,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="2:52" hidden="1">
+    <row r="8" spans="2:52">
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -7057,7 +6990,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="2:52" hidden="1">
+    <row r="9" spans="2:52">
       <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
@@ -7194,7 +7127,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="2:52" hidden="1">
+    <row r="10" spans="2:52">
       <c r="B10" s="98" t="s">
         <v>2</v>
       </c>
@@ -7331,7 +7264,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="2:52" hidden="1">
+    <row r="11" spans="2:52">
       <c r="B11" s="96" t="s">
         <v>2</v>
       </c>
@@ -7468,7 +7401,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="2:52" hidden="1">
+    <row r="12" spans="2:52">
       <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
@@ -7605,7 +7538,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="2:52" hidden="1">
+    <row r="13" spans="2:52">
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -7742,7 +7675,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="2:52" hidden="1">
+    <row r="14" spans="2:52">
       <c r="B14" s="26" t="s">
         <v>2</v>
       </c>
@@ -7880,7 +7813,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="2:52" hidden="1">
+    <row r="15" spans="2:52">
       <c r="B15" s="27" t="s">
         <v>2</v>
       </c>
@@ -8017,7 +7950,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="2:52" hidden="1">
+    <row r="16" spans="2:52">
       <c r="B16" s="27" t="s">
         <v>2</v>
       </c>
@@ -8154,7 +8087,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="2:52" ht="16.5" hidden="1" thickBot="1">
+    <row r="17" spans="2:52" ht="16.5" thickBot="1">
       <c r="B17" s="115" t="s">
         <v>2</v>
       </c>
@@ -8291,7 +8224,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="2:52" hidden="1">
+    <row r="18" spans="2:52" ht="16.5" thickTop="1">
       <c r="B18" s="41" t="s">
         <v>2</v>
       </c>
@@ -8428,7 +8361,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:52" hidden="1">
+    <row r="19" spans="2:52">
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -8565,7 +8498,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="2:52" hidden="1">
+    <row r="20" spans="2:52">
       <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
@@ -8702,7 +8635,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:52" hidden="1">
+    <row r="21" spans="2:52">
       <c r="B21" s="27" t="s">
         <v>2</v>
       </c>
@@ -8839,7 +8772,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="2:52" hidden="1">
+    <row r="22" spans="2:52">
       <c r="B22" s="27" t="s">
         <v>2</v>
       </c>
@@ -8976,7 +8909,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="2:52" hidden="1">
+    <row r="23" spans="2:52">
       <c r="B23" s="27" t="s">
         <v>2</v>
       </c>
@@ -9266,7 +9199,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="2:52" hidden="1">
+    <row r="25" spans="2:52">
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -9403,7 +9336,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="2:52" hidden="1">
+    <row r="26" spans="2:52">
       <c r="B26" s="27" t="s">
         <v>2</v>
       </c>
@@ -9536,7 +9469,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="2:52" hidden="1">
+    <row r="27" spans="2:52">
       <c r="B27" s="27" t="s">
         <v>2</v>
       </c>
@@ -9673,7 +9606,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:52" hidden="1">
+    <row r="28" spans="2:52">
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -9810,7 +9743,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="2:52" hidden="1">
+    <row r="29" spans="2:52">
       <c r="B29" s="26" t="s">
         <v>2</v>
       </c>
@@ -9947,7 +9880,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="2:52" hidden="1">
+    <row r="30" spans="2:52">
       <c r="B30" s="27" t="s">
         <v>2</v>
       </c>
@@ -10084,7 +10017,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="2:52" hidden="1">
+    <row r="31" spans="2:52">
       <c r="B31" s="27" t="s">
         <v>2</v>
       </c>
@@ -10221,7 +10154,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="2:52" hidden="1">
+    <row r="32" spans="2:52">
       <c r="B32" s="27" t="s">
         <v>2</v>
       </c>
@@ -10358,7 +10291,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="2:52" hidden="1">
+    <row r="33" spans="2:52">
       <c r="B33" s="27" t="s">
         <v>2</v>
       </c>
@@ -10650,7 +10583,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="2:52" hidden="1">
+    <row r="35" spans="2:52">
       <c r="B35" s="26" t="s">
         <v>2</v>
       </c>
@@ -10787,7 +10720,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="2:52" hidden="1">
+    <row r="36" spans="2:52">
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
@@ -10924,7 +10857,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="2:52" hidden="1">
+    <row r="37" spans="2:52">
       <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
@@ -11061,7 +10994,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="2:52" hidden="1">
+    <row r="38" spans="2:52">
       <c r="B38" s="66" t="s">
         <v>2</v>
       </c>
@@ -11508,7 +11441,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="2:52" ht="16.5" thickBot="1">
+    <row r="41" spans="2:52">
       <c r="B41" s="26" t="s">
         <v>2</v>
       </c>
@@ -11663,7 +11596,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="2:52" ht="16.5" hidden="1" thickBot="1">
+    <row r="42" spans="2:52">
       <c r="B42" s="26" t="s">
         <v>2</v>
       </c>
@@ -11800,7 +11733,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="2:52" ht="16.5" hidden="1" thickBot="1">
+    <row r="43" spans="2:52">
       <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
@@ -11937,7 +11870,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="2:52" ht="16.5" hidden="1" thickBot="1">
+    <row r="44" spans="2:52" ht="16.5" thickBot="1">
       <c r="B44" s="66" t="s">
         <v>2</v>
       </c>
@@ -12384,7 +12317,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="2:52" hidden="1">
+    <row r="47" spans="2:52">
       <c r="B47" s="26" t="s">
         <v>2</v>
       </c>
@@ -12676,7 +12609,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="2:52" hidden="1">
+    <row r="49" spans="2:52">
       <c r="B49" s="26" t="s">
         <v>2</v>
       </c>
@@ -12968,7 +12901,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="2:52" hidden="1">
+    <row r="51" spans="2:52">
       <c r="B51" s="207" t="s">
         <v>2</v>
       </c>
@@ -13105,7 +13038,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:52" hidden="1">
+    <row r="52" spans="2:52">
       <c r="B52" s="26" t="s">
         <v>2</v>
       </c>
@@ -13552,7 +13485,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="2:52" hidden="1">
+    <row r="55" spans="2:52">
       <c r="B55" s="26" t="s">
         <v>2</v>
       </c>
@@ -13689,7 +13622,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="2:52">
+    <row r="56" spans="2:52" ht="16.5" thickBot="1">
       <c r="B56" s="66" t="s">
         <v>2</v>
       </c>
@@ -13844,7 +13777,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="2:52" s="199" customFormat="1" ht="17.25" hidden="1" thickTop="1" thickBot="1">
+    <row r="57" spans="2:52" s="199" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
       <c r="B57" s="208" t="s">
         <v>2</v>
       </c>
@@ -13981,7 +13914,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="2:52" hidden="1">
+    <row r="58" spans="2:52">
       <c r="B58" s="27" t="s">
         <v>2</v>
       </c>
@@ -14118,7 +14051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="2:52" hidden="1">
+    <row r="59" spans="2:52">
       <c r="B59" s="27" t="s">
         <v>2</v>
       </c>
@@ -14255,7 +14188,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="2:52" hidden="1">
+    <row r="60" spans="2:52">
       <c r="B60" s="27" t="s">
         <v>2</v>
       </c>
@@ -14857,7 +14790,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="2:52">
+    <row r="64" spans="2:52" ht="16.5" thickBot="1">
       <c r="B64" s="66" t="s">
         <v>2</v>
       </c>
@@ -15012,7 +14945,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="2:52" hidden="1">
+    <row r="65" spans="2:52">
       <c r="B65" s="155" t="s">
         <v>2</v>
       </c>
@@ -15149,7 +15082,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="2:52" hidden="1">
+    <row r="66" spans="2:52">
       <c r="B66" s="26" t="s">
         <v>2</v>
       </c>
@@ -18667,34 +18600,34 @@
     <mergeCell ref="B90:E90"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F74 F77:F88">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="75" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="74" priority="14" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",D93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F75">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="70" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F76">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="69" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F76)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Tweaked the progression and rotational offers!
Former-commit-id: 0749011ccbbc43f9fc39584aaf2e842e9c50ab7b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Offers.xlsx
+++ b/Docs/Content/HungryDragonContent_Offers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Settings" sheetId="4" r:id="rId2"/>
     <sheet name="ValidationData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3215" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3215" uniqueCount="376">
   <si>
     <t>[sku]</t>
   </si>
@@ -1094,21 +1094,9 @@
     <t>2.0</t>
   </si>
   <si>
-    <t>dragon_electic</t>
-  </si>
-  <si>
-    <t>dragon_blaze</t>
-  </si>
-  <si>
     <t>72:999</t>
   </si>
   <si>
-    <t>TID_STORE_PACK_PROMOTED1</t>
-  </si>
-  <si>
-    <t>dragon_chinese;dragon_classic</t>
-  </si>
-  <si>
     <t>dragon_chinese_2</t>
   </si>
   <si>
@@ -1164,6 +1152,9 @@
   </si>
   <si>
     <t>2.4</t>
+  </si>
+  <si>
+    <t>TID_STORE_PACK_PROGRESSIONPACK2</t>
   </si>
 </sst>
 </file>
@@ -2639,7 +2630,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="75">
     <dxf>
       <font>
         <b val="0"/>
@@ -5369,14 +5360,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -5543,7 +5526,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ88" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="offerPacksDefinitions" displayName="offerPacksDefinitions" ref="B2:AZ88" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="B2:AZ88"/>
   <tableColumns count="51">
     <tableColumn id="1" name="{offerPacksDefinitions}" dataDxfId="63"/>
@@ -5920,9 +5903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AZ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R80" sqref="R80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -9070,7 +9053,7 @@
         <v>10</v>
       </c>
       <c r="J24" s="30">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="K24" s="131" t="s">
         <v>126</v>
@@ -9079,7 +9062,7 @@
         <v>12</v>
       </c>
       <c r="M24" s="129">
-        <v>120000</v>
+        <v>150000</v>
       </c>
       <c r="N24" s="129" t="s">
         <v>126</v>
@@ -9187,7 +9170,7 @@
         <v>126</v>
       </c>
       <c r="AW24" s="20" t="s">
-        <v>171</v>
+        <v>327</v>
       </c>
       <c r="AX24" s="13" t="s">
         <v>126</v>
@@ -10571,7 +10554,7 @@
         <v>126</v>
       </c>
       <c r="AW34" s="20" t="s">
-        <v>171</v>
+        <v>327</v>
       </c>
       <c r="AX34" s="13" t="s">
         <v>126</v>
@@ -11274,7 +11257,7 @@
         <v>126</v>
       </c>
       <c r="AW39" s="20" t="s">
-        <v>171</v>
+        <v>327</v>
       </c>
       <c r="AX39" s="90" t="s">
         <v>126</v>
@@ -11315,7 +11298,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="30" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="L40" s="31" t="s">
         <v>49</v>
@@ -11324,7 +11307,7 @@
         <v>1</v>
       </c>
       <c r="N40" s="31" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="O40" s="32" t="s">
         <v>49</v>
@@ -1